<commit_message>
Continue implementing equivalent loads
</commit_message>
<xml_diff>
--- a/theory/FEM matriisit.xlsx
+++ b/theory/FEM matriisit.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ville\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ohjelmointi\2_Rust\idfem\theory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{759548A5-DADE-4612-84F7-0A10332A923C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DA3B9F8-1214-4D8A-AE58-AEAAAB67122B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-22230" yWindow="0" windowWidth="22335" windowHeight="20985" xr2:uid="{27180542-B0D2-4BFE-946B-7857B24C93C8}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -611,7 +611,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="155">
+  <cellXfs count="151">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1005,13 +1005,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="11" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1020,7 +1016,31 @@
     <cellStyle name="Neutraali" xfId="1" builtinId="28"/>
     <cellStyle name="Normaali" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -1050,59 +1070,6 @@
         <color auto="1"/>
       </font>
       <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1170,16 +1137,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>539263</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>456437</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>42241</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>604489</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>397565</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>14813</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1202,8 +1169,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4254013" y="133350"/>
-          <a:ext cx="1932126" cy="2676525"/>
+          <a:off x="6055480" y="340415"/>
+          <a:ext cx="5515324" cy="7526311"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1681,8 +1648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94F9BDF3-3EE6-4BFB-9734-CB047BC6E804}">
   <dimension ref="B1:CW233"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AG36" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AQ57" sqref="AQ57"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -2362,15 +2329,15 @@
         <v>0</v>
       </c>
       <c r="BD9" s="15">
-        <f>L20</f>
+        <f t="shared" ref="BD9:BF11" si="2">L20</f>
         <v>700000</v>
       </c>
       <c r="BE9" s="15">
-        <f>M20</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="BF9" s="15">
-        <f>N20</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="BG9" s="4">
@@ -2383,15 +2350,15 @@
         <v>0</v>
       </c>
       <c r="BJ9" s="15">
-        <f>O20</f>
+        <f t="shared" ref="BJ9:BL11" si="3">O20</f>
         <v>-700000</v>
       </c>
       <c r="BK9" s="15">
-        <f>P20</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="BL9" s="15">
-        <f>Q20</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="BM9" s="16"/>
@@ -2495,15 +2462,15 @@
         <v>0</v>
       </c>
       <c r="BD10" s="15">
-        <f>L21</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="BE10" s="15">
-        <f>M21</f>
+        <f t="shared" si="2"/>
         <v>777.77777777777783</v>
       </c>
       <c r="BF10" s="15">
-        <f>N21</f>
+        <f t="shared" si="2"/>
         <v>2333333.3333333335</v>
       </c>
       <c r="BG10" s="4">
@@ -2516,15 +2483,15 @@
         <v>0</v>
       </c>
       <c r="BJ10" s="15">
-        <f>O21</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="BK10" s="15">
-        <f>P21</f>
+        <f t="shared" si="3"/>
         <v>-777.77777777777783</v>
       </c>
       <c r="BL10" s="15">
-        <f>Q21</f>
+        <f t="shared" si="3"/>
         <v>2333333.3333333335</v>
       </c>
       <c r="BM10" s="16"/>
@@ -2627,15 +2594,15 @@
         <v>0</v>
       </c>
       <c r="BD11" s="15">
-        <f>L22</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="BE11" s="15">
-        <f>M22</f>
+        <f t="shared" si="2"/>
         <v>2333333.3333333335</v>
       </c>
       <c r="BF11" s="15">
-        <f>N22</f>
+        <f t="shared" si="2"/>
         <v>9333333333.333334</v>
       </c>
       <c r="BG11" s="4">
@@ -2648,15 +2615,15 @@
         <v>0</v>
       </c>
       <c r="BJ11" s="15">
-        <f>O22</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="BK11" s="15">
-        <f>P22</f>
+        <f t="shared" si="3"/>
         <v>-2333333.3333333335</v>
       </c>
       <c r="BL11" s="15">
-        <f>Q22</f>
+        <f t="shared" si="3"/>
         <v>4666666666.666667</v>
       </c>
       <c r="BM11" s="16"/>
@@ -3036,15 +3003,15 @@
         <v>0</v>
       </c>
       <c r="BD15" s="15">
-        <f>L23</f>
+        <f t="shared" ref="BD15:BF17" si="4">L23</f>
         <v>-700000</v>
       </c>
       <c r="BE15" s="15">
-        <f>M23</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="BF15" s="15">
-        <f>N23</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="BG15" s="4">
@@ -3057,15 +3024,15 @@
         <v>0</v>
       </c>
       <c r="BJ15" s="15">
-        <f>O23</f>
+        <f t="shared" ref="BJ15:BL17" si="5">O23</f>
         <v>700000</v>
       </c>
       <c r="BK15" s="15">
-        <f>P23</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="BL15" s="15">
-        <f>Q23</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="BM15" s="16"/>
@@ -3160,15 +3127,15 @@
         <v>0</v>
       </c>
       <c r="BD16" s="15">
-        <f>L24</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="BE16" s="15">
-        <f>M24</f>
+        <f t="shared" si="4"/>
         <v>-777.77777777777783</v>
       </c>
       <c r="BF16" s="15">
-        <f>N24</f>
+        <f t="shared" si="4"/>
         <v>-2333333.3333333335</v>
       </c>
       <c r="BG16" s="4">
@@ -3181,15 +3148,15 @@
         <v>0</v>
       </c>
       <c r="BJ16" s="15">
-        <f>O24</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="BK16" s="15">
-        <f>P24</f>
+        <f t="shared" si="5"/>
         <v>777.77777777777783</v>
       </c>
       <c r="BL16" s="15">
-        <f>Q24</f>
+        <f t="shared" si="5"/>
         <v>-2333333.3333333335</v>
       </c>
       <c r="BM16" s="16"/>
@@ -3252,15 +3219,15 @@
         <v>0</v>
       </c>
       <c r="BD17" s="15">
-        <f>L25</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="BE17" s="15">
-        <f>M25</f>
+        <f t="shared" si="4"/>
         <v>2333333.3333333335</v>
       </c>
       <c r="BF17" s="15">
-        <f>N25</f>
+        <f t="shared" si="4"/>
         <v>4666666666.666667</v>
       </c>
       <c r="BG17" s="4">
@@ -3273,15 +3240,15 @@
         <v>0</v>
       </c>
       <c r="BJ17" s="15">
-        <f>O25</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="BK17" s="15">
-        <f>P25</f>
+        <f t="shared" si="5"/>
         <v>-2333333.3333333335</v>
       </c>
       <c r="BL17" s="15">
-        <f>Q25</f>
+        <f t="shared" si="5"/>
         <v>9333333333.333334</v>
       </c>
       <c r="BM17" s="16"/>
@@ -3367,27 +3334,27 @@
     </row>
     <row r="20" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B20" s="37">
-        <f t="shared" ref="B20:G21" si="2">$B36*B$45+$C36*B$46+$D36*B$47+$E36*B$48+$F36*B$49+$G36*B$50</f>
+        <f t="shared" ref="B20:G21" si="6">$B36*B$45+$C36*B$46+$D36*B$47+$E36*B$48+$F36*B$49+$G36*B$50</f>
         <v>328.125</v>
       </c>
       <c r="C20" s="37">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>3.2140046849512931E-11</v>
       </c>
       <c r="D20" s="37">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-656250</v>
       </c>
       <c r="E20" s="37">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-328.125</v>
       </c>
       <c r="F20" s="37">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-3.2140046849512931E-11</v>
       </c>
       <c r="G20" s="37">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-656250</v>
       </c>
       <c r="I20" s="40">
@@ -3395,27 +3362,27 @@
         <v>-20000</v>
       </c>
       <c r="L20" s="19">
-        <f t="shared" ref="L20:Q25" si="3">$L37*L$46+$M37*L$47+$N37*L$48+$O37*L$49+$P37*L$50+$Q37*L$51</f>
+        <f t="shared" ref="L20:Q25" si="7">$L37*L$46+$M37*L$47+$N37*L$48+$O37*L$49+$P37*L$50+$Q37*L$51</f>
         <v>700000</v>
       </c>
       <c r="M20" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N20" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="O20" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-700000</v>
       </c>
       <c r="P20" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Q20" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="S20" s="40">
@@ -3423,27 +3390,27 @@
         <v>0</v>
       </c>
       <c r="V20" s="20">
-        <f t="shared" ref="V20:AA21" si="4">$V37*B$45+$W37*B$46+$X37*B$47+$Y37*B$48+$Z37*B$49+$AA37*B$50</f>
+        <f t="shared" ref="V20:AA21" si="8">$V37*B$45+$W37*B$46+$X37*B$47+$Y37*B$48+$Z37*B$49+$AA37*B$50</f>
         <v>328.125</v>
       </c>
       <c r="W20" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>3.2140046849512931E-11</v>
       </c>
       <c r="X20" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>-656250</v>
       </c>
       <c r="Y20" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>-328.125</v>
       </c>
       <c r="Z20" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>-3.2140046849512931E-11</v>
       </c>
       <c r="AA20" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>-656250</v>
       </c>
       <c r="AC20" s="40">
@@ -3456,27 +3423,27 @@
     </row>
     <row r="21" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B21" s="37">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>3.2140046849512931E-11</v>
       </c>
       <c r="C21" s="37">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>525000</v>
       </c>
       <c r="D21" s="37">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>4.0200183676689094E-11</v>
       </c>
       <c r="E21" s="37">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-3.2140046849512931E-11</v>
       </c>
       <c r="F21" s="37">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-525000</v>
       </c>
       <c r="G21" s="37">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>4.0200183676689094E-11</v>
       </c>
       <c r="I21" s="40">
@@ -3484,27 +3451,27 @@
         <v>1570.0000000000011</v>
       </c>
       <c r="L21" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="M21" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>777.77777777777783</v>
       </c>
       <c r="N21" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2333333.3333333335</v>
       </c>
       <c r="O21" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="P21" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-777.77777777777783</v>
       </c>
       <c r="Q21" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2333333.3333333335</v>
       </c>
       <c r="S21" s="40">
@@ -3512,27 +3479,27 @@
         <v>34710</v>
       </c>
       <c r="V21" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>3.2140046849512931E-11</v>
       </c>
       <c r="W21" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>525000</v>
       </c>
       <c r="X21" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>4.0200183676689094E-11</v>
       </c>
       <c r="Y21" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>-3.2140046849512931E-11</v>
       </c>
       <c r="Z21" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>-525000</v>
       </c>
       <c r="AA21" s="20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>4.0200183676689094E-11</v>
       </c>
       <c r="AC21" s="40">
@@ -3583,23 +3550,23 @@
     </row>
     <row r="22" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B22" s="37">
-        <f t="shared" ref="B22:F25" si="5">$B38*B$45+$C38*B$46+$D38*B$47+$E38*B$48+$F38*B$49+$G38*B$50</f>
+        <f t="shared" ref="B22:F25" si="9">$B38*B$45+$C38*B$46+$D38*B$47+$E38*B$48+$F38*B$49+$G38*B$50</f>
         <v>-656250</v>
       </c>
       <c r="C22" s="37">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>4.0200183676689094E-11</v>
       </c>
       <c r="D22" s="37">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>1750000000</v>
       </c>
       <c r="E22" s="37">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>656250</v>
       </c>
       <c r="F22" s="37">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>-4.0200183676689094E-11</v>
       </c>
       <c r="G22" s="37">
@@ -3611,27 +3578,27 @@
         <v>13333333.333333334</v>
       </c>
       <c r="L22" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="M22" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2333333.3333333335</v>
       </c>
       <c r="N22" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>9333333333.333334</v>
       </c>
       <c r="O22" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="P22" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-2333333.3333333335</v>
       </c>
       <c r="Q22" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>4666666666.666667</v>
       </c>
       <c r="S22" s="40">
@@ -3639,23 +3606,23 @@
         <v>34710000</v>
       </c>
       <c r="V22" s="20">
-        <f t="shared" ref="V22:Z25" si="6">$V39*B$45+$W39*B$46+$X39*B$47+$Y39*B$48+$Z39*B$49+$AA39*B$50</f>
+        <f t="shared" ref="V22:Z25" si="10">$V39*B$45+$W39*B$46+$X39*B$47+$Y39*B$48+$Z39*B$49+$AA39*B$50</f>
         <v>-656250</v>
       </c>
       <c r="W22" s="20">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>4.0200183676689094E-11</v>
       </c>
       <c r="X22" s="20">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>1750000000</v>
       </c>
       <c r="Y22" s="20">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>656250</v>
       </c>
       <c r="Z22" s="20">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>-4.0200183676689094E-11</v>
       </c>
       <c r="AA22" s="20">
@@ -3709,23 +3676,23 @@
     </row>
     <row r="23" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B23" s="37">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>-328.125</v>
       </c>
       <c r="C23" s="37">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>-3.2140046849512931E-11</v>
       </c>
       <c r="D23" s="37">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>656250</v>
       </c>
       <c r="E23" s="37">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>328.125</v>
       </c>
       <c r="F23" s="37">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>3.2140046849512931E-11</v>
       </c>
       <c r="G23" s="37">
@@ -3737,27 +3704,27 @@
         <v>-20000</v>
       </c>
       <c r="L23" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-700000</v>
       </c>
       <c r="M23" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N23" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="O23" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>700000</v>
       </c>
       <c r="P23" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="Q23" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="S23" s="40">
@@ -3765,23 +3732,23 @@
         <v>0</v>
       </c>
       <c r="V23" s="20">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>-328.125</v>
       </c>
       <c r="W23" s="20">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>-3.2140046849512931E-11</v>
       </c>
       <c r="X23" s="20">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>656250</v>
       </c>
       <c r="Y23" s="20">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>328.125</v>
       </c>
       <c r="Z23" s="20">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>3.2140046849512931E-11</v>
       </c>
       <c r="AA23" s="20">
@@ -3835,23 +3802,23 @@
     </row>
     <row r="24" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B24" s="37">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>-3.2140046849512931E-11</v>
       </c>
       <c r="C24" s="37">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>-525000</v>
       </c>
       <c r="D24" s="37">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>-4.0200183676689094E-11</v>
       </c>
       <c r="E24" s="37">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>3.2140046849512931E-11</v>
       </c>
       <c r="F24" s="37">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>525000</v>
       </c>
       <c r="G24" s="37">
@@ -3863,27 +3830,27 @@
         <v>1570.0000000000011</v>
       </c>
       <c r="L24" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="M24" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-777.77777777777783</v>
       </c>
       <c r="N24" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-2333333.3333333335</v>
       </c>
       <c r="O24" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="P24" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>777.77777777777783</v>
       </c>
       <c r="Q24" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-2333333.3333333335</v>
       </c>
       <c r="S24" s="40">
@@ -3891,23 +3858,23 @@
         <v>34710</v>
       </c>
       <c r="V24" s="20">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>-3.2140046849512931E-11</v>
       </c>
       <c r="W24" s="20">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>-525000</v>
       </c>
       <c r="X24" s="20">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>-4.0200183676689094E-11</v>
       </c>
       <c r="Y24" s="20">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>3.2140046849512931E-11</v>
       </c>
       <c r="Z24" s="20">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>525000</v>
       </c>
       <c r="AA24" s="20">
@@ -3961,23 +3928,23 @@
     </row>
     <row r="25" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B25" s="37">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>-656250</v>
       </c>
       <c r="C25" s="37">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>4.0200183676689094E-11</v>
       </c>
       <c r="D25" s="37">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>875000000</v>
       </c>
       <c r="E25" s="37">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>656250</v>
       </c>
       <c r="F25" s="37">
-        <f t="shared" si="5"/>
+        <f t="shared" si="9"/>
         <v>-4.0200183676689094E-11</v>
       </c>
       <c r="G25" s="37">
@@ -3990,27 +3957,27 @@
       </c>
       <c r="K25" s="2"/>
       <c r="L25" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="M25" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>2333333.3333333335</v>
       </c>
       <c r="N25" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>4666666666.666667</v>
       </c>
       <c r="O25" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="P25" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>-2333333.3333333335</v>
       </c>
       <c r="Q25" s="19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>9333333333.333334</v>
       </c>
       <c r="S25" s="40">
@@ -4019,23 +3986,23 @@
       </c>
       <c r="U25" s="2"/>
       <c r="V25" s="20">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>-656250</v>
       </c>
       <c r="W25" s="20">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>4.0200183676689094E-11</v>
       </c>
       <c r="X25" s="20">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>875000000</v>
       </c>
       <c r="Y25" s="20">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>656250</v>
       </c>
       <c r="Z25" s="20">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>-4.0200183676689094E-11</v>
       </c>
       <c r="AA25" s="20">
@@ -4140,7 +4107,7 @@
       <c r="B27" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="I27" s="148" t="s">
+      <c r="I27" s="147" t="s">
         <v>33</v>
       </c>
       <c r="L27" s="2" t="s">
@@ -4291,27 +4258,27 @@
         <v>0</v>
       </c>
       <c r="AQ28" s="17">
-        <f t="shared" ref="AQ28:AV33" si="7">V20</f>
+        <f t="shared" ref="AQ28:AV33" si="11">V20</f>
         <v>328.125</v>
       </c>
       <c r="AR28" s="17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>3.2140046849512931E-11</v>
       </c>
       <c r="AS28" s="17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>-656250</v>
       </c>
       <c r="AT28" s="17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>-328.125</v>
       </c>
       <c r="AU28" s="17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>-3.2140046849512931E-11</v>
       </c>
       <c r="AV28" s="17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>-656250</v>
       </c>
       <c r="AW28" s="4"/>
@@ -4422,32 +4389,32 @@
         <v>0</v>
       </c>
       <c r="AQ29" s="17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>3.2140046849512931E-11</v>
       </c>
       <c r="AR29" s="17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>525000</v>
       </c>
       <c r="AS29" s="17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>4.0200183676689094E-11</v>
       </c>
       <c r="AT29" s="17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>-3.2140046849512931E-11</v>
       </c>
       <c r="AU29" s="17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>-525000</v>
       </c>
       <c r="AV29" s="17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>4.0200183676689094E-11</v>
       </c>
       <c r="AW29" s="4"/>
       <c r="AX29" s="3">
-        <f t="shared" ref="AX29:AX33" si="8">AC21</f>
+        <f t="shared" ref="AX29:AX33" si="12">AC21</f>
         <v>1569.9999999999989</v>
       </c>
       <c r="AY29" s="10"/>
@@ -4553,32 +4520,32 @@
         <v>0</v>
       </c>
       <c r="AQ30" s="17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>-656250</v>
       </c>
       <c r="AR30" s="17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>4.0200183676689094E-11</v>
       </c>
       <c r="AS30" s="17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>1750000000</v>
       </c>
       <c r="AT30" s="17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>656250</v>
       </c>
       <c r="AU30" s="17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>-4.0200183676689094E-11</v>
       </c>
       <c r="AV30" s="17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>875000000</v>
       </c>
       <c r="AW30" s="4"/>
       <c r="AX30" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>-13333333.333333334</v>
       </c>
       <c r="AY30" s="8"/>
@@ -4677,32 +4644,32 @@
         <v>0</v>
       </c>
       <c r="AQ31" s="17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>-328.125</v>
       </c>
       <c r="AR31" s="17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>-3.2140046849512931E-11</v>
       </c>
       <c r="AS31" s="17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>656250</v>
       </c>
       <c r="AT31" s="17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>328.125</v>
       </c>
       <c r="AU31" s="17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>3.2140046849512931E-11</v>
       </c>
       <c r="AV31" s="17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>656250</v>
       </c>
       <c r="AW31" s="4"/>
       <c r="AX31" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>20000</v>
       </c>
       <c r="AY31" s="8"/>
@@ -4809,32 +4776,32 @@
         <v>0</v>
       </c>
       <c r="AQ32" s="17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>-3.2140046849512931E-11</v>
       </c>
       <c r="AR32" s="17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>-525000</v>
       </c>
       <c r="AS32" s="17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>-4.0200183676689094E-11</v>
       </c>
       <c r="AT32" s="17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>3.2140046849512931E-11</v>
       </c>
       <c r="AU32" s="17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>525000</v>
       </c>
       <c r="AV32" s="17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>-4.0200183676689094E-11</v>
       </c>
       <c r="AW32" s="4"/>
       <c r="AX32" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>1569.9999999999989</v>
       </c>
       <c r="AY32" s="10"/>
@@ -4940,32 +4907,32 @@
         <v>0</v>
       </c>
       <c r="AQ33" s="17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>-656250</v>
       </c>
       <c r="AR33" s="17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>4.0200183676689094E-11</v>
       </c>
       <c r="AS33" s="17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>875000000</v>
       </c>
       <c r="AT33" s="17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>656250</v>
       </c>
       <c r="AU33" s="17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>-4.0200183676689094E-11</v>
       </c>
       <c r="AV33" s="17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>1750000000</v>
       </c>
       <c r="AW33" s="4"/>
       <c r="AX33" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="12"/>
         <v>13333333.333333334</v>
       </c>
       <c r="AY33" s="8"/>
@@ -5005,27 +4972,27 @@
     </row>
     <row r="36" spans="2:83" x14ac:dyDescent="0.2">
       <c r="B36" s="38">
-        <f t="shared" ref="B36:G36" si="9">$B54*B28+$C54*B29+$D54*B30+$E54*B31+$F54*B32+$G54*B33</f>
+        <f t="shared" ref="B36:G36" si="13">$B54*B28+$C54*B29+$D54*B30+$E54*B31+$F54*B32+$G54*B33</f>
         <v>3.2160146941351275E-11</v>
       </c>
       <c r="C36" s="38">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>-328.125</v>
       </c>
       <c r="D36" s="38">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>-656250</v>
       </c>
       <c r="E36" s="38">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>-3.2160146941351275E-11</v>
       </c>
       <c r="F36" s="38">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>328.125</v>
       </c>
       <c r="G36" s="38">
-        <f t="shared" si="9"/>
+        <f t="shared" si="13"/>
         <v>-656250</v>
       </c>
       <c r="L36" s="2" t="s">
@@ -5037,372 +5004,372 @@
     </row>
     <row r="37" spans="2:83" x14ac:dyDescent="0.2">
       <c r="B37" s="38">
-        <f t="shared" ref="B37:G37" si="10">$B55*B28+$C55*B29+$D55*B30+$E55*B31+$F55*B32+$G55*B33</f>
+        <f t="shared" ref="B37:G37" si="14">$B55*B28+$C55*B29+$D55*B30+$E55*B31+$F55*B32+$G55*B33</f>
         <v>525000</v>
       </c>
       <c r="C37" s="38">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>2.0100091838344547E-14</v>
       </c>
       <c r="D37" s="38">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>4.0200183676689094E-11</v>
       </c>
       <c r="E37" s="38">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>-525000</v>
       </c>
       <c r="F37" s="38">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>-2.0100091838344547E-14</v>
       </c>
       <c r="G37" s="38">
-        <f t="shared" si="10"/>
+        <f t="shared" si="14"/>
         <v>4.0200183676689094E-11</v>
       </c>
       <c r="L37" s="38">
-        <f t="shared" ref="L37:Q42" si="11">$L55*L$28+$M55*L$29+$N55*L$30+$O55*L$31+$P55*L$32+$Q55*L$33</f>
+        <f t="shared" ref="L37:Q42" si="15">$L55*L$28+$M55*L$29+$N55*L$30+$O55*L$31+$P55*L$32+$Q55*L$33</f>
         <v>700000</v>
       </c>
       <c r="M37" s="38">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="N37" s="38">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="O37" s="38">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>-700000</v>
       </c>
       <c r="P37" s="38">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="Q37" s="38">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="V37" s="38">
-        <f t="shared" ref="V37:AA37" si="12">$V55*V28+$W55*V29+$X55*V30+$Y55*V31+$Z55*V32+$AA55*V33</f>
+        <f t="shared" ref="V37:AA37" si="16">$V55*V28+$W55*V29+$X55*V30+$Y55*V31+$Z55*V32+$AA55*V33</f>
         <v>3.2160146941351275E-11</v>
       </c>
       <c r="W37" s="38">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>-328.125</v>
       </c>
       <c r="X37" s="38">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>-656250</v>
       </c>
       <c r="Y37" s="38">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>-3.2160146941351275E-11</v>
       </c>
       <c r="Z37" s="38">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>328.125</v>
       </c>
       <c r="AA37" s="38">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>-656250</v>
       </c>
     </row>
     <row r="38" spans="2:83" x14ac:dyDescent="0.2">
       <c r="B38" s="38">
-        <f t="shared" ref="B38:G38" si="13">$B56*B28+$C56*B29+$D56*B30+$E56*B31+$F56*B32+$G56*B33</f>
+        <f t="shared" ref="B38:G38" si="17">$B56*B28+$C56*B29+$D56*B30+$E56*B31+$F56*B32+$G56*B33</f>
         <v>0</v>
       </c>
       <c r="C38" s="38">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>656250</v>
       </c>
       <c r="D38" s="38">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>1750000000</v>
       </c>
       <c r="E38" s="38">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="F38" s="38">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>-656250</v>
       </c>
       <c r="G38" s="38">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>875000000</v>
       </c>
       <c r="L38" s="38">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="M38" s="38">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>777.77777777777783</v>
       </c>
       <c r="N38" s="38">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>2333333.3333333335</v>
       </c>
       <c r="O38" s="38">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="P38" s="38">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>-777.77777777777783</v>
       </c>
       <c r="Q38" s="38">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>2333333.3333333335</v>
       </c>
       <c r="V38" s="38">
-        <f t="shared" ref="V38:AA38" si="14">$V56*V28+$W56*V29+$X56*V30+$Y56*V31+$Z56*V32+$AA56*V33</f>
+        <f t="shared" ref="V38:AA38" si="18">$V56*V28+$W56*V29+$X56*V30+$Y56*V31+$Z56*V32+$AA56*V33</f>
         <v>525000</v>
       </c>
       <c r="W38" s="38">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>2.0100091838344547E-14</v>
       </c>
       <c r="X38" s="38">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>4.0200183676689094E-11</v>
       </c>
       <c r="Y38" s="38">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>-525000</v>
       </c>
       <c r="Z38" s="38">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>-2.0100091838344547E-14</v>
       </c>
       <c r="AA38" s="38">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>4.0200183676689094E-11</v>
       </c>
     </row>
     <row r="39" spans="2:83" x14ac:dyDescent="0.2">
       <c r="B39" s="38">
-        <f t="shared" ref="B39:G41" si="15">$B57*B$28+$C57*B$29+$D57*B$30+$E57*B$31+$F57*B$32+$G57*B$33</f>
+        <f t="shared" ref="B39:G41" si="19">$B57*B$28+$C57*B$29+$D57*B$30+$E57*B$31+$F57*B$32+$G57*B$33</f>
         <v>-3.2160146941351275E-11</v>
       </c>
       <c r="C39" s="38">
+        <f t="shared" si="19"/>
+        <v>328.125</v>
+      </c>
+      <c r="D39" s="38">
+        <f t="shared" si="19"/>
+        <v>656250</v>
+      </c>
+      <c r="E39" s="38">
+        <f t="shared" si="19"/>
+        <v>3.2160146941351275E-11</v>
+      </c>
+      <c r="F39" s="38">
+        <f t="shared" si="19"/>
+        <v>-328.125</v>
+      </c>
+      <c r="G39" s="38">
+        <f t="shared" si="19"/>
+        <v>656250</v>
+      </c>
+      <c r="L39" s="38">
         <f t="shared" si="15"/>
-        <v>328.125</v>
-      </c>
-      <c r="D39" s="38">
+        <v>0</v>
+      </c>
+      <c r="M39" s="38">
         <f t="shared" si="15"/>
+        <v>2333333.3333333335</v>
+      </c>
+      <c r="N39" s="38">
+        <f t="shared" si="15"/>
+        <v>9333333333.333334</v>
+      </c>
+      <c r="O39" s="38">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="P39" s="38">
+        <f t="shared" si="15"/>
+        <v>-2333333.3333333335</v>
+      </c>
+      <c r="Q39" s="38">
+        <f t="shared" si="15"/>
+        <v>4666666666.666667</v>
+      </c>
+      <c r="V39" s="38">
+        <f t="shared" ref="V39:AA39" si="20">$V57*V28+$W57*V29+$X57*V30+$Y57*V31+$Z57*V32+$AA57*V33</f>
+        <v>0</v>
+      </c>
+      <c r="W39" s="38">
+        <f t="shared" si="20"/>
         <v>656250</v>
       </c>
-      <c r="E39" s="38">
-        <f t="shared" si="15"/>
-        <v>3.2160146941351275E-11</v>
-      </c>
-      <c r="F39" s="38">
-        <f t="shared" si="15"/>
-        <v>-328.125</v>
-      </c>
-      <c r="G39" s="38">
-        <f t="shared" si="15"/>
-        <v>656250</v>
-      </c>
-      <c r="L39" s="38">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="M39" s="38">
-        <f t="shared" si="11"/>
-        <v>2333333.3333333335</v>
-      </c>
-      <c r="N39" s="38">
-        <f t="shared" si="11"/>
-        <v>9333333333.333334</v>
-      </c>
-      <c r="O39" s="38">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="P39" s="38">
-        <f t="shared" si="11"/>
-        <v>-2333333.3333333335</v>
-      </c>
-      <c r="Q39" s="38">
-        <f t="shared" si="11"/>
-        <v>4666666666.666667</v>
-      </c>
-      <c r="V39" s="38">
-        <f t="shared" ref="V39:AA39" si="16">$V57*V28+$W57*V29+$X57*V30+$Y57*V31+$Z57*V32+$AA57*V33</f>
-        <v>0</v>
-      </c>
-      <c r="W39" s="38">
-        <f t="shared" si="16"/>
-        <v>656250</v>
-      </c>
       <c r="X39" s="38">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>1750000000</v>
       </c>
       <c r="Y39" s="38">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="Z39" s="38">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>-656250</v>
       </c>
       <c r="AA39" s="38">
-        <f t="shared" si="16"/>
+        <f t="shared" si="20"/>
         <v>875000000</v>
       </c>
     </row>
     <row r="40" spans="2:83" x14ac:dyDescent="0.2">
       <c r="B40" s="38">
+        <f t="shared" si="19"/>
+        <v>-525000</v>
+      </c>
+      <c r="C40" s="38">
+        <f t="shared" si="19"/>
+        <v>-2.0100091838344547E-14</v>
+      </c>
+      <c r="D40" s="38">
+        <f t="shared" si="19"/>
+        <v>-4.0200183676689094E-11</v>
+      </c>
+      <c r="E40" s="38">
+        <f t="shared" si="19"/>
+        <v>525000</v>
+      </c>
+      <c r="F40" s="38">
+        <f t="shared" si="19"/>
+        <v>2.0100091838344547E-14</v>
+      </c>
+      <c r="G40" s="38">
+        <f t="shared" si="19"/>
+        <v>-4.0200183676689094E-11</v>
+      </c>
+      <c r="L40" s="38">
         <f t="shared" si="15"/>
-        <v>-525000</v>
-      </c>
-      <c r="C40" s="38">
+        <v>-700000</v>
+      </c>
+      <c r="M40" s="38">
         <f t="shared" si="15"/>
-        <v>-2.0100091838344547E-14</v>
-      </c>
-      <c r="D40" s="38">
+        <v>0</v>
+      </c>
+      <c r="N40" s="38">
         <f t="shared" si="15"/>
-        <v>-4.0200183676689094E-11</v>
-      </c>
-      <c r="E40" s="38">
+        <v>0</v>
+      </c>
+      <c r="O40" s="38">
         <f t="shared" si="15"/>
-        <v>525000</v>
-      </c>
-      <c r="F40" s="38">
+        <v>700000</v>
+      </c>
+      <c r="P40" s="38">
         <f t="shared" si="15"/>
-        <v>2.0100091838344547E-14</v>
-      </c>
-      <c r="G40" s="38">
+        <v>0</v>
+      </c>
+      <c r="Q40" s="38">
         <f t="shared" si="15"/>
-        <v>-4.0200183676689094E-11</v>
-      </c>
-      <c r="L40" s="38">
-        <f t="shared" si="11"/>
-        <v>-700000</v>
-      </c>
-      <c r="M40" s="38">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="N40" s="38">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="O40" s="38">
-        <f t="shared" si="11"/>
-        <v>700000</v>
-      </c>
-      <c r="P40" s="38">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="Q40" s="38">
-        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="S40" s="2"/>
       <c r="V40" s="38">
-        <f t="shared" ref="V40:AA42" si="17">$V58*B$28+$W58*B$29+$X58*B$30+$Y58*B$31+$Z58*B$32+$AA58*B$33</f>
+        <f t="shared" ref="V40:AA42" si="21">$V58*B$28+$W58*B$29+$X58*B$30+$Y58*B$31+$Z58*B$32+$AA58*B$33</f>
         <v>-3.2160146941351275E-11</v>
       </c>
       <c r="W40" s="38">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>328.125</v>
       </c>
       <c r="X40" s="38">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>656250</v>
       </c>
       <c r="Y40" s="38">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>3.2160146941351275E-11</v>
       </c>
       <c r="Z40" s="38">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>-328.125</v>
       </c>
       <c r="AA40" s="38">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>656250</v>
       </c>
     </row>
     <row r="41" spans="2:83" x14ac:dyDescent="0.2">
       <c r="B41" s="38">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="C41" s="38">
+        <f t="shared" si="19"/>
+        <v>656250</v>
+      </c>
+      <c r="D41" s="38">
+        <f t="shared" si="19"/>
+        <v>875000000</v>
+      </c>
+      <c r="E41" s="38">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="F41" s="38">
+        <f t="shared" si="19"/>
+        <v>-656250</v>
+      </c>
+      <c r="G41" s="38">
+        <f t="shared" si="19"/>
+        <v>1750000000</v>
+      </c>
+      <c r="L41" s="38">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="C41" s="38">
+      <c r="M41" s="38">
         <f t="shared" si="15"/>
-        <v>656250</v>
-      </c>
-      <c r="D41" s="38">
+        <v>-777.77777777777783</v>
+      </c>
+      <c r="N41" s="38">
         <f t="shared" si="15"/>
-        <v>875000000</v>
-      </c>
-      <c r="E41" s="38">
+        <v>-2333333.3333333335</v>
+      </c>
+      <c r="O41" s="38">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="F41" s="38">
+      <c r="P41" s="38">
         <f t="shared" si="15"/>
-        <v>-656250</v>
-      </c>
-      <c r="G41" s="38">
+        <v>777.77777777777783</v>
+      </c>
+      <c r="Q41" s="38">
         <f t="shared" si="15"/>
-        <v>1750000000</v>
-      </c>
-      <c r="L41" s="38">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="M41" s="38">
-        <f t="shared" si="11"/>
-        <v>-777.77777777777783</v>
-      </c>
-      <c r="N41" s="38">
-        <f t="shared" si="11"/>
         <v>-2333333.3333333335</v>
       </c>
-      <c r="O41" s="38">
-        <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="P41" s="38">
-        <f t="shared" si="11"/>
-        <v>777.77777777777783</v>
-      </c>
-      <c r="Q41" s="38">
-        <f t="shared" si="11"/>
-        <v>-2333333.3333333335</v>
-      </c>
       <c r="V41" s="38">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>-525000</v>
       </c>
       <c r="W41" s="38">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>-2.0100091838344547E-14</v>
       </c>
       <c r="X41" s="38">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>-4.0200183676689094E-11</v>
       </c>
       <c r="Y41" s="38">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>525000</v>
       </c>
       <c r="Z41" s="38">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>2.0100091838344547E-14</v>
       </c>
       <c r="AA41" s="38">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>-4.0200183676689094E-11</v>
       </c>
       <c r="AJ41" s="2" t="s">
@@ -5415,51 +5382,51 @@
     </row>
     <row r="42" spans="2:83" x14ac:dyDescent="0.2">
       <c r="L42" s="38">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="M42" s="38">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>2333333.3333333335</v>
       </c>
       <c r="N42" s="38">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>4666666666.666667</v>
       </c>
       <c r="O42" s="38">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="P42" s="38">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>-2333333.3333333335</v>
       </c>
       <c r="Q42" s="38">
-        <f t="shared" si="11"/>
+        <f t="shared" si="15"/>
         <v>9333333333.333334</v>
       </c>
       <c r="V42" s="38">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="W42" s="38">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>656250</v>
       </c>
       <c r="X42" s="38">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>875000000</v>
       </c>
       <c r="Y42" s="38">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="Z42" s="38">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>-656250</v>
       </c>
       <c r="AA42" s="38">
-        <f t="shared" si="17"/>
+        <f t="shared" si="21"/>
         <v>1750000000</v>
       </c>
       <c r="AJ42" s="9"/>
@@ -5523,47 +5490,47 @@
         <v>328.125</v>
       </c>
       <c r="AL43" s="11">
-        <f t="shared" ref="AL43:AV43" si="18">AL6+BB6+AL22</f>
+        <f t="shared" ref="AL43:AV43" si="22">AL6+BB6+AL22</f>
         <v>3.2140046849512931E-11</v>
       </c>
       <c r="AM43" s="11">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>-656250</v>
       </c>
       <c r="AN43" s="11">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>-328.125</v>
       </c>
       <c r="AO43" s="11">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>-3.2140046849512931E-11</v>
       </c>
       <c r="AP43" s="11">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>-656250</v>
       </c>
       <c r="AQ43" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="AR43" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="AS43" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="AT43" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="AU43" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="AV43" s="7">
-        <f t="shared" si="18"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="AX43" s="4">
@@ -5573,7 +5540,7 @@
         <f>AX6+BN6+AX22</f>
         <v>-20000</v>
       </c>
-      <c r="BA43" s="149" t="s">
+      <c r="BA43" s="148" t="s">
         <v>55</v>
       </c>
     </row>
@@ -5586,61 +5553,61 @@
         <v>2</v>
       </c>
       <c r="AK44" s="11">
-        <f t="shared" ref="AK44:AK54" si="19">AK7+BA7+AK23</f>
+        <f t="shared" ref="AK44:AK54" si="23">AK7+BA7+AK23</f>
         <v>3.2140046849512931E-11</v>
       </c>
       <c r="AL44" s="11">
-        <f t="shared" ref="AL44:AL54" si="20">AL7+BB7+AL23</f>
+        <f t="shared" ref="AL44:AL54" si="24">AL7+BB7+AL23</f>
         <v>525000</v>
       </c>
       <c r="AM44" s="11">
-        <f t="shared" ref="AM44:AM54" si="21">AM7+BC7+AM23</f>
+        <f t="shared" ref="AM44:AM54" si="25">AM7+BC7+AM23</f>
         <v>4.0200183676689094E-11</v>
       </c>
       <c r="AN44" s="11">
-        <f t="shared" ref="AN44:AN54" si="22">AN7+BD7+AN23</f>
+        <f t="shared" ref="AN44:AN54" si="26">AN7+BD7+AN23</f>
         <v>-3.2140046849512931E-11</v>
       </c>
       <c r="AO44" s="11">
-        <f t="shared" ref="AO44:AO54" si="23">AO7+BE7+AO23</f>
+        <f t="shared" ref="AO44:AO54" si="27">AO7+BE7+AO23</f>
         <v>-525000</v>
       </c>
       <c r="AP44" s="11">
-        <f t="shared" ref="AP44:AP54" si="24">AP7+BF7+AP23</f>
+        <f t="shared" ref="AP44:AP54" si="28">AP7+BF7+AP23</f>
         <v>4.0200183676689094E-11</v>
       </c>
       <c r="AQ44" s="7">
-        <f t="shared" ref="AQ44:AQ54" si="25">AQ7+BG7+AQ23</f>
+        <f t="shared" ref="AQ44:AQ54" si="29">AQ7+BG7+AQ23</f>
         <v>0</v>
       </c>
       <c r="AR44" s="7">
-        <f t="shared" ref="AR44:AR54" si="26">AR7+BH7+AR23</f>
+        <f t="shared" ref="AR44:AR54" si="30">AR7+BH7+AR23</f>
         <v>0</v>
       </c>
       <c r="AS44" s="7">
-        <f t="shared" ref="AS44:AS54" si="27">AS7+BI7+AS23</f>
+        <f t="shared" ref="AS44:AS54" si="31">AS7+BI7+AS23</f>
         <v>0</v>
       </c>
       <c r="AT44" s="7">
-        <f t="shared" ref="AT44:AT54" si="28">AT7+BJ7+AT23</f>
+        <f t="shared" ref="AT44:AT54" si="32">AT7+BJ7+AT23</f>
         <v>0</v>
       </c>
       <c r="AU44" s="7">
-        <f t="shared" ref="AU44:AU54" si="29">AU7+BK7+AU23</f>
+        <f t="shared" ref="AU44:AU54" si="33">AU7+BK7+AU23</f>
         <v>0</v>
       </c>
       <c r="AV44" s="7">
-        <f t="shared" ref="AV44:AV54" si="30">AV7+BL7+AV23</f>
+        <f t="shared" ref="AV44:AV54" si="34">AV7+BL7+AV23</f>
         <v>0</v>
       </c>
       <c r="AX44" s="4">
         <v>0</v>
       </c>
       <c r="AZ44" s="3">
-        <f t="shared" ref="AZ44:AZ54" si="31">AX7+BN7+AX23</f>
+        <f t="shared" ref="AZ44:AZ54" si="35">AX7+BN7+AX23</f>
         <v>1570.0000000000011</v>
       </c>
-      <c r="BA44" s="149" t="s">
+      <c r="BA44" s="148" t="s">
         <v>54</v>
       </c>
     </row>
@@ -5676,58 +5643,58 @@
         <v>3</v>
       </c>
       <c r="AK45" s="11">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>-656250</v>
       </c>
       <c r="AL45" s="11">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>4.0200183676689094E-11</v>
       </c>
       <c r="AM45" s="11">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>1750000000</v>
       </c>
       <c r="AN45" s="11">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>656250</v>
       </c>
       <c r="AO45" s="11">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>-4.0200183676689094E-11</v>
       </c>
       <c r="AP45" s="11">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>875000000</v>
       </c>
       <c r="AQ45" s="7">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="AR45" s="7">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="AS45" s="7">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="AT45" s="7">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="AU45" s="7">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="AV45" s="7">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="AX45" s="4" t="s">
         <v>42</v>
       </c>
       <c r="AZ45" s="3">
-        <f t="shared" si="31"/>
+        <f t="shared" si="35"/>
         <v>13333333.333333334</v>
       </c>
     </row>
@@ -5797,58 +5764,58 @@
         <v>4</v>
       </c>
       <c r="AK46" s="11">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>-328.125</v>
       </c>
       <c r="AL46" s="11">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>-3.2140046849512931E-11</v>
       </c>
       <c r="AM46" s="11">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>656250</v>
       </c>
       <c r="AN46" s="18">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>700328.125</v>
       </c>
       <c r="AO46" s="18">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>3.2140046849512931E-11</v>
       </c>
       <c r="AP46" s="18">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>656250</v>
       </c>
       <c r="AQ46" s="16">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="AR46" s="7">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="AS46" s="7">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="AT46" s="19">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>-700000</v>
       </c>
       <c r="AU46" s="15">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="AV46" s="15">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="AX46" s="4" t="s">
         <v>43</v>
       </c>
       <c r="AZ46" s="3">
-        <f t="shared" si="31"/>
+        <f t="shared" si="35"/>
         <v>-20000</v>
       </c>
       <c r="CE46" s="2"/>
@@ -5917,51 +5884,51 @@
         <v>5</v>
       </c>
       <c r="AK47" s="11">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>-3.2140046849512931E-11</v>
       </c>
       <c r="AL47" s="11">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>-525000</v>
       </c>
       <c r="AM47" s="11">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>-4.0200183676689094E-11</v>
       </c>
       <c r="AN47" s="18">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>3.2140046849512931E-11</v>
       </c>
       <c r="AO47" s="18">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>525777.77777777775</v>
       </c>
       <c r="AP47" s="18">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>2333333.3333333335</v>
       </c>
       <c r="AQ47" s="16">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="AR47" s="7">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="AS47" s="7">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="AT47" s="19">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="AU47" s="15">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>-777.77777777777783</v>
       </c>
       <c r="AV47" s="15">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>2333333.3333333335</v>
       </c>
       <c r="AX47" s="4" t="s">
@@ -6036,58 +6003,58 @@
         <v>6</v>
       </c>
       <c r="AK48" s="11">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>-656250</v>
       </c>
       <c r="AL48" s="11">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>4.0200183676689094E-11</v>
       </c>
       <c r="AM48" s="11">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>875000000</v>
       </c>
       <c r="AN48" s="18">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>656250</v>
       </c>
       <c r="AO48" s="18">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>2333333.3333333335</v>
       </c>
       <c r="AP48" s="18">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>11083333333.333334</v>
       </c>
       <c r="AQ48" s="7">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="AR48" s="7">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="AS48" s="7">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="AT48" s="19">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="AU48" s="19">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>-2333333.3333333335</v>
       </c>
       <c r="AV48" s="19">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>4666666666.666667</v>
       </c>
       <c r="AX48" s="4" t="s">
         <v>45</v>
       </c>
       <c r="AZ48" s="3">
-        <f t="shared" si="31"/>
+        <f t="shared" si="35"/>
         <v>21376666.666666664</v>
       </c>
     </row>
@@ -6159,61 +6126,61 @@
         <v>7</v>
       </c>
       <c r="AK49" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="AL49" s="7">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="AM49" s="7">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="AN49" s="16">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="AO49" s="16">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AP49" s="7">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="AQ49" s="17">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>328.125</v>
       </c>
       <c r="AR49" s="20">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>3.2140046849512931E-11</v>
       </c>
       <c r="AS49" s="20">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>-656250</v>
       </c>
       <c r="AT49" s="20">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>-328.125</v>
       </c>
       <c r="AU49" s="17">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>-3.2140046849512931E-11</v>
       </c>
       <c r="AV49" s="17">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>-656250</v>
       </c>
       <c r="AX49" s="4">
         <v>0</v>
       </c>
       <c r="AZ49" s="3">
-        <f t="shared" si="31"/>
+        <f t="shared" si="35"/>
         <v>20000</v>
       </c>
-      <c r="BA49" s="149" t="s">
+      <c r="BA49" s="148" t="s">
         <v>56</v>
       </c>
       <c r="CW49" s="2"/>
@@ -6285,61 +6252,61 @@
         <v>8</v>
       </c>
       <c r="AK50" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="AL50" s="7">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="AM50" s="7">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="AN50" s="7">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="AO50" s="7">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AP50" s="7">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="AQ50" s="20">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>3.2140046849512931E-11</v>
       </c>
       <c r="AR50" s="17">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>525000</v>
       </c>
       <c r="AS50" s="17">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>4.0200183676689094E-11</v>
       </c>
       <c r="AT50" s="17">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>-3.2140046849512931E-11</v>
       </c>
       <c r="AU50" s="17">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>-525000</v>
       </c>
       <c r="AV50" s="17">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>4.0200183676689094E-11</v>
       </c>
       <c r="AX50" s="4">
         <v>0</v>
       </c>
       <c r="AZ50" s="3">
-        <f t="shared" si="31"/>
+        <f t="shared" si="35"/>
         <v>1569.9999999999989</v>
       </c>
-      <c r="BA50" s="149" t="s">
+      <c r="BA50" s="148" t="s">
         <v>57</v>
       </c>
       <c r="BK50" s="2"/>
@@ -6392,58 +6359,58 @@
         <v>9</v>
       </c>
       <c r="AK51" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="AL51" s="7">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="AM51" s="7">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="AN51" s="7">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="AO51" s="7">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AP51" s="7">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="AQ51" s="20">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>-656250</v>
       </c>
       <c r="AR51" s="17">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>4.0200183676689094E-11</v>
       </c>
       <c r="AS51" s="17">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>1750000000</v>
       </c>
       <c r="AT51" s="17">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>656250</v>
       </c>
       <c r="AU51" s="17">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>-4.0200183676689094E-11</v>
       </c>
       <c r="AV51" s="17">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>875000000</v>
       </c>
       <c r="AX51" s="4" t="s">
         <v>46</v>
       </c>
       <c r="AZ51" s="3">
-        <f t="shared" si="31"/>
+        <f t="shared" si="35"/>
         <v>-13333333.333333334</v>
       </c>
       <c r="BB51" s="4"/>
@@ -6467,58 +6434,58 @@
         <v>10</v>
       </c>
       <c r="AK52" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="AL52" s="7">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="AM52" s="7">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="AN52" s="19">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>-700000</v>
       </c>
       <c r="AO52" s="19">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="AP52" s="19">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="AQ52" s="20">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>-328.125</v>
       </c>
       <c r="AR52" s="17">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>-3.2140046849512931E-11</v>
       </c>
       <c r="AS52" s="17">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>656250</v>
       </c>
       <c r="AT52" s="21">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>700328.125</v>
       </c>
       <c r="AU52" s="21">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>3.2140046849512931E-11</v>
       </c>
       <c r="AV52" s="21">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>656250</v>
       </c>
       <c r="AX52" s="4" t="s">
         <v>47</v>
       </c>
       <c r="AZ52" s="3">
-        <f t="shared" si="31"/>
+        <f t="shared" si="35"/>
         <v>20000</v>
       </c>
       <c r="BB52" s="12"/>
@@ -6545,58 +6512,58 @@
         <v>11</v>
       </c>
       <c r="AK53" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="AL53" s="7">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="AM53" s="7">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="AN53" s="15">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="AO53" s="15">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>-777.77777777777783</v>
       </c>
       <c r="AP53" s="19">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>-2333333.3333333335</v>
       </c>
       <c r="AQ53" s="17">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>-3.2140046849512931E-11</v>
       </c>
       <c r="AR53" s="17">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>-525000</v>
       </c>
       <c r="AS53" s="17">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>-4.0200183676689094E-11</v>
       </c>
       <c r="AT53" s="21">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>3.2140046849512931E-11</v>
       </c>
       <c r="AU53" s="21">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>525777.77777777775</v>
       </c>
       <c r="AV53" s="21">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>-2333333.3333333335</v>
       </c>
       <c r="AX53" s="4" t="s">
         <v>48</v>
       </c>
       <c r="AZ53" s="3">
-        <f t="shared" si="31"/>
+        <f t="shared" si="35"/>
         <v>36280</v>
       </c>
       <c r="BB53" s="12"/>
@@ -6651,58 +6618,58 @@
         <v>12</v>
       </c>
       <c r="AK54" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="AL54" s="7">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="AM54" s="7">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="AN54" s="15">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="AO54" s="15">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>2333333.3333333335</v>
       </c>
       <c r="AP54" s="19">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>4666666666.666667</v>
       </c>
       <c r="AQ54" s="17">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>-656250</v>
       </c>
       <c r="AR54" s="17">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>4.0200183676689094E-11</v>
       </c>
       <c r="AS54" s="17">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>875000000</v>
       </c>
       <c r="AT54" s="21">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>656250</v>
       </c>
       <c r="AU54" s="21">
-        <f t="shared" si="29"/>
+        <f t="shared" si="33"/>
         <v>-2333333.3333333335</v>
       </c>
       <c r="AV54" s="21">
-        <f t="shared" si="30"/>
+        <f t="shared" si="34"/>
         <v>11083333333.333334</v>
       </c>
       <c r="AX54" s="4" t="s">
         <v>49</v>
       </c>
       <c r="AZ54" s="3">
-        <f t="shared" si="31"/>
+        <f t="shared" si="35"/>
         <v>-21376666.666666664</v>
       </c>
       <c r="BB54" s="12"/>
@@ -7197,7 +7164,7 @@
         <f>AX45</f>
         <v>r13</v>
       </c>
-      <c r="AV60" s="150" cm="1">
+      <c r="AV60" s="149" cm="1">
         <f t="array" ref="AV60:AV63">AZ45:AZ48</f>
         <v>13333333.333333334</v>
       </c>
@@ -7419,7 +7386,7 @@
         <f>AX51</f>
         <v>r33</v>
       </c>
-      <c r="AV64" s="151" cm="1">
+      <c r="AV64" s="3" cm="1">
         <f t="array" ref="AV64:AV67">AZ51:AZ54</f>
         <v>-13333333.333333334</v>
       </c>
@@ -7470,7 +7437,7 @@
         <f>AX52</f>
         <v>r41</v>
       </c>
-      <c r="AV65" s="147">
+      <c r="AV65" s="1">
         <v>20000</v>
       </c>
       <c r="BB65" s="12"/>
@@ -7509,7 +7476,7 @@
         <f>AX53</f>
         <v>r42</v>
       </c>
-      <c r="AV66" s="147">
+      <c r="AV66" s="1">
         <v>36280</v>
       </c>
     </row>
@@ -7546,7 +7513,7 @@
         <f>AX54</f>
         <v>r43</v>
       </c>
-      <c r="AV67" s="147">
+      <c r="AV67" s="1">
         <v>-21376666.666666664</v>
       </c>
     </row>
@@ -7555,7 +7522,7 @@
       <c r="BR68" s="66"/>
     </row>
     <row r="69" spans="5:74" x14ac:dyDescent="0.2">
-      <c r="AJ69" s="153" t="s">
+      <c r="AJ69" s="2" t="s">
         <v>58</v>
       </c>
       <c r="BR69" s="66"/>
@@ -7570,13 +7537,13 @@
       <c r="AP70" s="9"/>
       <c r="AQ70" s="9"/>
       <c r="AR70" s="9"/>
-      <c r="AS70" s="152" t="s">
+      <c r="AS70" s="1" t="s">
         <v>1</v>
       </c>
       <c r="AT70" s="145" t="s">
         <v>52</v>
       </c>
-      <c r="AU70" s="154" t="s">
+      <c r="AU70" s="150" t="s">
         <v>51</v>
       </c>
       <c r="AV70" s="9" t="s">
@@ -9716,17 +9683,17 @@
       <c r="BF233" s="50"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="AK43:AV54">
+    <cfRule type="expression" dxfId="4" priority="1">
+      <formula>ABS(AK43)&lt;0.1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="BR172:BR174">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>"VIRHE!"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"OK!"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AK43:AV54">
-    <cfRule type="expression" dxfId="2" priority="1">
-      <formula>ABS(AK43)&lt;0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Implement handle_point_load and tests for it
</commit_message>
<xml_diff>
--- a/theory/FEM matriisit.xlsx
+++ b/theory/FEM matriisit.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ohjelmointi\2_Rust\idfem\theory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DA3B9F8-1214-4D8A-AE58-AEAAAB67122B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFF4E6F1-CB7A-4BB4-9CD6-1B7B34BB2EE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22230" yWindow="0" windowWidth="22335" windowHeight="20985" xr2:uid="{27180542-B0D2-4BFE-946B-7857B24C93C8}"/>
+    <workbookView xWindow="-22230" yWindow="0" windowWidth="22335" windowHeight="20880" xr2:uid="{27180542-B0D2-4BFE-946B-7857B24C93C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Ilman vapautuksia" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="82">
   <si>
     <t>°</t>
   </si>
@@ -309,9 +309,6 @@
     <t>+Q32</t>
   </si>
   <si>
-    <t>Tuntemattomien siirtymien käänteismatriisi</t>
-  </si>
-  <si>
     <t>mrad</t>
   </si>
   <si>
@@ -319,6 +316,69 @@
   </si>
   <si>
     <t>rad</t>
+  </si>
+  <si>
+    <t>Momenttikuorma</t>
+  </si>
+  <si>
+    <t>Suunta</t>
+  </si>
+  <si>
+    <t>Positiivinen vastapäivään</t>
+  </si>
+  <si>
+    <t>Siirtymä (pituussuunnassa)</t>
+  </si>
+  <si>
+    <t>⮕</t>
+  </si>
+  <si>
+    <t>⬆</t>
+  </si>
+  <si>
+    <t>⟲</t>
+  </si>
+  <si>
+    <t>Matriisi</t>
+  </si>
+  <si>
+    <t>Alkupää</t>
+  </si>
+  <si>
+    <t>Loppupää</t>
+  </si>
+  <si>
+    <t>suunta</t>
+  </si>
+  <si>
+    <t>Lokaali</t>
+  </si>
+  <si>
+    <t>Globaalit arvot</t>
+  </si>
+  <si>
+    <t>Lokaalit arvot</t>
+  </si>
+  <si>
+    <t>Pysty</t>
+  </si>
+  <si>
+    <t>Vaaka</t>
+  </si>
+  <si>
+    <t>Muut kuormat muunnetaan pistekuormiksi ekvivalenttien kuormituskaavioiden mukaan ajatellen, että 'elementin' alku ja loppupiste on samassa kohtaa, kuin voiman alku ja loppupiste</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>etäisyys (a)</t>
+  </si>
+  <si>
+    <t>(Huomaa -1* alussa)</t>
+  </si>
+  <si>
+    <t>Positiivinen venymä</t>
   </si>
 </sst>
 </file>
@@ -611,7 +671,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="151">
+  <cellXfs count="153">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1011,6 +1071,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutraali" xfId="1" builtinId="28"/>
@@ -1144,7 +1210,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>397565</xdr:colOff>
+      <xdr:colOff>372717</xdr:colOff>
       <xdr:row>52</xdr:row>
       <xdr:rowOff>14813</xdr:rowOff>
     </xdr:to>
@@ -1171,6 +1237,94 @@
         <a:xfrm>
           <a:off x="6055480" y="340415"/>
           <a:ext cx="5515324" cy="7526311"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>41413</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>552251</xdr:colOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>66261</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Kuva 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9307D9D9-7156-701D-D272-FACC579DAAF3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3147391" y="11620500"/>
+          <a:ext cx="3616817" cy="3197087"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>488673</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>50110</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>221987</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>72398</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Kuva 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{61598652-8122-D8F1-BC81-D8E9EEC9F958}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7313543" y="11521523"/>
+          <a:ext cx="4106531" cy="2258592"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1646,10 +1800,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94F9BDF3-3EE6-4BFB-9734-CB047BC6E804}">
-  <dimension ref="B1:CW233"/>
+  <dimension ref="B1:CW227"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" topLeftCell="C24" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F73" sqref="F73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1661,7 +1815,8 @@
     <col min="8" max="8" width="9.140625" style="1"/>
     <col min="9" max="9" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="9.140625" style="1"/>
-    <col min="12" max="14" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="17" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="9.140625" style="1"/>
@@ -2815,7 +2970,7 @@
         <v>0.78500000000000003</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L14" s="1" t="s">
         <v>12</v>
@@ -2825,7 +2980,7 @@
         <v>1.57</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="V14" s="1" t="s">
         <v>12</v>
@@ -2835,7 +2990,7 @@
         <v>0.78500000000000003</v>
       </c>
       <c r="Z14" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AJ14" s="81">
         <v>9</v>
@@ -2927,7 +3082,7 @@
         <v>10</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L15" s="1" t="s">
         <v>19</v>
@@ -2937,7 +3092,7 @@
         <v>10</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="V15" s="1" t="s">
         <v>19</v>
@@ -2947,7 +3102,7 @@
         <v>10</v>
       </c>
       <c r="Z15" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AJ15" s="81">
         <v>10</v>
@@ -7246,6 +7401,15 @@
       <c r="CE61" s="45"/>
     </row>
     <row r="62" spans="2:101" x14ac:dyDescent="0.2">
+      <c r="M62" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="N62" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="O62" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="W62" s="4"/>
       <c r="AD62" s="4"/>
       <c r="AJ62" s="9">
@@ -7298,6 +7462,21 @@
       <c r="CA62" s="63"/>
     </row>
     <row r="63" spans="2:101" x14ac:dyDescent="0.2">
+      <c r="I63" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="K63" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="M63" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="N63" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="O63" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="W63" s="4"/>
       <c r="AD63" s="4"/>
       <c r="AJ63" s="9">
@@ -7350,799 +7529,854 @@
       <c r="CA63" s="63"/>
     </row>
     <row r="64" spans="2:101" x14ac:dyDescent="0.2">
-      <c r="W64" s="4"/>
-      <c r="AD64" s="4"/>
-      <c r="AJ64" s="9">
+      <c r="H64" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I64" s="1">
+        <v>10</v>
+      </c>
+      <c r="J64" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="AK64" s="7" cm="1">
-        <f t="array" ref="AK64:AN67">AM51:AP54</f>
-        <v>0</v>
-      </c>
-      <c r="AL64" s="7">
-        <v>0</v>
-      </c>
-      <c r="AM64" s="7">
-        <v>0</v>
-      </c>
-      <c r="AN64" s="7">
-        <v>0</v>
-      </c>
-      <c r="AO64" s="7" cm="1">
-        <f t="array" ref="AO64:AR67">AS51:AV54</f>
-        <v>1750000000</v>
-      </c>
-      <c r="AP64" s="7">
-        <v>656250</v>
-      </c>
-      <c r="AQ64" s="7">
-        <v>-4.0200183676689094E-11</v>
-      </c>
-      <c r="AR64" s="7">
-        <v>875000000</v>
-      </c>
-      <c r="AS64" s="7"/>
-      <c r="AT64" s="7" t="str">
-        <f>AX51</f>
-        <v>r33</v>
-      </c>
-      <c r="AV64" s="3" cm="1">
-        <f t="array" ref="AV64:AV67">AZ51:AZ54</f>
-        <v>-13333333.333333334</v>
-      </c>
-      <c r="BB64" s="12"/>
-      <c r="BE64" s="12"/>
-      <c r="BK64" s="7"/>
-      <c r="BL64" s="4"/>
-      <c r="BM64" s="4"/>
-      <c r="BN64" s="4"/>
-      <c r="BO64" s="4"/>
-      <c r="BP64" s="4"/>
-      <c r="BR64" s="4"/>
-      <c r="BT64" s="6"/>
-      <c r="BV64" s="4"/>
-      <c r="BY64" s="65"/>
-      <c r="CA64" s="63"/>
+      <c r="K64" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="L64" s="3">
+        <f>COS(RADIANS(I65-E4))*I64</f>
+        <v>6.1257422745431001E-16</v>
+      </c>
+      <c r="M64" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="N64" s="3">
+        <f>-I67/E6*L64</f>
+        <v>-3.06287113727155E-16</v>
+      </c>
+      <c r="O64" s="3">
+        <f>-I66/E6*L64</f>
+        <v>-3.06287113727155E-16</v>
+      </c>
+      <c r="AJ64" s="9"/>
+      <c r="AK64" s="9"/>
+      <c r="AL64" s="9"/>
+      <c r="AM64" s="9"/>
+      <c r="AN64" s="9"/>
+      <c r="AO64" s="9"/>
+      <c r="AP64" s="9"/>
+      <c r="AQ64" s="9"/>
+      <c r="AR64" s="9"/>
+      <c r="AS64" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AT64" s="145" t="s">
+        <v>52</v>
+      </c>
+      <c r="AU64" s="150" t="s">
+        <v>51</v>
+      </c>
+      <c r="AV64" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="BR64" s="66"/>
     </row>
     <row r="65" spans="5:74" x14ac:dyDescent="0.2">
+      <c r="H65" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I65" s="1">
+        <v>0</v>
+      </c>
+      <c r="J65" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K65" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="L65" s="3">
+        <f>SIN(RADIANS(I65-E4))*I64</f>
+        <v>-10</v>
+      </c>
+      <c r="M65" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="N65" s="3">
+        <f>I67^2*(3*I66+I67)/E6^3*L65</f>
+        <v>-5</v>
+      </c>
+      <c r="O65" s="3">
+        <f>I66^2*(I66+3*I67)/E6^3*L65</f>
+        <v>-5</v>
+      </c>
       <c r="AJ65" s="9">
+        <v>3</v>
+      </c>
+      <c r="AK65" s="1" t="e">
+        <f t="array" ref="AK65:AR72">MINVERSE(AK60:AR63)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AL65" s="1" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AM65" s="1" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AN65" s="1" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AO65" s="1" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AP65" s="1" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AQ65" s="1" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AR65" s="1" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AT65" s="3" cm="1">
+        <f t="array" ref="AT65:AT68">AV60:AV63</f>
+        <v>13333333.333333334</v>
+      </c>
+      <c r="AV65" s="1" t="e" cm="1">
+        <f t="array" ref="AV65">MMULT(AK65:AR72,AT65:AT72)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AW65" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AX65" s="1" t="e">
+        <f>1000*AV65</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AY65" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="BR65" s="66"/>
+    </row>
+    <row r="66" spans="5:74" x14ac:dyDescent="0.2">
+      <c r="H66" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="I66" s="1">
+        <v>2000</v>
+      </c>
+      <c r="J66" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M66" s="152" t="s">
+        <v>67</v>
+      </c>
+      <c r="N66" s="3">
+        <f>I66*I67^2/E6^2*L65</f>
+        <v>-5000</v>
+      </c>
+      <c r="O66" s="3">
+        <f>-1*I66^2*I67/E6^2*L65</f>
+        <v>5000</v>
+      </c>
+      <c r="P66" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="AJ66" s="9">
+        <v>4</v>
+      </c>
+      <c r="AK66" s="1" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AL66" s="3" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AM66" s="3" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AN66" s="1" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AO66" s="1" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AP66" s="1" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AQ66" s="1" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AR66" s="1" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AT66" s="1">
+        <v>-20000</v>
+      </c>
+      <c r="AW66" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="BC66" s="29"/>
+      <c r="BD66" s="29"/>
+      <c r="BR66" s="66"/>
+    </row>
+    <row r="67" spans="5:74" x14ac:dyDescent="0.2">
+      <c r="H67" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I67" s="25">
+        <f>E6-I66</f>
+        <v>2000</v>
+      </c>
+      <c r="M67" s="34"/>
+      <c r="AJ67" s="9">
+        <v>5</v>
+      </c>
+      <c r="AK67" s="1" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AL67" s="3" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AM67" s="3" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AN67" s="1" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AO67" s="1" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AP67" s="1" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AQ67" s="1" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AR67" s="1" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AT67" s="1">
+        <v>36280</v>
+      </c>
+      <c r="AW67" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="BR67" s="66"/>
+    </row>
+    <row r="68" spans="5:74" x14ac:dyDescent="0.2">
+      <c r="F68" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H68" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="M68" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="AJ68" s="9">
+        <v>6</v>
+      </c>
+      <c r="AK68" s="1" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AL68" s="1" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AM68" s="1" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AN68" s="1" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AO68" s="1" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AP68" s="1" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AQ68" s="1" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AR68" s="1" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AT68" s="1">
+        <v>21376666.666666664</v>
+      </c>
+      <c r="AW68" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AX68" s="1">
+        <f>1000*AV68</f>
+        <v>0</v>
+      </c>
+      <c r="AY68" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="BR68" s="66"/>
+    </row>
+    <row r="69" spans="5:74" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M69" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="AJ69" s="9">
+        <v>9</v>
+      </c>
+      <c r="AK69" s="1" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AL69" s="1" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AM69" s="1" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AN69" s="1" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AO69" s="1" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AP69" s="1" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AQ69" s="1" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AR69" s="1" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AW69" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AX69" s="1">
+        <f>1000*AV69</f>
+        <v>0</v>
+      </c>
+      <c r="AY69" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="BR69" s="66"/>
+    </row>
+    <row r="70" spans="5:74" x14ac:dyDescent="0.2">
+      <c r="E70" s="26"/>
+      <c r="M70" s="152" t="s">
+        <v>67</v>
+      </c>
+      <c r="AG70" s="2"/>
+      <c r="AH70" s="2"/>
+      <c r="AJ70" s="9">
         <v>10</v>
       </c>
-      <c r="AK65" s="7">
-        <v>0</v>
-      </c>
-      <c r="AL65" s="7">
-        <v>-700000</v>
-      </c>
-      <c r="AM65" s="7">
-        <v>0</v>
-      </c>
-      <c r="AN65" s="7">
-        <v>0</v>
-      </c>
-      <c r="AO65" s="7">
-        <v>656250</v>
-      </c>
-      <c r="AP65" s="7">
-        <v>700328.125</v>
-      </c>
-      <c r="AQ65" s="7">
-        <v>3.2140046849512931E-11</v>
-      </c>
-      <c r="AR65" s="7">
-        <v>656250</v>
-      </c>
-      <c r="AS65" s="7"/>
-      <c r="AT65" s="7" t="str">
-        <f>AX52</f>
-        <v>r41</v>
-      </c>
-      <c r="AV65" s="1">
-        <v>20000</v>
-      </c>
-      <c r="BB65" s="12"/>
-      <c r="BE65" s="12"/>
-    </row>
-    <row r="66" spans="5:74" x14ac:dyDescent="0.2">
-      <c r="AJ66" s="9">
+      <c r="AK70" s="1" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AL70" s="1" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AM70" s="1" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AN70" s="1" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AO70" s="3" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AP70" s="1" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AQ70" s="1" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AR70" s="1" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AW70" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="71" spans="5:74" x14ac:dyDescent="0.2">
+      <c r="AG71" s="2"/>
+      <c r="AH71" s="2"/>
+      <c r="AI71" s="2"/>
+      <c r="AJ71" s="9">
         <v>11</v>
       </c>
-      <c r="AK66" s="3">
-        <v>0</v>
-      </c>
-      <c r="AL66" s="3">
-        <v>0</v>
-      </c>
-      <c r="AM66" s="3">
-        <v>-777.77777777777783</v>
-      </c>
-      <c r="AN66" s="3">
-        <v>-2333333.3333333335</v>
-      </c>
-      <c r="AO66" s="3">
-        <v>-4.0200183676689094E-11</v>
-      </c>
-      <c r="AP66" s="3">
-        <v>3.2140046849512931E-11</v>
-      </c>
-      <c r="AQ66" s="3">
-        <v>525777.77777777775</v>
-      </c>
-      <c r="AR66" s="3">
-        <v>-2333333.3333333335</v>
-      </c>
-      <c r="AS66" s="3"/>
-      <c r="AT66" s="7" t="str">
-        <f>AX53</f>
-        <v>r42</v>
-      </c>
-      <c r="AV66" s="1">
-        <v>36280</v>
-      </c>
-    </row>
-    <row r="67" spans="5:74" x14ac:dyDescent="0.2">
-      <c r="AJ67" s="9">
+      <c r="AK71" s="1" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AL71" s="1" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AM71" s="1" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AN71" s="1" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AO71" s="3" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AP71" s="1" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AQ71" s="1" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AR71" s="1" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AW71" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" spans="5:74" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F72" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="H72" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="M72" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="AJ72" s="9">
         <v>12</v>
       </c>
-      <c r="AK67" s="3">
-        <v>0</v>
-      </c>
-      <c r="AL67" s="3">
-        <v>0</v>
-      </c>
-      <c r="AM67" s="3">
-        <v>2333333.3333333335</v>
-      </c>
-      <c r="AN67" s="3">
-        <v>4666666666.666667</v>
-      </c>
-      <c r="AO67" s="3">
-        <v>875000000</v>
-      </c>
-      <c r="AP67" s="3">
-        <v>656250</v>
-      </c>
-      <c r="AQ67" s="3">
-        <v>-2333333.3333333335</v>
-      </c>
-      <c r="AR67" s="3">
-        <v>11083333333.333334</v>
-      </c>
-      <c r="AS67" s="3"/>
-      <c r="AT67" s="7" t="str">
-        <f>AX54</f>
-        <v>r43</v>
-      </c>
-      <c r="AV67" s="1">
-        <v>-21376666.666666664</v>
-      </c>
-    </row>
-    <row r="68" spans="5:74" x14ac:dyDescent="0.2">
-      <c r="BO68" s="2"/>
-      <c r="BR68" s="66"/>
-    </row>
-    <row r="69" spans="5:74" x14ac:dyDescent="0.2">
-      <c r="AJ69" s="2" t="s">
+      <c r="AK72" s="1" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AL72" s="1" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AM72" s="1" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AN72" s="1" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AO72" s="1" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AP72" s="1" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AQ72" s="1" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AR72" s="1" t="e">
+        <v>#VALUE!</v>
+      </c>
+      <c r="AW72" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AX72" s="1">
+        <f>1000*AV72</f>
+        <v>0</v>
+      </c>
+      <c r="AY72" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="BR69" s="66"/>
-    </row>
-    <row r="70" spans="5:74" x14ac:dyDescent="0.2">
-      <c r="AJ70" s="9"/>
-      <c r="AK70" s="9"/>
-      <c r="AL70" s="9"/>
-      <c r="AM70" s="9"/>
-      <c r="AN70" s="9"/>
-      <c r="AO70" s="9"/>
-      <c r="AP70" s="9"/>
-      <c r="AQ70" s="9"/>
-      <c r="AR70" s="9"/>
-      <c r="AS70" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="AT70" s="145" t="s">
-        <v>52</v>
-      </c>
-      <c r="AU70" s="150" t="s">
-        <v>51</v>
-      </c>
-      <c r="AV70" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="BR70" s="66"/>
-    </row>
-    <row r="71" spans="5:74" x14ac:dyDescent="0.2">
-      <c r="AJ71" s="9">
-        <v>3</v>
-      </c>
-      <c r="AK71" s="1">
-        <f t="array" ref="AK71:AR78">MINVERSE(AK60:AR67)</f>
-        <v>1.485340598131857E-9</v>
-      </c>
-      <c r="AL71" s="1">
-        <v>-2.4291188322375727E-6</v>
-      </c>
-      <c r="AM71" s="1">
-        <v>-3.1746031746004912E-10</v>
-      </c>
-      <c r="AN71" s="1">
-        <v>-5.9849292283921501E-12</v>
-      </c>
-      <c r="AO71" s="1">
-        <v>8.7201389922218198E-10</v>
-      </c>
-      <c r="AP71" s="1">
-        <v>-2.4288705857505882E-6</v>
-      </c>
-      <c r="AQ71" s="1">
-        <v>3.1746031746034778E-10</v>
-      </c>
-      <c r="AR71" s="1">
-        <v>7.7625140868576821E-11</v>
-      </c>
-      <c r="AT71" s="3" cm="1">
-        <f t="array" ref="AT71:AT78">AV60:AV67</f>
-        <v>13333333.333333334</v>
-      </c>
-      <c r="AV71" s="1" cm="1">
-        <f t="array" ref="AV71:AV78">MMULT(AK71:AR78,AT71:AT78)</f>
-        <v>6.395349650095826E-3</v>
-      </c>
-      <c r="AW71" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="AX71" s="1">
-        <f>1000*AV71</f>
-        <v>6.3953496500958256</v>
-      </c>
-      <c r="AY71" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="BR71" s="66"/>
-    </row>
-    <row r="72" spans="5:74" x14ac:dyDescent="0.2">
-      <c r="AJ72" s="9">
-        <v>4</v>
-      </c>
-      <c r="AK72" s="1">
-        <v>-2.4291188322375723E-6</v>
-      </c>
-      <c r="AL72" s="3">
-        <v>6.6687169148831986E-3</v>
-      </c>
-      <c r="AM72" s="3">
-        <v>1.2698412698405332E-6</v>
-      </c>
-      <c r="AN72" s="1">
-        <v>-1.4330002168725296E-7</v>
-      </c>
-      <c r="AO72" s="1">
-        <v>-2.4288705857505873E-6</v>
-      </c>
-      <c r="AP72" s="1">
-        <v>6.6680026618329271E-3</v>
-      </c>
-      <c r="AQ72" s="1">
-        <v>-1.2698412698413532E-6</v>
-      </c>
-      <c r="AR72" s="1">
-        <v>-1.4326082487351951E-7</v>
-      </c>
-      <c r="AT72" s="1">
-        <v>-20000</v>
-      </c>
-      <c r="AV72" s="1">
-        <v>-1.8432911386823125E-2</v>
-      </c>
-      <c r="AW72" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="BC72" s="29"/>
-      <c r="BD72" s="29"/>
-      <c r="BR72" s="66"/>
-    </row>
-    <row r="73" spans="5:74" x14ac:dyDescent="0.2">
-      <c r="AJ73" s="9">
-        <v>5</v>
-      </c>
-      <c r="AK73" s="1">
-        <v>-3.1746031746013711E-10</v>
-      </c>
-      <c r="AL73" s="3">
-        <v>1.2698412698411596E-6</v>
-      </c>
-      <c r="AM73" s="3">
-        <v>1.9047619047619047E-6</v>
-      </c>
-      <c r="AN73" s="1">
-        <v>-3.1746031746026796E-10</v>
-      </c>
-      <c r="AO73" s="1">
-        <v>-3.174603174602724E-10</v>
-      </c>
-      <c r="AP73" s="1">
-        <v>1.2698412698409161E-6</v>
-      </c>
-      <c r="AQ73" s="1">
-        <v>-3.8064789415719652E-22</v>
-      </c>
-      <c r="AR73" s="1">
-        <v>-3.1746031746016089E-10</v>
-      </c>
-      <c r="AT73" s="1">
-        <v>36280</v>
-      </c>
-      <c r="AV73" s="1">
-        <v>6.9104761904756534E-2</v>
-      </c>
-      <c r="AW73" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="BR73" s="66"/>
+    </row>
+    <row r="73" spans="5:74" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M73" s="34" t="s">
+        <v>66</v>
+      </c>
+      <c r="BB73" s="4"/>
+      <c r="BK73" s="2"/>
     </row>
     <row r="74" spans="5:74" x14ac:dyDescent="0.2">
-      <c r="AJ74" s="9">
-        <v>6</v>
-      </c>
-      <c r="AK74" s="1">
-        <v>-5.9849292283919748E-12</v>
-      </c>
-      <c r="AL74" s="1">
-        <v>-1.4330002168725354E-7</v>
-      </c>
-      <c r="AM74" s="1">
-        <v>-3.1746031746030166E-10</v>
-      </c>
-      <c r="AN74" s="1">
-        <v>1.1944487472222402E-10</v>
-      </c>
-      <c r="AO74" s="1">
-        <v>7.7625140868576614E-11</v>
-      </c>
-      <c r="AP74" s="1">
-        <v>-1.4326082487351898E-7</v>
-      </c>
-      <c r="AQ74" s="1">
-        <v>3.1746031746031929E-10</v>
-      </c>
-      <c r="AR74" s="1">
-        <v>-4.780466308201401E-11</v>
-      </c>
-      <c r="AT74" s="1">
-        <v>21376666.666666664</v>
-      </c>
-      <c r="AV74" s="1">
-        <v>2.4612206214437047E-3</v>
-      </c>
-      <c r="AW74" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="AX74" s="1">
-        <f>1000*AV74</f>
-        <v>2.4612206214437049</v>
-      </c>
-      <c r="AY74" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="BR74" s="66"/>
+      <c r="M74" s="152" t="s">
+        <v>67</v>
+      </c>
+      <c r="AZ74" s="12"/>
+      <c r="BB74" s="12"/>
+      <c r="BE74" s="12"/>
+      <c r="BK74" s="6"/>
+      <c r="BL74" s="6"/>
+      <c r="BM74" s="6"/>
+      <c r="BN74" s="6"/>
+      <c r="BO74" s="6"/>
+      <c r="BP74" s="6"/>
+      <c r="BR74" s="67"/>
+      <c r="BT74" s="4"/>
+      <c r="BV74" s="68"/>
     </row>
     <row r="75" spans="5:74" x14ac:dyDescent="0.2">
-      <c r="AJ75" s="9">
-        <v>9</v>
-      </c>
-      <c r="AK75" s="1">
-        <v>8.7201389922218157E-10</v>
-      </c>
-      <c r="AL75" s="1">
-        <v>-2.4288705857505873E-6</v>
-      </c>
-      <c r="AM75" s="1">
-        <v>-3.1746031746004912E-10</v>
-      </c>
-      <c r="AN75" s="1">
-        <v>7.7625140868576395E-11</v>
-      </c>
-      <c r="AO75" s="1">
-        <v>1.4853405981318572E-9</v>
-      </c>
-      <c r="AP75" s="1">
-        <v>-2.4291188322375736E-6</v>
-      </c>
-      <c r="AQ75" s="1">
-        <v>3.1746031746034788E-10</v>
-      </c>
-      <c r="AR75" s="1">
-        <v>-5.9849292283917535E-12</v>
-      </c>
-      <c r="AT75" s="1">
-        <v>-13333333.333333334</v>
-      </c>
-      <c r="AV75" s="1">
-        <v>-6.3953496500958676E-3</v>
-      </c>
-      <c r="AW75" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="AX75" s="1">
-        <f>1000*AV75</f>
-        <v>-6.3953496500958673</v>
-      </c>
-      <c r="AY75" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="BR75" s="66"/>
+      <c r="G75" s="151"/>
+      <c r="M75" s="34"/>
+      <c r="AZ75" s="12"/>
+      <c r="BB75" s="12"/>
+      <c r="BE75" s="12"/>
+      <c r="BK75" s="6"/>
+      <c r="BL75" s="6"/>
+      <c r="BM75" s="6"/>
+      <c r="BN75" s="6"/>
+      <c r="BO75" s="6"/>
+      <c r="BP75" s="6"/>
+      <c r="BR75" s="67"/>
+      <c r="BT75" s="4"/>
+      <c r="BV75" s="68"/>
     </row>
     <row r="76" spans="5:74" x14ac:dyDescent="0.2">
-      <c r="E76" s="26"/>
-      <c r="F76" s="25"/>
-      <c r="AG76" s="2"/>
-      <c r="AH76" s="2"/>
-      <c r="AJ76" s="9">
-        <v>10</v>
-      </c>
-      <c r="AK76" s="1">
-        <v>-2.4288705857505865E-6</v>
-      </c>
-      <c r="AL76" s="1">
-        <v>6.6680026618329237E-3</v>
-      </c>
-      <c r="AM76" s="1">
-        <v>1.2698412698405332E-6</v>
-      </c>
-      <c r="AN76" s="1">
-        <v>-1.432608248735184E-7</v>
-      </c>
-      <c r="AO76" s="3">
-        <v>-2.4291188322375727E-6</v>
-      </c>
-      <c r="AP76" s="1">
-        <v>6.6687169148832003E-3</v>
-      </c>
-      <c r="AQ76" s="1">
-        <v>-1.2698412698413532E-6</v>
-      </c>
-      <c r="AR76" s="1">
-        <v>-1.4330002168725404E-7</v>
-      </c>
-      <c r="AT76" s="1">
-        <v>20000</v>
-      </c>
-      <c r="AV76" s="1">
-        <v>1.8432911386937256E-2</v>
-      </c>
-      <c r="AW76" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="F76" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="M76" s="34"/>
+      <c r="AZ76" s="12"/>
+      <c r="BB76" s="12"/>
+      <c r="BE76" s="12"/>
+      <c r="BK76" s="6"/>
+      <c r="BL76" s="6"/>
+      <c r="BM76" s="6"/>
+      <c r="BN76" s="6"/>
+      <c r="BO76" s="6"/>
+      <c r="BP76" s="6"/>
+      <c r="BQ76" s="4"/>
+      <c r="BR76" s="67"/>
+      <c r="BS76" s="4"/>
+      <c r="BT76" s="4"/>
+      <c r="BU76" s="4"/>
+      <c r="BV76" s="68"/>
     </row>
     <row r="77" spans="5:74" x14ac:dyDescent="0.2">
-      <c r="AG77" s="2"/>
-      <c r="AH77" s="2"/>
-      <c r="AI77" s="2"/>
-      <c r="AJ77" s="9">
-        <v>11</v>
-      </c>
-      <c r="AK77" s="1">
-        <v>3.1746031746034638E-10</v>
-      </c>
-      <c r="AL77" s="1">
-        <v>-1.2698412698413493E-6</v>
-      </c>
-      <c r="AM77" s="1">
-        <v>6.2275328606048644E-23</v>
-      </c>
-      <c r="AN77" s="1">
-        <v>3.1746031746031909E-10</v>
-      </c>
-      <c r="AO77" s="3">
-        <v>3.1746031746034654E-10</v>
-      </c>
-      <c r="AP77" s="1">
-        <v>-1.2698412698413498E-6</v>
-      </c>
-      <c r="AQ77" s="1">
-        <v>1.9047619047619049E-6</v>
-      </c>
-      <c r="AR77" s="1">
-        <v>3.1746031746031929E-10</v>
-      </c>
-      <c r="AT77" s="1">
-        <v>36280</v>
-      </c>
-      <c r="AV77" s="1">
-        <v>6.9104761904761891E-2</v>
-      </c>
-      <c r="AW77" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="M77" s="152"/>
+      <c r="AZ77" s="30"/>
+      <c r="BB77" s="4"/>
+      <c r="BE77" s="4"/>
+      <c r="BK77" s="6"/>
+      <c r="BL77" s="6"/>
+      <c r="BM77" s="6"/>
+      <c r="BN77" s="6"/>
+      <c r="BO77" s="6"/>
+      <c r="BP77" s="6"/>
+      <c r="BR77" s="67"/>
+      <c r="BT77" s="4"/>
+      <c r="BV77" s="68"/>
     </row>
     <row r="78" spans="5:74" x14ac:dyDescent="0.2">
-      <c r="AJ78" s="9">
-        <v>12</v>
-      </c>
-      <c r="AK78" s="1">
-        <v>7.7625140868576589E-11</v>
-      </c>
-      <c r="AL78" s="1">
-        <v>-1.4326082487351892E-7</v>
-      </c>
-      <c r="AM78" s="1">
-        <v>-3.1746031746030166E-10</v>
-      </c>
-      <c r="AN78" s="1">
-        <v>-4.7804663082014004E-11</v>
-      </c>
-      <c r="AO78" s="1">
-        <v>-5.9849292283919458E-12</v>
-      </c>
-      <c r="AP78" s="1">
-        <v>-1.4330002168725351E-7</v>
-      </c>
-      <c r="AQ78" s="1">
-        <v>3.1746031746031924E-10</v>
-      </c>
-      <c r="AR78" s="1">
-        <v>1.1944487472222405E-10</v>
-      </c>
-      <c r="AT78" s="1">
-        <v>-21376666.666666664</v>
-      </c>
-      <c r="AV78" s="1">
-        <v>-2.461220621443706E-3</v>
-      </c>
-      <c r="AW78" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="AX78" s="1">
-        <f>1000*AV78</f>
-        <v>-2.4612206214437062</v>
-      </c>
-      <c r="AY78" s="1" t="s">
-        <v>59</v>
-      </c>
+      <c r="AZ78" s="4"/>
+      <c r="BB78" s="4"/>
+      <c r="BE78" s="12"/>
+      <c r="BK78" s="6"/>
+      <c r="BL78" s="6"/>
+      <c r="BM78" s="6"/>
+      <c r="BN78" s="6"/>
+      <c r="BO78" s="6"/>
+      <c r="BP78" s="6"/>
+      <c r="BR78" s="67"/>
+      <c r="BT78" s="4"/>
+      <c r="BV78" s="68"/>
     </row>
     <row r="79" spans="5:74" x14ac:dyDescent="0.2">
+      <c r="AY79" s="4"/>
+      <c r="AZ79" s="30"/>
+      <c r="BA79" s="4"/>
       <c r="BB79" s="4"/>
-      <c r="BK79" s="2"/>
+      <c r="BC79" s="28"/>
+      <c r="BD79" s="28"/>
+      <c r="BE79" s="12"/>
+      <c r="BK79" s="6"/>
+      <c r="BL79" s="6"/>
+      <c r="BM79" s="6"/>
+      <c r="BN79" s="6"/>
+      <c r="BO79" s="6"/>
+      <c r="BP79" s="6"/>
+      <c r="BR79" s="67"/>
+      <c r="BT79" s="4"/>
+      <c r="BV79" s="68"/>
     </row>
     <row r="80" spans="5:74" x14ac:dyDescent="0.2">
-      <c r="AZ80" s="12"/>
-      <c r="BB80" s="12"/>
+      <c r="AY80" s="4"/>
+      <c r="AZ80" s="30"/>
+      <c r="BA80" s="4"/>
+      <c r="BB80" s="4"/>
+      <c r="BC80" s="28"/>
+      <c r="BD80" s="28"/>
       <c r="BE80" s="12"/>
-      <c r="BK80" s="6"/>
-      <c r="BL80" s="6"/>
-      <c r="BM80" s="6"/>
-      <c r="BN80" s="6"/>
-      <c r="BO80" s="6"/>
-      <c r="BP80" s="6"/>
-      <c r="BR80" s="67"/>
-      <c r="BT80" s="4"/>
-      <c r="BV80" s="68"/>
-    </row>
-    <row r="81" spans="51:83" x14ac:dyDescent="0.2">
-      <c r="AZ81" s="12"/>
+    </row>
+    <row r="81" spans="52:83" x14ac:dyDescent="0.2">
+      <c r="AZ81" s="4"/>
       <c r="BB81" s="12"/>
       <c r="BE81" s="12"/>
-      <c r="BK81" s="6"/>
-      <c r="BL81" s="6"/>
-      <c r="BM81" s="6"/>
-      <c r="BN81" s="6"/>
-      <c r="BO81" s="6"/>
-      <c r="BP81" s="6"/>
-      <c r="BR81" s="67"/>
-      <c r="BT81" s="4"/>
-      <c r="BV81" s="68"/>
-    </row>
-    <row r="82" spans="51:83" x14ac:dyDescent="0.2">
-      <c r="AZ82" s="12"/>
+      <c r="BK81" s="2"/>
+    </row>
+    <row r="82" spans="52:83" x14ac:dyDescent="0.2">
+      <c r="AZ82" s="4"/>
       <c r="BB82" s="12"/>
       <c r="BE82" s="12"/>
-      <c r="BK82" s="6"/>
-      <c r="BL82" s="6"/>
-      <c r="BM82" s="6"/>
-      <c r="BN82" s="6"/>
-      <c r="BO82" s="6"/>
-      <c r="BP82" s="6"/>
-      <c r="BQ82" s="4"/>
+      <c r="BK82" s="7"/>
+      <c r="BL82" s="7"/>
+      <c r="BM82" s="7"/>
+      <c r="BN82" s="7"/>
+      <c r="BO82" s="7"/>
+      <c r="BP82" s="7"/>
       <c r="BR82" s="67"/>
-      <c r="BS82" s="4"/>
-      <c r="BT82" s="4"/>
-      <c r="BU82" s="4"/>
-      <c r="BV82" s="68"/>
-    </row>
-    <row r="83" spans="51:83" x14ac:dyDescent="0.2">
-      <c r="AZ83" s="30"/>
-      <c r="BB83" s="4"/>
-      <c r="BE83" s="4"/>
-      <c r="BK83" s="6"/>
-      <c r="BL83" s="6"/>
-      <c r="BM83" s="6"/>
-      <c r="BN83" s="6"/>
-      <c r="BO83" s="6"/>
-      <c r="BP83" s="6"/>
+      <c r="BT82" s="6"/>
+      <c r="BV82" s="4"/>
+      <c r="BY82" s="65"/>
+      <c r="CA82" s="63"/>
+    </row>
+    <row r="83" spans="52:83" x14ac:dyDescent="0.2">
+      <c r="AZ83" s="12"/>
+      <c r="BB83" s="12"/>
+      <c r="BE83" s="12"/>
+      <c r="BK83" s="7"/>
+      <c r="BL83" s="7"/>
+      <c r="BM83" s="7"/>
+      <c r="BN83" s="7"/>
+      <c r="BO83" s="7"/>
+      <c r="BP83" s="7"/>
       <c r="BR83" s="67"/>
-      <c r="BT83" s="4"/>
-      <c r="BV83" s="68"/>
-    </row>
-    <row r="84" spans="51:83" x14ac:dyDescent="0.2">
-      <c r="AZ84" s="4"/>
-      <c r="BB84" s="4"/>
+      <c r="BT83" s="7"/>
+      <c r="BV83" s="4"/>
+      <c r="BY83" s="65"/>
+      <c r="CA83" s="63"/>
+      <c r="CE83" s="45"/>
+    </row>
+    <row r="84" spans="52:83" x14ac:dyDescent="0.2">
+      <c r="AZ84" s="12"/>
+      <c r="BB84" s="12"/>
       <c r="BE84" s="12"/>
-      <c r="BK84" s="6"/>
-      <c r="BL84" s="6"/>
-      <c r="BM84" s="6"/>
-      <c r="BN84" s="6"/>
-      <c r="BO84" s="6"/>
-      <c r="BP84" s="6"/>
+      <c r="BK84" s="7"/>
+      <c r="BL84" s="7"/>
+      <c r="BM84" s="7"/>
+      <c r="BN84" s="7"/>
+      <c r="BO84" s="7"/>
+      <c r="BP84" s="7"/>
+      <c r="BQ84" s="4"/>
       <c r="BR84" s="67"/>
-      <c r="BT84" s="4"/>
-      <c r="BV84" s="68"/>
-    </row>
-    <row r="85" spans="51:83" x14ac:dyDescent="0.2">
-      <c r="AY85" s="4"/>
-      <c r="AZ85" s="30"/>
-      <c r="BA85" s="4"/>
+      <c r="BS84" s="4"/>
+      <c r="BT84" s="7"/>
+      <c r="BU84" s="4"/>
+      <c r="BV84" s="4"/>
+      <c r="BW84" s="4"/>
+      <c r="BX84" s="4"/>
+      <c r="BY84" s="65"/>
+      <c r="BZ84" s="4"/>
+      <c r="CA84" s="63"/>
+    </row>
+    <row r="85" spans="52:83" x14ac:dyDescent="0.2">
+      <c r="AZ85" s="4"/>
       <c r="BB85" s="4"/>
-      <c r="BC85" s="28"/>
-      <c r="BD85" s="28"/>
       <c r="BE85" s="12"/>
-      <c r="BK85" s="6"/>
-      <c r="BL85" s="6"/>
-      <c r="BM85" s="6"/>
-      <c r="BN85" s="6"/>
-      <c r="BO85" s="6"/>
-      <c r="BP85" s="6"/>
+      <c r="BK85" s="7"/>
+      <c r="BL85" s="7"/>
+      <c r="BM85" s="7"/>
+      <c r="BN85" s="7"/>
+      <c r="BO85" s="7"/>
+      <c r="BP85" s="7"/>
       <c r="BR85" s="67"/>
-      <c r="BT85" s="4"/>
-      <c r="BV85" s="68"/>
-    </row>
-    <row r="86" spans="51:83" x14ac:dyDescent="0.2">
-      <c r="AY86" s="4"/>
-      <c r="AZ86" s="30"/>
-      <c r="BA86" s="4"/>
+      <c r="BT85" s="6"/>
+      <c r="BV85" s="4"/>
+      <c r="BY85" s="65"/>
+      <c r="CA85" s="63"/>
+    </row>
+    <row r="86" spans="52:83" x14ac:dyDescent="0.2">
+      <c r="AZ86" s="4"/>
       <c r="BB86" s="4"/>
-      <c r="BC86" s="28"/>
-      <c r="BD86" s="28"/>
       <c r="BE86" s="12"/>
-    </row>
-    <row r="87" spans="51:83" x14ac:dyDescent="0.2">
+      <c r="BK86" s="7"/>
+      <c r="BL86" s="7"/>
+      <c r="BM86" s="7"/>
+      <c r="BN86" s="7"/>
+      <c r="BO86" s="7"/>
+      <c r="BP86" s="7"/>
+      <c r="BR86" s="67"/>
+      <c r="BT86" s="7"/>
+      <c r="BV86" s="4"/>
+      <c r="BY86" s="65"/>
+      <c r="CA86" s="63"/>
+    </row>
+    <row r="87" spans="52:83" x14ac:dyDescent="0.2">
       <c r="AZ87" s="4"/>
-      <c r="BB87" s="12"/>
+      <c r="BB87" s="4"/>
       <c r="BE87" s="12"/>
-      <c r="BK87" s="2"/>
-    </row>
-    <row r="88" spans="51:83" x14ac:dyDescent="0.2">
-      <c r="AZ88" s="4"/>
-      <c r="BB88" s="12"/>
-      <c r="BE88" s="12"/>
-      <c r="BK88" s="7"/>
-      <c r="BL88" s="7"/>
-      <c r="BM88" s="7"/>
-      <c r="BN88" s="7"/>
-      <c r="BO88" s="7"/>
-      <c r="BP88" s="7"/>
-      <c r="BR88" s="67"/>
-      <c r="BT88" s="6"/>
-      <c r="BV88" s="4"/>
-      <c r="BY88" s="65"/>
-      <c r="CA88" s="63"/>
-    </row>
-    <row r="89" spans="51:83" x14ac:dyDescent="0.2">
-      <c r="AZ89" s="12"/>
-      <c r="BB89" s="12"/>
-      <c r="BE89" s="12"/>
-      <c r="BK89" s="7"/>
-      <c r="BL89" s="7"/>
-      <c r="BM89" s="7"/>
-      <c r="BN89" s="7"/>
-      <c r="BO89" s="7"/>
-      <c r="BP89" s="7"/>
-      <c r="BR89" s="67"/>
-      <c r="BT89" s="7"/>
-      <c r="BV89" s="4"/>
-      <c r="BY89" s="65"/>
-      <c r="CA89" s="63"/>
-      <c r="CE89" s="45"/>
-    </row>
-    <row r="90" spans="51:83" x14ac:dyDescent="0.2">
-      <c r="AZ90" s="12"/>
-      <c r="BB90" s="12"/>
-      <c r="BE90" s="12"/>
-      <c r="BK90" s="7"/>
-      <c r="BL90" s="7"/>
-      <c r="BM90" s="7"/>
-      <c r="BN90" s="7"/>
-      <c r="BO90" s="7"/>
-      <c r="BP90" s="7"/>
-      <c r="BQ90" s="4"/>
-      <c r="BR90" s="67"/>
-      <c r="BS90" s="4"/>
-      <c r="BT90" s="7"/>
-      <c r="BU90" s="4"/>
-      <c r="BV90" s="4"/>
-      <c r="BW90" s="4"/>
-      <c r="BX90" s="4"/>
-      <c r="BY90" s="65"/>
-      <c r="BZ90" s="4"/>
-      <c r="CA90" s="63"/>
-    </row>
-    <row r="91" spans="51:83" x14ac:dyDescent="0.2">
-      <c r="AZ91" s="4"/>
-      <c r="BB91" s="4"/>
-      <c r="BE91" s="12"/>
-      <c r="BK91" s="7"/>
-      <c r="BL91" s="7"/>
-      <c r="BM91" s="7"/>
-      <c r="BN91" s="7"/>
-      <c r="BO91" s="7"/>
-      <c r="BP91" s="7"/>
-      <c r="BR91" s="67"/>
-      <c r="BT91" s="6"/>
-      <c r="BV91" s="4"/>
-      <c r="BY91" s="65"/>
-      <c r="CA91" s="63"/>
-    </row>
-    <row r="92" spans="51:83" x14ac:dyDescent="0.2">
-      <c r="AZ92" s="4"/>
-      <c r="BB92" s="4"/>
-      <c r="BE92" s="12"/>
-      <c r="BK92" s="7"/>
-      <c r="BL92" s="7"/>
-      <c r="BM92" s="7"/>
-      <c r="BN92" s="7"/>
-      <c r="BO92" s="7"/>
-      <c r="BP92" s="7"/>
-      <c r="BR92" s="67"/>
-      <c r="BT92" s="7"/>
-      <c r="BV92" s="4"/>
-      <c r="BY92" s="65"/>
-      <c r="CA92" s="63"/>
-    </row>
-    <row r="93" spans="51:83" x14ac:dyDescent="0.2">
-      <c r="AZ93" s="4"/>
-      <c r="BB93" s="4"/>
-      <c r="BE93" s="12"/>
-      <c r="BK93" s="7"/>
-      <c r="BL93" s="7"/>
-      <c r="BM93" s="7"/>
-      <c r="BN93" s="7"/>
-      <c r="BO93" s="7"/>
-      <c r="BP93" s="7"/>
-      <c r="BR93" s="67"/>
-      <c r="BT93" s="7"/>
-      <c r="BV93" s="4"/>
-      <c r="BY93" s="65"/>
-      <c r="CA93" s="63"/>
-    </row>
-    <row r="100" spans="23:77" x14ac:dyDescent="0.2">
-      <c r="BC100" s="29"/>
-      <c r="BD100" s="29"/>
-    </row>
-    <row r="107" spans="23:77" x14ac:dyDescent="0.2">
-      <c r="BB107" s="4"/>
-    </row>
-    <row r="108" spans="23:77" x14ac:dyDescent="0.2">
-      <c r="AZ108" s="12"/>
+      <c r="BK87" s="7"/>
+      <c r="BL87" s="7"/>
+      <c r="BM87" s="7"/>
+      <c r="BN87" s="7"/>
+      <c r="BO87" s="7"/>
+      <c r="BP87" s="7"/>
+      <c r="BR87" s="67"/>
+      <c r="BT87" s="7"/>
+      <c r="BV87" s="4"/>
+      <c r="BY87" s="65"/>
+      <c r="CA87" s="63"/>
+    </row>
+    <row r="94" spans="52:83" x14ac:dyDescent="0.2">
+      <c r="BC94" s="29"/>
+      <c r="BD94" s="29"/>
+    </row>
+    <row r="101" spans="23:79" x14ac:dyDescent="0.2">
+      <c r="BB101" s="4"/>
+    </row>
+    <row r="102" spans="23:79" x14ac:dyDescent="0.2">
+      <c r="AZ102" s="12"/>
+      <c r="BB102" s="12"/>
+      <c r="BE102" s="12"/>
+      <c r="BK102" s="2"/>
+    </row>
+    <row r="103" spans="23:79" x14ac:dyDescent="0.2">
+      <c r="AZ103" s="12"/>
+      <c r="BB103" s="12"/>
+      <c r="BE103" s="12"/>
+      <c r="BK103" s="6"/>
+      <c r="BL103" s="6"/>
+      <c r="BM103" s="6"/>
+      <c r="BN103" s="6"/>
+      <c r="BO103" s="6"/>
+      <c r="BP103" s="6"/>
+      <c r="BR103" s="4"/>
+      <c r="BT103" s="4"/>
+      <c r="BV103" s="4"/>
+      <c r="BY103" s="4"/>
+    </row>
+    <row r="104" spans="23:79" x14ac:dyDescent="0.2">
+      <c r="W104" s="7"/>
+      <c r="X104" s="4"/>
+      <c r="Y104" s="4"/>
+      <c r="Z104" s="4"/>
+      <c r="AA104" s="4"/>
+      <c r="AB104" s="4"/>
+      <c r="AC104" s="4"/>
+      <c r="AD104" s="4"/>
+      <c r="AE104" s="4"/>
+      <c r="AF104" s="4"/>
+      <c r="AZ104" s="12"/>
+      <c r="BB104" s="12"/>
+      <c r="BE104" s="12"/>
+      <c r="BK104" s="6"/>
+      <c r="BL104" s="6"/>
+      <c r="BM104" s="6"/>
+      <c r="BN104" s="6"/>
+      <c r="BO104" s="6"/>
+      <c r="BP104" s="6"/>
+      <c r="BR104" s="4"/>
+      <c r="BT104" s="4"/>
+      <c r="BV104" s="4"/>
+      <c r="BY104" s="4"/>
+    </row>
+    <row r="105" spans="23:79" x14ac:dyDescent="0.2">
+      <c r="W105" s="4"/>
+      <c r="X105" s="7"/>
+      <c r="Y105" s="4"/>
+      <c r="Z105" s="4"/>
+      <c r="AA105" s="4"/>
+      <c r="AB105" s="4"/>
+      <c r="AC105" s="4"/>
+      <c r="AD105" s="4"/>
+      <c r="AE105" s="7"/>
+      <c r="AF105" s="4"/>
+      <c r="AZ105" s="30"/>
+      <c r="BB105" s="4"/>
+      <c r="BE105" s="4"/>
+      <c r="BK105" s="6"/>
+      <c r="BL105" s="6"/>
+      <c r="BM105" s="6"/>
+      <c r="BN105" s="6"/>
+      <c r="BO105" s="6"/>
+      <c r="BP105" s="6"/>
+      <c r="BQ105" s="4"/>
+      <c r="BR105" s="4"/>
+      <c r="BS105" s="4"/>
+      <c r="BT105" s="4"/>
+      <c r="BU105" s="4"/>
+      <c r="BV105" s="4"/>
+      <c r="BW105" s="4"/>
+      <c r="BX105" s="4"/>
+      <c r="BY105" s="4"/>
+    </row>
+    <row r="106" spans="23:79" x14ac:dyDescent="0.2">
+      <c r="W106" s="4"/>
+      <c r="X106" s="4"/>
+      <c r="Y106" s="7"/>
+      <c r="Z106" s="4"/>
+      <c r="AA106" s="7"/>
+      <c r="AB106" s="4"/>
+      <c r="AC106" s="4"/>
+      <c r="AD106" s="4"/>
+      <c r="AE106" s="4"/>
+      <c r="AF106" s="7"/>
+      <c r="AZ106" s="4"/>
+      <c r="BB106" s="4"/>
+      <c r="BE106" s="4"/>
+      <c r="BK106" s="6"/>
+      <c r="BL106" s="6"/>
+      <c r="BM106" s="6"/>
+      <c r="BN106" s="6"/>
+      <c r="BO106" s="6"/>
+      <c r="BP106" s="6"/>
+      <c r="BR106" s="67"/>
+      <c r="BT106" s="4"/>
+      <c r="BV106" s="4"/>
+      <c r="BY106" s="4"/>
+    </row>
+    <row r="107" spans="23:79" x14ac:dyDescent="0.2">
+      <c r="W107" s="4"/>
+      <c r="X107" s="4"/>
+      <c r="Y107" s="4"/>
+      <c r="Z107" s="4"/>
+      <c r="AA107" s="4"/>
+      <c r="AB107" s="4"/>
+      <c r="AC107" s="4"/>
+      <c r="AD107" s="4"/>
+      <c r="AE107" s="4"/>
+      <c r="AF107" s="4"/>
+      <c r="AZ107" s="12"/>
+      <c r="BB107" s="12"/>
+      <c r="BE107" s="12"/>
+      <c r="BK107" s="6"/>
+      <c r="BL107" s="6"/>
+      <c r="BM107" s="6"/>
+      <c r="BN107" s="6"/>
+      <c r="BO107" s="6"/>
+      <c r="BP107" s="6"/>
+      <c r="BR107" s="67"/>
+      <c r="BT107" s="4"/>
+      <c r="BV107" s="4"/>
+      <c r="BY107" s="4"/>
+    </row>
+    <row r="108" spans="23:79" x14ac:dyDescent="0.2">
+      <c r="W108" s="4"/>
+      <c r="X108" s="4"/>
+      <c r="Y108" s="7"/>
+      <c r="Z108" s="4"/>
+      <c r="AA108" s="7"/>
+      <c r="AB108" s="4"/>
+      <c r="AC108" s="4"/>
+      <c r="AD108" s="4"/>
+      <c r="AE108" s="4"/>
+      <c r="AF108" s="7"/>
+      <c r="AZ108" s="4"/>
       <c r="BB108" s="12"/>
-      <c r="BE108" s="12"/>
-      <c r="BK108" s="2"/>
-    </row>
-    <row r="109" spans="23:77" x14ac:dyDescent="0.2">
-      <c r="AZ109" s="12"/>
+      <c r="BE108" s="31"/>
+      <c r="BK108" s="6"/>
+      <c r="BL108" s="6"/>
+      <c r="BM108" s="6"/>
+      <c r="BN108" s="6"/>
+      <c r="BO108" s="6"/>
+      <c r="BP108" s="6"/>
+      <c r="BR108" s="67"/>
+      <c r="BT108" s="4"/>
+      <c r="BV108" s="4"/>
+      <c r="BY108" s="4"/>
+    </row>
+    <row r="109" spans="23:79" x14ac:dyDescent="0.2">
+      <c r="W109" s="4"/>
+      <c r="X109" s="4"/>
+      <c r="Y109" s="4"/>
+      <c r="Z109" s="4"/>
+      <c r="AA109" s="4"/>
+      <c r="AB109" s="4"/>
+      <c r="AC109" s="4"/>
+      <c r="AD109" s="4"/>
+      <c r="AE109" s="4"/>
+      <c r="AF109" s="4"/>
+      <c r="AZ109" s="4"/>
       <c r="BB109" s="12"/>
-      <c r="BE109" s="12"/>
-      <c r="BK109" s="6"/>
-      <c r="BL109" s="6"/>
-      <c r="BM109" s="6"/>
-      <c r="BN109" s="6"/>
-      <c r="BO109" s="6"/>
-      <c r="BP109" s="6"/>
-      <c r="BR109" s="4"/>
-      <c r="BT109" s="4"/>
-      <c r="BV109" s="4"/>
-      <c r="BY109" s="4"/>
-    </row>
-    <row r="110" spans="23:77" x14ac:dyDescent="0.2">
-      <c r="W110" s="7"/>
+      <c r="BE109" s="31"/>
+    </row>
+    <row r="110" spans="23:79" x14ac:dyDescent="0.2">
+      <c r="W110" s="4"/>
       <c r="X110" s="4"/>
       <c r="Y110" s="4"/>
       <c r="Z110" s="4"/>
@@ -8154,610 +8388,622 @@
       <c r="AF110" s="4"/>
       <c r="AZ110" s="12"/>
       <c r="BB110" s="12"/>
-      <c r="BE110" s="12"/>
-      <c r="BK110" s="6"/>
-      <c r="BL110" s="6"/>
-      <c r="BM110" s="6"/>
-      <c r="BN110" s="6"/>
-      <c r="BO110" s="6"/>
-      <c r="BP110" s="6"/>
-      <c r="BR110" s="4"/>
-      <c r="BT110" s="4"/>
-      <c r="BV110" s="4"/>
-      <c r="BY110" s="4"/>
-    </row>
-    <row r="111" spans="23:77" x14ac:dyDescent="0.2">
+      <c r="BE110" s="31"/>
+      <c r="BK110" s="2"/>
+    </row>
+    <row r="111" spans="23:79" x14ac:dyDescent="0.2">
       <c r="W111" s="4"/>
-      <c r="X111" s="7"/>
+      <c r="X111" s="4"/>
       <c r="Y111" s="4"/>
       <c r="Z111" s="4"/>
       <c r="AA111" s="4"/>
       <c r="AB111" s="4"/>
       <c r="AC111" s="4"/>
       <c r="AD111" s="4"/>
-      <c r="AE111" s="7"/>
+      <c r="AE111" s="4"/>
       <c r="AF111" s="4"/>
-      <c r="AZ111" s="30"/>
-      <c r="BB111" s="4"/>
-      <c r="BE111" s="4"/>
-      <c r="BK111" s="6"/>
-      <c r="BL111" s="6"/>
-      <c r="BM111" s="6"/>
-      <c r="BN111" s="6"/>
-      <c r="BO111" s="6"/>
-      <c r="BP111" s="6"/>
-      <c r="BQ111" s="4"/>
+      <c r="AZ111" s="12"/>
+      <c r="BB111" s="7"/>
+      <c r="BE111" s="31"/>
+      <c r="BK111" s="7"/>
+      <c r="BL111" s="7"/>
+      <c r="BM111" s="7"/>
+      <c r="BN111" s="7"/>
+      <c r="BO111" s="7"/>
+      <c r="BP111" s="7"/>
       <c r="BR111" s="4"/>
-      <c r="BS111" s="4"/>
-      <c r="BT111" s="4"/>
-      <c r="BU111" s="4"/>
+      <c r="BT111" s="6"/>
       <c r="BV111" s="4"/>
-      <c r="BW111" s="4"/>
-      <c r="BX111" s="4"/>
-      <c r="BY111" s="4"/>
-    </row>
-    <row r="112" spans="23:77" x14ac:dyDescent="0.2">
+      <c r="BY111" s="65"/>
+      <c r="CA111" s="63"/>
+    </row>
+    <row r="112" spans="23:79" x14ac:dyDescent="0.2">
       <c r="W112" s="4"/>
-      <c r="X112" s="4"/>
-      <c r="Y112" s="7"/>
+      <c r="X112" s="7"/>
+      <c r="Y112" s="4"/>
       <c r="Z112" s="4"/>
-      <c r="AA112" s="7"/>
+      <c r="AA112" s="4"/>
       <c r="AB112" s="4"/>
       <c r="AC112" s="4"/>
       <c r="AD112" s="4"/>
-      <c r="AE112" s="4"/>
-      <c r="AF112" s="7"/>
-      <c r="AZ112" s="4"/>
-      <c r="BB112" s="4"/>
-      <c r="BE112" s="4"/>
-      <c r="BK112" s="6"/>
-      <c r="BL112" s="6"/>
-      <c r="BM112" s="6"/>
-      <c r="BN112" s="6"/>
-      <c r="BO112" s="6"/>
-      <c r="BP112" s="6"/>
-      <c r="BR112" s="67"/>
-      <c r="BT112" s="4"/>
+      <c r="AE112" s="7"/>
+      <c r="AF112" s="4"/>
+      <c r="AZ112" s="12"/>
+      <c r="BB112" s="7"/>
+      <c r="BE112" s="31"/>
+      <c r="BK112" s="7"/>
+      <c r="BL112" s="7"/>
+      <c r="BM112" s="7"/>
+      <c r="BN112" s="7"/>
+      <c r="BO112" s="7"/>
+      <c r="BP112" s="7"/>
+      <c r="BR112" s="4"/>
+      <c r="BT112" s="6"/>
       <c r="BV112" s="4"/>
-      <c r="BY112" s="4"/>
+      <c r="BY112" s="65"/>
+      <c r="CA112" s="63"/>
     </row>
     <row r="113" spans="2:79" x14ac:dyDescent="0.2">
       <c r="W113" s="4"/>
       <c r="X113" s="4"/>
-      <c r="Y113" s="4"/>
+      <c r="Y113" s="7"/>
       <c r="Z113" s="4"/>
-      <c r="AA113" s="4"/>
+      <c r="AA113" s="7"/>
       <c r="AB113" s="4"/>
       <c r="AC113" s="4"/>
       <c r="AD113" s="4"/>
       <c r="AE113" s="4"/>
-      <c r="AF113" s="4"/>
-      <c r="AZ113" s="12"/>
-      <c r="BB113" s="12"/>
-      <c r="BE113" s="12"/>
-      <c r="BK113" s="6"/>
-      <c r="BL113" s="6"/>
-      <c r="BM113" s="6"/>
-      <c r="BN113" s="6"/>
-      <c r="BO113" s="6"/>
-      <c r="BP113" s="6"/>
-      <c r="BR113" s="67"/>
-      <c r="BT113" s="4"/>
+      <c r="AF113" s="7"/>
+      <c r="AZ113" s="4"/>
+      <c r="BB113" s="4"/>
+      <c r="BE113" s="31"/>
+      <c r="BK113" s="7"/>
+      <c r="BL113" s="7"/>
+      <c r="BM113" s="7"/>
+      <c r="BN113" s="7"/>
+      <c r="BO113" s="7"/>
+      <c r="BP113" s="7"/>
+      <c r="BQ113" s="4"/>
+      <c r="BR113" s="4"/>
+      <c r="BS113" s="4"/>
+      <c r="BT113" s="6"/>
+      <c r="BU113" s="4"/>
       <c r="BV113" s="4"/>
-      <c r="BY113" s="4"/>
+      <c r="BW113" s="4"/>
+      <c r="BX113" s="4"/>
+      <c r="BY113" s="65"/>
+      <c r="BZ113" s="4"/>
+      <c r="CA113" s="63"/>
     </row>
     <row r="114" spans="2:79" x14ac:dyDescent="0.2">
       <c r="W114" s="4"/>
       <c r="X114" s="4"/>
-      <c r="Y114" s="7"/>
+      <c r="Y114" s="4"/>
       <c r="Z114" s="4"/>
-      <c r="AA114" s="7"/>
+      <c r="AA114" s="4"/>
       <c r="AB114" s="4"/>
       <c r="AC114" s="4"/>
       <c r="AD114" s="4"/>
       <c r="AE114" s="4"/>
-      <c r="AF114" s="7"/>
+      <c r="AF114" s="4"/>
       <c r="AZ114" s="4"/>
-      <c r="BB114" s="12"/>
+      <c r="BB114" s="4"/>
       <c r="BE114" s="31"/>
-      <c r="BK114" s="6"/>
-      <c r="BL114" s="6"/>
-      <c r="BM114" s="6"/>
-      <c r="BN114" s="6"/>
-      <c r="BO114" s="6"/>
-      <c r="BP114" s="6"/>
-      <c r="BR114" s="67"/>
-      <c r="BT114" s="4"/>
+      <c r="BK114" s="7"/>
+      <c r="BL114" s="7"/>
+      <c r="BM114" s="7"/>
+      <c r="BN114" s="7"/>
+      <c r="BO114" s="7"/>
+      <c r="BP114" s="7"/>
+      <c r="BR114" s="4"/>
+      <c r="BT114" s="6"/>
       <c r="BV114" s="4"/>
-      <c r="BY114" s="4"/>
+      <c r="BY114" s="65"/>
+      <c r="CA114" s="63"/>
     </row>
     <row r="115" spans="2:79" x14ac:dyDescent="0.2">
       <c r="W115" s="4"/>
       <c r="X115" s="4"/>
-      <c r="Y115" s="4"/>
+      <c r="Y115" s="7"/>
       <c r="Z115" s="4"/>
-      <c r="AA115" s="4"/>
+      <c r="AA115" s="7"/>
       <c r="AB115" s="4"/>
       <c r="AC115" s="4"/>
       <c r="AD115" s="4"/>
       <c r="AE115" s="4"/>
-      <c r="AF115" s="4"/>
+      <c r="AF115" s="7"/>
       <c r="AZ115" s="4"/>
-      <c r="BB115" s="12"/>
-      <c r="BE115" s="31"/>
+      <c r="BB115" s="4"/>
+      <c r="BE115" s="4"/>
+      <c r="BK115" s="7"/>
+      <c r="BL115" s="7"/>
+      <c r="BM115" s="7"/>
+      <c r="BN115" s="7"/>
+      <c r="BO115" s="7"/>
+      <c r="BP115" s="7"/>
+      <c r="BR115" s="4"/>
+      <c r="BT115" s="6"/>
+      <c r="BV115" s="4"/>
+      <c r="BY115" s="65"/>
+      <c r="CA115" s="63"/>
     </row>
     <row r="116" spans="2:79" x14ac:dyDescent="0.2">
-      <c r="W116" s="4"/>
-      <c r="X116" s="4"/>
-      <c r="Y116" s="4"/>
-      <c r="Z116" s="4"/>
-      <c r="AA116" s="4"/>
-      <c r="AB116" s="4"/>
-      <c r="AC116" s="4"/>
-      <c r="AD116" s="4"/>
-      <c r="AE116" s="4"/>
-      <c r="AF116" s="4"/>
-      <c r="AZ116" s="12"/>
-      <c r="BB116" s="12"/>
-      <c r="BE116" s="31"/>
-      <c r="BK116" s="2"/>
-    </row>
-    <row r="117" spans="2:79" x14ac:dyDescent="0.2">
-      <c r="W117" s="4"/>
-      <c r="X117" s="4"/>
-      <c r="Y117" s="4"/>
-      <c r="Z117" s="4"/>
-      <c r="AA117" s="4"/>
-      <c r="AB117" s="4"/>
-      <c r="AC117" s="4"/>
-      <c r="AD117" s="4"/>
-      <c r="AE117" s="4"/>
-      <c r="AF117" s="4"/>
-      <c r="AZ117" s="12"/>
-      <c r="BB117" s="7"/>
-      <c r="BE117" s="31"/>
-      <c r="BK117" s="7"/>
-      <c r="BL117" s="7"/>
-      <c r="BM117" s="7"/>
-      <c r="BN117" s="7"/>
-      <c r="BO117" s="7"/>
-      <c r="BP117" s="7"/>
-      <c r="BR117" s="4"/>
-      <c r="BT117" s="6"/>
-      <c r="BV117" s="4"/>
-      <c r="BY117" s="65"/>
-      <c r="CA117" s="63"/>
+      <c r="BK116" s="7"/>
+      <c r="BL116" s="7"/>
+      <c r="BM116" s="7"/>
+      <c r="BN116" s="7"/>
+      <c r="BO116" s="7"/>
+      <c r="BP116" s="7"/>
+      <c r="BR116" s="4"/>
+      <c r="BT116" s="6"/>
+      <c r="BV116" s="4"/>
+      <c r="BY116" s="65"/>
+      <c r="CA116" s="63"/>
     </row>
     <row r="118" spans="2:79" x14ac:dyDescent="0.2">
-      <c r="W118" s="4"/>
-      <c r="X118" s="7"/>
-      <c r="Y118" s="4"/>
-      <c r="Z118" s="4"/>
-      <c r="AA118" s="4"/>
-      <c r="AB118" s="4"/>
-      <c r="AC118" s="4"/>
-      <c r="AD118" s="4"/>
-      <c r="AE118" s="7"/>
-      <c r="AF118" s="4"/>
-      <c r="AZ118" s="12"/>
-      <c r="BB118" s="7"/>
-      <c r="BE118" s="31"/>
-      <c r="BK118" s="7"/>
-      <c r="BL118" s="7"/>
-      <c r="BM118" s="7"/>
-      <c r="BN118" s="7"/>
-      <c r="BO118" s="7"/>
-      <c r="BP118" s="7"/>
-      <c r="BR118" s="4"/>
-      <c r="BT118" s="6"/>
-      <c r="BV118" s="4"/>
-      <c r="BY118" s="65"/>
-      <c r="CA118" s="63"/>
+      <c r="B118" s="2"/>
+      <c r="AF118" s="2"/>
     </row>
     <row r="119" spans="2:79" x14ac:dyDescent="0.2">
-      <c r="W119" s="4"/>
-      <c r="X119" s="4"/>
-      <c r="Y119" s="7"/>
-      <c r="Z119" s="4"/>
-      <c r="AA119" s="7"/>
-      <c r="AB119" s="4"/>
-      <c r="AC119" s="4"/>
-      <c r="AD119" s="4"/>
-      <c r="AE119" s="4"/>
-      <c r="AF119" s="7"/>
-      <c r="AZ119" s="4"/>
-      <c r="BB119" s="4"/>
-      <c r="BE119" s="31"/>
-      <c r="BK119" s="7"/>
-      <c r="BL119" s="7"/>
-      <c r="BM119" s="7"/>
-      <c r="BN119" s="7"/>
-      <c r="BO119" s="7"/>
-      <c r="BP119" s="7"/>
-      <c r="BQ119" s="4"/>
-      <c r="BR119" s="4"/>
-      <c r="BS119" s="4"/>
-      <c r="BT119" s="6"/>
-      <c r="BU119" s="4"/>
-      <c r="BV119" s="4"/>
-      <c r="BW119" s="4"/>
-      <c r="BX119" s="4"/>
-      <c r="BY119" s="65"/>
-      <c r="BZ119" s="4"/>
-      <c r="CA119" s="63"/>
+      <c r="E119" s="26"/>
+      <c r="F119" s="25"/>
+      <c r="V119" s="4"/>
     </row>
     <row r="120" spans="2:79" x14ac:dyDescent="0.2">
-      <c r="W120" s="4"/>
-      <c r="X120" s="4"/>
-      <c r="Y120" s="4"/>
-      <c r="Z120" s="4"/>
-      <c r="AA120" s="4"/>
-      <c r="AB120" s="4"/>
-      <c r="AC120" s="4"/>
-      <c r="AD120" s="4"/>
-      <c r="AE120" s="4"/>
-      <c r="AF120" s="4"/>
-      <c r="AZ120" s="4"/>
-      <c r="BB120" s="4"/>
-      <c r="BE120" s="31"/>
-      <c r="BK120" s="7"/>
-      <c r="BL120" s="7"/>
-      <c r="BM120" s="7"/>
-      <c r="BN120" s="7"/>
-      <c r="BO120" s="7"/>
-      <c r="BP120" s="7"/>
-      <c r="BR120" s="4"/>
-      <c r="BT120" s="6"/>
-      <c r="BV120" s="4"/>
-      <c r="BY120" s="65"/>
-      <c r="CA120" s="63"/>
+      <c r="E120" s="26"/>
+      <c r="F120" s="25"/>
+      <c r="V120" s="4"/>
+      <c r="AW120" s="4"/>
+      <c r="AX120" s="4"/>
     </row>
     <row r="121" spans="2:79" x14ac:dyDescent="0.2">
-      <c r="W121" s="4"/>
-      <c r="X121" s="4"/>
-      <c r="Y121" s="7"/>
-      <c r="Z121" s="4"/>
-      <c r="AA121" s="7"/>
-      <c r="AB121" s="4"/>
-      <c r="AC121" s="4"/>
-      <c r="AD121" s="4"/>
-      <c r="AE121" s="4"/>
-      <c r="AF121" s="7"/>
-      <c r="AZ121" s="4"/>
-      <c r="BB121" s="4"/>
-      <c r="BE121" s="4"/>
-      <c r="BK121" s="7"/>
-      <c r="BL121" s="7"/>
-      <c r="BM121" s="7"/>
-      <c r="BN121" s="7"/>
-      <c r="BO121" s="7"/>
-      <c r="BP121" s="7"/>
-      <c r="BR121" s="4"/>
-      <c r="BT121" s="6"/>
-      <c r="BV121" s="4"/>
-      <c r="BY121" s="65"/>
-      <c r="CA121" s="63"/>
+      <c r="E121" s="26"/>
+      <c r="F121" s="25"/>
+      <c r="V121" s="4"/>
+      <c r="AW121" s="7"/>
+      <c r="AX121" s="7"/>
+      <c r="AZ121" s="12"/>
+      <c r="BB121" s="12"/>
+      <c r="BE121" s="31"/>
     </row>
     <row r="122" spans="2:79" x14ac:dyDescent="0.2">
-      <c r="BK122" s="7"/>
-      <c r="BL122" s="7"/>
-      <c r="BM122" s="7"/>
-      <c r="BN122" s="7"/>
-      <c r="BO122" s="7"/>
-      <c r="BP122" s="7"/>
-      <c r="BR122" s="4"/>
-      <c r="BT122" s="6"/>
-      <c r="BV122" s="4"/>
-      <c r="BY122" s="65"/>
-      <c r="CA122" s="63"/>
+      <c r="V122" s="4"/>
+      <c r="AW122" s="7"/>
+      <c r="AX122" s="7"/>
+      <c r="AZ122" s="12"/>
+      <c r="BB122" s="12"/>
+      <c r="BE122" s="31"/>
+    </row>
+    <row r="123" spans="2:79" x14ac:dyDescent="0.2">
+      <c r="V123" s="4"/>
+      <c r="AW123" s="7"/>
+      <c r="AX123" s="7"/>
+      <c r="AZ123" s="12"/>
+      <c r="BB123" s="12"/>
+      <c r="BE123" s="31"/>
     </row>
     <row r="124" spans="2:79" x14ac:dyDescent="0.2">
-      <c r="B124" s="2"/>
-      <c r="AF124" s="2"/>
+      <c r="V124" s="4"/>
+      <c r="AW124" s="7"/>
+      <c r="AX124" s="16"/>
+      <c r="AZ124" s="30"/>
+      <c r="BB124" s="7"/>
+      <c r="BE124" s="31"/>
     </row>
     <row r="125" spans="2:79" x14ac:dyDescent="0.2">
-      <c r="E125" s="26"/>
-      <c r="F125" s="25"/>
       <c r="V125" s="4"/>
+      <c r="AW125" s="7"/>
+      <c r="AX125" s="16"/>
+      <c r="AZ125" s="30"/>
+      <c r="BB125" s="7"/>
+      <c r="BE125" s="31"/>
     </row>
     <row r="126" spans="2:79" x14ac:dyDescent="0.2">
-      <c r="E126" s="26"/>
-      <c r="F126" s="25"/>
       <c r="V126" s="4"/>
-      <c r="AW126" s="4"/>
-      <c r="AX126" s="4"/>
+      <c r="AW126" s="7"/>
+      <c r="AX126" s="7"/>
+      <c r="AY126" s="4"/>
+      <c r="AZ126" s="30"/>
+      <c r="BB126" s="12"/>
+      <c r="BE126" s="31"/>
     </row>
     <row r="127" spans="2:79" x14ac:dyDescent="0.2">
-      <c r="E127" s="26"/>
-      <c r="F127" s="25"/>
       <c r="V127" s="4"/>
       <c r="AW127" s="7"/>
-      <c r="AX127" s="7"/>
-      <c r="AZ127" s="12"/>
+      <c r="AX127" s="16"/>
+      <c r="AZ127" s="30"/>
+      <c r="BA127" s="4"/>
       <c r="BB127" s="12"/>
+      <c r="BC127" s="28"/>
+      <c r="BD127" s="28"/>
       <c r="BE127" s="31"/>
     </row>
     <row r="128" spans="2:79" x14ac:dyDescent="0.2">
       <c r="V128" s="4"/>
-      <c r="AW128" s="7"/>
+      <c r="AW128" s="16"/>
       <c r="AX128" s="7"/>
-      <c r="AZ128" s="12"/>
+      <c r="AZ128" s="30"/>
       <c r="BB128" s="12"/>
       <c r="BE128" s="31"/>
     </row>
-    <row r="129" spans="22:76" x14ac:dyDescent="0.2">
+    <row r="129" spans="22:90" x14ac:dyDescent="0.2">
       <c r="V129" s="4"/>
-      <c r="AW129" s="7"/>
+      <c r="AW129" s="16"/>
       <c r="AX129" s="7"/>
-      <c r="AZ129" s="12"/>
+      <c r="AY129" s="3"/>
+      <c r="AZ129" s="30"/>
       <c r="BB129" s="12"/>
       <c r="BE129" s="31"/>
     </row>
-    <row r="130" spans="22:76" x14ac:dyDescent="0.2">
+    <row r="130" spans="22:90" x14ac:dyDescent="0.2">
       <c r="V130" s="4"/>
-      <c r="AW130" s="7"/>
-      <c r="AX130" s="16"/>
+      <c r="AW130" s="16"/>
+      <c r="AX130" s="7"/>
       <c r="AZ130" s="30"/>
-      <c r="BB130" s="7"/>
+      <c r="BB130" s="12"/>
       <c r="BE130" s="31"/>
     </row>
-    <row r="131" spans="22:76" x14ac:dyDescent="0.2">
+    <row r="131" spans="22:90" x14ac:dyDescent="0.2">
       <c r="V131" s="4"/>
-      <c r="AW131" s="7"/>
+      <c r="AW131" s="16"/>
       <c r="AX131" s="16"/>
       <c r="AZ131" s="30"/>
       <c r="BB131" s="7"/>
       <c r="BE131" s="31"/>
     </row>
-    <row r="132" spans="22:76" x14ac:dyDescent="0.2">
+    <row r="132" spans="22:90" x14ac:dyDescent="0.2">
       <c r="V132" s="4"/>
-      <c r="AW132" s="7"/>
-      <c r="AX132" s="7"/>
-      <c r="AY132" s="4"/>
+      <c r="AW132" s="16"/>
+      <c r="AX132" s="16"/>
       <c r="AZ132" s="30"/>
-      <c r="BB132" s="12"/>
+      <c r="BB132" s="7"/>
       <c r="BE132" s="31"/>
     </row>
-    <row r="133" spans="22:76" x14ac:dyDescent="0.2">
+    <row r="133" spans="22:90" x14ac:dyDescent="0.2">
       <c r="V133" s="4"/>
-      <c r="AW133" s="7"/>
-      <c r="AX133" s="16"/>
+      <c r="AJ133" s="4"/>
+      <c r="AK133" s="7"/>
+      <c r="AL133" s="7"/>
+      <c r="AM133" s="7"/>
+      <c r="AN133" s="7"/>
+      <c r="AO133" s="7"/>
+      <c r="AP133" s="7"/>
+      <c r="AQ133" s="7"/>
+      <c r="AR133" s="16"/>
+      <c r="AS133" s="16"/>
+      <c r="AT133" s="16"/>
+      <c r="AU133" s="16"/>
+      <c r="AV133" s="16"/>
+      <c r="AW133" s="16"/>
+      <c r="AX133" s="7"/>
       <c r="AZ133" s="30"/>
-      <c r="BA133" s="4"/>
       <c r="BB133" s="12"/>
-      <c r="BC133" s="28"/>
-      <c r="BD133" s="28"/>
       <c r="BE133" s="31"/>
     </row>
-    <row r="134" spans="22:76" x14ac:dyDescent="0.2">
+    <row r="134" spans="22:90" x14ac:dyDescent="0.2">
       <c r="V134" s="4"/>
-      <c r="AW134" s="16"/>
-      <c r="AX134" s="7"/>
+      <c r="AJ134" s="4"/>
+      <c r="AK134" s="7"/>
+      <c r="AL134" s="7"/>
+      <c r="AM134" s="7"/>
+      <c r="AN134" s="16"/>
+      <c r="AO134" s="16"/>
+      <c r="AP134" s="7"/>
+      <c r="AQ134" s="16"/>
+      <c r="AR134" s="8"/>
+      <c r="AS134" s="8"/>
+      <c r="AT134" s="8"/>
+      <c r="AU134" s="16"/>
+      <c r="AV134" s="16"/>
+      <c r="AW134" s="7"/>
+      <c r="AX134" s="16"/>
       <c r="AZ134" s="30"/>
       <c r="BB134" s="12"/>
       <c r="BE134" s="31"/>
     </row>
-    <row r="135" spans="22:76" x14ac:dyDescent="0.2">
+    <row r="135" spans="22:90" x14ac:dyDescent="0.2">
       <c r="V135" s="4"/>
-      <c r="AW135" s="16"/>
-      <c r="AX135" s="7"/>
-      <c r="AY135" s="3"/>
-      <c r="AZ135" s="30"/>
-      <c r="BB135" s="12"/>
-      <c r="BE135" s="31"/>
-    </row>
-    <row r="136" spans="22:76" x14ac:dyDescent="0.2">
+      <c r="AK135" s="32"/>
+      <c r="AL135" s="32"/>
+      <c r="AM135" s="32"/>
+    </row>
+    <row r="136" spans="22:90" x14ac:dyDescent="0.2">
       <c r="V136" s="4"/>
-      <c r="AW136" s="16"/>
-      <c r="AX136" s="7"/>
-      <c r="AZ136" s="30"/>
-      <c r="BB136" s="12"/>
-      <c r="BE136" s="31"/>
-    </row>
-    <row r="137" spans="22:76" x14ac:dyDescent="0.2">
-      <c r="V137" s="4"/>
-      <c r="AW137" s="16"/>
-      <c r="AX137" s="16"/>
-      <c r="AZ137" s="30"/>
-      <c r="BB137" s="7"/>
-      <c r="BE137" s="31"/>
-    </row>
-    <row r="138" spans="22:76" x14ac:dyDescent="0.2">
-      <c r="V138" s="4"/>
-      <c r="AW138" s="16"/>
-      <c r="AX138" s="16"/>
-      <c r="AZ138" s="30"/>
-      <c r="BB138" s="7"/>
-      <c r="BE138" s="31"/>
-    </row>
-    <row r="139" spans="22:76" x14ac:dyDescent="0.2">
-      <c r="V139" s="4"/>
-      <c r="AJ139" s="4"/>
-      <c r="AK139" s="7"/>
-      <c r="AL139" s="7"/>
-      <c r="AM139" s="7"/>
-      <c r="AN139" s="7"/>
-      <c r="AO139" s="7"/>
-      <c r="AP139" s="7"/>
-      <c r="AQ139" s="7"/>
-      <c r="AR139" s="16"/>
-      <c r="AS139" s="16"/>
-      <c r="AT139" s="16"/>
-      <c r="AU139" s="16"/>
-      <c r="AV139" s="16"/>
-      <c r="AW139" s="16"/>
-      <c r="AX139" s="7"/>
-      <c r="AZ139" s="30"/>
-      <c r="BB139" s="12"/>
-      <c r="BE139" s="31"/>
-    </row>
-    <row r="140" spans="22:76" x14ac:dyDescent="0.2">
-      <c r="V140" s="4"/>
-      <c r="AJ140" s="4"/>
-      <c r="AK140" s="7"/>
-      <c r="AL140" s="7"/>
-      <c r="AM140" s="7"/>
-      <c r="AN140" s="16"/>
-      <c r="AO140" s="16"/>
-      <c r="AP140" s="7"/>
-      <c r="AQ140" s="16"/>
-      <c r="AR140" s="8"/>
-      <c r="AS140" s="8"/>
-      <c r="AT140" s="8"/>
-      <c r="AU140" s="16"/>
-      <c r="AV140" s="16"/>
-      <c r="AW140" s="7"/>
-      <c r="AX140" s="16"/>
-      <c r="AZ140" s="30"/>
-      <c r="BB140" s="12"/>
-      <c r="BE140" s="31"/>
-    </row>
-    <row r="141" spans="22:76" x14ac:dyDescent="0.2">
-      <c r="V141" s="4"/>
-      <c r="AK141" s="32"/>
-      <c r="AL141" s="32"/>
-      <c r="AM141" s="32"/>
-    </row>
-    <row r="142" spans="22:76" x14ac:dyDescent="0.2">
-      <c r="V142" s="4"/>
-    </row>
-    <row r="143" spans="22:76" x14ac:dyDescent="0.2">
+    </row>
+    <row r="137" spans="22:90" x14ac:dyDescent="0.2">
+      <c r="BX137" s="33"/>
+    </row>
+    <row r="138" spans="22:90" x14ac:dyDescent="0.2">
+      <c r="BX138" s="33"/>
+    </row>
+    <row r="139" spans="22:90" x14ac:dyDescent="0.2">
+      <c r="BX139" s="33"/>
+    </row>
+    <row r="141" spans="22:90" x14ac:dyDescent="0.2">
+      <c r="BX141" s="33"/>
+      <c r="CL141" s="29"/>
+    </row>
+    <row r="142" spans="22:90" x14ac:dyDescent="0.2">
+      <c r="BX142" s="33"/>
+    </row>
+    <row r="143" spans="22:90" x14ac:dyDescent="0.2">
       <c r="BX143" s="33"/>
     </row>
-    <row r="144" spans="22:76" x14ac:dyDescent="0.2">
-      <c r="BX144" s="33"/>
-    </row>
-    <row r="145" spans="39:90" x14ac:dyDescent="0.2">
-      <c r="BX145" s="33"/>
-    </row>
-    <row r="147" spans="39:90" x14ac:dyDescent="0.2">
-      <c r="BX147" s="33"/>
-      <c r="CL147" s="29"/>
-    </row>
-    <row r="148" spans="39:90" x14ac:dyDescent="0.2">
-      <c r="BX148" s="33"/>
-    </row>
-    <row r="149" spans="39:90" x14ac:dyDescent="0.2">
-      <c r="BX149" s="33"/>
-    </row>
-    <row r="150" spans="39:90" x14ac:dyDescent="0.2">
+    <row r="144" spans="22:90" x14ac:dyDescent="0.2">
+      <c r="BL144" s="4"/>
+      <c r="BT144" s="2"/>
+    </row>
+    <row r="145" spans="39:92" x14ac:dyDescent="0.2">
+      <c r="BL145" s="4"/>
+      <c r="BN145" s="4"/>
+      <c r="BP145" s="4"/>
+      <c r="BR145" s="4"/>
+      <c r="BT145" s="6"/>
+      <c r="BU145" s="4"/>
+      <c r="BV145" s="4"/>
+      <c r="BW145" s="4"/>
+      <c r="BX145" s="4"/>
+      <c r="BY145" s="4"/>
+      <c r="BZ145" s="4"/>
+      <c r="CA145" s="42"/>
+      <c r="CB145" s="4"/>
+      <c r="CD145" s="4"/>
+      <c r="CF145" s="4"/>
+    </row>
+    <row r="146" spans="39:92" x14ac:dyDescent="0.2">
+      <c r="BL146" s="4"/>
+      <c r="BN146" s="4"/>
+      <c r="BP146" s="4"/>
+      <c r="BR146" s="4"/>
+      <c r="BT146" s="4"/>
+      <c r="BU146" s="6"/>
+      <c r="BV146" s="4"/>
+      <c r="BW146" s="4"/>
+      <c r="BX146" s="4"/>
+      <c r="BY146" s="4"/>
+      <c r="BZ146" s="4"/>
+      <c r="CA146" s="43"/>
+      <c r="CB146" s="4"/>
+      <c r="CD146" s="4"/>
+      <c r="CF146" s="4"/>
+    </row>
+    <row r="147" spans="39:92" x14ac:dyDescent="0.2">
+      <c r="BL147" s="4"/>
+      <c r="BN147" s="4"/>
+      <c r="BP147" s="4"/>
+      <c r="BR147" s="4"/>
+      <c r="BT147" s="4"/>
+      <c r="BU147" s="4"/>
+      <c r="BV147" s="4"/>
+      <c r="BW147" s="4"/>
+      <c r="BX147" s="4"/>
+      <c r="BY147" s="4"/>
+      <c r="BZ147" s="4"/>
+      <c r="CA147" s="42"/>
+      <c r="CB147" s="4"/>
+      <c r="CC147" s="4"/>
+      <c r="CD147" s="4"/>
+      <c r="CE147" s="4"/>
+      <c r="CF147" s="4"/>
+    </row>
+    <row r="148" spans="39:92" x14ac:dyDescent="0.2">
+      <c r="BL148" s="4"/>
+      <c r="BN148" s="4"/>
+      <c r="BP148" s="4"/>
+      <c r="BR148" s="4"/>
+      <c r="BT148" s="4"/>
+      <c r="BU148" s="4"/>
+      <c r="BV148" s="4"/>
+      <c r="BW148" s="6"/>
+      <c r="BX148" s="6"/>
+      <c r="BY148" s="4"/>
+      <c r="BZ148" s="4"/>
+      <c r="CA148" s="43"/>
+      <c r="CB148" s="7"/>
+      <c r="CD148" s="4"/>
+      <c r="CF148" s="7"/>
+    </row>
+    <row r="149" spans="39:92" x14ac:dyDescent="0.2">
+      <c r="AM149" s="2"/>
+      <c r="BL149" s="4"/>
+      <c r="BN149" s="4"/>
+      <c r="BP149" s="4"/>
+      <c r="BR149" s="4"/>
+      <c r="BT149" s="4"/>
+      <c r="BU149" s="4"/>
+      <c r="BV149" s="4"/>
+      <c r="BW149" s="4"/>
+      <c r="BX149" s="4"/>
+      <c r="BY149" s="6"/>
+      <c r="BZ149" s="4"/>
+      <c r="CA149" s="43"/>
+      <c r="CB149" s="7"/>
+      <c r="CD149" s="4"/>
+      <c r="CF149" s="7"/>
+    </row>
+    <row r="150" spans="39:92" x14ac:dyDescent="0.2">
+      <c r="AN150" s="4"/>
+      <c r="AO150" s="4"/>
+      <c r="AP150" s="4"/>
+      <c r="AQ150" s="4"/>
+      <c r="AR150" s="4"/>
+      <c r="AS150" s="4"/>
+      <c r="AT150" s="4"/>
+      <c r="AU150" s="4"/>
       <c r="BL150" s="4"/>
-      <c r="BT150" s="2"/>
-    </row>
-    <row r="151" spans="39:90" x14ac:dyDescent="0.2">
+      <c r="BN150" s="4"/>
+      <c r="BP150" s="4"/>
+      <c r="BR150" s="4"/>
+      <c r="BT150" s="4"/>
+      <c r="BU150" s="4"/>
+      <c r="BV150" s="4"/>
+      <c r="BW150" s="4"/>
+      <c r="BX150" s="4"/>
+      <c r="BY150" s="4"/>
+      <c r="BZ150" s="4"/>
+      <c r="CA150" s="43"/>
+      <c r="CB150" s="7"/>
+      <c r="CD150" s="4"/>
+      <c r="CF150" s="7"/>
+    </row>
+    <row r="151" spans="39:92" x14ac:dyDescent="0.2">
+      <c r="AM151" s="4"/>
+      <c r="AN151" s="7"/>
+      <c r="AO151" s="7"/>
+      <c r="AP151" s="7"/>
+      <c r="AQ151" s="7"/>
+      <c r="AR151" s="7"/>
+      <c r="AS151" s="7"/>
+      <c r="AT151" s="7"/>
+      <c r="AU151" s="7"/>
+      <c r="AV151" s="4"/>
+      <c r="AW151" s="12"/>
+      <c r="AX151" s="4"/>
+      <c r="AY151" s="7"/>
       <c r="BL151" s="4"/>
+      <c r="BM151" s="4"/>
       <c r="BN151" s="4"/>
+      <c r="BO151" s="4"/>
       <c r="BP151" s="4"/>
+      <c r="BQ151" s="28"/>
       <c r="BR151" s="4"/>
-      <c r="BT151" s="6"/>
-      <c r="BU151" s="4"/>
-      <c r="BV151" s="4"/>
-      <c r="BW151" s="4"/>
-      <c r="BX151" s="4"/>
-      <c r="BY151" s="4"/>
-      <c r="BZ151" s="4"/>
-      <c r="CA151" s="42"/>
-      <c r="CB151" s="4"/>
-      <c r="CD151" s="4"/>
-      <c r="CF151" s="4"/>
-    </row>
-    <row r="152" spans="39:90" x14ac:dyDescent="0.2">
-      <c r="BL152" s="4"/>
-      <c r="BN152" s="4"/>
-      <c r="BP152" s="4"/>
-      <c r="BR152" s="4"/>
-      <c r="BT152" s="4"/>
-      <c r="BU152" s="6"/>
-      <c r="BV152" s="4"/>
-      <c r="BW152" s="4"/>
-      <c r="BX152" s="4"/>
-      <c r="BY152" s="4"/>
-      <c r="BZ152" s="4"/>
-      <c r="CA152" s="43"/>
-      <c r="CB152" s="4"/>
-      <c r="CD152" s="4"/>
-      <c r="CF152" s="4"/>
-    </row>
-    <row r="153" spans="39:90" x14ac:dyDescent="0.2">
-      <c r="BL153" s="4"/>
-      <c r="BN153" s="4"/>
-      <c r="BP153" s="4"/>
-      <c r="BR153" s="4"/>
-      <c r="BT153" s="4"/>
+    </row>
+    <row r="152" spans="39:92" x14ac:dyDescent="0.2">
+      <c r="AM152" s="4"/>
+      <c r="AN152" s="7"/>
+      <c r="AO152" s="7"/>
+      <c r="AP152" s="7"/>
+      <c r="AQ152" s="7"/>
+      <c r="AR152" s="7"/>
+      <c r="AS152" s="7"/>
+      <c r="AT152" s="7"/>
+      <c r="AU152" s="7"/>
+      <c r="AW152" s="12"/>
+      <c r="AY152" s="7"/>
+      <c r="BL152" s="6"/>
+      <c r="BN152" s="12"/>
+      <c r="BP152" s="26"/>
+      <c r="BR152" s="16"/>
+      <c r="BT152" s="2"/>
+    </row>
+    <row r="153" spans="39:92" x14ac:dyDescent="0.2">
+      <c r="AM153" s="4"/>
+      <c r="AN153" s="7"/>
+      <c r="AO153" s="7"/>
+      <c r="AP153" s="7"/>
+      <c r="AQ153" s="7"/>
+      <c r="AR153" s="7"/>
+      <c r="AS153" s="7"/>
+      <c r="AT153" s="7"/>
+      <c r="AU153" s="7"/>
+      <c r="AW153" s="12"/>
+      <c r="AY153" s="7"/>
+      <c r="BL153" s="6"/>
+      <c r="BN153" s="12"/>
+      <c r="BP153" s="26"/>
+      <c r="BR153" s="22"/>
+      <c r="BT153" s="7"/>
       <c r="BU153" s="4"/>
-      <c r="BV153" s="4"/>
-      <c r="BW153" s="4"/>
-      <c r="BX153" s="4"/>
+      <c r="BV153" s="6"/>
+      <c r="BW153" s="7"/>
+      <c r="BX153" s="7"/>
       <c r="BY153" s="4"/>
-      <c r="BZ153" s="4"/>
-      <c r="CA153" s="42"/>
+      <c r="BZ153" s="6"/>
       <c r="CB153" s="4"/>
-      <c r="CC153" s="4"/>
       <c r="CD153" s="4"/>
-      <c r="CE153" s="4"/>
       <c r="CF153" s="4"/>
-    </row>
-    <row r="154" spans="39:90" x14ac:dyDescent="0.2">
-      <c r="BL154" s="4"/>
-      <c r="BN154" s="4"/>
-      <c r="BP154" s="4"/>
-      <c r="BR154" s="4"/>
+      <c r="CH153" s="44"/>
+    </row>
+    <row r="154" spans="39:92" x14ac:dyDescent="0.2">
+      <c r="AM154" s="4"/>
+      <c r="AN154" s="7"/>
+      <c r="AO154" s="7"/>
+      <c r="AP154" s="7"/>
+      <c r="AQ154" s="7"/>
+      <c r="AR154" s="7"/>
+      <c r="AS154" s="7"/>
+      <c r="AT154" s="7"/>
+      <c r="AU154" s="7"/>
+      <c r="AW154" s="12"/>
+      <c r="AY154" s="7"/>
+      <c r="BL154" s="6"/>
+      <c r="BN154" s="12"/>
+      <c r="BP154" s="26"/>
+      <c r="BR154" s="16"/>
       <c r="BT154" s="4"/>
-      <c r="BU154" s="4"/>
-      <c r="BV154" s="4"/>
-      <c r="BW154" s="6"/>
-      <c r="BX154" s="6"/>
-      <c r="BY154" s="4"/>
-      <c r="BZ154" s="4"/>
-      <c r="CA154" s="43"/>
-      <c r="CB154" s="7"/>
-      <c r="CD154" s="4"/>
-      <c r="CF154" s="7"/>
-    </row>
-    <row r="155" spans="39:90" x14ac:dyDescent="0.2">
-      <c r="AM155" s="2"/>
-      <c r="BL155" s="4"/>
-      <c r="BN155" s="4"/>
-      <c r="BP155" s="4"/>
-      <c r="BR155" s="4"/>
-      <c r="BT155" s="4"/>
-      <c r="BU155" s="4"/>
-      <c r="BV155" s="4"/>
-      <c r="BW155" s="4"/>
-      <c r="BX155" s="4"/>
-      <c r="BY155" s="6"/>
-      <c r="BZ155" s="4"/>
-      <c r="CA155" s="43"/>
-      <c r="CB155" s="7"/>
-      <c r="CD155" s="4"/>
-      <c r="CF155" s="7"/>
-    </row>
-    <row r="156" spans="39:90" x14ac:dyDescent="0.2">
-      <c r="AN156" s="4"/>
-      <c r="AO156" s="4"/>
-      <c r="AP156" s="4"/>
-      <c r="AQ156" s="4"/>
-      <c r="AR156" s="4"/>
-      <c r="AS156" s="4"/>
-      <c r="AT156" s="4"/>
-      <c r="AU156" s="4"/>
-      <c r="BL156" s="4"/>
-      <c r="BN156" s="4"/>
-      <c r="BP156" s="4"/>
-      <c r="BR156" s="4"/>
-      <c r="BT156" s="4"/>
+      <c r="BU154" s="7"/>
+      <c r="BV154" s="7"/>
+      <c r="BW154" s="4"/>
+      <c r="BX154" s="4"/>
+      <c r="BY154" s="7"/>
+      <c r="BZ154" s="7"/>
+      <c r="CB154" s="4"/>
+      <c r="CD154" s="7"/>
+      <c r="CF154" s="4"/>
+      <c r="CH154" s="44"/>
+    </row>
+    <row r="155" spans="39:92" x14ac:dyDescent="0.2">
+      <c r="AM155" s="4"/>
+      <c r="AN155" s="7"/>
+      <c r="AO155" s="7"/>
+      <c r="AP155" s="7"/>
+      <c r="AQ155" s="7"/>
+      <c r="AR155" s="7"/>
+      <c r="AS155" s="7"/>
+      <c r="AT155" s="7"/>
+      <c r="AU155" s="7"/>
+      <c r="AW155" s="12"/>
+      <c r="AY155" s="7"/>
+      <c r="BL155" s="6"/>
+      <c r="BN155" s="12"/>
+      <c r="BP155" s="7"/>
+      <c r="BR155" s="16"/>
+      <c r="BT155" s="6"/>
+      <c r="BU155" s="7"/>
+      <c r="BV155" s="7"/>
+      <c r="BW155" s="7"/>
+      <c r="BX155" s="7"/>
+      <c r="BY155" s="7"/>
+      <c r="BZ155" s="7"/>
+      <c r="CA155" s="4"/>
+      <c r="CB155" s="4"/>
+      <c r="CC155" s="4"/>
+      <c r="CD155" s="7"/>
+      <c r="CE155" s="4"/>
+      <c r="CF155" s="4"/>
+      <c r="CG155" s="4"/>
+      <c r="CH155" s="44"/>
+      <c r="CN155" s="45"/>
+    </row>
+    <row r="156" spans="39:92" x14ac:dyDescent="0.2">
+      <c r="AM156" s="4"/>
+      <c r="AN156" s="7"/>
+      <c r="AO156" s="7"/>
+      <c r="AP156" s="7"/>
+      <c r="AQ156" s="7"/>
+      <c r="AR156" s="7"/>
+      <c r="AS156" s="7"/>
+      <c r="AT156" s="7"/>
+      <c r="AU156" s="7"/>
+      <c r="AW156" s="12"/>
+      <c r="AY156" s="7"/>
+      <c r="BL156" s="6"/>
+      <c r="BN156" s="12"/>
+      <c r="BP156" s="7"/>
+      <c r="BR156" s="22"/>
+      <c r="BT156" s="7"/>
       <c r="BU156" s="4"/>
-      <c r="BV156" s="4"/>
-      <c r="BW156" s="4"/>
-      <c r="BX156" s="4"/>
+      <c r="BV156" s="6"/>
+      <c r="BW156" s="46"/>
+      <c r="BX156" s="46"/>
       <c r="BY156" s="4"/>
-      <c r="BZ156" s="4"/>
-      <c r="CA156" s="43"/>
+      <c r="BZ156" s="6"/>
       <c r="CB156" s="7"/>
       <c r="CD156" s="4"/>
-      <c r="CF156" s="7"/>
-    </row>
-    <row r="157" spans="39:90" x14ac:dyDescent="0.2">
+      <c r="CF156" s="4"/>
+      <c r="CH156" s="44"/>
+    </row>
+    <row r="157" spans="39:92" x14ac:dyDescent="0.2">
       <c r="AM157" s="4"/>
       <c r="AN157" s="7"/>
       <c r="AO157" s="7"/>
@@ -8767,19 +9013,27 @@
       <c r="AS157" s="7"/>
       <c r="AT157" s="7"/>
       <c r="AU157" s="7"/>
-      <c r="AV157" s="4"/>
       <c r="AW157" s="12"/>
-      <c r="AX157" s="4"/>
       <c r="AY157" s="7"/>
-      <c r="BL157" s="4"/>
-      <c r="BM157" s="4"/>
-      <c r="BN157" s="4"/>
-      <c r="BO157" s="4"/>
+      <c r="BD157" s="47"/>
+      <c r="BL157" s="6"/>
+      <c r="BN157" s="12"/>
+      <c r="BO157" s="32"/>
       <c r="BP157" s="4"/>
-      <c r="BQ157" s="28"/>
-      <c r="BR157" s="4"/>
-    </row>
-    <row r="158" spans="39:90" x14ac:dyDescent="0.2">
+      <c r="BR157" s="16"/>
+      <c r="BT157" s="4"/>
+      <c r="BU157" s="7"/>
+      <c r="BV157" s="7"/>
+      <c r="BW157" s="4"/>
+      <c r="BX157" s="4"/>
+      <c r="BY157" s="7"/>
+      <c r="BZ157" s="7"/>
+      <c r="CB157" s="7"/>
+      <c r="CD157" s="7"/>
+      <c r="CF157" s="4"/>
+      <c r="CH157" s="44"/>
+    </row>
+    <row r="158" spans="39:92" x14ac:dyDescent="0.2">
       <c r="AM158" s="4"/>
       <c r="AN158" s="7"/>
       <c r="AO158" s="7"/>
@@ -8791,160 +9045,80 @@
       <c r="AU158" s="7"/>
       <c r="AW158" s="12"/>
       <c r="AY158" s="7"/>
+      <c r="BD158" s="47"/>
       <c r="BL158" s="6"/>
-      <c r="BN158" s="12"/>
-      <c r="BP158" s="26"/>
-      <c r="BR158" s="16"/>
-      <c r="BT158" s="2"/>
-    </row>
-    <row r="159" spans="39:90" x14ac:dyDescent="0.2">
-      <c r="AM159" s="4"/>
-      <c r="AN159" s="7"/>
-      <c r="AO159" s="7"/>
-      <c r="AP159" s="7"/>
-      <c r="AQ159" s="7"/>
-      <c r="AR159" s="7"/>
-      <c r="AS159" s="7"/>
-      <c r="AT159" s="7"/>
-      <c r="AU159" s="7"/>
-      <c r="AW159" s="12"/>
-      <c r="AY159" s="7"/>
-      <c r="BL159" s="6"/>
-      <c r="BN159" s="12"/>
-      <c r="BP159" s="26"/>
-      <c r="BR159" s="22"/>
-      <c r="BT159" s="7"/>
-      <c r="BU159" s="4"/>
-      <c r="BV159" s="6"/>
-      <c r="BW159" s="7"/>
-      <c r="BX159" s="7"/>
-      <c r="BY159" s="4"/>
-      <c r="BZ159" s="6"/>
-      <c r="CB159" s="4"/>
-      <c r="CD159" s="4"/>
-      <c r="CF159" s="4"/>
-      <c r="CH159" s="44"/>
-    </row>
-    <row r="160" spans="39:90" x14ac:dyDescent="0.2">
-      <c r="AM160" s="4"/>
-      <c r="AN160" s="7"/>
-      <c r="AO160" s="7"/>
-      <c r="AP160" s="7"/>
-      <c r="AQ160" s="7"/>
-      <c r="AR160" s="7"/>
-      <c r="AS160" s="7"/>
-      <c r="AT160" s="7"/>
-      <c r="AU160" s="7"/>
-      <c r="AW160" s="12"/>
-      <c r="AY160" s="7"/>
-      <c r="BL160" s="6"/>
-      <c r="BN160" s="12"/>
-      <c r="BP160" s="26"/>
-      <c r="BR160" s="16"/>
-      <c r="BT160" s="4"/>
-      <c r="BU160" s="7"/>
-      <c r="BV160" s="7"/>
-      <c r="BW160" s="4"/>
-      <c r="BX160" s="4"/>
-      <c r="BY160" s="7"/>
-      <c r="BZ160" s="7"/>
-      <c r="CB160" s="4"/>
-      <c r="CD160" s="7"/>
-      <c r="CF160" s="4"/>
-      <c r="CH160" s="44"/>
-    </row>
-    <row r="161" spans="39:92" x14ac:dyDescent="0.2">
-      <c r="AM161" s="4"/>
-      <c r="AN161" s="7"/>
-      <c r="AO161" s="7"/>
-      <c r="AP161" s="7"/>
-      <c r="AQ161" s="7"/>
-      <c r="AR161" s="7"/>
-      <c r="AS161" s="7"/>
-      <c r="AT161" s="7"/>
-      <c r="AU161" s="7"/>
-      <c r="AW161" s="12"/>
-      <c r="AY161" s="7"/>
-      <c r="BL161" s="6"/>
-      <c r="BN161" s="12"/>
-      <c r="BP161" s="7"/>
-      <c r="BR161" s="16"/>
-      <c r="BT161" s="6"/>
-      <c r="BU161" s="7"/>
-      <c r="BV161" s="7"/>
-      <c r="BW161" s="7"/>
-      <c r="BX161" s="7"/>
-      <c r="BY161" s="7"/>
-      <c r="BZ161" s="7"/>
-      <c r="CA161" s="4"/>
-      <c r="CB161" s="4"/>
-      <c r="CC161" s="4"/>
-      <c r="CD161" s="7"/>
-      <c r="CE161" s="4"/>
-      <c r="CF161" s="4"/>
-      <c r="CG161" s="4"/>
-      <c r="CH161" s="44"/>
-      <c r="CN161" s="45"/>
-    </row>
-    <row r="162" spans="39:92" x14ac:dyDescent="0.2">
-      <c r="AM162" s="4"/>
-      <c r="AN162" s="7"/>
-      <c r="AO162" s="7"/>
-      <c r="AP162" s="7"/>
-      <c r="AQ162" s="7"/>
-      <c r="AR162" s="7"/>
-      <c r="AS162" s="7"/>
-      <c r="AT162" s="7"/>
-      <c r="AU162" s="7"/>
-      <c r="AW162" s="12"/>
-      <c r="AY162" s="7"/>
-      <c r="BL162" s="6"/>
-      <c r="BN162" s="12"/>
-      <c r="BP162" s="7"/>
-      <c r="BR162" s="22"/>
-      <c r="BT162" s="7"/>
-      <c r="BU162" s="4"/>
-      <c r="BV162" s="6"/>
-      <c r="BW162" s="46"/>
-      <c r="BX162" s="46"/>
-      <c r="BY162" s="4"/>
-      <c r="BZ162" s="6"/>
-      <c r="CB162" s="7"/>
-      <c r="CD162" s="4"/>
-      <c r="CF162" s="4"/>
-      <c r="CH162" s="44"/>
-    </row>
-    <row r="163" spans="39:92" x14ac:dyDescent="0.2">
-      <c r="AM163" s="4"/>
-      <c r="AN163" s="7"/>
-      <c r="AO163" s="7"/>
-      <c r="AP163" s="7"/>
-      <c r="AQ163" s="7"/>
-      <c r="AR163" s="7"/>
-      <c r="AS163" s="7"/>
-      <c r="AT163" s="7"/>
-      <c r="AU163" s="7"/>
-      <c r="AW163" s="12"/>
-      <c r="AY163" s="7"/>
-      <c r="BD163" s="47"/>
-      <c r="BL163" s="6"/>
-      <c r="BN163" s="12"/>
-      <c r="BO163" s="32"/>
-      <c r="BP163" s="4"/>
-      <c r="BR163" s="16"/>
-      <c r="BT163" s="4"/>
-      <c r="BU163" s="7"/>
-      <c r="BV163" s="7"/>
-      <c r="BW163" s="4"/>
-      <c r="BX163" s="4"/>
-      <c r="BY163" s="7"/>
-      <c r="BZ163" s="7"/>
-      <c r="CB163" s="7"/>
-      <c r="CD163" s="7"/>
-      <c r="CF163" s="4"/>
-      <c r="CH163" s="44"/>
-    </row>
-    <row r="164" spans="39:92" x14ac:dyDescent="0.2">
+      <c r="BN158" s="4"/>
+      <c r="BP158" s="4"/>
+      <c r="BR158" s="4"/>
+      <c r="BT158" s="6"/>
+      <c r="BU158" s="7"/>
+      <c r="BV158" s="7"/>
+      <c r="BW158" s="6"/>
+      <c r="BX158" s="6"/>
+      <c r="BY158" s="7"/>
+      <c r="BZ158" s="7"/>
+      <c r="CB158" s="7"/>
+      <c r="CD158" s="7"/>
+      <c r="CF158" s="4"/>
+      <c r="CH158" s="48"/>
+    </row>
+    <row r="159" spans="39:92" x14ac:dyDescent="0.2">
+      <c r="BD159" s="47"/>
+      <c r="BR159" s="32"/>
+    </row>
+    <row r="160" spans="39:92" x14ac:dyDescent="0.2">
+      <c r="AS160" s="29"/>
+      <c r="BD160" s="47"/>
+      <c r="BK160" s="2"/>
+      <c r="BP160" s="32"/>
+    </row>
+    <row r="161" spans="39:91" x14ac:dyDescent="0.2">
+      <c r="BD161" s="47"/>
+      <c r="BJ161" s="4"/>
+      <c r="BK161" s="4"/>
+      <c r="BL161" s="4"/>
+      <c r="BM161" s="4"/>
+      <c r="BN161" s="4"/>
+      <c r="BO161" s="4"/>
+      <c r="BP161" s="4"/>
+      <c r="BQ161" s="4"/>
+      <c r="BR161" s="4"/>
+      <c r="BW161" s="49"/>
+      <c r="BX161" s="49"/>
+      <c r="CC161" s="29"/>
+    </row>
+    <row r="162" spans="39:91" x14ac:dyDescent="0.2">
+      <c r="AM162" s="2"/>
+      <c r="AZ162" s="50"/>
+      <c r="BA162" s="50"/>
+      <c r="BB162" s="50"/>
+      <c r="BC162" s="50"/>
+      <c r="BD162" s="47"/>
+      <c r="BK162" s="33"/>
+      <c r="BL162" s="33"/>
+      <c r="BN162" s="32"/>
+      <c r="BT162" s="2"/>
+      <c r="CA162" s="33"/>
+      <c r="CB162" s="33"/>
+      <c r="CC162" s="32"/>
+    </row>
+    <row r="163" spans="39:91" x14ac:dyDescent="0.2">
+      <c r="AN163" s="4"/>
+      <c r="AO163" s="4"/>
+      <c r="AP163" s="4"/>
+      <c r="AQ163" s="4"/>
+      <c r="AR163" s="4"/>
+      <c r="AS163" s="4"/>
+      <c r="AT163" s="4"/>
+      <c r="AU163" s="4"/>
+      <c r="AZ163" s="50"/>
+      <c r="BA163" s="50"/>
+      <c r="BB163" s="50"/>
+      <c r="BC163" s="50"/>
+      <c r="BD163" s="50"/>
+      <c r="BE163" s="50"/>
+    </row>
+    <row r="164" spans="39:91" x14ac:dyDescent="0.2">
       <c r="AM164" s="4"/>
       <c r="AN164" s="7"/>
       <c r="AO164" s="7"/>
@@ -8954,82 +9128,158 @@
       <c r="AS164" s="7"/>
       <c r="AT164" s="7"/>
       <c r="AU164" s="7"/>
-      <c r="AW164" s="12"/>
-      <c r="AY164" s="7"/>
-      <c r="BD164" s="47"/>
-      <c r="BL164" s="6"/>
-      <c r="BN164" s="4"/>
-      <c r="BP164" s="4"/>
-      <c r="BR164" s="4"/>
-      <c r="BT164" s="6"/>
-      <c r="BU164" s="7"/>
-      <c r="BV164" s="7"/>
-      <c r="BW164" s="6"/>
-      <c r="BX164" s="6"/>
-      <c r="BY164" s="7"/>
-      <c r="BZ164" s="7"/>
-      <c r="CB164" s="7"/>
-      <c r="CD164" s="7"/>
-      <c r="CF164" s="4"/>
-      <c r="CH164" s="48"/>
-    </row>
-    <row r="165" spans="39:92" x14ac:dyDescent="0.2">
-      <c r="BD165" s="47"/>
-      <c r="BR165" s="32"/>
-    </row>
-    <row r="166" spans="39:92" x14ac:dyDescent="0.2">
-      <c r="AS166" s="29"/>
-      <c r="BD166" s="47"/>
-      <c r="BK166" s="2"/>
-      <c r="BP166" s="32"/>
-    </row>
-    <row r="167" spans="39:92" x14ac:dyDescent="0.2">
-      <c r="BD167" s="47"/>
-      <c r="BJ167" s="4"/>
-      <c r="BK167" s="4"/>
-      <c r="BL167" s="4"/>
-      <c r="BM167" s="4"/>
-      <c r="BN167" s="4"/>
-      <c r="BO167" s="4"/>
-      <c r="BP167" s="4"/>
-      <c r="BQ167" s="4"/>
-      <c r="BR167" s="4"/>
-      <c r="BW167" s="49"/>
-      <c r="BX167" s="49"/>
-      <c r="CC167" s="29"/>
-    </row>
-    <row r="168" spans="39:92" x14ac:dyDescent="0.2">
-      <c r="AM168" s="2"/>
+      <c r="AV164" s="4"/>
+      <c r="AW164" s="3"/>
+      <c r="AX164" s="4"/>
+      <c r="AY164" s="12"/>
+      <c r="AZ164" s="30"/>
+      <c r="BA164" s="51"/>
+      <c r="BB164" s="50"/>
+      <c r="BC164" s="50"/>
+      <c r="BD164" s="52"/>
+      <c r="BE164" s="50"/>
+      <c r="BQ164" s="33"/>
+    </row>
+    <row r="165" spans="39:91" x14ac:dyDescent="0.2">
+      <c r="AM165" s="4"/>
+      <c r="AN165" s="7"/>
+      <c r="AO165" s="7"/>
+      <c r="AP165" s="7"/>
+      <c r="AQ165" s="7"/>
+      <c r="AR165" s="7"/>
+      <c r="AS165" s="7"/>
+      <c r="AT165" s="7"/>
+      <c r="AU165" s="7"/>
+      <c r="AW165" s="3"/>
+      <c r="AY165" s="12"/>
+      <c r="AZ165" s="50"/>
+      <c r="BA165" s="51"/>
+      <c r="BB165" s="50"/>
+      <c r="BC165" s="50"/>
+      <c r="BD165" s="52"/>
+      <c r="BE165" s="50"/>
+      <c r="BK165" s="2"/>
+      <c r="BT165" s="2"/>
+      <c r="BY165" s="2"/>
+    </row>
+    <row r="166" spans="39:91" x14ac:dyDescent="0.2">
+      <c r="AM166" s="4"/>
+      <c r="AN166" s="7"/>
+      <c r="AO166" s="7"/>
+      <c r="AP166" s="7"/>
+      <c r="AQ166" s="7"/>
+      <c r="AR166" s="7"/>
+      <c r="AS166" s="7"/>
+      <c r="AT166" s="7"/>
+      <c r="AU166" s="7"/>
+      <c r="AW166" s="3"/>
+      <c r="AY166" s="12"/>
+      <c r="AZ166" s="50"/>
+      <c r="BA166" s="51"/>
+      <c r="BB166" s="53"/>
+      <c r="BC166" s="50"/>
+      <c r="BD166" s="54"/>
+      <c r="BE166" s="50"/>
+      <c r="BP166" s="55"/>
+      <c r="BQ166" s="56"/>
+      <c r="BR166" s="57"/>
+      <c r="BT166" s="12"/>
+      <c r="BU166" s="58"/>
+      <c r="BV166" s="2"/>
+      <c r="BY166" s="12"/>
+      <c r="BZ166" s="56"/>
+      <c r="CA166" s="2"/>
+    </row>
+    <row r="167" spans="39:91" x14ac:dyDescent="0.2">
+      <c r="AM167" s="4"/>
+      <c r="AN167" s="7"/>
+      <c r="AO167" s="7"/>
+      <c r="AP167" s="7"/>
+      <c r="AQ167" s="7"/>
+      <c r="AR167" s="7"/>
+      <c r="AS167" s="7"/>
+      <c r="AT167" s="7"/>
+      <c r="AU167" s="7"/>
+      <c r="AW167" s="3"/>
+      <c r="AY167" s="12"/>
+      <c r="BA167" s="51"/>
+      <c r="BB167" s="53"/>
+      <c r="BC167" s="50"/>
+      <c r="BD167" s="52"/>
+      <c r="BE167" s="50"/>
+      <c r="BP167" s="55"/>
+      <c r="BQ167" s="56"/>
+      <c r="BR167" s="57"/>
+      <c r="BT167" s="12"/>
+      <c r="BU167" s="58"/>
+      <c r="BV167" s="2"/>
+      <c r="BY167" s="12"/>
+      <c r="BZ167" s="56"/>
+      <c r="CA167" s="2"/>
+    </row>
+    <row r="168" spans="39:91" x14ac:dyDescent="0.2">
+      <c r="AM168" s="4"/>
+      <c r="AN168" s="7"/>
+      <c r="AO168" s="7"/>
+      <c r="AP168" s="7"/>
+      <c r="AQ168" s="7"/>
+      <c r="AR168" s="7"/>
+      <c r="AS168" s="7"/>
+      <c r="AT168" s="7"/>
+      <c r="AU168" s="7"/>
+      <c r="AW168" s="3"/>
+      <c r="AY168" s="12"/>
       <c r="AZ168" s="50"/>
-      <c r="BA168" s="50"/>
+      <c r="BA168" s="51"/>
       <c r="BB168" s="50"/>
       <c r="BC168" s="50"/>
-      <c r="BD168" s="47"/>
-      <c r="BK168" s="33"/>
-      <c r="BL168" s="33"/>
-      <c r="BN168" s="32"/>
-      <c r="BT168" s="2"/>
-      <c r="CA168" s="33"/>
-      <c r="CB168" s="33"/>
-      <c r="CC168" s="32"/>
-    </row>
-    <row r="169" spans="39:92" x14ac:dyDescent="0.2">
-      <c r="AN169" s="4"/>
-      <c r="AO169" s="4"/>
-      <c r="AP169" s="4"/>
-      <c r="AQ169" s="4"/>
-      <c r="AR169" s="4"/>
-      <c r="AS169" s="4"/>
-      <c r="AT169" s="4"/>
-      <c r="AU169" s="4"/>
+      <c r="BD168" s="52"/>
+      <c r="BE168" s="50"/>
+      <c r="BP168" s="55"/>
+      <c r="BQ168" s="56"/>
+      <c r="BR168" s="57"/>
+      <c r="BT168" s="12"/>
+      <c r="BU168" s="58"/>
+      <c r="BV168" s="2"/>
+      <c r="BW168" s="59"/>
+      <c r="BX168" s="59"/>
+      <c r="BY168" s="12"/>
+      <c r="BZ168" s="56"/>
+      <c r="CA168" s="2"/>
+    </row>
+    <row r="169" spans="39:91" x14ac:dyDescent="0.2">
+      <c r="AM169" s="4"/>
+      <c r="AN169" s="7"/>
+      <c r="AO169" s="7"/>
+      <c r="AP169" s="7"/>
+      <c r="AQ169" s="7"/>
+      <c r="AR169" s="7"/>
+      <c r="AS169" s="7"/>
+      <c r="AT169" s="7"/>
+      <c r="AU169" s="7"/>
+      <c r="AW169" s="3"/>
+      <c r="AY169" s="12"/>
       <c r="AZ169" s="50"/>
-      <c r="BA169" s="50"/>
+      <c r="BA169" s="51"/>
       <c r="BB169" s="50"/>
       <c r="BC169" s="50"/>
-      <c r="BD169" s="50"/>
+      <c r="BD169" s="52"/>
       <c r="BE169" s="50"/>
-    </row>
-    <row r="170" spans="39:92" x14ac:dyDescent="0.2">
+      <c r="BL169" s="60"/>
+      <c r="BM169" s="61"/>
+      <c r="BN169" s="61"/>
+      <c r="BP169" s="55"/>
+      <c r="BQ169" s="56"/>
+      <c r="BT169" s="12"/>
+      <c r="BU169" s="58"/>
+      <c r="BV169" s="2"/>
+      <c r="BW169" s="59"/>
+      <c r="BX169" s="59"/>
+      <c r="BY169" s="12"/>
+      <c r="BZ169" s="56"/>
+      <c r="CA169" s="2"/>
+    </row>
+    <row r="170" spans="39:91" x14ac:dyDescent="0.2">
       <c r="AM170" s="4"/>
       <c r="AN170" s="7"/>
       <c r="AO170" s="7"/>
@@ -9039,19 +9289,24 @@
       <c r="AS170" s="7"/>
       <c r="AT170" s="7"/>
       <c r="AU170" s="7"/>
-      <c r="AV170" s="4"/>
       <c r="AW170" s="3"/>
-      <c r="AX170" s="4"/>
       <c r="AY170" s="12"/>
-      <c r="AZ170" s="30"/>
+      <c r="AZ170" s="50"/>
       <c r="BA170" s="51"/>
-      <c r="BB170" s="50"/>
+      <c r="BB170" s="53"/>
       <c r="BC170" s="50"/>
       <c r="BD170" s="52"/>
       <c r="BE170" s="50"/>
-      <c r="BQ170" s="33"/>
-    </row>
-    <row r="171" spans="39:92" x14ac:dyDescent="0.2">
+      <c r="BP170" s="55"/>
+      <c r="BQ170" s="47"/>
+      <c r="BT170" s="12"/>
+      <c r="BU170" s="58"/>
+      <c r="BV170" s="2"/>
+      <c r="BY170" s="12"/>
+      <c r="BZ170" s="56"/>
+      <c r="CA170" s="2"/>
+    </row>
+    <row r="171" spans="39:91" x14ac:dyDescent="0.2">
       <c r="AM171" s="4"/>
       <c r="AN171" s="7"/>
       <c r="AO171" s="7"/>
@@ -9065,157 +9320,88 @@
       <c r="AY171" s="12"/>
       <c r="AZ171" s="50"/>
       <c r="BA171" s="51"/>
-      <c r="BB171" s="50"/>
+      <c r="BB171" s="53"/>
       <c r="BC171" s="50"/>
       <c r="BD171" s="52"/>
       <c r="BE171" s="50"/>
-      <c r="BK171" s="2"/>
-      <c r="BT171" s="2"/>
-      <c r="BY171" s="2"/>
-    </row>
-    <row r="172" spans="39:92" x14ac:dyDescent="0.2">
-      <c r="AM172" s="4"/>
-      <c r="AN172" s="7"/>
-      <c r="AO172" s="7"/>
-      <c r="AP172" s="7"/>
-      <c r="AQ172" s="7"/>
-      <c r="AR172" s="7"/>
-      <c r="AS172" s="7"/>
-      <c r="AT172" s="7"/>
-      <c r="AU172" s="7"/>
-      <c r="AW172" s="3"/>
-      <c r="AY172" s="12"/>
-      <c r="AZ172" s="50"/>
-      <c r="BA172" s="51"/>
-      <c r="BB172" s="53"/>
+      <c r="BP171" s="55"/>
+      <c r="BQ171" s="47"/>
+      <c r="BT171" s="12"/>
+      <c r="BU171" s="58"/>
+      <c r="BV171" s="2"/>
+      <c r="BY171" s="12"/>
+      <c r="BZ171" s="56"/>
+      <c r="CA171" s="2"/>
+      <c r="CF171" s="2"/>
+    </row>
+    <row r="172" spans="39:91" x14ac:dyDescent="0.2">
+      <c r="BB172" s="50"/>
       <c r="BC172" s="50"/>
-      <c r="BD172" s="54"/>
+      <c r="BD172" s="50"/>
       <c r="BE172" s="50"/>
-      <c r="BP172" s="55"/>
-      <c r="BQ172" s="56"/>
-      <c r="BR172" s="57"/>
-      <c r="BT172" s="12"/>
-      <c r="BU172" s="58"/>
-      <c r="BV172" s="2"/>
+      <c r="BW172" s="59"/>
+      <c r="BX172" s="59"/>
       <c r="BY172" s="12"/>
       <c r="BZ172" s="56"/>
       <c r="CA172" s="2"/>
     </row>
-    <row r="173" spans="39:92" x14ac:dyDescent="0.2">
-      <c r="AM173" s="4"/>
-      <c r="AN173" s="7"/>
-      <c r="AO173" s="7"/>
-      <c r="AP173" s="7"/>
-      <c r="AQ173" s="7"/>
-      <c r="AR173" s="7"/>
-      <c r="AS173" s="7"/>
-      <c r="AT173" s="7"/>
-      <c r="AU173" s="7"/>
-      <c r="AW173" s="3"/>
-      <c r="AY173" s="12"/>
-      <c r="BA173" s="51"/>
-      <c r="BB173" s="53"/>
+    <row r="173" spans="39:91" x14ac:dyDescent="0.2">
+      <c r="AZ173" s="50"/>
+      <c r="BA173" s="50"/>
+      <c r="BB173" s="62"/>
       <c r="BC173" s="50"/>
-      <c r="BD173" s="52"/>
+      <c r="BD173" s="50"/>
       <c r="BE173" s="50"/>
-      <c r="BP173" s="55"/>
-      <c r="BQ173" s="56"/>
-      <c r="BR173" s="57"/>
-      <c r="BT173" s="12"/>
-      <c r="BU173" s="58"/>
-      <c r="BV173" s="2"/>
+      <c r="BF173" s="50"/>
+      <c r="BW173" s="59"/>
+      <c r="BX173" s="59"/>
       <c r="BY173" s="12"/>
       <c r="BZ173" s="56"/>
       <c r="CA173" s="2"/>
     </row>
-    <row r="174" spans="39:92" x14ac:dyDescent="0.2">
-      <c r="AM174" s="4"/>
-      <c r="AN174" s="7"/>
-      <c r="AO174" s="7"/>
-      <c r="AP174" s="7"/>
-      <c r="AQ174" s="7"/>
-      <c r="AR174" s="7"/>
-      <c r="AS174" s="7"/>
-      <c r="AT174" s="7"/>
-      <c r="AU174" s="7"/>
-      <c r="AW174" s="3"/>
-      <c r="AY174" s="12"/>
+    <row r="174" spans="39:91" x14ac:dyDescent="0.2">
       <c r="AZ174" s="50"/>
-      <c r="BA174" s="51"/>
+      <c r="BA174" s="50"/>
       <c r="BB174" s="50"/>
       <c r="BC174" s="50"/>
-      <c r="BD174" s="52"/>
+      <c r="BD174" s="50"/>
       <c r="BE174" s="50"/>
-      <c r="BP174" s="55"/>
-      <c r="BQ174" s="56"/>
-      <c r="BR174" s="57"/>
-      <c r="BT174" s="12"/>
-      <c r="BU174" s="58"/>
-      <c r="BV174" s="2"/>
-      <c r="BW174" s="59"/>
-      <c r="BX174" s="59"/>
-      <c r="BY174" s="12"/>
-      <c r="BZ174" s="56"/>
-      <c r="CA174" s="2"/>
-    </row>
-    <row r="175" spans="39:92" x14ac:dyDescent="0.2">
-      <c r="AM175" s="4"/>
-      <c r="AN175" s="7"/>
-      <c r="AO175" s="7"/>
-      <c r="AP175" s="7"/>
-      <c r="AQ175" s="7"/>
-      <c r="AR175" s="7"/>
-      <c r="AS175" s="7"/>
-      <c r="AT175" s="7"/>
-      <c r="AU175" s="7"/>
-      <c r="AW175" s="3"/>
-      <c r="AY175" s="12"/>
+      <c r="BF174" s="50"/>
+    </row>
+    <row r="175" spans="39:91" x14ac:dyDescent="0.2">
+      <c r="AM175" s="2"/>
       <c r="AZ175" s="50"/>
-      <c r="BA175" s="51"/>
+      <c r="BA175" s="50"/>
       <c r="BB175" s="50"/>
       <c r="BC175" s="50"/>
-      <c r="BD175" s="52"/>
+      <c r="BD175" s="50"/>
       <c r="BE175" s="50"/>
-      <c r="BL175" s="60"/>
-      <c r="BM175" s="61"/>
-      <c r="BN175" s="61"/>
-      <c r="BP175" s="55"/>
-      <c r="BQ175" s="56"/>
-      <c r="BT175" s="12"/>
-      <c r="BU175" s="58"/>
-      <c r="BV175" s="2"/>
-      <c r="BW175" s="59"/>
-      <c r="BX175" s="59"/>
-      <c r="BY175" s="12"/>
-      <c r="BZ175" s="56"/>
-      <c r="CA175" s="2"/>
-    </row>
-    <row r="176" spans="39:92" x14ac:dyDescent="0.2">
-      <c r="AM176" s="4"/>
-      <c r="AN176" s="7"/>
-      <c r="AO176" s="7"/>
-      <c r="AP176" s="7"/>
-      <c r="AQ176" s="7"/>
-      <c r="AR176" s="7"/>
-      <c r="AS176" s="7"/>
-      <c r="AT176" s="7"/>
-      <c r="AU176" s="7"/>
-      <c r="AW176" s="3"/>
-      <c r="AY176" s="12"/>
+      <c r="BF175" s="50"/>
+    </row>
+    <row r="176" spans="39:91" x14ac:dyDescent="0.2">
+      <c r="AN176" s="4"/>
+      <c r="AO176" s="4"/>
+      <c r="AP176" s="4"/>
+      <c r="AQ176" s="4"/>
+      <c r="AR176" s="4"/>
+      <c r="AS176" s="4"/>
+      <c r="AT176" s="4"/>
+      <c r="AU176" s="4"/>
+      <c r="AW176" s="7"/>
       <c r="AZ176" s="50"/>
-      <c r="BA176" s="51"/>
-      <c r="BB176" s="53"/>
+      <c r="BA176" s="50"/>
+      <c r="BB176" s="50"/>
       <c r="BC176" s="50"/>
-      <c r="BD176" s="52"/>
+      <c r="BD176" s="50"/>
       <c r="BE176" s="50"/>
-      <c r="BP176" s="55"/>
-      <c r="BQ176" s="47"/>
-      <c r="BT176" s="12"/>
-      <c r="BU176" s="58"/>
-      <c r="BV176" s="2"/>
-      <c r="BY176" s="12"/>
-      <c r="BZ176" s="56"/>
-      <c r="CA176" s="2"/>
+      <c r="BF176" s="50"/>
+      <c r="BK176" s="2"/>
+      <c r="BP176" s="2"/>
+      <c r="BT176" s="2"/>
+      <c r="BY176" s="2"/>
+      <c r="CD176" s="2"/>
+      <c r="CI176" s="2"/>
+      <c r="CM176" s="2"/>
     </row>
     <row r="177" spans="39:93" x14ac:dyDescent="0.2">
       <c r="AM177" s="4"/>
@@ -9223,375 +9409,294 @@
       <c r="AO177" s="7"/>
       <c r="AP177" s="7"/>
       <c r="AQ177" s="7"/>
-      <c r="AR177" s="7"/>
-      <c r="AS177" s="7"/>
-      <c r="AT177" s="7"/>
-      <c r="AU177" s="7"/>
-      <c r="AW177" s="3"/>
-      <c r="AY177" s="12"/>
+      <c r="AR177" s="6"/>
+      <c r="AS177" s="6"/>
+      <c r="AT177" s="6"/>
+      <c r="AU177" s="6"/>
+      <c r="AW177" s="7"/>
+      <c r="AY177" s="7"/>
       <c r="AZ177" s="50"/>
-      <c r="BA177" s="51"/>
-      <c r="BB177" s="53"/>
-      <c r="BC177" s="50"/>
-      <c r="BD177" s="52"/>
+      <c r="BA177" s="26"/>
+      <c r="BB177" s="50"/>
+      <c r="BC177" s="48"/>
+      <c r="BD177" s="48"/>
       <c r="BE177" s="50"/>
-      <c r="BP177" s="55"/>
+      <c r="BF177" s="63"/>
+      <c r="BK177" s="26"/>
+      <c r="BL177" s="47"/>
+      <c r="BM177" s="2"/>
+      <c r="BP177" s="4"/>
       <c r="BQ177" s="47"/>
-      <c r="BT177" s="12"/>
-      <c r="BU177" s="58"/>
+      <c r="BR177" s="2"/>
+      <c r="BT177" s="4"/>
+      <c r="BU177" s="47"/>
       <c r="BV177" s="2"/>
-      <c r="BY177" s="12"/>
-      <c r="BZ177" s="56"/>
+      <c r="BY177" s="4"/>
+      <c r="BZ177" s="47"/>
       <c r="CA177" s="2"/>
+      <c r="CD177" s="4"/>
+      <c r="CE177" s="47"/>
       <c r="CF177" s="2"/>
+      <c r="CI177" s="4"/>
+      <c r="CJ177" s="47"/>
+      <c r="CK177" s="2"/>
+      <c r="CM177" s="4"/>
+      <c r="CN177" s="47"/>
+      <c r="CO177" s="2"/>
     </row>
     <row r="178" spans="39:93" x14ac:dyDescent="0.2">
+      <c r="AM178" s="4"/>
+      <c r="AN178" s="7"/>
+      <c r="AO178" s="7"/>
+      <c r="AP178" s="7"/>
+      <c r="AQ178" s="7"/>
+      <c r="AR178" s="6"/>
+      <c r="AS178" s="6"/>
+      <c r="AT178" s="6"/>
+      <c r="AU178" s="6"/>
+      <c r="AW178" s="7"/>
+      <c r="AY178" s="7"/>
+      <c r="AZ178" s="50"/>
+      <c r="BA178" s="26"/>
       <c r="BB178" s="50"/>
-      <c r="BC178" s="50"/>
-      <c r="BD178" s="50"/>
+      <c r="BC178" s="48"/>
+      <c r="BD178" s="48"/>
       <c r="BE178" s="50"/>
-      <c r="BW178" s="59"/>
-      <c r="BX178" s="59"/>
-      <c r="BY178" s="12"/>
-      <c r="BZ178" s="56"/>
+      <c r="BF178" s="63"/>
+      <c r="BK178" s="26"/>
+      <c r="BL178" s="47"/>
+      <c r="BM178" s="2"/>
+      <c r="BP178" s="4"/>
+      <c r="BQ178" s="47"/>
+      <c r="BR178" s="2"/>
+      <c r="BT178" s="4"/>
+      <c r="BU178" s="47"/>
+      <c r="BV178" s="2"/>
+      <c r="BY178" s="4"/>
+      <c r="BZ178" s="47"/>
       <c r="CA178" s="2"/>
+      <c r="CD178" s="4"/>
+      <c r="CE178" s="47"/>
+      <c r="CF178" s="2"/>
+      <c r="CI178" s="4"/>
+      <c r="CJ178" s="47"/>
+      <c r="CK178" s="2"/>
+      <c r="CM178" s="4"/>
+      <c r="CN178" s="47"/>
+      <c r="CO178" s="2"/>
     </row>
     <row r="179" spans="39:93" x14ac:dyDescent="0.2">
-      <c r="AZ179" s="50"/>
-      <c r="BA179" s="50"/>
-      <c r="BB179" s="62"/>
-      <c r="BC179" s="50"/>
-      <c r="BD179" s="50"/>
-      <c r="BE179" s="50"/>
-      <c r="BF179" s="50"/>
-      <c r="BW179" s="59"/>
-      <c r="BX179" s="59"/>
-      <c r="BY179" s="12"/>
-      <c r="BZ179" s="56"/>
+      <c r="AM179" s="4"/>
+      <c r="AN179" s="7"/>
+      <c r="AO179" s="7"/>
+      <c r="AP179" s="7"/>
+      <c r="AQ179" s="7"/>
+      <c r="AR179" s="6"/>
+      <c r="AS179" s="6"/>
+      <c r="AT179" s="6"/>
+      <c r="AU179" s="6"/>
+      <c r="AV179" s="4"/>
+      <c r="AW179" s="7"/>
+      <c r="AX179" s="4"/>
+      <c r="AY179" s="7"/>
+      <c r="AZ179" s="30"/>
+      <c r="BA179" s="26"/>
+      <c r="BB179" s="30"/>
+      <c r="BC179" s="48"/>
+      <c r="BD179" s="48"/>
+      <c r="BE179" s="30"/>
+      <c r="BF179" s="63"/>
+      <c r="BK179" s="26"/>
+      <c r="BL179" s="47"/>
+      <c r="BM179" s="2"/>
+      <c r="BP179" s="4"/>
+      <c r="BQ179" s="47"/>
+      <c r="BR179" s="2"/>
+      <c r="BT179" s="4"/>
+      <c r="BU179" s="47"/>
+      <c r="BV179" s="2"/>
+      <c r="BY179" s="4"/>
+      <c r="BZ179" s="47"/>
       <c r="CA179" s="2"/>
+      <c r="CD179" s="4"/>
+      <c r="CE179" s="47"/>
+      <c r="CF179" s="2"/>
+      <c r="CI179" s="4"/>
+      <c r="CJ179" s="47"/>
+      <c r="CK179" s="2"/>
+      <c r="CM179" s="4"/>
+      <c r="CN179" s="47"/>
+      <c r="CO179" s="2"/>
     </row>
     <row r="180" spans="39:93" x14ac:dyDescent="0.2">
+      <c r="AM180" s="4"/>
+      <c r="AN180" s="4"/>
+      <c r="AO180" s="4"/>
+      <c r="AP180" s="4"/>
+      <c r="AQ180" s="4"/>
+      <c r="AR180" s="7"/>
+      <c r="AS180" s="7"/>
+      <c r="AT180" s="7"/>
+      <c r="AU180" s="7"/>
+      <c r="AW180" s="7"/>
+      <c r="AY180" s="7"/>
       <c r="AZ180" s="50"/>
-      <c r="BA180" s="50"/>
+      <c r="BA180" s="26"/>
       <c r="BB180" s="50"/>
-      <c r="BC180" s="50"/>
-      <c r="BD180" s="50"/>
+      <c r="BC180" s="48"/>
+      <c r="BD180" s="48"/>
       <c r="BE180" s="50"/>
-      <c r="BF180" s="50"/>
+      <c r="BF180" s="63"/>
+      <c r="BK180" s="26"/>
+      <c r="BL180" s="47"/>
+      <c r="BM180" s="2"/>
+      <c r="BP180" s="4"/>
+      <c r="BQ180" s="47"/>
+      <c r="BR180" s="2"/>
+      <c r="BT180" s="4"/>
+      <c r="BU180" s="47"/>
+      <c r="BV180" s="2"/>
+      <c r="BY180" s="4"/>
+      <c r="BZ180" s="47"/>
+      <c r="CA180" s="2"/>
+      <c r="CD180" s="4"/>
+      <c r="CE180" s="47"/>
+      <c r="CF180" s="2"/>
+      <c r="CI180" s="4"/>
+      <c r="CJ180" s="47"/>
+      <c r="CK180" s="2"/>
+      <c r="CM180" s="4"/>
+      <c r="CN180" s="47"/>
+      <c r="CO180" s="2"/>
     </row>
     <row r="181" spans="39:93" x14ac:dyDescent="0.2">
-      <c r="AM181" s="2"/>
+      <c r="AM181" s="4"/>
+      <c r="AN181" s="4"/>
+      <c r="AO181" s="4"/>
+      <c r="AP181" s="4"/>
+      <c r="AQ181" s="4"/>
+      <c r="AR181" s="7"/>
+      <c r="AS181" s="7"/>
+      <c r="AT181" s="7"/>
+      <c r="AU181" s="7"/>
+      <c r="AW181" s="7"/>
+      <c r="AY181" s="7"/>
       <c r="AZ181" s="50"/>
-      <c r="BA181" s="50"/>
+      <c r="BA181" s="26"/>
       <c r="BB181" s="50"/>
-      <c r="BC181" s="50"/>
-      <c r="BD181" s="50"/>
+      <c r="BC181" s="48"/>
+      <c r="BD181" s="48"/>
       <c r="BE181" s="50"/>
-      <c r="BF181" s="50"/>
+      <c r="BF181" s="63"/>
+      <c r="BK181" s="26"/>
+      <c r="BL181" s="47"/>
+      <c r="BM181" s="2"/>
+      <c r="BP181" s="4"/>
+      <c r="BQ181" s="47"/>
+      <c r="BR181" s="2"/>
+      <c r="BT181" s="4"/>
+      <c r="BU181" s="47"/>
+      <c r="BV181" s="2"/>
+      <c r="BY181" s="4"/>
+      <c r="BZ181" s="47"/>
+      <c r="CA181" s="2"/>
+      <c r="CD181" s="4"/>
+      <c r="CE181" s="47"/>
+      <c r="CF181" s="2"/>
+      <c r="CI181" s="4"/>
+      <c r="CJ181" s="47"/>
+      <c r="CK181" s="2"/>
+      <c r="CM181" s="4"/>
+      <c r="CN181" s="47"/>
+      <c r="CO181" s="2"/>
     </row>
     <row r="182" spans="39:93" x14ac:dyDescent="0.2">
+      <c r="AM182" s="4"/>
       <c r="AN182" s="4"/>
       <c r="AO182" s="4"/>
       <c r="AP182" s="4"/>
       <c r="AQ182" s="4"/>
-      <c r="AR182" s="4"/>
-      <c r="AS182" s="4"/>
-      <c r="AT182" s="4"/>
-      <c r="AU182" s="4"/>
+      <c r="AR182" s="7"/>
+      <c r="AS182" s="7"/>
+      <c r="AT182" s="7"/>
+      <c r="AU182" s="7"/>
       <c r="AW182" s="7"/>
+      <c r="AY182" s="7"/>
       <c r="AZ182" s="50"/>
-      <c r="BA182" s="50"/>
+      <c r="BA182" s="26"/>
       <c r="BB182" s="50"/>
-      <c r="BC182" s="50"/>
-      <c r="BD182" s="50"/>
+      <c r="BC182" s="48"/>
+      <c r="BD182" s="48"/>
       <c r="BE182" s="50"/>
-      <c r="BF182" s="50"/>
-      <c r="BK182" s="2"/>
-      <c r="BP182" s="2"/>
-      <c r="BT182" s="2"/>
-      <c r="BY182" s="2"/>
-      <c r="CD182" s="2"/>
-      <c r="CI182" s="2"/>
-      <c r="CM182" s="2"/>
+      <c r="BF182" s="63"/>
+      <c r="BK182" s="26"/>
+      <c r="BL182" s="47"/>
+      <c r="BM182" s="2"/>
+      <c r="BP182" s="4"/>
+      <c r="BQ182" s="47"/>
+      <c r="BR182" s="2"/>
+      <c r="BT182" s="4"/>
+      <c r="BU182" s="47"/>
+      <c r="BV182" s="2"/>
+      <c r="BY182" s="4"/>
+      <c r="BZ182" s="47"/>
+      <c r="CA182" s="2"/>
+      <c r="CD182" s="4"/>
+      <c r="CE182" s="47"/>
+      <c r="CF182" s="2"/>
+      <c r="CI182" s="4"/>
+      <c r="CJ182" s="47"/>
+      <c r="CK182" s="2"/>
+      <c r="CM182" s="4"/>
+      <c r="CN182" s="47"/>
+      <c r="CO182" s="2"/>
     </row>
     <row r="183" spans="39:93" x14ac:dyDescent="0.2">
-      <c r="AM183" s="4"/>
-      <c r="AN183" s="7"/>
-      <c r="AO183" s="7"/>
-      <c r="AP183" s="7"/>
-      <c r="AQ183" s="7"/>
-      <c r="AR183" s="6"/>
-      <c r="AS183" s="6"/>
-      <c r="AT183" s="6"/>
-      <c r="AU183" s="6"/>
       <c r="AW183" s="7"/>
-      <c r="AY183" s="7"/>
       <c r="AZ183" s="50"/>
-      <c r="BA183" s="26"/>
+      <c r="BA183" s="50"/>
       <c r="BB183" s="50"/>
-      <c r="BC183" s="48"/>
-      <c r="BD183" s="48"/>
+      <c r="BC183" s="50"/>
+      <c r="BD183" s="50"/>
       <c r="BE183" s="50"/>
-      <c r="BF183" s="63"/>
-      <c r="BK183" s="26"/>
-      <c r="BL183" s="47"/>
-      <c r="BM183" s="2"/>
-      <c r="BP183" s="4"/>
-      <c r="BQ183" s="47"/>
-      <c r="BR183" s="2"/>
-      <c r="BT183" s="4"/>
-      <c r="BU183" s="47"/>
-      <c r="BV183" s="2"/>
-      <c r="BY183" s="4"/>
-      <c r="BZ183" s="47"/>
-      <c r="CA183" s="2"/>
-      <c r="CD183" s="4"/>
-      <c r="CE183" s="47"/>
-      <c r="CF183" s="2"/>
-      <c r="CI183" s="4"/>
-      <c r="CJ183" s="47"/>
-      <c r="CK183" s="2"/>
-      <c r="CM183" s="4"/>
-      <c r="CN183" s="47"/>
-      <c r="CO183" s="2"/>
+      <c r="BF183" s="50"/>
+      <c r="BT183" s="47"/>
     </row>
     <row r="184" spans="39:93" x14ac:dyDescent="0.2">
-      <c r="AM184" s="4"/>
-      <c r="AN184" s="7"/>
-      <c r="AO184" s="7"/>
-      <c r="AP184" s="7"/>
-      <c r="AQ184" s="7"/>
-      <c r="AR184" s="6"/>
-      <c r="AS184" s="6"/>
-      <c r="AT184" s="6"/>
-      <c r="AU184" s="6"/>
       <c r="AW184" s="7"/>
-      <c r="AY184" s="7"/>
-      <c r="AZ184" s="50"/>
-      <c r="BA184" s="26"/>
-      <c r="BB184" s="50"/>
-      <c r="BC184" s="48"/>
-      <c r="BD184" s="48"/>
       <c r="BE184" s="50"/>
-      <c r="BF184" s="63"/>
-      <c r="BK184" s="26"/>
-      <c r="BL184" s="47"/>
-      <c r="BM184" s="2"/>
-      <c r="BP184" s="4"/>
-      <c r="BQ184" s="47"/>
-      <c r="BR184" s="2"/>
-      <c r="BT184" s="4"/>
-      <c r="BU184" s="47"/>
-      <c r="BV184" s="2"/>
-      <c r="BY184" s="4"/>
-      <c r="BZ184" s="47"/>
-      <c r="CA184" s="2"/>
-      <c r="CD184" s="4"/>
-      <c r="CE184" s="47"/>
-      <c r="CF184" s="2"/>
-      <c r="CI184" s="4"/>
-      <c r="CJ184" s="47"/>
-      <c r="CK184" s="2"/>
-      <c r="CM184" s="4"/>
-      <c r="CN184" s="47"/>
-      <c r="CO184" s="2"/>
+      <c r="BF184" s="50"/>
     </row>
     <row r="185" spans="39:93" x14ac:dyDescent="0.2">
-      <c r="AM185" s="4"/>
-      <c r="AN185" s="7"/>
-      <c r="AO185" s="7"/>
-      <c r="AP185" s="7"/>
-      <c r="AQ185" s="7"/>
-      <c r="AR185" s="6"/>
-      <c r="AS185" s="6"/>
-      <c r="AT185" s="6"/>
-      <c r="AU185" s="6"/>
-      <c r="AV185" s="4"/>
       <c r="AW185" s="7"/>
-      <c r="AX185" s="4"/>
-      <c r="AY185" s="7"/>
-      <c r="AZ185" s="30"/>
-      <c r="BA185" s="26"/>
-      <c r="BB185" s="30"/>
-      <c r="BC185" s="48"/>
-      <c r="BD185" s="48"/>
-      <c r="BE185" s="30"/>
-      <c r="BF185" s="63"/>
-      <c r="BK185" s="26"/>
-      <c r="BL185" s="47"/>
-      <c r="BM185" s="2"/>
-      <c r="BP185" s="4"/>
-      <c r="BQ185" s="47"/>
-      <c r="BR185" s="2"/>
-      <c r="BT185" s="4"/>
-      <c r="BU185" s="47"/>
-      <c r="BV185" s="2"/>
-      <c r="BY185" s="4"/>
-      <c r="BZ185" s="47"/>
-      <c r="CA185" s="2"/>
-      <c r="CD185" s="4"/>
-      <c r="CE185" s="47"/>
-      <c r="CF185" s="2"/>
-      <c r="CI185" s="4"/>
-      <c r="CJ185" s="47"/>
-      <c r="CK185" s="2"/>
-      <c r="CM185" s="4"/>
-      <c r="CN185" s="47"/>
-      <c r="CO185" s="2"/>
+      <c r="AZ185" s="50"/>
+      <c r="BA185" s="50"/>
+      <c r="BB185" s="50"/>
+      <c r="BC185" s="50"/>
+      <c r="BD185" s="50"/>
+      <c r="BE185" s="50"/>
+      <c r="BF185" s="50"/>
+      <c r="BK185" s="2"/>
+      <c r="BR185" s="64"/>
     </row>
     <row r="186" spans="39:93" x14ac:dyDescent="0.2">
-      <c r="AM186" s="4"/>
-      <c r="AN186" s="4"/>
-      <c r="AO186" s="4"/>
-      <c r="AP186" s="4"/>
-      <c r="AQ186" s="4"/>
-      <c r="AR186" s="7"/>
-      <c r="AS186" s="7"/>
-      <c r="AT186" s="7"/>
-      <c r="AU186" s="7"/>
       <c r="AW186" s="7"/>
-      <c r="AY186" s="7"/>
-      <c r="AZ186" s="50"/>
-      <c r="BA186" s="26"/>
-      <c r="BB186" s="50"/>
-      <c r="BC186" s="48"/>
-      <c r="BD186" s="48"/>
-      <c r="BE186" s="50"/>
-      <c r="BF186" s="63"/>
-      <c r="BK186" s="26"/>
-      <c r="BL186" s="47"/>
+      <c r="BL186" s="56"/>
       <c r="BM186" s="2"/>
-      <c r="BP186" s="4"/>
-      <c r="BQ186" s="47"/>
-      <c r="BR186" s="2"/>
-      <c r="BT186" s="4"/>
-      <c r="BU186" s="47"/>
-      <c r="BV186" s="2"/>
-      <c r="BY186" s="4"/>
-      <c r="BZ186" s="47"/>
-      <c r="CA186" s="2"/>
-      <c r="CD186" s="4"/>
-      <c r="CE186" s="47"/>
-      <c r="CF186" s="2"/>
-      <c r="CI186" s="4"/>
-      <c r="CJ186" s="47"/>
-      <c r="CK186" s="2"/>
-      <c r="CM186" s="4"/>
-      <c r="CN186" s="47"/>
-      <c r="CO186" s="2"/>
     </row>
     <row r="187" spans="39:93" x14ac:dyDescent="0.2">
-      <c r="AM187" s="4"/>
-      <c r="AN187" s="4"/>
-      <c r="AO187" s="4"/>
-      <c r="AP187" s="4"/>
-      <c r="AQ187" s="4"/>
-      <c r="AR187" s="7"/>
-      <c r="AS187" s="7"/>
-      <c r="AT187" s="7"/>
-      <c r="AU187" s="7"/>
-      <c r="AW187" s="7"/>
-      <c r="AY187" s="7"/>
-      <c r="AZ187" s="50"/>
-      <c r="BA187" s="26"/>
-      <c r="BB187" s="50"/>
-      <c r="BC187" s="48"/>
-      <c r="BD187" s="48"/>
-      <c r="BE187" s="50"/>
-      <c r="BF187" s="63"/>
-      <c r="BK187" s="26"/>
-      <c r="BL187" s="47"/>
+      <c r="BL187" s="56"/>
       <c r="BM187" s="2"/>
-      <c r="BP187" s="4"/>
-      <c r="BQ187" s="47"/>
-      <c r="BR187" s="2"/>
-      <c r="BT187" s="4"/>
-      <c r="BU187" s="47"/>
-      <c r="BV187" s="2"/>
-      <c r="BY187" s="4"/>
-      <c r="BZ187" s="47"/>
-      <c r="CA187" s="2"/>
-      <c r="CD187" s="4"/>
-      <c r="CE187" s="47"/>
-      <c r="CF187" s="2"/>
-      <c r="CI187" s="4"/>
-      <c r="CJ187" s="47"/>
-      <c r="CK187" s="2"/>
-      <c r="CM187" s="4"/>
-      <c r="CN187" s="47"/>
-      <c r="CO187" s="2"/>
-    </row>
-    <row r="188" spans="39:93" x14ac:dyDescent="0.2">
-      <c r="AM188" s="4"/>
-      <c r="AN188" s="4"/>
-      <c r="AO188" s="4"/>
-      <c r="AP188" s="4"/>
-      <c r="AQ188" s="4"/>
-      <c r="AR188" s="7"/>
-      <c r="AS188" s="7"/>
-      <c r="AT188" s="7"/>
-      <c r="AU188" s="7"/>
-      <c r="AW188" s="7"/>
-      <c r="AY188" s="7"/>
-      <c r="AZ188" s="50"/>
-      <c r="BA188" s="26"/>
-      <c r="BB188" s="50"/>
-      <c r="BC188" s="48"/>
-      <c r="BD188" s="48"/>
-      <c r="BE188" s="50"/>
-      <c r="BF188" s="63"/>
-      <c r="BK188" s="26"/>
-      <c r="BL188" s="47"/>
-      <c r="BM188" s="2"/>
-      <c r="BP188" s="4"/>
-      <c r="BQ188" s="47"/>
-      <c r="BR188" s="2"/>
-      <c r="BT188" s="4"/>
-      <c r="BU188" s="47"/>
-      <c r="BV188" s="2"/>
-      <c r="BY188" s="4"/>
-      <c r="BZ188" s="47"/>
-      <c r="CA188" s="2"/>
-      <c r="CD188" s="4"/>
-      <c r="CE188" s="47"/>
-      <c r="CF188" s="2"/>
-      <c r="CI188" s="4"/>
-      <c r="CJ188" s="47"/>
-      <c r="CK188" s="2"/>
-      <c r="CM188" s="4"/>
-      <c r="CN188" s="47"/>
-      <c r="CO188" s="2"/>
-    </row>
-    <row r="189" spans="39:93" x14ac:dyDescent="0.2">
-      <c r="AW189" s="7"/>
-      <c r="AZ189" s="50"/>
-      <c r="BA189" s="50"/>
-      <c r="BB189" s="50"/>
-      <c r="BC189" s="50"/>
-      <c r="BD189" s="50"/>
-      <c r="BE189" s="50"/>
-      <c r="BF189" s="50"/>
-      <c r="BT189" s="47"/>
     </row>
     <row r="190" spans="39:93" x14ac:dyDescent="0.2">
-      <c r="AW190" s="7"/>
-      <c r="BE190" s="50"/>
-      <c r="BF190" s="50"/>
+      <c r="BL190" s="56"/>
+      <c r="BM190" s="2"/>
     </row>
     <row r="191" spans="39:93" x14ac:dyDescent="0.2">
-      <c r="AW191" s="7"/>
-      <c r="AZ191" s="50"/>
-      <c r="BA191" s="50"/>
-      <c r="BB191" s="50"/>
-      <c r="BC191" s="50"/>
-      <c r="BD191" s="50"/>
-      <c r="BE191" s="50"/>
-      <c r="BF191" s="50"/>
-      <c r="BK191" s="2"/>
-      <c r="BR191" s="64"/>
+      <c r="BL191" s="56"/>
+      <c r="BM191" s="2"/>
     </row>
     <row r="192" spans="39:93" x14ac:dyDescent="0.2">
-      <c r="AW192" s="7"/>
       <c r="BL192" s="56"/>
       <c r="BM192" s="2"/>
     </row>
@@ -9599,13 +9704,9 @@
       <c r="BL193" s="56"/>
       <c r="BM193" s="2"/>
     </row>
-    <row r="196" spans="64:65" x14ac:dyDescent="0.2">
-      <c r="BL196" s="56"/>
-      <c r="BM196" s="2"/>
-    </row>
-    <row r="197" spans="64:65" x14ac:dyDescent="0.2">
-      <c r="BL197" s="56"/>
-      <c r="BM197" s="2"/>
+    <row r="195" spans="64:65" x14ac:dyDescent="0.2">
+      <c r="BL195" s="56"/>
+      <c r="BM195" s="2"/>
     </row>
     <row r="198" spans="64:65" x14ac:dyDescent="0.2">
       <c r="BL198" s="56"/>
@@ -9615,17 +9716,17 @@
       <c r="BL199" s="56"/>
       <c r="BM199" s="2"/>
     </row>
+    <row r="200" spans="64:65" x14ac:dyDescent="0.2">
+      <c r="BL200" s="56"/>
+      <c r="BM200" s="2"/>
+    </row>
     <row r="201" spans="64:65" x14ac:dyDescent="0.2">
       <c r="BL201" s="56"/>
       <c r="BM201" s="2"/>
     </row>
-    <row r="204" spans="64:65" x14ac:dyDescent="0.2">
-      <c r="BL204" s="56"/>
-      <c r="BM204" s="2"/>
-    </row>
-    <row r="205" spans="64:65" x14ac:dyDescent="0.2">
-      <c r="BL205" s="56"/>
-      <c r="BM205" s="2"/>
+    <row r="203" spans="64:65" x14ac:dyDescent="0.2">
+      <c r="BL203" s="56"/>
+      <c r="BM203" s="2"/>
     </row>
     <row r="206" spans="64:65" x14ac:dyDescent="0.2">
       <c r="BL206" s="56"/>
@@ -9635,25 +9736,31 @@
       <c r="BL207" s="56"/>
       <c r="BM207" s="2"/>
     </row>
-    <row r="209" spans="64:65" x14ac:dyDescent="0.2">
+    <row r="208" spans="64:65" x14ac:dyDescent="0.2">
+      <c r="BL208" s="56"/>
+      <c r="BM208" s="2"/>
+    </row>
+    <row r="209" spans="58:65" x14ac:dyDescent="0.2">
       <c r="BL209" s="56"/>
       <c r="BM209" s="2"/>
     </row>
-    <row r="212" spans="64:65" x14ac:dyDescent="0.2">
-      <c r="BL212" s="56"/>
-      <c r="BM212" s="2"/>
-    </row>
-    <row r="213" spans="64:65" x14ac:dyDescent="0.2">
-      <c r="BL213" s="56"/>
-      <c r="BM213" s="2"/>
-    </row>
-    <row r="214" spans="64:65" x14ac:dyDescent="0.2">
-      <c r="BL214" s="56"/>
-      <c r="BM214" s="2"/>
-    </row>
-    <row r="215" spans="64:65" x14ac:dyDescent="0.2">
-      <c r="BL215" s="56"/>
-      <c r="BM215" s="2"/>
+    <row r="219" spans="58:65" x14ac:dyDescent="0.2">
+      <c r="BF219" s="50"/>
+    </row>
+    <row r="220" spans="58:65" x14ac:dyDescent="0.2">
+      <c r="BF220" s="50"/>
+    </row>
+    <row r="221" spans="58:65" x14ac:dyDescent="0.2">
+      <c r="BF221" s="50"/>
+    </row>
+    <row r="222" spans="58:65" x14ac:dyDescent="0.2">
+      <c r="BF222" s="50"/>
+    </row>
+    <row r="223" spans="58:65" x14ac:dyDescent="0.2">
+      <c r="BF223" s="50"/>
+    </row>
+    <row r="224" spans="58:65" x14ac:dyDescent="0.2">
+      <c r="BF224" s="50"/>
     </row>
     <row r="225" spans="58:58" x14ac:dyDescent="0.2">
       <c r="BF225" s="50"/>
@@ -9663,24 +9770,6 @@
     </row>
     <row r="227" spans="58:58" x14ac:dyDescent="0.2">
       <c r="BF227" s="50"/>
-    </row>
-    <row r="228" spans="58:58" x14ac:dyDescent="0.2">
-      <c r="BF228" s="50"/>
-    </row>
-    <row r="229" spans="58:58" x14ac:dyDescent="0.2">
-      <c r="BF229" s="50"/>
-    </row>
-    <row r="230" spans="58:58" x14ac:dyDescent="0.2">
-      <c r="BF230" s="50"/>
-    </row>
-    <row r="231" spans="58:58" x14ac:dyDescent="0.2">
-      <c r="BF231" s="50"/>
-    </row>
-    <row r="232" spans="58:58" x14ac:dyDescent="0.2">
-      <c r="BF232" s="50"/>
-    </row>
-    <row r="233" spans="58:58" x14ac:dyDescent="0.2">
-      <c r="BF233" s="50"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="AK43:AV54">
@@ -9688,7 +9777,7 @@
       <formula>ABS(AK43)&lt;0.1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BR172:BR174">
+  <conditionalFormatting sqref="BR166:BR168">
     <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
       <formula>"VIRHE!"</formula>
     </cfRule>

</xml_diff>

<commit_message>
Update theory .xls file
</commit_message>
<xml_diff>
--- a/theory/FEM matriisit.xlsx
+++ b/theory/FEM matriisit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ohjelmointi\2_Rust\idfem\theory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFF4E6F1-CB7A-4BB4-9CD6-1B7B34BB2EE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B462225D-41F4-4EF4-AAFE-70672ECC3602}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-22230" yWindow="0" windowWidth="22335" windowHeight="20880" xr2:uid="{27180542-B0D2-4BFE-946B-7857B24C93C8}"/>
   </bookViews>
@@ -327,6 +327,9 @@
     <t>Positiivinen vastapäivään</t>
   </si>
   <si>
+    <t>Positiivinen venymää</t>
+  </si>
+  <si>
     <t>Siirtymä (pituussuunnassa)</t>
   </si>
   <si>
@@ -376,9 +379,6 @@
   </si>
   <si>
     <t>(Huomaa -1* alussa)</t>
-  </si>
-  <si>
-    <t>Positiivinen venymä</t>
   </si>
 </sst>
 </file>
@@ -1203,16 +1203,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>456437</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>42241</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>481285</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>141633</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>372717</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>14813</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>271864</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>74544</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1235,8 +1235,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6055480" y="340415"/>
-          <a:ext cx="5515324" cy="7526311"/>
+          <a:off x="4208459" y="290720"/>
+          <a:ext cx="1662448" cy="2268607"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1802,8 +1802,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94F9BDF3-3EE6-4BFB-9734-CB047BC6E804}">
   <dimension ref="B1:CW227"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C24" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F73" sqref="F73"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1866,7 +1866,7 @@
         <v>18</v>
       </c>
       <c r="E4" s="35">
-        <v>90</v>
+        <v>120</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>0</v>
@@ -1903,14 +1903,14 @@
       </c>
       <c r="C5" s="25">
         <f>COS(RADIANS(E4))</f>
-        <v>6.1257422745431001E-17</v>
+        <v>-0.49999999999999978</v>
       </c>
       <c r="D5" s="34" t="s">
         <v>22</v>
       </c>
       <c r="E5" s="5">
         <f>SIN(RADIANS(E4))</f>
-        <v>1</v>
+        <v>0.86602540378443871</v>
       </c>
       <c r="L5" s="34" t="s">
         <v>21</v>
@@ -2057,27 +2057,27 @@
       </c>
       <c r="AK6" s="11">
         <f t="shared" ref="AK6:AP11" si="0">B20</f>
-        <v>328.125</v>
+        <v>131496.09374999988</v>
       </c>
       <c r="AL6" s="11">
         <f t="shared" si="0"/>
-        <v>3.2140046849512931E-11</v>
+        <v>-227189.58620060666</v>
       </c>
       <c r="AM6" s="11">
         <f t="shared" si="0"/>
-        <v>-656250</v>
+        <v>-568329.17123353796</v>
       </c>
       <c r="AN6" s="11">
         <f t="shared" si="0"/>
-        <v>-328.125</v>
+        <v>-131496.09374999988</v>
       </c>
       <c r="AO6" s="11">
         <f t="shared" si="0"/>
-        <v>-3.2140046849512931E-11</v>
+        <v>227189.58620060666</v>
       </c>
       <c r="AP6" s="11">
         <f t="shared" si="0"/>
-        <v>-656250</v>
+        <v>-568329.17123353796</v>
       </c>
       <c r="AQ6" s="4">
         <v>0</v>
@@ -2100,7 +2100,7 @@
       <c r="AW6" s="4"/>
       <c r="AX6" s="3">
         <f>I20</f>
-        <v>-20000</v>
+        <v>-18105.508075688773</v>
       </c>
       <c r="AZ6" s="81">
         <v>1</v>
@@ -2180,27 +2180,27 @@
       </c>
       <c r="AK7" s="11">
         <f t="shared" si="0"/>
-        <v>3.2140046849512931E-11</v>
+        <v>-227189.58620060669</v>
       </c>
       <c r="AL7" s="11">
         <f t="shared" si="0"/>
-        <v>525000</v>
+        <v>393832.03125000006</v>
       </c>
       <c r="AM7" s="11">
         <f t="shared" si="0"/>
-        <v>4.0200183676689094E-11</v>
+        <v>-328124.99999999983</v>
       </c>
       <c r="AN7" s="11">
         <f t="shared" si="0"/>
-        <v>-3.2140046849512931E-11</v>
+        <v>227189.58620060669</v>
       </c>
       <c r="AO7" s="11">
         <f t="shared" si="0"/>
-        <v>-525000</v>
+        <v>-393832.03125000006</v>
       </c>
       <c r="AP7" s="11">
         <f t="shared" si="0"/>
-        <v>4.0200183676689094E-11</v>
+        <v>-328124.99999999983</v>
       </c>
       <c r="AQ7" s="4">
         <v>0</v>
@@ -2223,7 +2223,7 @@
       <c r="AW7" s="4"/>
       <c r="AX7" s="3">
         <f t="shared" ref="AX7:AX11" si="1">I21</f>
-        <v>1570.0000000000011</v>
+        <v>-8640.3401160584272</v>
       </c>
       <c r="AZ7" s="81">
         <v>2</v>
@@ -2303,11 +2303,11 @@
       </c>
       <c r="AK8" s="11">
         <f t="shared" si="0"/>
-        <v>-656250</v>
+        <v>-568329.17123353796</v>
       </c>
       <c r="AL8" s="11">
         <f t="shared" si="0"/>
-        <v>4.0200183676689094E-11</v>
+        <v>-328124.99999999983</v>
       </c>
       <c r="AM8" s="11">
         <f t="shared" si="0"/>
@@ -2315,11 +2315,11 @@
       </c>
       <c r="AN8" s="11">
         <f t="shared" si="0"/>
-        <v>656250</v>
+        <v>568329.17123353796</v>
       </c>
       <c r="AO8" s="11">
         <f t="shared" si="0"/>
-        <v>-4.0200183676689094E-11</v>
+        <v>328124.99999999983</v>
       </c>
       <c r="AP8" s="11">
         <f t="shared" si="0"/>
@@ -2426,27 +2426,27 @@
       </c>
       <c r="AK9" s="11">
         <f t="shared" si="0"/>
-        <v>-328.125</v>
+        <v>-131496.09374999988</v>
       </c>
       <c r="AL9" s="11">
         <f t="shared" si="0"/>
-        <v>-3.2140046849512931E-11</v>
+        <v>227189.58620060666</v>
       </c>
       <c r="AM9" s="11">
         <f t="shared" si="0"/>
-        <v>656250</v>
+        <v>568329.17123353796</v>
       </c>
       <c r="AN9" s="11">
         <f t="shared" si="0"/>
-        <v>328.125</v>
+        <v>131496.09374999988</v>
       </c>
       <c r="AO9" s="11">
         <f t="shared" si="0"/>
-        <v>3.2140046849512931E-11</v>
+        <v>-227189.58620060666</v>
       </c>
       <c r="AP9" s="11">
         <f t="shared" si="0"/>
-        <v>656250</v>
+        <v>568329.17123353796</v>
       </c>
       <c r="AQ9" s="4">
         <v>0</v>
@@ -2469,7 +2469,7 @@
       <c r="AW9" s="4"/>
       <c r="AX9" s="3">
         <f t="shared" si="1"/>
-        <v>-20000</v>
+        <v>-18105.508075688773</v>
       </c>
       <c r="AZ9" s="81">
         <v>4</v>
@@ -2559,27 +2559,27 @@
       </c>
       <c r="AK10" s="11">
         <f t="shared" si="0"/>
-        <v>-3.2140046849512931E-11</v>
+        <v>227189.58620060669</v>
       </c>
       <c r="AL10" s="11">
         <f t="shared" si="0"/>
-        <v>-525000</v>
+        <v>-393832.03125000006</v>
       </c>
       <c r="AM10" s="11">
         <f t="shared" si="0"/>
-        <v>-4.0200183676689094E-11</v>
+        <v>328124.99999999983</v>
       </c>
       <c r="AN10" s="11">
         <f t="shared" si="0"/>
-        <v>3.2140046849512931E-11</v>
+        <v>-227189.58620060669</v>
       </c>
       <c r="AO10" s="11">
         <f t="shared" si="0"/>
-        <v>525000</v>
+        <v>393832.03125000006</v>
       </c>
       <c r="AP10" s="11">
         <f t="shared" si="0"/>
-        <v>-4.0200183676689094E-11</v>
+        <v>328124.99999999983</v>
       </c>
       <c r="AQ10" s="4">
         <v>0</v>
@@ -2602,7 +2602,7 @@
       <c r="AW10" s="4"/>
       <c r="AX10" s="3">
         <f>I24</f>
-        <v>1570.0000000000011</v>
+        <v>-8640.3401160584272</v>
       </c>
       <c r="AZ10" s="81">
         <v>5</v>
@@ -2691,11 +2691,11 @@
       </c>
       <c r="AK11" s="11">
         <f t="shared" si="0"/>
-        <v>-656250</v>
+        <v>-568329.17123353796</v>
       </c>
       <c r="AL11" s="11">
         <f t="shared" si="0"/>
-        <v>4.0200183676689094E-11</v>
+        <v>-328124.99999999983</v>
       </c>
       <c r="AM11" s="11">
         <f t="shared" si="0"/>
@@ -2703,11 +2703,11 @@
       </c>
       <c r="AN11" s="11">
         <f t="shared" si="0"/>
-        <v>656250</v>
+        <v>568329.17123353796</v>
       </c>
       <c r="AO11" s="11">
         <f t="shared" si="0"/>
-        <v>-4.0200183676689094E-11</v>
+        <v>328124.99999999983</v>
       </c>
       <c r="AP11" s="11">
         <f t="shared" si="0"/>
@@ -3490,31 +3490,31 @@
     <row r="20" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B20" s="37">
         <f t="shared" ref="B20:G21" si="6">$B36*B$45+$C36*B$46+$D36*B$47+$E36*B$48+$F36*B$49+$G36*B$50</f>
-        <v>328.125</v>
+        <v>131496.09374999988</v>
       </c>
       <c r="C20" s="37">
         <f t="shared" si="6"/>
-        <v>3.2140046849512931E-11</v>
+        <v>-227189.58620060666</v>
       </c>
       <c r="D20" s="37">
         <f t="shared" si="6"/>
-        <v>-656250</v>
+        <v>-568329.17123353796</v>
       </c>
       <c r="E20" s="37">
         <f t="shared" si="6"/>
-        <v>-328.125</v>
+        <v>-131496.09374999988</v>
       </c>
       <c r="F20" s="37">
         <f t="shared" si="6"/>
-        <v>-3.2140046849512931E-11</v>
+        <v>227189.58620060666</v>
       </c>
       <c r="G20" s="37">
         <f t="shared" si="6"/>
-        <v>-656250</v>
+        <v>-568329.17123353796</v>
       </c>
       <c r="I20" s="40">
         <f>B54*I28+C54*I29+D54*I30+E54*I31+F54*I32+G54*I33</f>
-        <v>-20000</v>
+        <v>-18105.508075688773</v>
       </c>
       <c r="L20" s="19">
         <f t="shared" ref="L20:Q25" si="7">$L37*L$46+$M37*L$47+$N37*L$48+$O37*L$49+$P37*L$50+$Q37*L$51</f>
@@ -3546,31 +3546,31 @@
       </c>
       <c r="V20" s="20">
         <f t="shared" ref="V20:AA21" si="8">$V37*B$45+$W37*B$46+$X37*B$47+$Y37*B$48+$Z37*B$49+$AA37*B$50</f>
-        <v>328.125</v>
+        <v>131496.09374999988</v>
       </c>
       <c r="W20" s="20">
         <f t="shared" si="8"/>
-        <v>3.2140046849512931E-11</v>
+        <v>-227189.58620060666</v>
       </c>
       <c r="X20" s="20">
         <f t="shared" si="8"/>
-        <v>-656250</v>
+        <v>-568329.17123353796</v>
       </c>
       <c r="Y20" s="20">
         <f t="shared" si="8"/>
-        <v>-328.125</v>
+        <v>-131496.09374999988</v>
       </c>
       <c r="Z20" s="20">
         <f t="shared" si="8"/>
-        <v>-3.2140046849512931E-11</v>
+        <v>227189.58620060666</v>
       </c>
       <c r="AA20" s="20">
         <f t="shared" si="8"/>
-        <v>-656250</v>
+        <v>-568329.17123353796</v>
       </c>
       <c r="AC20" s="40">
         <f>V55*AC28+W55*AC29+X55*AC30+Y55*AC31+Z55*AC32+AA55*AC33</f>
-        <v>20000</v>
+        <v>16535.508075688773</v>
       </c>
       <c r="AJ20" s="2" t="s">
         <v>40</v>
@@ -3579,31 +3579,31 @@
     <row r="21" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B21" s="37">
         <f t="shared" si="6"/>
-        <v>3.2140046849512931E-11</v>
+        <v>-227189.58620060669</v>
       </c>
       <c r="C21" s="37">
         <f t="shared" si="6"/>
-        <v>525000</v>
+        <v>393832.03125000006</v>
       </c>
       <c r="D21" s="37">
         <f t="shared" si="6"/>
-        <v>4.0200183676689094E-11</v>
+        <v>-328124.99999999983</v>
       </c>
       <c r="E21" s="37">
         <f t="shared" si="6"/>
-        <v>-3.2140046849512931E-11</v>
+        <v>227189.58620060669</v>
       </c>
       <c r="F21" s="37">
         <f t="shared" si="6"/>
-        <v>-525000</v>
+        <v>-393832.03125000006</v>
       </c>
       <c r="G21" s="37">
         <f t="shared" si="6"/>
-        <v>4.0200183676689094E-11</v>
+        <v>-328124.99999999983</v>
       </c>
       <c r="I21" s="40">
         <f>B55*I28+C55*I29+D55*I30+E55*I31+F55*I32+G55*I33</f>
-        <v>1570.0000000000011</v>
+        <v>-8640.3401160584272</v>
       </c>
       <c r="L21" s="19">
         <f t="shared" si="7"/>
@@ -3635,31 +3635,31 @@
       </c>
       <c r="V21" s="20">
         <f t="shared" si="8"/>
-        <v>3.2140046849512931E-11</v>
+        <v>-227189.58620060669</v>
       </c>
       <c r="W21" s="20">
         <f t="shared" si="8"/>
-        <v>525000</v>
+        <v>393832.03125000006</v>
       </c>
       <c r="X21" s="20">
         <f t="shared" si="8"/>
-        <v>4.0200183676689094E-11</v>
+        <v>-328124.99999999983</v>
       </c>
       <c r="Y21" s="20">
         <f t="shared" si="8"/>
-        <v>-3.2140046849512931E-11</v>
+        <v>227189.58620060669</v>
       </c>
       <c r="Z21" s="20">
         <f t="shared" si="8"/>
-        <v>-525000</v>
+        <v>-393832.03125000006</v>
       </c>
       <c r="AA21" s="20">
         <f t="shared" si="8"/>
-        <v>4.0200183676689094E-11</v>
+        <v>-328124.99999999983</v>
       </c>
       <c r="AC21" s="40">
         <f>V56*AC28+W56*AC29+X56*AC30+Y56*AC31+Z56*AC32+AA56*AC33</f>
-        <v>1569.9999999999989</v>
+        <v>11359.659883941566</v>
       </c>
       <c r="AJ21" s="9"/>
       <c r="AK21" s="81">
@@ -3706,11 +3706,11 @@
     <row r="22" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B22" s="37">
         <f t="shared" ref="B22:F25" si="9">$B38*B$45+$C38*B$46+$D38*B$47+$E38*B$48+$F38*B$49+$G38*B$50</f>
-        <v>-656250</v>
+        <v>-568329.17123353796</v>
       </c>
       <c r="C22" s="37">
         <f t="shared" si="9"/>
-        <v>4.0200183676689094E-11</v>
+        <v>-328124.99999999983</v>
       </c>
       <c r="D22" s="37">
         <f t="shared" si="9"/>
@@ -3718,11 +3718,11 @@
       </c>
       <c r="E22" s="37">
         <f t="shared" si="9"/>
-        <v>656250</v>
+        <v>568329.17123353796</v>
       </c>
       <c r="F22" s="37">
         <f t="shared" si="9"/>
-        <v>-4.0200183676689094E-11</v>
+        <v>328124.99999999983</v>
       </c>
       <c r="G22" s="37">
         <f>-1*$B38*G$45+$C38*G$46+$D38*G$47+$E38*G$48+$F38*G$49+$G38*G$50</f>
@@ -3762,11 +3762,11 @@
       </c>
       <c r="V22" s="20">
         <f t="shared" ref="V22:Z25" si="10">$V39*B$45+$W39*B$46+$X39*B$47+$Y39*B$48+$Z39*B$49+$AA39*B$50</f>
-        <v>-656250</v>
+        <v>-568329.17123353796</v>
       </c>
       <c r="W22" s="20">
         <f t="shared" si="10"/>
-        <v>4.0200183676689094E-11</v>
+        <v>-328124.99999999983</v>
       </c>
       <c r="X22" s="20">
         <f t="shared" si="10"/>
@@ -3774,11 +3774,11 @@
       </c>
       <c r="Y22" s="20">
         <f t="shared" si="10"/>
-        <v>656250</v>
+        <v>568329.17123353796</v>
       </c>
       <c r="Z22" s="20">
         <f t="shared" si="10"/>
-        <v>-4.0200183676689094E-11</v>
+        <v>328124.99999999983</v>
       </c>
       <c r="AA22" s="20">
         <f>-1*$V39*G$45+$W39*G$46+$X39*G$47+$Y39*G$48+$Z39*G$49+$AA39*G$50</f>
@@ -3832,31 +3832,31 @@
     <row r="23" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B23" s="37">
         <f t="shared" si="9"/>
-        <v>-328.125</v>
+        <v>-131496.09374999988</v>
       </c>
       <c r="C23" s="37">
         <f t="shared" si="9"/>
-        <v>-3.2140046849512931E-11</v>
+        <v>227189.58620060666</v>
       </c>
       <c r="D23" s="37">
         <f t="shared" si="9"/>
-        <v>656250</v>
+        <v>568329.17123353796</v>
       </c>
       <c r="E23" s="37">
         <f t="shared" si="9"/>
-        <v>328.125</v>
+        <v>131496.09374999988</v>
       </c>
       <c r="F23" s="37">
         <f t="shared" si="9"/>
-        <v>3.2140046849512931E-11</v>
+        <v>-227189.58620060666</v>
       </c>
       <c r="G23" s="37">
         <f>$B39*G$45+$C39*G$46+$D39*G$47+$E39*G$48+$F39*G$49+$G39*G$50</f>
-        <v>656250</v>
+        <v>568329.17123353796</v>
       </c>
       <c r="I23" s="40">
         <f>B57*I28+C57*I29+D57*I30+E57*I31+F57*I32+G57*I33</f>
-        <v>-20000</v>
+        <v>-18105.508075688773</v>
       </c>
       <c r="L23" s="19">
         <f t="shared" si="7"/>
@@ -3888,31 +3888,31 @@
       </c>
       <c r="V23" s="20">
         <f t="shared" si="10"/>
-        <v>-328.125</v>
+        <v>-131496.09374999988</v>
       </c>
       <c r="W23" s="20">
         <f t="shared" si="10"/>
-        <v>-3.2140046849512931E-11</v>
+        <v>227189.58620060666</v>
       </c>
       <c r="X23" s="20">
         <f t="shared" si="10"/>
-        <v>656250</v>
+        <v>568329.17123353796</v>
       </c>
       <c r="Y23" s="20">
         <f t="shared" si="10"/>
-        <v>328.125</v>
+        <v>131496.09374999988</v>
       </c>
       <c r="Z23" s="20">
         <f t="shared" si="10"/>
-        <v>3.2140046849512931E-11</v>
+        <v>-227189.58620060666</v>
       </c>
       <c r="AA23" s="20">
         <f>$V40*G$45+$W40*G$46+$X40*G$47+$Y40*G$48+$Z40*G$49+$AA40*G$50</f>
-        <v>656250</v>
+        <v>568329.17123353796</v>
       </c>
       <c r="AC23" s="40">
         <f>V58*AC28+W58*AC29+X58*AC30+Y58*AC31+Z58*AC32+AA58*AC33</f>
-        <v>20000</v>
+        <v>16535.508075688773</v>
       </c>
       <c r="AJ23" s="81">
         <v>2</v>
@@ -3958,31 +3958,31 @@
     <row r="24" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B24" s="37">
         <f t="shared" si="9"/>
-        <v>-3.2140046849512931E-11</v>
+        <v>227189.58620060669</v>
       </c>
       <c r="C24" s="37">
         <f t="shared" si="9"/>
-        <v>-525000</v>
+        <v>-393832.03125000006</v>
       </c>
       <c r="D24" s="37">
         <f t="shared" si="9"/>
-        <v>-4.0200183676689094E-11</v>
+        <v>328124.99999999983</v>
       </c>
       <c r="E24" s="37">
         <f t="shared" si="9"/>
-        <v>3.2140046849512931E-11</v>
+        <v>-227189.58620060669</v>
       </c>
       <c r="F24" s="37">
         <f t="shared" si="9"/>
-        <v>525000</v>
+        <v>393832.03125000006</v>
       </c>
       <c r="G24" s="37">
         <f>$B40*G$45+$C40*G$46+$D40*G$47+$E40*G$48+$F40*G$49+$G40*G$50</f>
-        <v>-4.0200183676689094E-11</v>
+        <v>328124.99999999983</v>
       </c>
       <c r="I24" s="40">
         <f>B58*I28+C58*I29+D58*I30+E58*I31+F58*I32+G58*I33</f>
-        <v>1570.0000000000011</v>
+        <v>-8640.3401160584272</v>
       </c>
       <c r="L24" s="19">
         <f t="shared" si="7"/>
@@ -4014,31 +4014,31 @@
       </c>
       <c r="V24" s="20">
         <f t="shared" si="10"/>
-        <v>-3.2140046849512931E-11</v>
+        <v>227189.58620060669</v>
       </c>
       <c r="W24" s="20">
         <f t="shared" si="10"/>
-        <v>-525000</v>
+        <v>-393832.03125000006</v>
       </c>
       <c r="X24" s="20">
         <f t="shared" si="10"/>
-        <v>-4.0200183676689094E-11</v>
+        <v>328124.99999999983</v>
       </c>
       <c r="Y24" s="20">
         <f t="shared" si="10"/>
-        <v>3.2140046849512931E-11</v>
+        <v>-227189.58620060669</v>
       </c>
       <c r="Z24" s="20">
         <f t="shared" si="10"/>
-        <v>525000</v>
+        <v>393832.03125000006</v>
       </c>
       <c r="AA24" s="20">
         <f>$V41*G$45+$W41*G$46+$X41*G$47+$Y41*G$48+$Z41*G$49+$AA41*G$50</f>
-        <v>-4.0200183676689094E-11</v>
+        <v>328124.99999999983</v>
       </c>
       <c r="AC24" s="40">
         <f>V59*AC28+W59*AC29+X59*AC30+Y59*AC31+Z59*AC32+AA59*AC33</f>
-        <v>1569.9999999999989</v>
+        <v>11359.659883941566</v>
       </c>
       <c r="AJ24" s="81">
         <v>3</v>
@@ -4084,11 +4084,11 @@
     <row r="25" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B25" s="37">
         <f t="shared" si="9"/>
-        <v>-656250</v>
+        <v>-568329.17123353796</v>
       </c>
       <c r="C25" s="37">
         <f t="shared" si="9"/>
-        <v>4.0200183676689094E-11</v>
+        <v>-328124.99999999983</v>
       </c>
       <c r="D25" s="37">
         <f t="shared" si="9"/>
@@ -4096,11 +4096,11 @@
       </c>
       <c r="E25" s="37">
         <f t="shared" si="9"/>
-        <v>656250</v>
+        <v>568329.17123353796</v>
       </c>
       <c r="F25" s="37">
         <f t="shared" si="9"/>
-        <v>-4.0200183676689094E-11</v>
+        <v>328124.99999999983</v>
       </c>
       <c r="G25" s="37">
         <f>$B41*G$45+$C41*G$46+$D41*G$47+$E41*G$48+$F41*G$49+$G41*G$50</f>
@@ -4142,11 +4142,11 @@
       <c r="U25" s="2"/>
       <c r="V25" s="20">
         <f t="shared" si="10"/>
-        <v>-656250</v>
+        <v>-568329.17123353796</v>
       </c>
       <c r="W25" s="20">
         <f t="shared" si="10"/>
-        <v>4.0200183676689094E-11</v>
+        <v>-328124.99999999983</v>
       </c>
       <c r="X25" s="20">
         <f t="shared" si="10"/>
@@ -4154,11 +4154,11 @@
       </c>
       <c r="Y25" s="20">
         <f t="shared" si="10"/>
-        <v>656250</v>
+        <v>568329.17123353796</v>
       </c>
       <c r="Z25" s="20">
         <f t="shared" si="10"/>
-        <v>-4.0200183676689094E-11</v>
+        <v>328124.99999999983</v>
       </c>
       <c r="AA25" s="20">
         <f>$V42*G$45+$W42*G$46+$X42*G$47+$Y42*G$48+$Z42*G$49+$AA42*G$50</f>
@@ -4414,32 +4414,32 @@
       </c>
       <c r="AQ28" s="17">
         <f t="shared" ref="AQ28:AV33" si="11">V20</f>
-        <v>328.125</v>
+        <v>131496.09374999988</v>
       </c>
       <c r="AR28" s="17">
         <f t="shared" si="11"/>
-        <v>3.2140046849512931E-11</v>
+        <v>-227189.58620060666</v>
       </c>
       <c r="AS28" s="17">
         <f t="shared" si="11"/>
-        <v>-656250</v>
+        <v>-568329.17123353796</v>
       </c>
       <c r="AT28" s="17">
         <f t="shared" si="11"/>
-        <v>-328.125</v>
+        <v>-131496.09374999988</v>
       </c>
       <c r="AU28" s="17">
         <f t="shared" si="11"/>
-        <v>-3.2140046849512931E-11</v>
+        <v>227189.58620060666</v>
       </c>
       <c r="AV28" s="17">
         <f t="shared" si="11"/>
-        <v>-656250</v>
+        <v>-568329.17123353796</v>
       </c>
       <c r="AW28" s="4"/>
       <c r="AX28" s="3">
         <f>AC20</f>
-        <v>20000</v>
+        <v>16535.508075688773</v>
       </c>
       <c r="AY28" s="8"/>
     </row>
@@ -4545,32 +4545,32 @@
       </c>
       <c r="AQ29" s="17">
         <f t="shared" si="11"/>
-        <v>3.2140046849512931E-11</v>
+        <v>-227189.58620060669</v>
       </c>
       <c r="AR29" s="17">
         <f t="shared" si="11"/>
-        <v>525000</v>
+        <v>393832.03125000006</v>
       </c>
       <c r="AS29" s="17">
         <f t="shared" si="11"/>
-        <v>4.0200183676689094E-11</v>
+        <v>-328124.99999999983</v>
       </c>
       <c r="AT29" s="17">
         <f t="shared" si="11"/>
-        <v>-3.2140046849512931E-11</v>
+        <v>227189.58620060669</v>
       </c>
       <c r="AU29" s="17">
         <f t="shared" si="11"/>
-        <v>-525000</v>
+        <v>-393832.03125000006</v>
       </c>
       <c r="AV29" s="17">
         <f t="shared" si="11"/>
-        <v>4.0200183676689094E-11</v>
+        <v>-328124.99999999983</v>
       </c>
       <c r="AW29" s="4"/>
       <c r="AX29" s="3">
         <f t="shared" ref="AX29:AX33" si="12">AC21</f>
-        <v>1569.9999999999989</v>
+        <v>11359.659883941566</v>
       </c>
       <c r="AY29" s="10"/>
     </row>
@@ -4676,11 +4676,11 @@
       </c>
       <c r="AQ30" s="17">
         <f t="shared" si="11"/>
-        <v>-656250</v>
+        <v>-568329.17123353796</v>
       </c>
       <c r="AR30" s="17">
         <f t="shared" si="11"/>
-        <v>4.0200183676689094E-11</v>
+        <v>-328124.99999999983</v>
       </c>
       <c r="AS30" s="17">
         <f t="shared" si="11"/>
@@ -4688,11 +4688,11 @@
       </c>
       <c r="AT30" s="17">
         <f t="shared" si="11"/>
-        <v>656250</v>
+        <v>568329.17123353796</v>
       </c>
       <c r="AU30" s="17">
         <f t="shared" si="11"/>
-        <v>-4.0200183676689094E-11</v>
+        <v>328124.99999999983</v>
       </c>
       <c r="AV30" s="17">
         <f t="shared" si="11"/>
@@ -4800,32 +4800,32 @@
       </c>
       <c r="AQ31" s="17">
         <f t="shared" si="11"/>
-        <v>-328.125</v>
+        <v>-131496.09374999988</v>
       </c>
       <c r="AR31" s="17">
         <f t="shared" si="11"/>
-        <v>-3.2140046849512931E-11</v>
+        <v>227189.58620060666</v>
       </c>
       <c r="AS31" s="17">
         <f t="shared" si="11"/>
-        <v>656250</v>
+        <v>568329.17123353796</v>
       </c>
       <c r="AT31" s="17">
         <f t="shared" si="11"/>
-        <v>328.125</v>
+        <v>131496.09374999988</v>
       </c>
       <c r="AU31" s="17">
         <f t="shared" si="11"/>
-        <v>3.2140046849512931E-11</v>
+        <v>-227189.58620060666</v>
       </c>
       <c r="AV31" s="17">
         <f t="shared" si="11"/>
-        <v>656250</v>
+        <v>568329.17123353796</v>
       </c>
       <c r="AW31" s="4"/>
       <c r="AX31" s="3">
         <f t="shared" si="12"/>
-        <v>20000</v>
+        <v>16535.508075688773</v>
       </c>
       <c r="AY31" s="8"/>
     </row>
@@ -4932,32 +4932,32 @@
       </c>
       <c r="AQ32" s="17">
         <f t="shared" si="11"/>
-        <v>-3.2140046849512931E-11</v>
+        <v>227189.58620060669</v>
       </c>
       <c r="AR32" s="17">
         <f t="shared" si="11"/>
-        <v>-525000</v>
+        <v>-393832.03125000006</v>
       </c>
       <c r="AS32" s="17">
         <f t="shared" si="11"/>
-        <v>-4.0200183676689094E-11</v>
+        <v>328124.99999999983</v>
       </c>
       <c r="AT32" s="17">
         <f t="shared" si="11"/>
-        <v>3.2140046849512931E-11</v>
+        <v>-227189.58620060669</v>
       </c>
       <c r="AU32" s="17">
         <f t="shared" si="11"/>
-        <v>525000</v>
+        <v>393832.03125000006</v>
       </c>
       <c r="AV32" s="17">
         <f t="shared" si="11"/>
-        <v>-4.0200183676689094E-11</v>
+        <v>328124.99999999983</v>
       </c>
       <c r="AW32" s="4"/>
       <c r="AX32" s="3">
         <f t="shared" si="12"/>
-        <v>1569.9999999999989</v>
+        <v>11359.659883941566</v>
       </c>
       <c r="AY32" s="10"/>
     </row>
@@ -5063,11 +5063,11 @@
       </c>
       <c r="AQ33" s="17">
         <f t="shared" si="11"/>
-        <v>-656250</v>
+        <v>-568329.17123353796</v>
       </c>
       <c r="AR33" s="17">
         <f t="shared" si="11"/>
-        <v>4.0200183676689094E-11</v>
+        <v>-328124.99999999983</v>
       </c>
       <c r="AS33" s="17">
         <f t="shared" si="11"/>
@@ -5075,11 +5075,11 @@
       </c>
       <c r="AT33" s="17">
         <f t="shared" si="11"/>
-        <v>656250</v>
+        <v>568329.17123353796</v>
       </c>
       <c r="AU33" s="17">
         <f t="shared" si="11"/>
-        <v>-4.0200183676689094E-11</v>
+        <v>328124.99999999983</v>
       </c>
       <c r="AV33" s="17">
         <f t="shared" si="11"/>
@@ -5128,27 +5128,27 @@
     <row r="36" spans="2:83" x14ac:dyDescent="0.2">
       <c r="B36" s="38">
         <f t="shared" ref="B36:G36" si="13">$B54*B28+$C54*B29+$D54*B30+$E54*B31+$F54*B32+$G54*B33</f>
-        <v>3.2160146941351275E-11</v>
+        <v>-262499.99999999988</v>
       </c>
       <c r="C36" s="38">
         <f t="shared" si="13"/>
-        <v>-328.125</v>
+        <v>-284.16458561676893</v>
       </c>
       <c r="D36" s="38">
         <f t="shared" si="13"/>
-        <v>-656250</v>
+        <v>-568329.17123353796</v>
       </c>
       <c r="E36" s="38">
         <f t="shared" si="13"/>
-        <v>-3.2160146941351275E-11</v>
+        <v>262499.99999999988</v>
       </c>
       <c r="F36" s="38">
         <f t="shared" si="13"/>
-        <v>328.125</v>
+        <v>284.16458561676893</v>
       </c>
       <c r="G36" s="38">
         <f t="shared" si="13"/>
-        <v>-656250</v>
+        <v>-568329.17123353796</v>
       </c>
       <c r="L36" s="2" t="s">
         <v>30</v>
@@ -5160,27 +5160,27 @@
     <row r="37" spans="2:83" x14ac:dyDescent="0.2">
       <c r="B37" s="38">
         <f t="shared" ref="B37:G37" si="14">$B55*B28+$C55*B29+$D55*B30+$E55*B31+$F55*B32+$G55*B33</f>
-        <v>525000</v>
+        <v>454663.33698683034</v>
       </c>
       <c r="C37" s="38">
         <f t="shared" si="14"/>
-        <v>2.0100091838344547E-14</v>
+        <v>-164.06249999999991</v>
       </c>
       <c r="D37" s="38">
         <f t="shared" si="14"/>
-        <v>4.0200183676689094E-11</v>
+        <v>-328124.99999999983</v>
       </c>
       <c r="E37" s="38">
         <f t="shared" si="14"/>
-        <v>-525000</v>
+        <v>-454663.33698683034</v>
       </c>
       <c r="F37" s="38">
         <f t="shared" si="14"/>
-        <v>-2.0100091838344547E-14</v>
+        <v>164.06249999999991</v>
       </c>
       <c r="G37" s="38">
         <f t="shared" si="14"/>
-        <v>4.0200183676689094E-11</v>
+        <v>-328124.99999999983</v>
       </c>
       <c r="L37" s="38">
         <f t="shared" ref="L37:Q42" si="15">$L55*L$28+$M55*L$29+$N55*L$30+$O55*L$31+$P55*L$32+$Q55*L$33</f>
@@ -5208,27 +5208,27 @@
       </c>
       <c r="V37" s="38">
         <f t="shared" ref="V37:AA37" si="16">$V55*V28+$W55*V29+$X55*V30+$Y55*V31+$Z55*V32+$AA55*V33</f>
-        <v>3.2160146941351275E-11</v>
+        <v>-262499.99999999988</v>
       </c>
       <c r="W37" s="38">
         <f t="shared" si="16"/>
-        <v>-328.125</v>
+        <v>-284.16458561676893</v>
       </c>
       <c r="X37" s="38">
         <f t="shared" si="16"/>
-        <v>-656250</v>
+        <v>-568329.17123353796</v>
       </c>
       <c r="Y37" s="38">
         <f t="shared" si="16"/>
-        <v>-3.2160146941351275E-11</v>
+        <v>262499.99999999988</v>
       </c>
       <c r="Z37" s="38">
         <f t="shared" si="16"/>
-        <v>328.125</v>
+        <v>284.16458561676893</v>
       </c>
       <c r="AA37" s="38">
         <f t="shared" si="16"/>
-        <v>-656250</v>
+        <v>-568329.17123353796</v>
       </c>
     </row>
     <row r="38" spans="2:83" x14ac:dyDescent="0.2">
@@ -5282,53 +5282,53 @@
       </c>
       <c r="V38" s="38">
         <f t="shared" ref="V38:AA38" si="18">$V56*V28+$W56*V29+$X56*V30+$Y56*V31+$Z56*V32+$AA56*V33</f>
-        <v>525000</v>
+        <v>454663.33698683034</v>
       </c>
       <c r="W38" s="38">
         <f t="shared" si="18"/>
-        <v>2.0100091838344547E-14</v>
+        <v>-164.06249999999991</v>
       </c>
       <c r="X38" s="38">
         <f t="shared" si="18"/>
-        <v>4.0200183676689094E-11</v>
+        <v>-328124.99999999983</v>
       </c>
       <c r="Y38" s="38">
         <f t="shared" si="18"/>
-        <v>-525000</v>
+        <v>-454663.33698683034</v>
       </c>
       <c r="Z38" s="38">
         <f t="shared" si="18"/>
-        <v>-2.0100091838344547E-14</v>
+        <v>164.06249999999991</v>
       </c>
       <c r="AA38" s="38">
         <f t="shared" si="18"/>
-        <v>4.0200183676689094E-11</v>
+        <v>-328124.99999999983</v>
       </c>
     </row>
     <row r="39" spans="2:83" x14ac:dyDescent="0.2">
       <c r="B39" s="38">
         <f t="shared" ref="B39:G41" si="19">$B57*B$28+$C57*B$29+$D57*B$30+$E57*B$31+$F57*B$32+$G57*B$33</f>
-        <v>-3.2160146941351275E-11</v>
+        <v>262499.99999999988</v>
       </c>
       <c r="C39" s="38">
         <f t="shared" si="19"/>
-        <v>328.125</v>
+        <v>284.16458561676893</v>
       </c>
       <c r="D39" s="38">
         <f t="shared" si="19"/>
-        <v>656250</v>
+        <v>568329.17123353796</v>
       </c>
       <c r="E39" s="38">
         <f t="shared" si="19"/>
-        <v>3.2160146941351275E-11</v>
+        <v>-262499.99999999988</v>
       </c>
       <c r="F39" s="38">
         <f t="shared" si="19"/>
-        <v>-328.125</v>
+        <v>-284.16458561676893</v>
       </c>
       <c r="G39" s="38">
         <f t="shared" si="19"/>
-        <v>656250</v>
+        <v>568329.17123353796</v>
       </c>
       <c r="L39" s="38">
         <f t="shared" si="15"/>
@@ -5382,27 +5382,27 @@
     <row r="40" spans="2:83" x14ac:dyDescent="0.2">
       <c r="B40" s="38">
         <f t="shared" si="19"/>
-        <v>-525000</v>
+        <v>-454663.33698683034</v>
       </c>
       <c r="C40" s="38">
         <f t="shared" si="19"/>
-        <v>-2.0100091838344547E-14</v>
+        <v>164.06249999999991</v>
       </c>
       <c r="D40" s="38">
         <f t="shared" si="19"/>
-        <v>-4.0200183676689094E-11</v>
+        <v>328124.99999999983</v>
       </c>
       <c r="E40" s="38">
         <f t="shared" si="19"/>
-        <v>525000</v>
+        <v>454663.33698683034</v>
       </c>
       <c r="F40" s="38">
         <f t="shared" si="19"/>
-        <v>2.0100091838344547E-14</v>
+        <v>-164.06249999999991</v>
       </c>
       <c r="G40" s="38">
         <f t="shared" si="19"/>
-        <v>-4.0200183676689094E-11</v>
+        <v>328124.99999999983</v>
       </c>
       <c r="L40" s="38">
         <f t="shared" si="15"/>
@@ -5431,27 +5431,27 @@
       <c r="S40" s="2"/>
       <c r="V40" s="38">
         <f t="shared" ref="V40:AA42" si="21">$V58*B$28+$W58*B$29+$X58*B$30+$Y58*B$31+$Z58*B$32+$AA58*B$33</f>
-        <v>-3.2160146941351275E-11</v>
+        <v>262499.99999999988</v>
       </c>
       <c r="W40" s="38">
         <f t="shared" si="21"/>
-        <v>328.125</v>
+        <v>284.16458561676893</v>
       </c>
       <c r="X40" s="38">
         <f t="shared" si="21"/>
-        <v>656250</v>
+        <v>568329.17123353796</v>
       </c>
       <c r="Y40" s="38">
         <f t="shared" si="21"/>
-        <v>3.2160146941351275E-11</v>
+        <v>-262499.99999999988</v>
       </c>
       <c r="Z40" s="38">
         <f t="shared" si="21"/>
-        <v>-328.125</v>
+        <v>-284.16458561676893</v>
       </c>
       <c r="AA40" s="38">
         <f t="shared" si="21"/>
-        <v>656250</v>
+        <v>568329.17123353796</v>
       </c>
     </row>
     <row r="41" spans="2:83" x14ac:dyDescent="0.2">
@@ -5505,27 +5505,27 @@
       </c>
       <c r="V41" s="38">
         <f t="shared" si="21"/>
-        <v>-525000</v>
+        <v>-454663.33698683034</v>
       </c>
       <c r="W41" s="38">
         <f t="shared" si="21"/>
-        <v>-2.0100091838344547E-14</v>
+        <v>164.06249999999991</v>
       </c>
       <c r="X41" s="38">
         <f t="shared" si="21"/>
-        <v>-4.0200183676689094E-11</v>
+        <v>328124.99999999983</v>
       </c>
       <c r="Y41" s="38">
         <f t="shared" si="21"/>
-        <v>525000</v>
+        <v>454663.33698683034</v>
       </c>
       <c r="Z41" s="38">
         <f t="shared" si="21"/>
-        <v>2.0100091838344547E-14</v>
+        <v>-164.06249999999991</v>
       </c>
       <c r="AA41" s="38">
         <f t="shared" si="21"/>
-        <v>-4.0200183676689094E-11</v>
+        <v>328124.99999999983</v>
       </c>
       <c r="AJ41" s="2" t="s">
         <v>38</v>
@@ -5642,27 +5642,27 @@
       </c>
       <c r="AK43" s="11">
         <f>AK6+BA6+AK22</f>
-        <v>328.125</v>
+        <v>131496.09374999988</v>
       </c>
       <c r="AL43" s="11">
         <f t="shared" ref="AL43:AV43" si="22">AL6+BB6+AL22</f>
-        <v>3.2140046849512931E-11</v>
+        <v>-227189.58620060666</v>
       </c>
       <c r="AM43" s="11">
         <f t="shared" si="22"/>
-        <v>-656250</v>
+        <v>-568329.17123353796</v>
       </c>
       <c r="AN43" s="11">
         <f t="shared" si="22"/>
-        <v>-328.125</v>
+        <v>-131496.09374999988</v>
       </c>
       <c r="AO43" s="11">
         <f t="shared" si="22"/>
-        <v>-3.2140046849512931E-11</v>
+        <v>227189.58620060666</v>
       </c>
       <c r="AP43" s="11">
         <f t="shared" si="22"/>
-        <v>-656250</v>
+        <v>-568329.17123353796</v>
       </c>
       <c r="AQ43" s="7">
         <f t="shared" si="22"/>
@@ -5693,7 +5693,7 @@
       </c>
       <c r="AZ43" s="3">
         <f>AX6+BN6+AX22</f>
-        <v>-20000</v>
+        <v>-18105.508075688773</v>
       </c>
       <c r="BA43" s="148" t="s">
         <v>55</v>
@@ -5709,27 +5709,27 @@
       </c>
       <c r="AK44" s="11">
         <f t="shared" ref="AK44:AK54" si="23">AK7+BA7+AK23</f>
-        <v>3.2140046849512931E-11</v>
+        <v>-227189.58620060669</v>
       </c>
       <c r="AL44" s="11">
         <f t="shared" ref="AL44:AL54" si="24">AL7+BB7+AL23</f>
-        <v>525000</v>
+        <v>393832.03125000006</v>
       </c>
       <c r="AM44" s="11">
         <f t="shared" ref="AM44:AM54" si="25">AM7+BC7+AM23</f>
-        <v>4.0200183676689094E-11</v>
+        <v>-328124.99999999983</v>
       </c>
       <c r="AN44" s="11">
         <f t="shared" ref="AN44:AN54" si="26">AN7+BD7+AN23</f>
-        <v>-3.2140046849512931E-11</v>
+        <v>227189.58620060669</v>
       </c>
       <c r="AO44" s="11">
         <f t="shared" ref="AO44:AO54" si="27">AO7+BE7+AO23</f>
-        <v>-525000</v>
+        <v>-393832.03125000006</v>
       </c>
       <c r="AP44" s="11">
         <f t="shared" ref="AP44:AP54" si="28">AP7+BF7+AP23</f>
-        <v>4.0200183676689094E-11</v>
+        <v>-328124.99999999983</v>
       </c>
       <c r="AQ44" s="7">
         <f t="shared" ref="AQ44:AQ54" si="29">AQ7+BG7+AQ23</f>
@@ -5760,7 +5760,7 @@
       </c>
       <c r="AZ44" s="3">
         <f t="shared" ref="AZ44:AZ54" si="35">AX7+BN7+AX23</f>
-        <v>1570.0000000000011</v>
+        <v>-8640.3401160584272</v>
       </c>
       <c r="BA44" s="148" t="s">
         <v>54</v>
@@ -5769,11 +5769,11 @@
     <row r="45" spans="2:83" x14ac:dyDescent="0.2">
       <c r="B45" s="41">
         <f>$C$5</f>
-        <v>6.1257422745431001E-17</v>
+        <v>-0.49999999999999978</v>
       </c>
       <c r="C45" s="41">
         <f>$E$5</f>
-        <v>1</v>
+        <v>0.86602540378443871</v>
       </c>
       <c r="D45" s="41">
         <v>0</v>
@@ -5799,11 +5799,11 @@
       </c>
       <c r="AK45" s="11">
         <f t="shared" si="23"/>
-        <v>-656250</v>
+        <v>-568329.17123353796</v>
       </c>
       <c r="AL45" s="11">
         <f t="shared" si="24"/>
-        <v>4.0200183676689094E-11</v>
+        <v>-328124.99999999983</v>
       </c>
       <c r="AM45" s="11">
         <f t="shared" si="25"/>
@@ -5811,11 +5811,11 @@
       </c>
       <c r="AN45" s="11">
         <f t="shared" si="26"/>
-        <v>656250</v>
+        <v>568329.17123353796</v>
       </c>
       <c r="AO45" s="11">
         <f t="shared" si="27"/>
-        <v>-4.0200183676689094E-11</v>
+        <v>328124.99999999983</v>
       </c>
       <c r="AP45" s="11">
         <f t="shared" si="28"/>
@@ -5856,11 +5856,11 @@
     <row r="46" spans="2:83" x14ac:dyDescent="0.2">
       <c r="B46" s="41">
         <f>-$E$5</f>
-        <v>-1</v>
+        <v>-0.86602540378443871</v>
       </c>
       <c r="C46" s="41">
         <f>$C$5</f>
-        <v>6.1257422745431001E-17</v>
+        <v>-0.49999999999999978</v>
       </c>
       <c r="D46" s="41">
         <v>0</v>
@@ -5896,11 +5896,11 @@
       </c>
       <c r="V46" s="41">
         <f>$C$5</f>
-        <v>6.1257422745431001E-17</v>
+        <v>-0.49999999999999978</v>
       </c>
       <c r="W46" s="41">
         <f>$E$5</f>
-        <v>1</v>
+        <v>0.86602540378443871</v>
       </c>
       <c r="X46" s="41">
         <v>0</v>
@@ -5920,27 +5920,27 @@
       </c>
       <c r="AK46" s="11">
         <f t="shared" si="23"/>
-        <v>-328.125</v>
+        <v>-131496.09374999988</v>
       </c>
       <c r="AL46" s="11">
         <f t="shared" si="24"/>
-        <v>-3.2140046849512931E-11</v>
+        <v>227189.58620060666</v>
       </c>
       <c r="AM46" s="11">
         <f t="shared" si="25"/>
-        <v>656250</v>
+        <v>568329.17123353796</v>
       </c>
       <c r="AN46" s="18">
         <f t="shared" si="26"/>
-        <v>700328.125</v>
+        <v>831496.09374999988</v>
       </c>
       <c r="AO46" s="18">
         <f t="shared" si="27"/>
-        <v>3.2140046849512931E-11</v>
+        <v>-227189.58620060666</v>
       </c>
       <c r="AP46" s="18">
         <f t="shared" si="28"/>
-        <v>656250</v>
+        <v>568329.17123353796</v>
       </c>
       <c r="AQ46" s="16">
         <f t="shared" si="29"/>
@@ -5971,7 +5971,7 @@
       </c>
       <c r="AZ46" s="3">
         <f t="shared" si="35"/>
-        <v>-20000</v>
+        <v>-18105.508075688773</v>
       </c>
       <c r="CE46" s="2"/>
     </row>
@@ -6016,11 +6016,11 @@
       </c>
       <c r="V47" s="41">
         <f>-$E$5</f>
-        <v>-1</v>
+        <v>-0.86602540378443871</v>
       </c>
       <c r="W47" s="41">
         <f>$C$5</f>
-        <v>6.1257422745431001E-17</v>
+        <v>-0.49999999999999978</v>
       </c>
       <c r="X47" s="41">
         <v>0</v>
@@ -6040,27 +6040,27 @@
       </c>
       <c r="AK47" s="11">
         <f t="shared" si="23"/>
-        <v>-3.2140046849512931E-11</v>
+        <v>227189.58620060669</v>
       </c>
       <c r="AL47" s="11">
         <f t="shared" si="24"/>
-        <v>-525000</v>
+        <v>-393832.03125000006</v>
       </c>
       <c r="AM47" s="11">
         <f t="shared" si="25"/>
-        <v>-4.0200183676689094E-11</v>
+        <v>328124.99999999983</v>
       </c>
       <c r="AN47" s="18">
         <f t="shared" si="26"/>
-        <v>3.2140046849512931E-11</v>
+        <v>-227189.58620060669</v>
       </c>
       <c r="AO47" s="18">
         <f t="shared" si="27"/>
-        <v>525777.77777777775</v>
+        <v>394609.80902777781</v>
       </c>
       <c r="AP47" s="18">
         <f t="shared" si="28"/>
-        <v>2333333.3333333335</v>
+        <v>2661458.3333333335</v>
       </c>
       <c r="AQ47" s="16">
         <f t="shared" si="29"/>
@@ -6091,7 +6091,7 @@
       </c>
       <c r="AZ47" s="3">
         <f>AX10+BN10+AX26</f>
-        <v>36280</v>
+        <v>26069.659883941575</v>
       </c>
       <c r="BS47" s="3"/>
       <c r="CE47" s="2"/>
@@ -6108,11 +6108,11 @@
       </c>
       <c r="E48" s="41">
         <f>$C$5</f>
-        <v>6.1257422745431001E-17</v>
+        <v>-0.49999999999999978</v>
       </c>
       <c r="F48" s="41">
         <f>$E$5</f>
-        <v>1</v>
+        <v>0.86602540378443871</v>
       </c>
       <c r="G48" s="41">
         <v>0</v>
@@ -6159,11 +6159,11 @@
       </c>
       <c r="AK48" s="11">
         <f t="shared" si="23"/>
-        <v>-656250</v>
+        <v>-568329.17123353796</v>
       </c>
       <c r="AL48" s="11">
         <f t="shared" si="24"/>
-        <v>4.0200183676689094E-11</v>
+        <v>-328124.99999999983</v>
       </c>
       <c r="AM48" s="11">
         <f t="shared" si="25"/>
@@ -6171,11 +6171,11 @@
       </c>
       <c r="AN48" s="18">
         <f t="shared" si="26"/>
-        <v>656250</v>
+        <v>568329.17123353796</v>
       </c>
       <c r="AO48" s="18">
         <f t="shared" si="27"/>
-        <v>2333333.3333333335</v>
+        <v>2661458.3333333335</v>
       </c>
       <c r="AP48" s="18">
         <f t="shared" si="28"/>
@@ -6225,11 +6225,11 @@
       </c>
       <c r="E49" s="41">
         <f>-$E$5</f>
-        <v>-1</v>
+        <v>-0.86602540378443871</v>
       </c>
       <c r="F49" s="41">
         <f>$C$5</f>
-        <v>6.1257422745431001E-17</v>
+        <v>-0.49999999999999978</v>
       </c>
       <c r="G49" s="41">
         <v>0</v>
@@ -6265,11 +6265,11 @@
       </c>
       <c r="Y49" s="41">
         <f>$C$5</f>
-        <v>6.1257422745431001E-17</v>
+        <v>-0.49999999999999978</v>
       </c>
       <c r="Z49" s="41">
         <f>$E$5</f>
-        <v>1</v>
+        <v>0.86602540378443871</v>
       </c>
       <c r="AA49" s="41">
         <v>0</v>
@@ -6306,34 +6306,34 @@
       </c>
       <c r="AQ49" s="17">
         <f t="shared" si="29"/>
-        <v>328.125</v>
+        <v>131496.09374999988</v>
       </c>
       <c r="AR49" s="20">
         <f t="shared" si="30"/>
-        <v>3.2140046849512931E-11</v>
+        <v>-227189.58620060666</v>
       </c>
       <c r="AS49" s="20">
         <f t="shared" si="31"/>
-        <v>-656250</v>
+        <v>-568329.17123353796</v>
       </c>
       <c r="AT49" s="20">
         <f t="shared" si="32"/>
-        <v>-328.125</v>
+        <v>-131496.09374999988</v>
       </c>
       <c r="AU49" s="17">
         <f t="shared" si="33"/>
-        <v>-3.2140046849512931E-11</v>
+        <v>227189.58620060666</v>
       </c>
       <c r="AV49" s="17">
         <f t="shared" si="34"/>
-        <v>-656250</v>
+        <v>-568329.17123353796</v>
       </c>
       <c r="AX49" s="4">
         <v>0</v>
       </c>
       <c r="AZ49" s="3">
         <f t="shared" si="35"/>
-        <v>20000</v>
+        <v>16535.508075688773</v>
       </c>
       <c r="BA49" s="148" t="s">
         <v>56</v>
@@ -6391,11 +6391,11 @@
       </c>
       <c r="Y50" s="41">
         <f>-$E$5</f>
-        <v>-1</v>
+        <v>-0.86602540378443871</v>
       </c>
       <c r="Z50" s="41">
         <f>$C$5</f>
-        <v>6.1257422745431001E-17</v>
+        <v>-0.49999999999999978</v>
       </c>
       <c r="AA50" s="41">
         <v>0</v>
@@ -6432,34 +6432,34 @@
       </c>
       <c r="AQ50" s="20">
         <f t="shared" si="29"/>
-        <v>3.2140046849512931E-11</v>
+        <v>-227189.58620060669</v>
       </c>
       <c r="AR50" s="17">
         <f t="shared" si="30"/>
-        <v>525000</v>
+        <v>393832.03125000006</v>
       </c>
       <c r="AS50" s="17">
         <f t="shared" si="31"/>
-        <v>4.0200183676689094E-11</v>
+        <v>-328124.99999999983</v>
       </c>
       <c r="AT50" s="17">
         <f t="shared" si="32"/>
-        <v>-3.2140046849512931E-11</v>
+        <v>227189.58620060669</v>
       </c>
       <c r="AU50" s="17">
         <f t="shared" si="33"/>
-        <v>-525000</v>
+        <v>-393832.03125000006</v>
       </c>
       <c r="AV50" s="17">
         <f t="shared" si="34"/>
-        <v>4.0200183676689094E-11</v>
+        <v>-328124.99999999983</v>
       </c>
       <c r="AX50" s="4">
         <v>0</v>
       </c>
       <c r="AZ50" s="3">
         <f t="shared" si="35"/>
-        <v>1569.9999999999989</v>
+        <v>11359.659883941566</v>
       </c>
       <c r="BA50" s="148" t="s">
         <v>57</v>
@@ -6539,11 +6539,11 @@
       </c>
       <c r="AQ51" s="20">
         <f t="shared" si="29"/>
-        <v>-656250</v>
+        <v>-568329.17123353796</v>
       </c>
       <c r="AR51" s="17">
         <f t="shared" si="30"/>
-        <v>4.0200183676689094E-11</v>
+        <v>-328124.99999999983</v>
       </c>
       <c r="AS51" s="17">
         <f t="shared" si="31"/>
@@ -6551,11 +6551,11 @@
       </c>
       <c r="AT51" s="17">
         <f t="shared" si="32"/>
-        <v>656250</v>
+        <v>568329.17123353796</v>
       </c>
       <c r="AU51" s="17">
         <f t="shared" si="33"/>
-        <v>-4.0200183676689094E-11</v>
+        <v>328124.99999999983</v>
       </c>
       <c r="AV51" s="17">
         <f t="shared" si="34"/>
@@ -6614,34 +6614,34 @@
       </c>
       <c r="AQ52" s="20">
         <f t="shared" si="29"/>
-        <v>-328.125</v>
+        <v>-131496.09374999988</v>
       </c>
       <c r="AR52" s="17">
         <f t="shared" si="30"/>
-        <v>-3.2140046849512931E-11</v>
+        <v>227189.58620060666</v>
       </c>
       <c r="AS52" s="17">
         <f t="shared" si="31"/>
-        <v>656250</v>
+        <v>568329.17123353796</v>
       </c>
       <c r="AT52" s="21">
         <f t="shared" si="32"/>
-        <v>700328.125</v>
+        <v>831496.09374999988</v>
       </c>
       <c r="AU52" s="21">
         <f t="shared" si="33"/>
-        <v>3.2140046849512931E-11</v>
+        <v>-227189.58620060666</v>
       </c>
       <c r="AV52" s="21">
         <f t="shared" si="34"/>
-        <v>656250</v>
+        <v>568329.17123353796</v>
       </c>
       <c r="AX52" s="4" t="s">
         <v>47</v>
       </c>
       <c r="AZ52" s="3">
         <f t="shared" si="35"/>
-        <v>20000</v>
+        <v>16535.508075688773</v>
       </c>
       <c r="BB52" s="12"/>
       <c r="BE52" s="16"/>
@@ -6692,34 +6692,34 @@
       </c>
       <c r="AQ53" s="17">
         <f t="shared" si="29"/>
-        <v>-3.2140046849512931E-11</v>
+        <v>227189.58620060669</v>
       </c>
       <c r="AR53" s="17">
         <f t="shared" si="30"/>
-        <v>-525000</v>
+        <v>-393832.03125000006</v>
       </c>
       <c r="AS53" s="17">
         <f t="shared" si="31"/>
-        <v>-4.0200183676689094E-11</v>
+        <v>328124.99999999983</v>
       </c>
       <c r="AT53" s="21">
         <f t="shared" si="32"/>
-        <v>3.2140046849512931E-11</v>
+        <v>-227189.58620060669</v>
       </c>
       <c r="AU53" s="21">
         <f t="shared" si="33"/>
-        <v>525777.77777777775</v>
+        <v>394609.80902777781</v>
       </c>
       <c r="AV53" s="21">
         <f t="shared" si="34"/>
-        <v>-2333333.3333333335</v>
+        <v>-2005208.3333333337</v>
       </c>
       <c r="AX53" s="4" t="s">
         <v>48</v>
       </c>
       <c r="AZ53" s="3">
         <f t="shared" si="35"/>
-        <v>36280</v>
+        <v>46069.659883941567</v>
       </c>
       <c r="BB53" s="12"/>
       <c r="BE53" s="16"/>
@@ -6742,11 +6742,11 @@
     <row r="54" spans="2:101" x14ac:dyDescent="0.2">
       <c r="B54" s="41">
         <f>$C$5</f>
-        <v>6.1257422745431001E-17</v>
+        <v>-0.49999999999999978</v>
       </c>
       <c r="C54" s="41">
         <f>-$E$5</f>
-        <v>-1</v>
+        <v>-0.86602540378443871</v>
       </c>
       <c r="D54" s="41">
         <v>0</v>
@@ -6798,11 +6798,11 @@
       </c>
       <c r="AQ54" s="17">
         <f t="shared" si="29"/>
-        <v>-656250</v>
+        <v>-568329.17123353796</v>
       </c>
       <c r="AR54" s="17">
         <f t="shared" si="30"/>
-        <v>4.0200183676689094E-11</v>
+        <v>-328124.99999999983</v>
       </c>
       <c r="AS54" s="17">
         <f t="shared" si="31"/>
@@ -6810,11 +6810,11 @@
       </c>
       <c r="AT54" s="21">
         <f t="shared" si="32"/>
-        <v>656250</v>
+        <v>568329.17123353796</v>
       </c>
       <c r="AU54" s="21">
         <f t="shared" si="33"/>
-        <v>-2333333.3333333335</v>
+        <v>-2005208.3333333337</v>
       </c>
       <c r="AV54" s="21">
         <f t="shared" si="34"/>
@@ -6843,11 +6843,11 @@
     <row r="55" spans="2:101" x14ac:dyDescent="0.2">
       <c r="B55" s="41">
         <f>$E$5</f>
-        <v>1</v>
+        <v>0.86602540378443871</v>
       </c>
       <c r="C55" s="41">
         <f>$C$5</f>
-        <v>6.1257422745431001E-17</v>
+        <v>-0.49999999999999978</v>
       </c>
       <c r="D55" s="41">
         <v>0</v>
@@ -6883,11 +6883,11 @@
       </c>
       <c r="V55" s="41">
         <f>$C$5</f>
-        <v>6.1257422745431001E-17</v>
+        <v>-0.49999999999999978</v>
       </c>
       <c r="W55" s="41">
         <f>-$E$5</f>
-        <v>-1</v>
+        <v>-0.86602540378443871</v>
       </c>
       <c r="X55" s="41">
         <v>0</v>
@@ -6960,11 +6960,11 @@
       </c>
       <c r="V56" s="41">
         <f>$E$5</f>
-        <v>1</v>
+        <v>0.86602540378443871</v>
       </c>
       <c r="W56" s="41">
         <f>$C$5</f>
-        <v>6.1257422745431001E-17</v>
+        <v>-0.49999999999999978</v>
       </c>
       <c r="X56" s="41">
         <v>0</v>
@@ -7007,11 +7007,11 @@
       </c>
       <c r="E57" s="41">
         <f>$C$5</f>
-        <v>6.1257422745431001E-17</v>
+        <v>-0.49999999999999978</v>
       </c>
       <c r="F57" s="41">
         <f>-$E$5</f>
-        <v>-1</v>
+        <v>-0.86602540378443871</v>
       </c>
       <c r="G57" s="41">
         <v>0</v>
@@ -7071,11 +7071,11 @@
       </c>
       <c r="E58" s="41">
         <f>$E$5</f>
-        <v>1</v>
+        <v>0.86602540378443871</v>
       </c>
       <c r="F58" s="41">
         <f>$C$5</f>
-        <v>6.1257422745431001E-17</v>
+        <v>-0.49999999999999978</v>
       </c>
       <c r="G58" s="41">
         <v>0</v>
@@ -7111,11 +7111,11 @@
       </c>
       <c r="Y58" s="41">
         <f>$C$5</f>
-        <v>6.1257422745431001E-17</v>
+        <v>-0.49999999999999978</v>
       </c>
       <c r="Z58" s="41">
         <f>-$E$5</f>
-        <v>-1</v>
+        <v>-0.86602540378443871</v>
       </c>
       <c r="AA58" s="41">
         <v>0</v>
@@ -7184,11 +7184,11 @@
       </c>
       <c r="Y59" s="41">
         <f>$E$5</f>
-        <v>1</v>
+        <v>0.86602540378443871</v>
       </c>
       <c r="Z59" s="41">
         <f>$C$5</f>
-        <v>6.1257422745431001E-17</v>
+        <v>-0.49999999999999978</v>
       </c>
       <c r="AA59" s="41">
         <v>0</v>
@@ -7293,10 +7293,10 @@
         <v>1750000000</v>
       </c>
       <c r="AL60" s="3">
-        <v>656250</v>
+        <v>568329.17123353796</v>
       </c>
       <c r="AM60" s="3">
-        <v>-4.0200183676689094E-11</v>
+        <v>328124.99999999983</v>
       </c>
       <c r="AN60" s="3">
         <v>875000000</v>
@@ -7344,16 +7344,16 @@
         <v>4</v>
       </c>
       <c r="AK61" s="3">
-        <v>656250</v>
+        <v>568329.17123353796</v>
       </c>
       <c r="AL61" s="3">
-        <v>700328.125</v>
+        <v>831496.09374999988</v>
       </c>
       <c r="AM61" s="3">
-        <v>3.2140046849512931E-11</v>
+        <v>-227189.58620060666</v>
       </c>
       <c r="AN61" s="3">
-        <v>656250</v>
+        <v>568329.17123353796</v>
       </c>
       <c r="AO61" s="3">
         <v>0</v>
@@ -7373,7 +7373,7 @@
         <v>r21</v>
       </c>
       <c r="AV61" s="146">
-        <v>-20000</v>
+        <v>-18105.508075688773</v>
       </c>
       <c r="BA61" s="4"/>
       <c r="BB61" s="12"/>
@@ -7402,13 +7402,13 @@
     </row>
     <row r="62" spans="2:101" x14ac:dyDescent="0.2">
       <c r="M62" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="N62" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="O62" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="W62" s="4"/>
       <c r="AD62" s="4"/>
@@ -7416,16 +7416,16 @@
         <v>5</v>
       </c>
       <c r="AK62" s="3">
-        <v>-4.0200183676689094E-11</v>
+        <v>328124.99999999983</v>
       </c>
       <c r="AL62" s="3">
-        <v>3.2140046849512931E-11</v>
+        <v>-227189.58620060669</v>
       </c>
       <c r="AM62" s="3">
-        <v>525777.77777777775</v>
+        <v>394609.80902777781</v>
       </c>
       <c r="AN62" s="3">
-        <v>2333333.3333333335</v>
+        <v>2661458.3333333335</v>
       </c>
       <c r="AO62" s="3">
         <v>0</v>
@@ -7445,7 +7445,7 @@
         <v>r22</v>
       </c>
       <c r="AV62" s="146">
-        <v>36280</v>
+        <v>26069.659883941575</v>
       </c>
       <c r="BB62" s="12"/>
       <c r="BE62" s="12"/>
@@ -7463,19 +7463,19 @@
     </row>
     <row r="63" spans="2:101" x14ac:dyDescent="0.2">
       <c r="I63" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="K63" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="M63" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="N63" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="O63" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="N63" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="O63" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="W63" s="4"/>
       <c r="AD63" s="4"/>
@@ -7486,10 +7486,10 @@
         <v>875000000</v>
       </c>
       <c r="AL63" s="3">
-        <v>656250</v>
+        <v>568329.17123353796</v>
       </c>
       <c r="AM63" s="3">
-        <v>2333333.3333333335</v>
+        <v>2661458.3333333335</v>
       </c>
       <c r="AN63" s="3">
         <v>11083333333.333334</v>
@@ -7533,28 +7533,28 @@
         <v>20</v>
       </c>
       <c r="I64" s="1">
+        <v>10000</v>
+      </c>
+      <c r="J64" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J64" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="K64" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="L64" s="3">
         <f>COS(RADIANS(I65-E4))*I64</f>
-        <v>6.1257422745431001E-16</v>
+        <v>-4999.9999999999982</v>
       </c>
       <c r="M64" s="34" t="s">
-        <v>65</v>
-      </c>
-      <c r="N64" s="3">
+        <v>66</v>
+      </c>
+      <c r="N64" s="27">
         <f>-I67/E6*L64</f>
-        <v>-3.06287113727155E-16</v>
-      </c>
-      <c r="O64" s="3">
+        <v>2499.9999999999991</v>
+      </c>
+      <c r="O64" s="27">
         <f>-I66/E6*L64</f>
-        <v>-3.06287113727155E-16</v>
+        <v>2499.9999999999991</v>
       </c>
       <c r="AJ64" s="9"/>
       <c r="AK64" s="9"/>
@@ -7590,22 +7590,22 @@
         <v>0</v>
       </c>
       <c r="K65" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="L65" s="3">
         <f>SIN(RADIANS(I65-E4))*I64</f>
-        <v>-10</v>
+        <v>-8660.2540378443864</v>
       </c>
       <c r="M65" s="34" t="s">
-        <v>66</v>
-      </c>
-      <c r="N65" s="3">
+        <v>67</v>
+      </c>
+      <c r="N65" s="27">
         <f>I67^2*(3*I66+I67)/E6^3*L65</f>
-        <v>-5</v>
-      </c>
-      <c r="O65" s="3">
+        <v>-4330.1270189221932</v>
+      </c>
+      <c r="O65" s="27">
         <f>I66^2*(I66+3*I67)/E6^3*L65</f>
-        <v>-5</v>
+        <v>-4330.1270189221932</v>
       </c>
       <c r="AJ65" s="9">
         <v>3</v>
@@ -7657,7 +7657,7 @@
     </row>
     <row r="66" spans="5:74" x14ac:dyDescent="0.2">
       <c r="H66" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="I66" s="1">
         <v>2000</v>
@@ -7666,18 +7666,18 @@
         <v>3</v>
       </c>
       <c r="M66" s="152" t="s">
-        <v>67</v>
-      </c>
-      <c r="N66" s="3">
+        <v>68</v>
+      </c>
+      <c r="N66" s="27">
         <f>I66*I67^2/E6^2*L65</f>
-        <v>-5000</v>
-      </c>
-      <c r="O66" s="3">
+        <v>-4330127.018922193</v>
+      </c>
+      <c r="O66" s="27">
         <f>-1*I66^2*I67/E6^2*L65</f>
-        <v>5000</v>
+        <v>4330127.018922193</v>
       </c>
       <c r="P66" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="AJ66" s="9">
         <v>4</v>
@@ -7707,7 +7707,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="AT66" s="1">
-        <v>-20000</v>
+        <v>-18105.508075688773</v>
       </c>
       <c r="AW66" s="1" t="s">
         <v>3</v>
@@ -7718,7 +7718,7 @@
     </row>
     <row r="67" spans="5:74" x14ac:dyDescent="0.2">
       <c r="H67" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I67" s="25">
         <f>E6-I66</f>
@@ -7753,7 +7753,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="AT67" s="1">
-        <v>36280</v>
+        <v>26069.659883941575</v>
       </c>
       <c r="AW67" s="1" t="s">
         <v>3</v>
@@ -7768,7 +7768,7 @@
         <v>61</v>
       </c>
       <c r="M68" s="34" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="AJ68" s="9">
         <v>6</v>
@@ -7814,7 +7814,7 @@
     </row>
     <row r="69" spans="5:74" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="M69" s="34" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="AJ69" s="9">
         <v>9</v>
@@ -7858,7 +7858,7 @@
     <row r="70" spans="5:74" x14ac:dyDescent="0.2">
       <c r="E70" s="26"/>
       <c r="M70" s="152" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AG70" s="2"/>
       <c r="AH70" s="2"/>
@@ -7930,13 +7930,13 @@
     </row>
     <row r="72" spans="5:74" ht="12" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F72" s="1" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="H72" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="M72" s="34" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="AJ72" s="9">
         <v>12</v>
@@ -7978,14 +7978,14 @@
     </row>
     <row r="73" spans="5:74" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="M73" s="34" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="BB73" s="4"/>
       <c r="BK73" s="2"/>
     </row>
     <row r="74" spans="5:74" x14ac:dyDescent="0.2">
       <c r="M74" s="152" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="AZ74" s="12"/>
       <c r="BB74" s="12"/>
@@ -8018,7 +8018,7 @@
     </row>
     <row r="76" spans="5:74" x14ac:dyDescent="0.2">
       <c r="F76" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="M76" s="34"/>
       <c r="AZ76" s="12"/>

</xml_diff>

<commit_message>
Equivalent line loads work (with tests)
</commit_message>
<xml_diff>
--- a/theory/FEM matriisit.xlsx
+++ b/theory/FEM matriisit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ohjelmointi\2_Rust\idfem\theory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B462225D-41F4-4EF4-AAFE-70672ECC3602}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D983DBF-4AE4-4125-93E3-791C25DC504B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-22230" yWindow="0" windowWidth="22335" windowHeight="20880" xr2:uid="{27180542-B0D2-4BFE-946B-7857B24C93C8}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="88">
   <si>
     <t>°</t>
   </si>
@@ -380,6 +380,24 @@
   <si>
     <t>(Huomaa -1* alussa)</t>
   </si>
+  <si>
+    <t>Kuorma</t>
+  </si>
+  <si>
+    <t>N (/Nmm)</t>
+  </si>
+  <si>
+    <t>Huom! Pystykuorma osoittaa alaspäin! Vaikuttaa siihen, miten ekvivalentit kuormat (horisontaalinen ja momentt)</t>
+  </si>
+  <si>
+    <t>pitää ohjelmassa huomioida (toisin kuin vaakasuuntainen, joka jo osoittaa oikealle (0°))</t>
+  </si>
+  <si>
+    <t>Lukkovoimaesimerkissä kuorma osoittaa alaspäin positiivisena</t>
+  </si>
+  <si>
+    <t>mutta SIN(kulma) antaa negatiivisen arvon alaspäin osoittaville voimille</t>
+  </si>
 </sst>
 </file>
 
@@ -671,7 +689,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="153">
+  <cellXfs count="155">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1077,6 +1095,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="164" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutraali" xfId="1" builtinId="28"/>
@@ -1438,16 +1458,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>19051</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>525878</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>171451</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>459203</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1470,7 +1490,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="676275" y="209551"/>
+          <a:off x="0" y="0"/>
           <a:ext cx="6555203" cy="9105900"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1803,7 +1823,7 @@
   <dimension ref="B1:CW227"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1866,7 +1886,7 @@
         <v>18</v>
       </c>
       <c r="E4" s="35">
-        <v>120</v>
+        <v>90</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>0</v>
@@ -1903,14 +1923,14 @@
       </c>
       <c r="C5" s="25">
         <f>COS(RADIANS(E4))</f>
-        <v>-0.49999999999999978</v>
+        <v>6.1257422745431001E-17</v>
       </c>
       <c r="D5" s="34" t="s">
         <v>22</v>
       </c>
       <c r="E5" s="5">
         <f>SIN(RADIANS(E4))</f>
-        <v>0.86602540378443871</v>
+        <v>1</v>
       </c>
       <c r="L5" s="34" t="s">
         <v>21</v>
@@ -2057,27 +2077,27 @@
       </c>
       <c r="AK6" s="11">
         <f t="shared" ref="AK6:AP11" si="0">B20</f>
-        <v>131496.09374999988</v>
+        <v>328.125</v>
       </c>
       <c r="AL6" s="11">
         <f t="shared" si="0"/>
-        <v>-227189.58620060666</v>
+        <v>3.2140046849512931E-11</v>
       </c>
       <c r="AM6" s="11">
         <f t="shared" si="0"/>
-        <v>-568329.17123353796</v>
+        <v>-656250</v>
       </c>
       <c r="AN6" s="11">
         <f t="shared" si="0"/>
-        <v>-131496.09374999988</v>
+        <v>-328.125</v>
       </c>
       <c r="AO6" s="11">
         <f t="shared" si="0"/>
-        <v>227189.58620060666</v>
+        <v>-3.2140046849512931E-11</v>
       </c>
       <c r="AP6" s="11">
         <f t="shared" si="0"/>
-        <v>-568329.17123353796</v>
+        <v>-656250</v>
       </c>
       <c r="AQ6" s="4">
         <v>0</v>
@@ -2100,7 +2120,7 @@
       <c r="AW6" s="4"/>
       <c r="AX6" s="3">
         <f>I20</f>
-        <v>-18105.508075688773</v>
+        <v>-20000</v>
       </c>
       <c r="AZ6" s="81">
         <v>1</v>
@@ -2180,27 +2200,27 @@
       </c>
       <c r="AK7" s="11">
         <f t="shared" si="0"/>
-        <v>-227189.58620060669</v>
+        <v>3.2140046849512931E-11</v>
       </c>
       <c r="AL7" s="11">
         <f t="shared" si="0"/>
-        <v>393832.03125000006</v>
+        <v>525000</v>
       </c>
       <c r="AM7" s="11">
         <f t="shared" si="0"/>
-        <v>-328124.99999999983</v>
+        <v>4.0200183676689094E-11</v>
       </c>
       <c r="AN7" s="11">
         <f t="shared" si="0"/>
-        <v>227189.58620060669</v>
+        <v>-3.2140046849512931E-11</v>
       </c>
       <c r="AO7" s="11">
         <f t="shared" si="0"/>
-        <v>-393832.03125000006</v>
+        <v>-525000</v>
       </c>
       <c r="AP7" s="11">
         <f t="shared" si="0"/>
-        <v>-328124.99999999983</v>
+        <v>4.0200183676689094E-11</v>
       </c>
       <c r="AQ7" s="4">
         <v>0</v>
@@ -2223,7 +2243,7 @@
       <c r="AW7" s="4"/>
       <c r="AX7" s="3">
         <f t="shared" ref="AX7:AX11" si="1">I21</f>
-        <v>-8640.3401160584272</v>
+        <v>1570.0000000000011</v>
       </c>
       <c r="AZ7" s="81">
         <v>2</v>
@@ -2303,11 +2323,11 @@
       </c>
       <c r="AK8" s="11">
         <f t="shared" si="0"/>
-        <v>-568329.17123353796</v>
+        <v>-656250</v>
       </c>
       <c r="AL8" s="11">
         <f t="shared" si="0"/>
-        <v>-328124.99999999983</v>
+        <v>4.0200183676689094E-11</v>
       </c>
       <c r="AM8" s="11">
         <f t="shared" si="0"/>
@@ -2315,11 +2335,11 @@
       </c>
       <c r="AN8" s="11">
         <f t="shared" si="0"/>
-        <v>568329.17123353796</v>
+        <v>656250</v>
       </c>
       <c r="AO8" s="11">
         <f t="shared" si="0"/>
-        <v>328124.99999999983</v>
+        <v>-4.0200183676689094E-11</v>
       </c>
       <c r="AP8" s="11">
         <f t="shared" si="0"/>
@@ -2426,27 +2446,27 @@
       </c>
       <c r="AK9" s="11">
         <f t="shared" si="0"/>
-        <v>-131496.09374999988</v>
+        <v>-328.125</v>
       </c>
       <c r="AL9" s="11">
         <f t="shared" si="0"/>
-        <v>227189.58620060666</v>
+        <v>-3.2140046849512931E-11</v>
       </c>
       <c r="AM9" s="11">
         <f t="shared" si="0"/>
-        <v>568329.17123353796</v>
+        <v>656250</v>
       </c>
       <c r="AN9" s="11">
         <f t="shared" si="0"/>
-        <v>131496.09374999988</v>
+        <v>328.125</v>
       </c>
       <c r="AO9" s="11">
         <f t="shared" si="0"/>
-        <v>-227189.58620060666</v>
+        <v>3.2140046849512931E-11</v>
       </c>
       <c r="AP9" s="11">
         <f t="shared" si="0"/>
-        <v>568329.17123353796</v>
+        <v>656250</v>
       </c>
       <c r="AQ9" s="4">
         <v>0</v>
@@ -2469,7 +2489,7 @@
       <c r="AW9" s="4"/>
       <c r="AX9" s="3">
         <f t="shared" si="1"/>
-        <v>-18105.508075688773</v>
+        <v>-20000</v>
       </c>
       <c r="AZ9" s="81">
         <v>4</v>
@@ -2559,27 +2579,27 @@
       </c>
       <c r="AK10" s="11">
         <f t="shared" si="0"/>
-        <v>227189.58620060669</v>
+        <v>-3.2140046849512931E-11</v>
       </c>
       <c r="AL10" s="11">
         <f t="shared" si="0"/>
-        <v>-393832.03125000006</v>
+        <v>-525000</v>
       </c>
       <c r="AM10" s="11">
         <f t="shared" si="0"/>
-        <v>328124.99999999983</v>
+        <v>-4.0200183676689094E-11</v>
       </c>
       <c r="AN10" s="11">
         <f t="shared" si="0"/>
-        <v>-227189.58620060669</v>
+        <v>3.2140046849512931E-11</v>
       </c>
       <c r="AO10" s="11">
         <f t="shared" si="0"/>
-        <v>393832.03125000006</v>
+        <v>525000</v>
       </c>
       <c r="AP10" s="11">
         <f t="shared" si="0"/>
-        <v>328124.99999999983</v>
+        <v>-4.0200183676689094E-11</v>
       </c>
       <c r="AQ10" s="4">
         <v>0</v>
@@ -2602,7 +2622,7 @@
       <c r="AW10" s="4"/>
       <c r="AX10" s="3">
         <f>I24</f>
-        <v>-8640.3401160584272</v>
+        <v>1570.0000000000011</v>
       </c>
       <c r="AZ10" s="81">
         <v>5</v>
@@ -2691,11 +2711,11 @@
       </c>
       <c r="AK11" s="11">
         <f t="shared" si="0"/>
-        <v>-568329.17123353796</v>
+        <v>-656250</v>
       </c>
       <c r="AL11" s="11">
         <f t="shared" si="0"/>
-        <v>-328124.99999999983</v>
+        <v>4.0200183676689094E-11</v>
       </c>
       <c r="AM11" s="11">
         <f t="shared" si="0"/>
@@ -2703,11 +2723,11 @@
       </c>
       <c r="AN11" s="11">
         <f t="shared" si="0"/>
-        <v>568329.17123353796</v>
+        <v>656250</v>
       </c>
       <c r="AO11" s="11">
         <f t="shared" si="0"/>
-        <v>328124.99999999983</v>
+        <v>-4.0200183676689094E-11</v>
       </c>
       <c r="AP11" s="11">
         <f t="shared" si="0"/>
@@ -3490,31 +3510,31 @@
     <row r="20" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B20" s="37">
         <f t="shared" ref="B20:G21" si="6">$B36*B$45+$C36*B$46+$D36*B$47+$E36*B$48+$F36*B$49+$G36*B$50</f>
-        <v>131496.09374999988</v>
+        <v>328.125</v>
       </c>
       <c r="C20" s="37">
         <f t="shared" si="6"/>
-        <v>-227189.58620060666</v>
+        <v>3.2140046849512931E-11</v>
       </c>
       <c r="D20" s="37">
         <f t="shared" si="6"/>
-        <v>-568329.17123353796</v>
+        <v>-656250</v>
       </c>
       <c r="E20" s="37">
         <f t="shared" si="6"/>
-        <v>-131496.09374999988</v>
+        <v>-328.125</v>
       </c>
       <c r="F20" s="37">
         <f t="shared" si="6"/>
-        <v>227189.58620060666</v>
+        <v>-3.2140046849512931E-11</v>
       </c>
       <c r="G20" s="37">
         <f t="shared" si="6"/>
-        <v>-568329.17123353796</v>
+        <v>-656250</v>
       </c>
       <c r="I20" s="40">
         <f>B54*I28+C54*I29+D54*I30+E54*I31+F54*I32+G54*I33</f>
-        <v>-18105.508075688773</v>
+        <v>-20000</v>
       </c>
       <c r="L20" s="19">
         <f t="shared" ref="L20:Q25" si="7">$L37*L$46+$M37*L$47+$N37*L$48+$O37*L$49+$P37*L$50+$Q37*L$51</f>
@@ -3546,31 +3566,31 @@
       </c>
       <c r="V20" s="20">
         <f t="shared" ref="V20:AA21" si="8">$V37*B$45+$W37*B$46+$X37*B$47+$Y37*B$48+$Z37*B$49+$AA37*B$50</f>
-        <v>131496.09374999988</v>
+        <v>328.125</v>
       </c>
       <c r="W20" s="20">
         <f t="shared" si="8"/>
-        <v>-227189.58620060666</v>
+        <v>3.2140046849512931E-11</v>
       </c>
       <c r="X20" s="20">
         <f t="shared" si="8"/>
-        <v>-568329.17123353796</v>
+        <v>-656250</v>
       </c>
       <c r="Y20" s="20">
         <f t="shared" si="8"/>
-        <v>-131496.09374999988</v>
+        <v>-328.125</v>
       </c>
       <c r="Z20" s="20">
         <f t="shared" si="8"/>
-        <v>227189.58620060666</v>
+        <v>-3.2140046849512931E-11</v>
       </c>
       <c r="AA20" s="20">
         <f t="shared" si="8"/>
-        <v>-568329.17123353796</v>
+        <v>-656250</v>
       </c>
       <c r="AC20" s="40">
         <f>V55*AC28+W55*AC29+X55*AC30+Y55*AC31+Z55*AC32+AA55*AC33</f>
-        <v>16535.508075688773</v>
+        <v>20000</v>
       </c>
       <c r="AJ20" s="2" t="s">
         <v>40</v>
@@ -3579,31 +3599,31 @@
     <row r="21" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B21" s="37">
         <f t="shared" si="6"/>
-        <v>-227189.58620060669</v>
+        <v>3.2140046849512931E-11</v>
       </c>
       <c r="C21" s="37">
         <f t="shared" si="6"/>
-        <v>393832.03125000006</v>
+        <v>525000</v>
       </c>
       <c r="D21" s="37">
         <f t="shared" si="6"/>
-        <v>-328124.99999999983</v>
+        <v>4.0200183676689094E-11</v>
       </c>
       <c r="E21" s="37">
         <f t="shared" si="6"/>
-        <v>227189.58620060669</v>
+        <v>-3.2140046849512931E-11</v>
       </c>
       <c r="F21" s="37">
         <f t="shared" si="6"/>
-        <v>-393832.03125000006</v>
+        <v>-525000</v>
       </c>
       <c r="G21" s="37">
         <f t="shared" si="6"/>
-        <v>-328124.99999999983</v>
+        <v>4.0200183676689094E-11</v>
       </c>
       <c r="I21" s="40">
         <f>B55*I28+C55*I29+D55*I30+E55*I31+F55*I32+G55*I33</f>
-        <v>-8640.3401160584272</v>
+        <v>1570.0000000000011</v>
       </c>
       <c r="L21" s="19">
         <f t="shared" si="7"/>
@@ -3635,31 +3655,31 @@
       </c>
       <c r="V21" s="20">
         <f t="shared" si="8"/>
-        <v>-227189.58620060669</v>
+        <v>3.2140046849512931E-11</v>
       </c>
       <c r="W21" s="20">
         <f t="shared" si="8"/>
-        <v>393832.03125000006</v>
+        <v>525000</v>
       </c>
       <c r="X21" s="20">
         <f t="shared" si="8"/>
-        <v>-328124.99999999983</v>
+        <v>4.0200183676689094E-11</v>
       </c>
       <c r="Y21" s="20">
         <f t="shared" si="8"/>
-        <v>227189.58620060669</v>
+        <v>-3.2140046849512931E-11</v>
       </c>
       <c r="Z21" s="20">
         <f t="shared" si="8"/>
-        <v>-393832.03125000006</v>
+        <v>-525000</v>
       </c>
       <c r="AA21" s="20">
         <f t="shared" si="8"/>
-        <v>-328124.99999999983</v>
+        <v>4.0200183676689094E-11</v>
       </c>
       <c r="AC21" s="40">
         <f>V56*AC28+W56*AC29+X56*AC30+Y56*AC31+Z56*AC32+AA56*AC33</f>
-        <v>11359.659883941566</v>
+        <v>1569.9999999999989</v>
       </c>
       <c r="AJ21" s="9"/>
       <c r="AK21" s="81">
@@ -3706,11 +3726,11 @@
     <row r="22" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B22" s="37">
         <f t="shared" ref="B22:F25" si="9">$B38*B$45+$C38*B$46+$D38*B$47+$E38*B$48+$F38*B$49+$G38*B$50</f>
-        <v>-568329.17123353796</v>
+        <v>-656250</v>
       </c>
       <c r="C22" s="37">
         <f t="shared" si="9"/>
-        <v>-328124.99999999983</v>
+        <v>4.0200183676689094E-11</v>
       </c>
       <c r="D22" s="37">
         <f t="shared" si="9"/>
@@ -3718,11 +3738,11 @@
       </c>
       <c r="E22" s="37">
         <f t="shared" si="9"/>
-        <v>568329.17123353796</v>
+        <v>656250</v>
       </c>
       <c r="F22" s="37">
         <f t="shared" si="9"/>
-        <v>328124.99999999983</v>
+        <v>-4.0200183676689094E-11</v>
       </c>
       <c r="G22" s="37">
         <f>-1*$B38*G$45+$C38*G$46+$D38*G$47+$E38*G$48+$F38*G$49+$G38*G$50</f>
@@ -3762,11 +3782,11 @@
       </c>
       <c r="V22" s="20">
         <f t="shared" ref="V22:Z25" si="10">$V39*B$45+$W39*B$46+$X39*B$47+$Y39*B$48+$Z39*B$49+$AA39*B$50</f>
-        <v>-568329.17123353796</v>
+        <v>-656250</v>
       </c>
       <c r="W22" s="20">
         <f t="shared" si="10"/>
-        <v>-328124.99999999983</v>
+        <v>4.0200183676689094E-11</v>
       </c>
       <c r="X22" s="20">
         <f t="shared" si="10"/>
@@ -3774,11 +3794,11 @@
       </c>
       <c r="Y22" s="20">
         <f t="shared" si="10"/>
-        <v>568329.17123353796</v>
+        <v>656250</v>
       </c>
       <c r="Z22" s="20">
         <f t="shared" si="10"/>
-        <v>328124.99999999983</v>
+        <v>-4.0200183676689094E-11</v>
       </c>
       <c r="AA22" s="20">
         <f>-1*$V39*G$45+$W39*G$46+$X39*G$47+$Y39*G$48+$Z39*G$49+$AA39*G$50</f>
@@ -3832,31 +3852,31 @@
     <row r="23" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B23" s="37">
         <f t="shared" si="9"/>
-        <v>-131496.09374999988</v>
+        <v>-328.125</v>
       </c>
       <c r="C23" s="37">
         <f t="shared" si="9"/>
-        <v>227189.58620060666</v>
+        <v>-3.2140046849512931E-11</v>
       </c>
       <c r="D23" s="37">
         <f t="shared" si="9"/>
-        <v>568329.17123353796</v>
+        <v>656250</v>
       </c>
       <c r="E23" s="37">
         <f t="shared" si="9"/>
-        <v>131496.09374999988</v>
+        <v>328.125</v>
       </c>
       <c r="F23" s="37">
         <f t="shared" si="9"/>
-        <v>-227189.58620060666</v>
+        <v>3.2140046849512931E-11</v>
       </c>
       <c r="G23" s="37">
         <f>$B39*G$45+$C39*G$46+$D39*G$47+$E39*G$48+$F39*G$49+$G39*G$50</f>
-        <v>568329.17123353796</v>
+        <v>656250</v>
       </c>
       <c r="I23" s="40">
         <f>B57*I28+C57*I29+D57*I30+E57*I31+F57*I32+G57*I33</f>
-        <v>-18105.508075688773</v>
+        <v>-20000</v>
       </c>
       <c r="L23" s="19">
         <f t="shared" si="7"/>
@@ -3888,31 +3908,31 @@
       </c>
       <c r="V23" s="20">
         <f t="shared" si="10"/>
-        <v>-131496.09374999988</v>
+        <v>-328.125</v>
       </c>
       <c r="W23" s="20">
         <f t="shared" si="10"/>
-        <v>227189.58620060666</v>
+        <v>-3.2140046849512931E-11</v>
       </c>
       <c r="X23" s="20">
         <f t="shared" si="10"/>
-        <v>568329.17123353796</v>
+        <v>656250</v>
       </c>
       <c r="Y23" s="20">
         <f t="shared" si="10"/>
-        <v>131496.09374999988</v>
+        <v>328.125</v>
       </c>
       <c r="Z23" s="20">
         <f t="shared" si="10"/>
-        <v>-227189.58620060666</v>
+        <v>3.2140046849512931E-11</v>
       </c>
       <c r="AA23" s="20">
         <f>$V40*G$45+$W40*G$46+$X40*G$47+$Y40*G$48+$Z40*G$49+$AA40*G$50</f>
-        <v>568329.17123353796</v>
+        <v>656250</v>
       </c>
       <c r="AC23" s="40">
         <f>V58*AC28+W58*AC29+X58*AC30+Y58*AC31+Z58*AC32+AA58*AC33</f>
-        <v>16535.508075688773</v>
+        <v>20000</v>
       </c>
       <c r="AJ23" s="81">
         <v>2</v>
@@ -3958,31 +3978,31 @@
     <row r="24" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B24" s="37">
         <f t="shared" si="9"/>
-        <v>227189.58620060669</v>
+        <v>-3.2140046849512931E-11</v>
       </c>
       <c r="C24" s="37">
         <f t="shared" si="9"/>
-        <v>-393832.03125000006</v>
+        <v>-525000</v>
       </c>
       <c r="D24" s="37">
         <f t="shared" si="9"/>
-        <v>328124.99999999983</v>
+        <v>-4.0200183676689094E-11</v>
       </c>
       <c r="E24" s="37">
         <f t="shared" si="9"/>
-        <v>-227189.58620060669</v>
+        <v>3.2140046849512931E-11</v>
       </c>
       <c r="F24" s="37">
         <f t="shared" si="9"/>
-        <v>393832.03125000006</v>
+        <v>525000</v>
       </c>
       <c r="G24" s="37">
         <f>$B40*G$45+$C40*G$46+$D40*G$47+$E40*G$48+$F40*G$49+$G40*G$50</f>
-        <v>328124.99999999983</v>
+        <v>-4.0200183676689094E-11</v>
       </c>
       <c r="I24" s="40">
         <f>B58*I28+C58*I29+D58*I30+E58*I31+F58*I32+G58*I33</f>
-        <v>-8640.3401160584272</v>
+        <v>1570.0000000000011</v>
       </c>
       <c r="L24" s="19">
         <f t="shared" si="7"/>
@@ -4014,31 +4034,31 @@
       </c>
       <c r="V24" s="20">
         <f t="shared" si="10"/>
-        <v>227189.58620060669</v>
+        <v>-3.2140046849512931E-11</v>
       </c>
       <c r="W24" s="20">
         <f t="shared" si="10"/>
-        <v>-393832.03125000006</v>
+        <v>-525000</v>
       </c>
       <c r="X24" s="20">
         <f t="shared" si="10"/>
-        <v>328124.99999999983</v>
+        <v>-4.0200183676689094E-11</v>
       </c>
       <c r="Y24" s="20">
         <f t="shared" si="10"/>
-        <v>-227189.58620060669</v>
+        <v>3.2140046849512931E-11</v>
       </c>
       <c r="Z24" s="20">
         <f t="shared" si="10"/>
-        <v>393832.03125000006</v>
+        <v>525000</v>
       </c>
       <c r="AA24" s="20">
         <f>$V41*G$45+$W41*G$46+$X41*G$47+$Y41*G$48+$Z41*G$49+$AA41*G$50</f>
-        <v>328124.99999999983</v>
+        <v>-4.0200183676689094E-11</v>
       </c>
       <c r="AC24" s="40">
         <f>V59*AC28+W59*AC29+X59*AC30+Y59*AC31+Z59*AC32+AA59*AC33</f>
-        <v>11359.659883941566</v>
+        <v>1569.9999999999989</v>
       </c>
       <c r="AJ24" s="81">
         <v>3</v>
@@ -4084,11 +4104,11 @@
     <row r="25" spans="2:66" x14ac:dyDescent="0.2">
       <c r="B25" s="37">
         <f t="shared" si="9"/>
-        <v>-568329.17123353796</v>
+        <v>-656250</v>
       </c>
       <c r="C25" s="37">
         <f t="shared" si="9"/>
-        <v>-328124.99999999983</v>
+        <v>4.0200183676689094E-11</v>
       </c>
       <c r="D25" s="37">
         <f t="shared" si="9"/>
@@ -4096,11 +4116,11 @@
       </c>
       <c r="E25" s="37">
         <f t="shared" si="9"/>
-        <v>568329.17123353796</v>
+        <v>656250</v>
       </c>
       <c r="F25" s="37">
         <f t="shared" si="9"/>
-        <v>328124.99999999983</v>
+        <v>-4.0200183676689094E-11</v>
       </c>
       <c r="G25" s="37">
         <f>$B41*G$45+$C41*G$46+$D41*G$47+$E41*G$48+$F41*G$49+$G41*G$50</f>
@@ -4142,11 +4162,11 @@
       <c r="U25" s="2"/>
       <c r="V25" s="20">
         <f t="shared" si="10"/>
-        <v>-568329.17123353796</v>
+        <v>-656250</v>
       </c>
       <c r="W25" s="20">
         <f t="shared" si="10"/>
-        <v>-328124.99999999983</v>
+        <v>4.0200183676689094E-11</v>
       </c>
       <c r="X25" s="20">
         <f t="shared" si="10"/>
@@ -4154,11 +4174,11 @@
       </c>
       <c r="Y25" s="20">
         <f t="shared" si="10"/>
-        <v>568329.17123353796</v>
+        <v>656250</v>
       </c>
       <c r="Z25" s="20">
         <f t="shared" si="10"/>
-        <v>328124.99999999983</v>
+        <v>-4.0200183676689094E-11</v>
       </c>
       <c r="AA25" s="20">
         <f>$V42*G$45+$W42*G$46+$X42*G$47+$Y42*G$48+$Z42*G$49+$AA42*G$50</f>
@@ -4414,32 +4434,32 @@
       </c>
       <c r="AQ28" s="17">
         <f t="shared" ref="AQ28:AV33" si="11">V20</f>
-        <v>131496.09374999988</v>
+        <v>328.125</v>
       </c>
       <c r="AR28" s="17">
         <f t="shared" si="11"/>
-        <v>-227189.58620060666</v>
+        <v>3.2140046849512931E-11</v>
       </c>
       <c r="AS28" s="17">
         <f t="shared" si="11"/>
-        <v>-568329.17123353796</v>
+        <v>-656250</v>
       </c>
       <c r="AT28" s="17">
         <f t="shared" si="11"/>
-        <v>-131496.09374999988</v>
+        <v>-328.125</v>
       </c>
       <c r="AU28" s="17">
         <f t="shared" si="11"/>
-        <v>227189.58620060666</v>
+        <v>-3.2140046849512931E-11</v>
       </c>
       <c r="AV28" s="17">
         <f t="shared" si="11"/>
-        <v>-568329.17123353796</v>
+        <v>-656250</v>
       </c>
       <c r="AW28" s="4"/>
       <c r="AX28" s="3">
         <f>AC20</f>
-        <v>16535.508075688773</v>
+        <v>20000</v>
       </c>
       <c r="AY28" s="8"/>
     </row>
@@ -4545,32 +4565,32 @@
       </c>
       <c r="AQ29" s="17">
         <f t="shared" si="11"/>
-        <v>-227189.58620060669</v>
+        <v>3.2140046849512931E-11</v>
       </c>
       <c r="AR29" s="17">
         <f t="shared" si="11"/>
-        <v>393832.03125000006</v>
+        <v>525000</v>
       </c>
       <c r="AS29" s="17">
         <f t="shared" si="11"/>
-        <v>-328124.99999999983</v>
+        <v>4.0200183676689094E-11</v>
       </c>
       <c r="AT29" s="17">
         <f t="shared" si="11"/>
-        <v>227189.58620060669</v>
+        <v>-3.2140046849512931E-11</v>
       </c>
       <c r="AU29" s="17">
         <f t="shared" si="11"/>
-        <v>-393832.03125000006</v>
+        <v>-525000</v>
       </c>
       <c r="AV29" s="17">
         <f t="shared" si="11"/>
-        <v>-328124.99999999983</v>
+        <v>4.0200183676689094E-11</v>
       </c>
       <c r="AW29" s="4"/>
       <c r="AX29" s="3">
         <f t="shared" ref="AX29:AX33" si="12">AC21</f>
-        <v>11359.659883941566</v>
+        <v>1569.9999999999989</v>
       </c>
       <c r="AY29" s="10"/>
     </row>
@@ -4676,11 +4696,11 @@
       </c>
       <c r="AQ30" s="17">
         <f t="shared" si="11"/>
-        <v>-568329.17123353796</v>
+        <v>-656250</v>
       </c>
       <c r="AR30" s="17">
         <f t="shared" si="11"/>
-        <v>-328124.99999999983</v>
+        <v>4.0200183676689094E-11</v>
       </c>
       <c r="AS30" s="17">
         <f t="shared" si="11"/>
@@ -4688,11 +4708,11 @@
       </c>
       <c r="AT30" s="17">
         <f t="shared" si="11"/>
-        <v>568329.17123353796</v>
+        <v>656250</v>
       </c>
       <c r="AU30" s="17">
         <f t="shared" si="11"/>
-        <v>328124.99999999983</v>
+        <v>-4.0200183676689094E-11</v>
       </c>
       <c r="AV30" s="17">
         <f t="shared" si="11"/>
@@ -4800,32 +4820,32 @@
       </c>
       <c r="AQ31" s="17">
         <f t="shared" si="11"/>
-        <v>-131496.09374999988</v>
+        <v>-328.125</v>
       </c>
       <c r="AR31" s="17">
         <f t="shared" si="11"/>
-        <v>227189.58620060666</v>
+        <v>-3.2140046849512931E-11</v>
       </c>
       <c r="AS31" s="17">
         <f t="shared" si="11"/>
-        <v>568329.17123353796</v>
+        <v>656250</v>
       </c>
       <c r="AT31" s="17">
         <f t="shared" si="11"/>
-        <v>131496.09374999988</v>
+        <v>328.125</v>
       </c>
       <c r="AU31" s="17">
         <f t="shared" si="11"/>
-        <v>-227189.58620060666</v>
+        <v>3.2140046849512931E-11</v>
       </c>
       <c r="AV31" s="17">
         <f t="shared" si="11"/>
-        <v>568329.17123353796</v>
+        <v>656250</v>
       </c>
       <c r="AW31" s="4"/>
       <c r="AX31" s="3">
         <f t="shared" si="12"/>
-        <v>16535.508075688773</v>
+        <v>20000</v>
       </c>
       <c r="AY31" s="8"/>
     </row>
@@ -4932,32 +4952,32 @@
       </c>
       <c r="AQ32" s="17">
         <f t="shared" si="11"/>
-        <v>227189.58620060669</v>
+        <v>-3.2140046849512931E-11</v>
       </c>
       <c r="AR32" s="17">
         <f t="shared" si="11"/>
-        <v>-393832.03125000006</v>
+        <v>-525000</v>
       </c>
       <c r="AS32" s="17">
         <f t="shared" si="11"/>
-        <v>328124.99999999983</v>
+        <v>-4.0200183676689094E-11</v>
       </c>
       <c r="AT32" s="17">
         <f t="shared" si="11"/>
-        <v>-227189.58620060669</v>
+        <v>3.2140046849512931E-11</v>
       </c>
       <c r="AU32" s="17">
         <f t="shared" si="11"/>
-        <v>393832.03125000006</v>
+        <v>525000</v>
       </c>
       <c r="AV32" s="17">
         <f t="shared" si="11"/>
-        <v>328124.99999999983</v>
+        <v>-4.0200183676689094E-11</v>
       </c>
       <c r="AW32" s="4"/>
       <c r="AX32" s="3">
         <f t="shared" si="12"/>
-        <v>11359.659883941566</v>
+        <v>1569.9999999999989</v>
       </c>
       <c r="AY32" s="10"/>
     </row>
@@ -5063,11 +5083,11 @@
       </c>
       <c r="AQ33" s="17">
         <f t="shared" si="11"/>
-        <v>-568329.17123353796</v>
+        <v>-656250</v>
       </c>
       <c r="AR33" s="17">
         <f t="shared" si="11"/>
-        <v>-328124.99999999983</v>
+        <v>4.0200183676689094E-11</v>
       </c>
       <c r="AS33" s="17">
         <f t="shared" si="11"/>
@@ -5075,11 +5095,11 @@
       </c>
       <c r="AT33" s="17">
         <f t="shared" si="11"/>
-        <v>568329.17123353796</v>
+        <v>656250</v>
       </c>
       <c r="AU33" s="17">
         <f t="shared" si="11"/>
-        <v>328124.99999999983</v>
+        <v>-4.0200183676689094E-11</v>
       </c>
       <c r="AV33" s="17">
         <f t="shared" si="11"/>
@@ -5128,27 +5148,27 @@
     <row r="36" spans="2:83" x14ac:dyDescent="0.2">
       <c r="B36" s="38">
         <f t="shared" ref="B36:G36" si="13">$B54*B28+$C54*B29+$D54*B30+$E54*B31+$F54*B32+$G54*B33</f>
-        <v>-262499.99999999988</v>
+        <v>3.2160146941351275E-11</v>
       </c>
       <c r="C36" s="38">
         <f t="shared" si="13"/>
-        <v>-284.16458561676893</v>
+        <v>-328.125</v>
       </c>
       <c r="D36" s="38">
         <f t="shared" si="13"/>
-        <v>-568329.17123353796</v>
+        <v>-656250</v>
       </c>
       <c r="E36" s="38">
         <f t="shared" si="13"/>
-        <v>262499.99999999988</v>
+        <v>-3.2160146941351275E-11</v>
       </c>
       <c r="F36" s="38">
         <f t="shared" si="13"/>
-        <v>284.16458561676893</v>
+        <v>328.125</v>
       </c>
       <c r="G36" s="38">
         <f t="shared" si="13"/>
-        <v>-568329.17123353796</v>
+        <v>-656250</v>
       </c>
       <c r="L36" s="2" t="s">
         <v>30</v>
@@ -5160,27 +5180,27 @@
     <row r="37" spans="2:83" x14ac:dyDescent="0.2">
       <c r="B37" s="38">
         <f t="shared" ref="B37:G37" si="14">$B55*B28+$C55*B29+$D55*B30+$E55*B31+$F55*B32+$G55*B33</f>
-        <v>454663.33698683034</v>
+        <v>525000</v>
       </c>
       <c r="C37" s="38">
         <f t="shared" si="14"/>
-        <v>-164.06249999999991</v>
+        <v>2.0100091838344547E-14</v>
       </c>
       <c r="D37" s="38">
         <f t="shared" si="14"/>
-        <v>-328124.99999999983</v>
+        <v>4.0200183676689094E-11</v>
       </c>
       <c r="E37" s="38">
         <f t="shared" si="14"/>
-        <v>-454663.33698683034</v>
+        <v>-525000</v>
       </c>
       <c r="F37" s="38">
         <f t="shared" si="14"/>
-        <v>164.06249999999991</v>
+        <v>-2.0100091838344547E-14</v>
       </c>
       <c r="G37" s="38">
         <f t="shared" si="14"/>
-        <v>-328124.99999999983</v>
+        <v>4.0200183676689094E-11</v>
       </c>
       <c r="L37" s="38">
         <f t="shared" ref="L37:Q42" si="15">$L55*L$28+$M55*L$29+$N55*L$30+$O55*L$31+$P55*L$32+$Q55*L$33</f>
@@ -5208,27 +5228,27 @@
       </c>
       <c r="V37" s="38">
         <f t="shared" ref="V37:AA37" si="16">$V55*V28+$W55*V29+$X55*V30+$Y55*V31+$Z55*V32+$AA55*V33</f>
-        <v>-262499.99999999988</v>
+        <v>3.2160146941351275E-11</v>
       </c>
       <c r="W37" s="38">
         <f t="shared" si="16"/>
-        <v>-284.16458561676893</v>
+        <v>-328.125</v>
       </c>
       <c r="X37" s="38">
         <f t="shared" si="16"/>
-        <v>-568329.17123353796</v>
+        <v>-656250</v>
       </c>
       <c r="Y37" s="38">
         <f t="shared" si="16"/>
-        <v>262499.99999999988</v>
+        <v>-3.2160146941351275E-11</v>
       </c>
       <c r="Z37" s="38">
         <f t="shared" si="16"/>
-        <v>284.16458561676893</v>
+        <v>328.125</v>
       </c>
       <c r="AA37" s="38">
         <f t="shared" si="16"/>
-        <v>-568329.17123353796</v>
+        <v>-656250</v>
       </c>
     </row>
     <row r="38" spans="2:83" x14ac:dyDescent="0.2">
@@ -5282,53 +5302,53 @@
       </c>
       <c r="V38" s="38">
         <f t="shared" ref="V38:AA38" si="18">$V56*V28+$W56*V29+$X56*V30+$Y56*V31+$Z56*V32+$AA56*V33</f>
-        <v>454663.33698683034</v>
+        <v>525000</v>
       </c>
       <c r="W38" s="38">
         <f t="shared" si="18"/>
-        <v>-164.06249999999991</v>
+        <v>2.0100091838344547E-14</v>
       </c>
       <c r="X38" s="38">
         <f t="shared" si="18"/>
-        <v>-328124.99999999983</v>
+        <v>4.0200183676689094E-11</v>
       </c>
       <c r="Y38" s="38">
         <f t="shared" si="18"/>
-        <v>-454663.33698683034</v>
+        <v>-525000</v>
       </c>
       <c r="Z38" s="38">
         <f t="shared" si="18"/>
-        <v>164.06249999999991</v>
+        <v>-2.0100091838344547E-14</v>
       </c>
       <c r="AA38" s="38">
         <f t="shared" si="18"/>
-        <v>-328124.99999999983</v>
+        <v>4.0200183676689094E-11</v>
       </c>
     </row>
     <row r="39" spans="2:83" x14ac:dyDescent="0.2">
       <c r="B39" s="38">
         <f t="shared" ref="B39:G41" si="19">$B57*B$28+$C57*B$29+$D57*B$30+$E57*B$31+$F57*B$32+$G57*B$33</f>
-        <v>262499.99999999988</v>
+        <v>-3.2160146941351275E-11</v>
       </c>
       <c r="C39" s="38">
         <f t="shared" si="19"/>
-        <v>284.16458561676893</v>
+        <v>328.125</v>
       </c>
       <c r="D39" s="38">
         <f t="shared" si="19"/>
-        <v>568329.17123353796</v>
+        <v>656250</v>
       </c>
       <c r="E39" s="38">
         <f t="shared" si="19"/>
-        <v>-262499.99999999988</v>
+        <v>3.2160146941351275E-11</v>
       </c>
       <c r="F39" s="38">
         <f t="shared" si="19"/>
-        <v>-284.16458561676893</v>
+        <v>-328.125</v>
       </c>
       <c r="G39" s="38">
         <f t="shared" si="19"/>
-        <v>568329.17123353796</v>
+        <v>656250</v>
       </c>
       <c r="L39" s="38">
         <f t="shared" si="15"/>
@@ -5382,27 +5402,27 @@
     <row r="40" spans="2:83" x14ac:dyDescent="0.2">
       <c r="B40" s="38">
         <f t="shared" si="19"/>
-        <v>-454663.33698683034</v>
+        <v>-525000</v>
       </c>
       <c r="C40" s="38">
         <f t="shared" si="19"/>
-        <v>164.06249999999991</v>
+        <v>-2.0100091838344547E-14</v>
       </c>
       <c r="D40" s="38">
         <f t="shared" si="19"/>
-        <v>328124.99999999983</v>
+        <v>-4.0200183676689094E-11</v>
       </c>
       <c r="E40" s="38">
         <f t="shared" si="19"/>
-        <v>454663.33698683034</v>
+        <v>525000</v>
       </c>
       <c r="F40" s="38">
         <f t="shared" si="19"/>
-        <v>-164.06249999999991</v>
+        <v>2.0100091838344547E-14</v>
       </c>
       <c r="G40" s="38">
         <f t="shared" si="19"/>
-        <v>328124.99999999983</v>
+        <v>-4.0200183676689094E-11</v>
       </c>
       <c r="L40" s="38">
         <f t="shared" si="15"/>
@@ -5431,27 +5451,27 @@
       <c r="S40" s="2"/>
       <c r="V40" s="38">
         <f t="shared" ref="V40:AA42" si="21">$V58*B$28+$W58*B$29+$X58*B$30+$Y58*B$31+$Z58*B$32+$AA58*B$33</f>
-        <v>262499.99999999988</v>
+        <v>-3.2160146941351275E-11</v>
       </c>
       <c r="W40" s="38">
         <f t="shared" si="21"/>
-        <v>284.16458561676893</v>
+        <v>328.125</v>
       </c>
       <c r="X40" s="38">
         <f t="shared" si="21"/>
-        <v>568329.17123353796</v>
+        <v>656250</v>
       </c>
       <c r="Y40" s="38">
         <f t="shared" si="21"/>
-        <v>-262499.99999999988</v>
+        <v>3.2160146941351275E-11</v>
       </c>
       <c r="Z40" s="38">
         <f t="shared" si="21"/>
-        <v>-284.16458561676893</v>
+        <v>-328.125</v>
       </c>
       <c r="AA40" s="38">
         <f t="shared" si="21"/>
-        <v>568329.17123353796</v>
+        <v>656250</v>
       </c>
     </row>
     <row r="41" spans="2:83" x14ac:dyDescent="0.2">
@@ -5505,27 +5525,27 @@
       </c>
       <c r="V41" s="38">
         <f t="shared" si="21"/>
-        <v>-454663.33698683034</v>
+        <v>-525000</v>
       </c>
       <c r="W41" s="38">
         <f t="shared" si="21"/>
-        <v>164.06249999999991</v>
+        <v>-2.0100091838344547E-14</v>
       </c>
       <c r="X41" s="38">
         <f t="shared" si="21"/>
-        <v>328124.99999999983</v>
+        <v>-4.0200183676689094E-11</v>
       </c>
       <c r="Y41" s="38">
         <f t="shared" si="21"/>
-        <v>454663.33698683034</v>
+        <v>525000</v>
       </c>
       <c r="Z41" s="38">
         <f t="shared" si="21"/>
-        <v>-164.06249999999991</v>
+        <v>2.0100091838344547E-14</v>
       </c>
       <c r="AA41" s="38">
         <f t="shared" si="21"/>
-        <v>328124.99999999983</v>
+        <v>-4.0200183676689094E-11</v>
       </c>
       <c r="AJ41" s="2" t="s">
         <v>38</v>
@@ -5642,27 +5662,27 @@
       </c>
       <c r="AK43" s="11">
         <f>AK6+BA6+AK22</f>
-        <v>131496.09374999988</v>
+        <v>328.125</v>
       </c>
       <c r="AL43" s="11">
         <f t="shared" ref="AL43:AV43" si="22">AL6+BB6+AL22</f>
-        <v>-227189.58620060666</v>
+        <v>3.2140046849512931E-11</v>
       </c>
       <c r="AM43" s="11">
         <f t="shared" si="22"/>
-        <v>-568329.17123353796</v>
+        <v>-656250</v>
       </c>
       <c r="AN43" s="11">
         <f t="shared" si="22"/>
-        <v>-131496.09374999988</v>
+        <v>-328.125</v>
       </c>
       <c r="AO43" s="11">
         <f t="shared" si="22"/>
-        <v>227189.58620060666</v>
+        <v>-3.2140046849512931E-11</v>
       </c>
       <c r="AP43" s="11">
         <f t="shared" si="22"/>
-        <v>-568329.17123353796</v>
+        <v>-656250</v>
       </c>
       <c r="AQ43" s="7">
         <f t="shared" si="22"/>
@@ -5693,7 +5713,7 @@
       </c>
       <c r="AZ43" s="3">
         <f>AX6+BN6+AX22</f>
-        <v>-18105.508075688773</v>
+        <v>-20000</v>
       </c>
       <c r="BA43" s="148" t="s">
         <v>55</v>
@@ -5709,27 +5729,27 @@
       </c>
       <c r="AK44" s="11">
         <f t="shared" ref="AK44:AK54" si="23">AK7+BA7+AK23</f>
-        <v>-227189.58620060669</v>
+        <v>3.2140046849512931E-11</v>
       </c>
       <c r="AL44" s="11">
         <f t="shared" ref="AL44:AL54" si="24">AL7+BB7+AL23</f>
-        <v>393832.03125000006</v>
+        <v>525000</v>
       </c>
       <c r="AM44" s="11">
         <f t="shared" ref="AM44:AM54" si="25">AM7+BC7+AM23</f>
-        <v>-328124.99999999983</v>
+        <v>4.0200183676689094E-11</v>
       </c>
       <c r="AN44" s="11">
         <f t="shared" ref="AN44:AN54" si="26">AN7+BD7+AN23</f>
-        <v>227189.58620060669</v>
+        <v>-3.2140046849512931E-11</v>
       </c>
       <c r="AO44" s="11">
         <f t="shared" ref="AO44:AO54" si="27">AO7+BE7+AO23</f>
-        <v>-393832.03125000006</v>
+        <v>-525000</v>
       </c>
       <c r="AP44" s="11">
         <f t="shared" ref="AP44:AP54" si="28">AP7+BF7+AP23</f>
-        <v>-328124.99999999983</v>
+        <v>4.0200183676689094E-11</v>
       </c>
       <c r="AQ44" s="7">
         <f t="shared" ref="AQ44:AQ54" si="29">AQ7+BG7+AQ23</f>
@@ -5760,7 +5780,7 @@
       </c>
       <c r="AZ44" s="3">
         <f t="shared" ref="AZ44:AZ54" si="35">AX7+BN7+AX23</f>
-        <v>-8640.3401160584272</v>
+        <v>1570.0000000000011</v>
       </c>
       <c r="BA44" s="148" t="s">
         <v>54</v>
@@ -5769,11 +5789,11 @@
     <row r="45" spans="2:83" x14ac:dyDescent="0.2">
       <c r="B45" s="41">
         <f>$C$5</f>
-        <v>-0.49999999999999978</v>
+        <v>6.1257422745431001E-17</v>
       </c>
       <c r="C45" s="41">
         <f>$E$5</f>
-        <v>0.86602540378443871</v>
+        <v>1</v>
       </c>
       <c r="D45" s="41">
         <v>0</v>
@@ -5799,11 +5819,11 @@
       </c>
       <c r="AK45" s="11">
         <f t="shared" si="23"/>
-        <v>-568329.17123353796</v>
+        <v>-656250</v>
       </c>
       <c r="AL45" s="11">
         <f t="shared" si="24"/>
-        <v>-328124.99999999983</v>
+        <v>4.0200183676689094E-11</v>
       </c>
       <c r="AM45" s="11">
         <f t="shared" si="25"/>
@@ -5811,11 +5831,11 @@
       </c>
       <c r="AN45" s="11">
         <f t="shared" si="26"/>
-        <v>568329.17123353796</v>
+        <v>656250</v>
       </c>
       <c r="AO45" s="11">
         <f t="shared" si="27"/>
-        <v>328124.99999999983</v>
+        <v>-4.0200183676689094E-11</v>
       </c>
       <c r="AP45" s="11">
         <f t="shared" si="28"/>
@@ -5856,11 +5876,11 @@
     <row r="46" spans="2:83" x14ac:dyDescent="0.2">
       <c r="B46" s="41">
         <f>-$E$5</f>
-        <v>-0.86602540378443871</v>
+        <v>-1</v>
       </c>
       <c r="C46" s="41">
         <f>$C$5</f>
-        <v>-0.49999999999999978</v>
+        <v>6.1257422745431001E-17</v>
       </c>
       <c r="D46" s="41">
         <v>0</v>
@@ -5896,11 +5916,11 @@
       </c>
       <c r="V46" s="41">
         <f>$C$5</f>
-        <v>-0.49999999999999978</v>
+        <v>6.1257422745431001E-17</v>
       </c>
       <c r="W46" s="41">
         <f>$E$5</f>
-        <v>0.86602540378443871</v>
+        <v>1</v>
       </c>
       <c r="X46" s="41">
         <v>0</v>
@@ -5920,27 +5940,27 @@
       </c>
       <c r="AK46" s="11">
         <f t="shared" si="23"/>
-        <v>-131496.09374999988</v>
+        <v>-328.125</v>
       </c>
       <c r="AL46" s="11">
         <f t="shared" si="24"/>
-        <v>227189.58620060666</v>
+        <v>-3.2140046849512931E-11</v>
       </c>
       <c r="AM46" s="11">
         <f t="shared" si="25"/>
-        <v>568329.17123353796</v>
+        <v>656250</v>
       </c>
       <c r="AN46" s="18">
         <f t="shared" si="26"/>
-        <v>831496.09374999988</v>
+        <v>700328.125</v>
       </c>
       <c r="AO46" s="18">
         <f t="shared" si="27"/>
-        <v>-227189.58620060666</v>
+        <v>3.2140046849512931E-11</v>
       </c>
       <c r="AP46" s="18">
         <f t="shared" si="28"/>
-        <v>568329.17123353796</v>
+        <v>656250</v>
       </c>
       <c r="AQ46" s="16">
         <f t="shared" si="29"/>
@@ -5971,7 +5991,7 @@
       </c>
       <c r="AZ46" s="3">
         <f t="shared" si="35"/>
-        <v>-18105.508075688773</v>
+        <v>-20000</v>
       </c>
       <c r="CE46" s="2"/>
     </row>
@@ -6016,11 +6036,11 @@
       </c>
       <c r="V47" s="41">
         <f>-$E$5</f>
-        <v>-0.86602540378443871</v>
+        <v>-1</v>
       </c>
       <c r="W47" s="41">
         <f>$C$5</f>
-        <v>-0.49999999999999978</v>
+        <v>6.1257422745431001E-17</v>
       </c>
       <c r="X47" s="41">
         <v>0</v>
@@ -6040,27 +6060,27 @@
       </c>
       <c r="AK47" s="11">
         <f t="shared" si="23"/>
-        <v>227189.58620060669</v>
+        <v>-3.2140046849512931E-11</v>
       </c>
       <c r="AL47" s="11">
         <f t="shared" si="24"/>
-        <v>-393832.03125000006</v>
+        <v>-525000</v>
       </c>
       <c r="AM47" s="11">
         <f t="shared" si="25"/>
-        <v>328124.99999999983</v>
+        <v>-4.0200183676689094E-11</v>
       </c>
       <c r="AN47" s="18">
         <f t="shared" si="26"/>
-        <v>-227189.58620060669</v>
+        <v>3.2140046849512931E-11</v>
       </c>
       <c r="AO47" s="18">
         <f t="shared" si="27"/>
-        <v>394609.80902777781</v>
+        <v>525777.77777777775</v>
       </c>
       <c r="AP47" s="18">
         <f t="shared" si="28"/>
-        <v>2661458.3333333335</v>
+        <v>2333333.3333333335</v>
       </c>
       <c r="AQ47" s="16">
         <f t="shared" si="29"/>
@@ -6091,7 +6111,7 @@
       </c>
       <c r="AZ47" s="3">
         <f>AX10+BN10+AX26</f>
-        <v>26069.659883941575</v>
+        <v>36280</v>
       </c>
       <c r="BS47" s="3"/>
       <c r="CE47" s="2"/>
@@ -6108,11 +6128,11 @@
       </c>
       <c r="E48" s="41">
         <f>$C$5</f>
-        <v>-0.49999999999999978</v>
+        <v>6.1257422745431001E-17</v>
       </c>
       <c r="F48" s="41">
         <f>$E$5</f>
-        <v>0.86602540378443871</v>
+        <v>1</v>
       </c>
       <c r="G48" s="41">
         <v>0</v>
@@ -6159,11 +6179,11 @@
       </c>
       <c r="AK48" s="11">
         <f t="shared" si="23"/>
-        <v>-568329.17123353796</v>
+        <v>-656250</v>
       </c>
       <c r="AL48" s="11">
         <f t="shared" si="24"/>
-        <v>-328124.99999999983</v>
+        <v>4.0200183676689094E-11</v>
       </c>
       <c r="AM48" s="11">
         <f t="shared" si="25"/>
@@ -6171,11 +6191,11 @@
       </c>
       <c r="AN48" s="18">
         <f t="shared" si="26"/>
-        <v>568329.17123353796</v>
+        <v>656250</v>
       </c>
       <c r="AO48" s="18">
         <f t="shared" si="27"/>
-        <v>2661458.3333333335</v>
+        <v>2333333.3333333335</v>
       </c>
       <c r="AP48" s="18">
         <f t="shared" si="28"/>
@@ -6225,11 +6245,11 @@
       </c>
       <c r="E49" s="41">
         <f>-$E$5</f>
-        <v>-0.86602540378443871</v>
+        <v>-1</v>
       </c>
       <c r="F49" s="41">
         <f>$C$5</f>
-        <v>-0.49999999999999978</v>
+        <v>6.1257422745431001E-17</v>
       </c>
       <c r="G49" s="41">
         <v>0</v>
@@ -6265,11 +6285,11 @@
       </c>
       <c r="Y49" s="41">
         <f>$C$5</f>
-        <v>-0.49999999999999978</v>
+        <v>6.1257422745431001E-17</v>
       </c>
       <c r="Z49" s="41">
         <f>$E$5</f>
-        <v>0.86602540378443871</v>
+        <v>1</v>
       </c>
       <c r="AA49" s="41">
         <v>0</v>
@@ -6306,34 +6326,34 @@
       </c>
       <c r="AQ49" s="17">
         <f t="shared" si="29"/>
-        <v>131496.09374999988</v>
+        <v>328.125</v>
       </c>
       <c r="AR49" s="20">
         <f t="shared" si="30"/>
-        <v>-227189.58620060666</v>
+        <v>3.2140046849512931E-11</v>
       </c>
       <c r="AS49" s="20">
         <f t="shared" si="31"/>
-        <v>-568329.17123353796</v>
+        <v>-656250</v>
       </c>
       <c r="AT49" s="20">
         <f t="shared" si="32"/>
-        <v>-131496.09374999988</v>
+        <v>-328.125</v>
       </c>
       <c r="AU49" s="17">
         <f t="shared" si="33"/>
-        <v>227189.58620060666</v>
+        <v>-3.2140046849512931E-11</v>
       </c>
       <c r="AV49" s="17">
         <f t="shared" si="34"/>
-        <v>-568329.17123353796</v>
+        <v>-656250</v>
       </c>
       <c r="AX49" s="4">
         <v>0</v>
       </c>
       <c r="AZ49" s="3">
         <f t="shared" si="35"/>
-        <v>16535.508075688773</v>
+        <v>20000</v>
       </c>
       <c r="BA49" s="148" t="s">
         <v>56</v>
@@ -6391,11 +6411,11 @@
       </c>
       <c r="Y50" s="41">
         <f>-$E$5</f>
-        <v>-0.86602540378443871</v>
+        <v>-1</v>
       </c>
       <c r="Z50" s="41">
         <f>$C$5</f>
-        <v>-0.49999999999999978</v>
+        <v>6.1257422745431001E-17</v>
       </c>
       <c r="AA50" s="41">
         <v>0</v>
@@ -6432,34 +6452,34 @@
       </c>
       <c r="AQ50" s="20">
         <f t="shared" si="29"/>
-        <v>-227189.58620060669</v>
+        <v>3.2140046849512931E-11</v>
       </c>
       <c r="AR50" s="17">
         <f t="shared" si="30"/>
-        <v>393832.03125000006</v>
+        <v>525000</v>
       </c>
       <c r="AS50" s="17">
         <f t="shared" si="31"/>
-        <v>-328124.99999999983</v>
+        <v>4.0200183676689094E-11</v>
       </c>
       <c r="AT50" s="17">
         <f t="shared" si="32"/>
-        <v>227189.58620060669</v>
+        <v>-3.2140046849512931E-11</v>
       </c>
       <c r="AU50" s="17">
         <f t="shared" si="33"/>
-        <v>-393832.03125000006</v>
+        <v>-525000</v>
       </c>
       <c r="AV50" s="17">
         <f t="shared" si="34"/>
-        <v>-328124.99999999983</v>
+        <v>4.0200183676689094E-11</v>
       </c>
       <c r="AX50" s="4">
         <v>0</v>
       </c>
       <c r="AZ50" s="3">
         <f t="shared" si="35"/>
-        <v>11359.659883941566</v>
+        <v>1569.9999999999989</v>
       </c>
       <c r="BA50" s="148" t="s">
         <v>57</v>
@@ -6539,11 +6559,11 @@
       </c>
       <c r="AQ51" s="20">
         <f t="shared" si="29"/>
-        <v>-568329.17123353796</v>
+        <v>-656250</v>
       </c>
       <c r="AR51" s="17">
         <f t="shared" si="30"/>
-        <v>-328124.99999999983</v>
+        <v>4.0200183676689094E-11</v>
       </c>
       <c r="AS51" s="17">
         <f t="shared" si="31"/>
@@ -6551,11 +6571,11 @@
       </c>
       <c r="AT51" s="17">
         <f t="shared" si="32"/>
-        <v>568329.17123353796</v>
+        <v>656250</v>
       </c>
       <c r="AU51" s="17">
         <f t="shared" si="33"/>
-        <v>328124.99999999983</v>
+        <v>-4.0200183676689094E-11</v>
       </c>
       <c r="AV51" s="17">
         <f t="shared" si="34"/>
@@ -6614,34 +6634,34 @@
       </c>
       <c r="AQ52" s="20">
         <f t="shared" si="29"/>
-        <v>-131496.09374999988</v>
+        <v>-328.125</v>
       </c>
       <c r="AR52" s="17">
         <f t="shared" si="30"/>
-        <v>227189.58620060666</v>
+        <v>-3.2140046849512931E-11</v>
       </c>
       <c r="AS52" s="17">
         <f t="shared" si="31"/>
-        <v>568329.17123353796</v>
+        <v>656250</v>
       </c>
       <c r="AT52" s="21">
         <f t="shared" si="32"/>
-        <v>831496.09374999988</v>
+        <v>700328.125</v>
       </c>
       <c r="AU52" s="21">
         <f t="shared" si="33"/>
-        <v>-227189.58620060666</v>
+        <v>3.2140046849512931E-11</v>
       </c>
       <c r="AV52" s="21">
         <f t="shared" si="34"/>
-        <v>568329.17123353796</v>
+        <v>656250</v>
       </c>
       <c r="AX52" s="4" t="s">
         <v>47</v>
       </c>
       <c r="AZ52" s="3">
         <f t="shared" si="35"/>
-        <v>16535.508075688773</v>
+        <v>20000</v>
       </c>
       <c r="BB52" s="12"/>
       <c r="BE52" s="16"/>
@@ -6692,34 +6712,34 @@
       </c>
       <c r="AQ53" s="17">
         <f t="shared" si="29"/>
-        <v>227189.58620060669</v>
+        <v>-3.2140046849512931E-11</v>
       </c>
       <c r="AR53" s="17">
         <f t="shared" si="30"/>
-        <v>-393832.03125000006</v>
+        <v>-525000</v>
       </c>
       <c r="AS53" s="17">
         <f t="shared" si="31"/>
-        <v>328124.99999999983</v>
+        <v>-4.0200183676689094E-11</v>
       </c>
       <c r="AT53" s="21">
         <f t="shared" si="32"/>
-        <v>-227189.58620060669</v>
+        <v>3.2140046849512931E-11</v>
       </c>
       <c r="AU53" s="21">
         <f t="shared" si="33"/>
-        <v>394609.80902777781</v>
+        <v>525777.77777777775</v>
       </c>
       <c r="AV53" s="21">
         <f t="shared" si="34"/>
-        <v>-2005208.3333333337</v>
+        <v>-2333333.3333333335</v>
       </c>
       <c r="AX53" s="4" t="s">
         <v>48</v>
       </c>
       <c r="AZ53" s="3">
         <f t="shared" si="35"/>
-        <v>46069.659883941567</v>
+        <v>36280</v>
       </c>
       <c r="BB53" s="12"/>
       <c r="BE53" s="16"/>
@@ -6742,11 +6762,11 @@
     <row r="54" spans="2:101" x14ac:dyDescent="0.2">
       <c r="B54" s="41">
         <f>$C$5</f>
-        <v>-0.49999999999999978</v>
+        <v>6.1257422745431001E-17</v>
       </c>
       <c r="C54" s="41">
         <f>-$E$5</f>
-        <v>-0.86602540378443871</v>
+        <v>-1</v>
       </c>
       <c r="D54" s="41">
         <v>0</v>
@@ -6798,11 +6818,11 @@
       </c>
       <c r="AQ54" s="17">
         <f t="shared" si="29"/>
-        <v>-568329.17123353796</v>
+        <v>-656250</v>
       </c>
       <c r="AR54" s="17">
         <f t="shared" si="30"/>
-        <v>-328124.99999999983</v>
+        <v>4.0200183676689094E-11</v>
       </c>
       <c r="AS54" s="17">
         <f t="shared" si="31"/>
@@ -6810,11 +6830,11 @@
       </c>
       <c r="AT54" s="21">
         <f t="shared" si="32"/>
-        <v>568329.17123353796</v>
+        <v>656250</v>
       </c>
       <c r="AU54" s="21">
         <f t="shared" si="33"/>
-        <v>-2005208.3333333337</v>
+        <v>-2333333.3333333335</v>
       </c>
       <c r="AV54" s="21">
         <f t="shared" si="34"/>
@@ -6843,11 +6863,11 @@
     <row r="55" spans="2:101" x14ac:dyDescent="0.2">
       <c r="B55" s="41">
         <f>$E$5</f>
-        <v>0.86602540378443871</v>
+        <v>1</v>
       </c>
       <c r="C55" s="41">
         <f>$C$5</f>
-        <v>-0.49999999999999978</v>
+        <v>6.1257422745431001E-17</v>
       </c>
       <c r="D55" s="41">
         <v>0</v>
@@ -6883,11 +6903,11 @@
       </c>
       <c r="V55" s="41">
         <f>$C$5</f>
-        <v>-0.49999999999999978</v>
+        <v>6.1257422745431001E-17</v>
       </c>
       <c r="W55" s="41">
         <f>-$E$5</f>
-        <v>-0.86602540378443871</v>
+        <v>-1</v>
       </c>
       <c r="X55" s="41">
         <v>0</v>
@@ -6960,11 +6980,11 @@
       </c>
       <c r="V56" s="41">
         <f>$E$5</f>
-        <v>0.86602540378443871</v>
+        <v>1</v>
       </c>
       <c r="W56" s="41">
         <f>$C$5</f>
-        <v>-0.49999999999999978</v>
+        <v>6.1257422745431001E-17</v>
       </c>
       <c r="X56" s="41">
         <v>0</v>
@@ -7007,11 +7027,11 @@
       </c>
       <c r="E57" s="41">
         <f>$C$5</f>
-        <v>-0.49999999999999978</v>
+        <v>6.1257422745431001E-17</v>
       </c>
       <c r="F57" s="41">
         <f>-$E$5</f>
-        <v>-0.86602540378443871</v>
+        <v>-1</v>
       </c>
       <c r="G57" s="41">
         <v>0</v>
@@ -7071,11 +7091,11 @@
       </c>
       <c r="E58" s="41">
         <f>$E$5</f>
-        <v>0.86602540378443871</v>
+        <v>1</v>
       </c>
       <c r="F58" s="41">
         <f>$C$5</f>
-        <v>-0.49999999999999978</v>
+        <v>6.1257422745431001E-17</v>
       </c>
       <c r="G58" s="41">
         <v>0</v>
@@ -7111,11 +7131,11 @@
       </c>
       <c r="Y58" s="41">
         <f>$C$5</f>
-        <v>-0.49999999999999978</v>
+        <v>6.1257422745431001E-17</v>
       </c>
       <c r="Z58" s="41">
         <f>-$E$5</f>
-        <v>-0.86602540378443871</v>
+        <v>-1</v>
       </c>
       <c r="AA58" s="41">
         <v>0</v>
@@ -7184,11 +7204,11 @@
       </c>
       <c r="Y59" s="41">
         <f>$E$5</f>
-        <v>0.86602540378443871</v>
+        <v>1</v>
       </c>
       <c r="Z59" s="41">
         <f>$C$5</f>
-        <v>-0.49999999999999978</v>
+        <v>6.1257422745431001E-17</v>
       </c>
       <c r="AA59" s="41">
         <v>0</v>
@@ -7293,10 +7313,10 @@
         <v>1750000000</v>
       </c>
       <c r="AL60" s="3">
-        <v>568329.17123353796</v>
+        <v>656250</v>
       </c>
       <c r="AM60" s="3">
-        <v>328124.99999999983</v>
+        <v>-4.0200183676689094E-11</v>
       </c>
       <c r="AN60" s="3">
         <v>875000000</v>
@@ -7344,16 +7364,16 @@
         <v>4</v>
       </c>
       <c r="AK61" s="3">
-        <v>568329.17123353796</v>
+        <v>656250</v>
       </c>
       <c r="AL61" s="3">
-        <v>831496.09374999988</v>
+        <v>700328.125</v>
       </c>
       <c r="AM61" s="3">
-        <v>-227189.58620060666</v>
+        <v>3.2140046849512931E-11</v>
       </c>
       <c r="AN61" s="3">
-        <v>568329.17123353796</v>
+        <v>656250</v>
       </c>
       <c r="AO61" s="3">
         <v>0</v>
@@ -7373,7 +7393,7 @@
         <v>r21</v>
       </c>
       <c r="AV61" s="146">
-        <v>-18105.508075688773</v>
+        <v>-20000</v>
       </c>
       <c r="BA61" s="4"/>
       <c r="BB61" s="12"/>
@@ -7416,16 +7436,16 @@
         <v>5</v>
       </c>
       <c r="AK62" s="3">
-        <v>328124.99999999983</v>
+        <v>-4.0200183676689094E-11</v>
       </c>
       <c r="AL62" s="3">
-        <v>-227189.58620060669</v>
+        <v>3.2140046849512931E-11</v>
       </c>
       <c r="AM62" s="3">
-        <v>394609.80902777781</v>
+        <v>525777.77777777775</v>
       </c>
       <c r="AN62" s="3">
-        <v>2661458.3333333335</v>
+        <v>2333333.3333333335</v>
       </c>
       <c r="AO62" s="3">
         <v>0</v>
@@ -7445,7 +7465,7 @@
         <v>r22</v>
       </c>
       <c r="AV62" s="146">
-        <v>26069.659883941575</v>
+        <v>36280</v>
       </c>
       <c r="BB62" s="12"/>
       <c r="BE62" s="12"/>
@@ -7486,10 +7506,10 @@
         <v>875000000</v>
       </c>
       <c r="AL63" s="3">
-        <v>568329.17123353796</v>
+        <v>656250</v>
       </c>
       <c r="AM63" s="3">
-        <v>2661458.3333333335</v>
+        <v>2333333.3333333335</v>
       </c>
       <c r="AN63" s="3">
         <v>11083333333.333334</v>
@@ -7530,31 +7550,34 @@
     </row>
     <row r="64" spans="2:101" x14ac:dyDescent="0.2">
       <c r="H64" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I64" s="1">
+        <v>82</v>
+      </c>
+      <c r="I64" s="154">
         <v>10000</v>
       </c>
       <c r="J64" s="1" t="s">
-        <v>10</v>
+        <v>83</v>
       </c>
       <c r="K64" s="1" t="s">
         <v>77</v>
       </c>
       <c r="L64" s="3">
         <f>COS(RADIANS(I65-E4))*I64</f>
-        <v>-4999.9999999999982</v>
+        <v>6.1257422745431001E-13</v>
       </c>
       <c r="M64" s="34" t="s">
         <v>66</v>
       </c>
       <c r="N64" s="27">
         <f>-I67/E6*L64</f>
-        <v>2499.9999999999991</v>
+        <v>-3.06287113727155E-13</v>
       </c>
       <c r="O64" s="27">
         <f>-I66/E6*L64</f>
-        <v>2499.9999999999991</v>
+        <v>-3.06287113727155E-13</v>
+      </c>
+      <c r="P64" s="1" t="s">
+        <v>86</v>
       </c>
       <c r="AJ64" s="9"/>
       <c r="AK64" s="9"/>
@@ -7583,7 +7606,7 @@
       <c r="H65" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="I65" s="1">
+      <c r="I65" s="154">
         <v>0</v>
       </c>
       <c r="J65" s="1" t="s">
@@ -7594,18 +7617,21 @@
       </c>
       <c r="L65" s="3">
         <f>SIN(RADIANS(I65-E4))*I64</f>
-        <v>-8660.2540378443864</v>
+        <v>-10000</v>
       </c>
       <c r="M65" s="34" t="s">
         <v>67</v>
       </c>
       <c r="N65" s="27">
-        <f>I67^2*(3*I66+I67)/E6^3*L65</f>
-        <v>-4330.1270189221932</v>
+        <f>-1*I67^2*(3*I66+I67)/E6^3*L65</f>
+        <v>5000</v>
       </c>
       <c r="O65" s="27">
-        <f>I66^2*(I66+3*I67)/E6^3*L65</f>
-        <v>-4330.1270189221932</v>
+        <f>-1*I66^2*(I66+3*I67)/E6^3*L65</f>
+        <v>5000</v>
+      </c>
+      <c r="P65" s="1" t="s">
+        <v>87</v>
       </c>
       <c r="AJ65" s="9">
         <v>3</v>
@@ -7659,7 +7685,7 @@
       <c r="H66" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="I66" s="1">
+      <c r="I66" s="154">
         <v>2000</v>
       </c>
       <c r="J66" s="1" t="s">
@@ -7669,12 +7695,12 @@
         <v>68</v>
       </c>
       <c r="N66" s="27">
-        <f>I66*I67^2/E6^2*L65</f>
-        <v>-4330127.018922193</v>
+        <f>-1*I66*I67^2/E6^2*L65</f>
+        <v>5000000</v>
       </c>
       <c r="O66" s="27">
-        <f>-1*I66^2*I67/E6^2*L65</f>
-        <v>4330127.018922193</v>
+        <f>I66^2*I67/E6^2*L65</f>
+        <v>-5000000</v>
       </c>
       <c r="P66" s="1" t="s">
         <v>81</v>
@@ -7707,7 +7733,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="AT66" s="1">
-        <v>-18105.508075688773</v>
+        <v>-20000</v>
       </c>
       <c r="AW66" s="1" t="s">
         <v>3</v>
@@ -7720,7 +7746,7 @@
       <c r="H67" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="I67" s="25">
+      <c r="I67" s="153">
         <f>E6-I66</f>
         <v>2000</v>
       </c>
@@ -7753,7 +7779,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="AT67" s="1">
-        <v>26069.659883941575</v>
+        <v>36280</v>
       </c>
       <c r="AW67" s="1" t="s">
         <v>3</v>
@@ -7761,9 +7787,6 @@
       <c r="BR67" s="66"/>
     </row>
     <row r="68" spans="5:74" x14ac:dyDescent="0.2">
-      <c r="F68" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="H68" s="1" t="s">
         <v>61</v>
       </c>
@@ -7813,8 +7836,19 @@
       <c r="BR68" s="66"/>
     </row>
     <row r="69" spans="5:74" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H69" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="M69" s="34" t="s">
         <v>67</v>
+      </c>
+      <c r="N69" s="1">
+        <f>6*I66*I67/E6^3*I64</f>
+        <v>3.75</v>
+      </c>
+      <c r="O69" s="1">
+        <f>-6*I66*I67/E6^3*I64</f>
+        <v>-3.75</v>
       </c>
       <c r="AJ69" s="9">
         <v>9</v>
@@ -7859,6 +7893,14 @@
       <c r="E70" s="26"/>
       <c r="M70" s="152" t="s">
         <v>68</v>
+      </c>
+      <c r="N70" s="1">
+        <f>I67*(2*I66-I67)/E6^2*I64</f>
+        <v>2500</v>
+      </c>
+      <c r="O70" s="1">
+        <f>I66*(2*I67-I66)/E6^2*I64</f>
+        <v>2500</v>
       </c>
       <c r="AG70" s="2"/>
       <c r="AH70" s="2"/>
@@ -7929,9 +7971,6 @@
       </c>
     </row>
     <row r="72" spans="5:74" ht="12" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F72" s="1" t="s">
-        <v>64</v>
-      </c>
       <c r="H72" s="1" t="s">
         <v>65</v>
       </c>
@@ -7977,6 +8016,9 @@
       </c>
     </row>
     <row r="73" spans="5:74" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H73" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="M73" s="34" t="s">
         <v>67</v>
       </c>
@@ -18153,14 +18195,25 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A31214F-D315-442C-9106-A983B611689D}">
-  <dimension ref="A1"/>
+  <dimension ref="L24:L25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O28" sqref="O28"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="24" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L24" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="25" spans="12:12" x14ac:dyDescent="0.25">
+      <c r="L25" t="s">
+        <v>85</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Implement support for strain and thermal loads
</commit_message>
<xml_diff>
--- a/theory/FEM matriisit.xlsx
+++ b/theory/FEM matriisit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ohjelmointi\2_Rust\idfem\theory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D983DBF-4AE4-4125-93E3-791C25DC504B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{094C6094-8C9E-4147-9A93-651BD2647B12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-22230" yWindow="0" windowWidth="22335" windowHeight="20880" xr2:uid="{27180542-B0D2-4BFE-946B-7857B24C93C8}"/>
   </bookViews>
@@ -403,12 +403,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.000000"/>
     <numFmt numFmtId="166" formatCode="0.000E+00"/>
     <numFmt numFmtId="167" formatCode="0.0"/>
     <numFmt numFmtId="168" formatCode="0.00000"/>
+    <numFmt numFmtId="169" formatCode="0.0000E+00"/>
   </numFmts>
   <fonts count="15" x14ac:knownFonts="1">
     <font>
@@ -689,7 +690,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="155">
+  <cellXfs count="157">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1097,6 +1098,12 @@
     </xf>
     <xf numFmtId="164" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="169" fontId="6" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="2" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutraali" xfId="1" builtinId="28"/>
@@ -1823,7 +1830,7 @@
   <dimension ref="B1:CW227"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -2243,7 +2250,7 @@
       <c r="AW7" s="4"/>
       <c r="AX7" s="3">
         <f t="shared" ref="AX7:AX11" si="1">I21</f>
-        <v>1570.0000000000011</v>
+        <v>1.22514845490862E-12</v>
       </c>
       <c r="AZ7" s="81">
         <v>2</v>
@@ -2622,7 +2629,7 @@
       <c r="AW10" s="4"/>
       <c r="AX10" s="3">
         <f>I24</f>
-        <v>1570.0000000000011</v>
+        <v>1.22514845490862E-12</v>
       </c>
       <c r="AZ10" s="81">
         <v>5</v>
@@ -2671,7 +2678,7 @@
       </c>
       <c r="BM10" s="16"/>
       <c r="BN10" s="1">
-        <v>34710</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="11" spans="2:66" ht="13.5" x14ac:dyDescent="0.2">
@@ -2803,7 +2810,7 @@
       </c>
       <c r="BM11" s="16"/>
       <c r="BN11" s="1">
-        <v>34710000</v>
+        <v>30000000</v>
       </c>
     </row>
     <row r="12" spans="2:66" x14ac:dyDescent="0.2">
@@ -2986,8 +2993,7 @@
         <v>12</v>
       </c>
       <c r="E14" s="14">
-        <f>100*100*7850*10/1000000000</f>
-        <v>0.78500000000000003</v>
+        <v>0</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>59</v>
@@ -2996,8 +3002,7 @@
         <v>12</v>
       </c>
       <c r="O14" s="14">
-        <f>200*100*7850*10/1000000000</f>
-        <v>1.57</v>
+        <v>0</v>
       </c>
       <c r="P14" s="1" t="s">
         <v>59</v>
@@ -3006,8 +3011,7 @@
         <v>12</v>
       </c>
       <c r="Y14" s="14">
-        <f>100*100*7850*10/1000000000</f>
-        <v>0.78500000000000003</v>
+        <v>0</v>
       </c>
       <c r="Z14" s="1" t="s">
         <v>59</v>
@@ -3221,8 +3225,7 @@
         <v>53</v>
       </c>
       <c r="E16" s="14">
-        <f>10*1000</f>
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>10</v>
@@ -3231,8 +3234,7 @@
         <v>53</v>
       </c>
       <c r="O16" s="14">
-        <f>10*1000</f>
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="P16" s="1" t="s">
         <v>10</v>
@@ -3242,8 +3244,7 @@
         <v>53</v>
       </c>
       <c r="Y16" s="14">
-        <f>10*1000</f>
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="Z16" s="1" t="s">
         <v>10</v>
@@ -3336,7 +3337,7 @@
       </c>
       <c r="BM16" s="16"/>
       <c r="BN16" s="12">
-        <v>34710</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="17" spans="2:66" x14ac:dyDescent="0.2">
@@ -3428,7 +3429,7 @@
       </c>
       <c r="BM17" s="16"/>
       <c r="BN17" s="12">
-        <v>-34710000</v>
+        <v>-30000000</v>
       </c>
     </row>
     <row r="18" spans="2:66" x14ac:dyDescent="0.2">
@@ -3532,7 +3533,7 @@
         <f t="shared" si="6"/>
         <v>-656250</v>
       </c>
-      <c r="I20" s="40">
+      <c r="I20" s="155">
         <f>B54*I28+C54*I29+D54*I30+E54*I31+F54*I32+G54*I33</f>
         <v>-20000</v>
       </c>
@@ -3621,9 +3622,9 @@
         <f t="shared" si="6"/>
         <v>4.0200183676689094E-11</v>
       </c>
-      <c r="I21" s="40">
+      <c r="I21" s="155">
         <f>B55*I28+C55*I29+D55*I30+E55*I31+F55*I32+G55*I33</f>
-        <v>1570.0000000000011</v>
+        <v>1.22514845490862E-12</v>
       </c>
       <c r="L21" s="19">
         <f t="shared" si="7"/>
@@ -3651,7 +3652,7 @@
       </c>
       <c r="S21" s="40">
         <f>L56*S28+M56*S29+N56*S30+O56*S31+P56*S32+Q56*S33</f>
-        <v>34710</v>
+        <v>30000</v>
       </c>
       <c r="V21" s="20">
         <f t="shared" si="8"/>
@@ -3679,7 +3680,7 @@
       </c>
       <c r="AC21" s="40">
         <f>V56*AC28+W56*AC29+X56*AC30+Y56*AC31+Z56*AC32+AA56*AC33</f>
-        <v>1569.9999999999989</v>
+        <v>-1.22514845490862E-12</v>
       </c>
       <c r="AJ21" s="9"/>
       <c r="AK21" s="81">
@@ -3748,7 +3749,7 @@
         <f>-1*$B38*G$45+$C38*G$46+$D38*G$47+$E38*G$48+$F38*G$49+$G38*G$50</f>
         <v>875000000</v>
       </c>
-      <c r="I22" s="40">
+      <c r="I22" s="155">
         <f>B56*I28+C56*I29+D56*I30+E56*I31+F56*I32+G56*I33</f>
         <v>13333333.333333334</v>
       </c>
@@ -3778,7 +3779,7 @@
       </c>
       <c r="S22" s="40">
         <f>L57*S28+M57*S29+N57*S30+O57*S31+P57*S32+Q57*S33</f>
-        <v>34710000</v>
+        <v>30000000</v>
       </c>
       <c r="V22" s="20">
         <f t="shared" ref="V22:Z25" si="10">$V39*B$45+$W39*B$46+$X39*B$47+$Y39*B$48+$Z39*B$49+$AA39*B$50</f>
@@ -3874,7 +3875,7 @@
         <f>$B39*G$45+$C39*G$46+$D39*G$47+$E39*G$48+$F39*G$49+$G39*G$50</f>
         <v>656250</v>
       </c>
-      <c r="I23" s="40">
+      <c r="I23" s="155">
         <f>B57*I28+C57*I29+D57*I30+E57*I31+F57*I32+G57*I33</f>
         <v>-20000</v>
       </c>
@@ -4000,9 +4001,9 @@
         <f>$B40*G$45+$C40*G$46+$D40*G$47+$E40*G$48+$F40*G$49+$G40*G$50</f>
         <v>-4.0200183676689094E-11</v>
       </c>
-      <c r="I24" s="40">
+      <c r="I24" s="155">
         <f>B58*I28+C58*I29+D58*I30+E58*I31+F58*I32+G58*I33</f>
-        <v>1570.0000000000011</v>
+        <v>1.22514845490862E-12</v>
       </c>
       <c r="L24" s="19">
         <f t="shared" si="7"/>
@@ -4030,7 +4031,7 @@
       </c>
       <c r="S24" s="40">
         <f>L59*S28+M59*S29+N59*S30+O59*S31+P59*S32+Q59*S33</f>
-        <v>34710</v>
+        <v>30000</v>
       </c>
       <c r="V24" s="20">
         <f t="shared" si="10"/>
@@ -4058,7 +4059,7 @@
       </c>
       <c r="AC24" s="40">
         <f>V59*AC28+W59*AC29+X59*AC30+Y59*AC31+Z59*AC32+AA59*AC33</f>
-        <v>1569.9999999999989</v>
+        <v>-1.22514845490862E-12</v>
       </c>
       <c r="AJ24" s="81">
         <v>3</v>
@@ -4126,7 +4127,7 @@
         <f>$B41*G$45+$C41*G$46+$D41*G$47+$E41*G$48+$F41*G$49+$G41*G$50</f>
         <v>1750000000</v>
       </c>
-      <c r="I25" s="40">
+      <c r="I25" s="155">
         <f>B59*I28+C59*I29+D59*I30+E59*I31+F59*I32+G59*I33</f>
         <v>-13333333.333333334</v>
       </c>
@@ -4157,7 +4158,7 @@
       </c>
       <c r="S25" s="40">
         <f>L60*S28+M60*S29+N60*S30+O60*S31+P60*S32+Q60*S33</f>
-        <v>-34710000</v>
+        <v>-30000000</v>
       </c>
       <c r="U25" s="2"/>
       <c r="V25" s="20">
@@ -4362,7 +4363,7 @@
       </c>
       <c r="I28" s="38">
         <f>E6/2*E14</f>
-        <v>1570</v>
+        <v>0</v>
       </c>
       <c r="L28" s="38">
         <f>$O$10/O6</f>
@@ -4409,7 +4410,7 @@
       </c>
       <c r="AC28" s="38">
         <f>Y6/2*Y14</f>
-        <v>1570</v>
+        <v>0</v>
       </c>
       <c r="AJ28" s="81">
         <v>7</v>
@@ -4514,7 +4515,7 @@
       </c>
       <c r="S29" s="38">
         <f>O6/2*(O14+O15)</f>
-        <v>34710</v>
+        <v>30000</v>
       </c>
       <c r="V29" s="39">
         <v>0</v>
@@ -4590,7 +4591,7 @@
       <c r="AW29" s="4"/>
       <c r="AX29" s="3">
         <f t="shared" ref="AX29:AX33" si="12">AC21</f>
-        <v>1569.9999999999989</v>
+        <v>-1.22514845490862E-12</v>
       </c>
       <c r="AY29" s="10"/>
     </row>
@@ -4645,7 +4646,7 @@
       </c>
       <c r="S30" s="38">
         <f>1*((O14+O15)*O6^2)/12</f>
-        <v>34710000</v>
+        <v>30000000</v>
       </c>
       <c r="V30" s="39">
         <v>0</v>
@@ -4748,7 +4749,7 @@
       </c>
       <c r="I31" s="38">
         <f>E6/2*E14</f>
-        <v>1570</v>
+        <v>0</v>
       </c>
       <c r="L31" s="38">
         <f>-$O$10/O6</f>
@@ -4795,7 +4796,7 @@
       </c>
       <c r="AC31" s="38">
         <f>Y6/2*Y14</f>
-        <v>1570</v>
+        <v>0</v>
       </c>
       <c r="AJ31" s="81">
         <v>10</v>
@@ -4901,7 +4902,7 @@
       <c r="R32" s="2"/>
       <c r="S32" s="38">
         <f>O6/2*(O14+O15)</f>
-        <v>34710</v>
+        <v>30000</v>
       </c>
       <c r="V32" s="39">
         <v>0</v>
@@ -4977,7 +4978,7 @@
       <c r="AW32" s="4"/>
       <c r="AX32" s="3">
         <f t="shared" si="12"/>
-        <v>1569.9999999999989</v>
+        <v>-1.22514845490862E-12</v>
       </c>
       <c r="AY32" s="10"/>
     </row>
@@ -5032,7 +5033,7 @@
       </c>
       <c r="S33" s="38">
         <f>-1*((O14+O15)*O6^2)/12</f>
-        <v>-34710000</v>
+        <v>-30000000</v>
       </c>
       <c r="V33" s="39">
         <v>0</v>
@@ -5780,31 +5781,31 @@
       </c>
       <c r="AZ44" s="3">
         <f t="shared" ref="AZ44:AZ54" si="35">AX7+BN7+AX23</f>
-        <v>1570.0000000000011</v>
+        <v>1.22514845490862E-12</v>
       </c>
       <c r="BA44" s="148" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="45" spans="2:83" x14ac:dyDescent="0.2">
-      <c r="B45" s="41">
+      <c r="B45" s="156">
         <f>$C$5</f>
         <v>6.1257422745431001E-17</v>
       </c>
-      <c r="C45" s="41">
+      <c r="C45" s="156">
         <f>$E$5</f>
         <v>1</v>
       </c>
-      <c r="D45" s="41">
-        <v>0</v>
-      </c>
-      <c r="E45" s="41">
-        <v>0</v>
-      </c>
-      <c r="F45" s="41">
-        <v>0</v>
-      </c>
-      <c r="G45" s="41">
+      <c r="D45" s="156">
+        <v>0</v>
+      </c>
+      <c r="E45" s="156">
+        <v>0</v>
+      </c>
+      <c r="F45" s="156">
+        <v>0</v>
+      </c>
+      <c r="G45" s="156">
         <v>0</v>
       </c>
       <c r="L45" s="2" t="s">
@@ -5874,64 +5875,64 @@
       </c>
     </row>
     <row r="46" spans="2:83" x14ac:dyDescent="0.2">
-      <c r="B46" s="41">
+      <c r="B46" s="156">
         <f>-$E$5</f>
         <v>-1</v>
       </c>
-      <c r="C46" s="41">
+      <c r="C46" s="156">
         <f>$C$5</f>
         <v>6.1257422745431001E-17</v>
       </c>
-      <c r="D46" s="41">
-        <v>0</v>
-      </c>
-      <c r="E46" s="41">
-        <v>0</v>
-      </c>
-      <c r="F46" s="41">
-        <v>0</v>
-      </c>
-      <c r="G46" s="41">
-        <v>0</v>
-      </c>
-      <c r="L46" s="41">
+      <c r="D46" s="156">
+        <v>0</v>
+      </c>
+      <c r="E46" s="156">
+        <v>0</v>
+      </c>
+      <c r="F46" s="156">
+        <v>0</v>
+      </c>
+      <c r="G46" s="156">
+        <v>0</v>
+      </c>
+      <c r="L46" s="156">
         <f>$M$5</f>
         <v>1</v>
       </c>
-      <c r="M46" s="41">
+      <c r="M46" s="156">
         <f>$O$5</f>
         <v>0</v>
       </c>
-      <c r="N46" s="41">
-        <v>0</v>
-      </c>
-      <c r="O46" s="41">
-        <v>0</v>
-      </c>
-      <c r="P46" s="41">
-        <v>0</v>
-      </c>
-      <c r="Q46" s="41">
-        <v>0</v>
-      </c>
-      <c r="V46" s="41">
+      <c r="N46" s="156">
+        <v>0</v>
+      </c>
+      <c r="O46" s="156">
+        <v>0</v>
+      </c>
+      <c r="P46" s="156">
+        <v>0</v>
+      </c>
+      <c r="Q46" s="156">
+        <v>0</v>
+      </c>
+      <c r="V46" s="156">
         <f>$C$5</f>
         <v>6.1257422745431001E-17</v>
       </c>
-      <c r="W46" s="41">
+      <c r="W46" s="156">
         <f>$E$5</f>
         <v>1</v>
       </c>
-      <c r="X46" s="41">
-        <v>0</v>
-      </c>
-      <c r="Y46" s="41">
-        <v>0</v>
-      </c>
-      <c r="Z46" s="41">
-        <v>0</v>
-      </c>
-      <c r="AA46" s="41">
+      <c r="X46" s="156">
+        <v>0</v>
+      </c>
+      <c r="Y46" s="156">
+        <v>0</v>
+      </c>
+      <c r="Z46" s="156">
+        <v>0</v>
+      </c>
+      <c r="AA46" s="156">
         <v>0</v>
       </c>
       <c r="AE46" s="10"/>
@@ -5996,62 +5997,62 @@
       <c r="CE46" s="2"/>
     </row>
     <row r="47" spans="2:83" x14ac:dyDescent="0.2">
-      <c r="B47" s="41">
-        <v>0</v>
-      </c>
-      <c r="C47" s="41">
-        <v>0</v>
-      </c>
-      <c r="D47" s="41">
+      <c r="B47" s="156">
+        <v>0</v>
+      </c>
+      <c r="C47" s="156">
+        <v>0</v>
+      </c>
+      <c r="D47" s="156">
         <v>1</v>
       </c>
-      <c r="E47" s="41">
-        <v>0</v>
-      </c>
-      <c r="F47" s="41">
-        <v>0</v>
-      </c>
-      <c r="G47" s="41">
-        <v>0</v>
-      </c>
-      <c r="L47" s="41">
+      <c r="E47" s="156">
+        <v>0</v>
+      </c>
+      <c r="F47" s="156">
+        <v>0</v>
+      </c>
+      <c r="G47" s="156">
+        <v>0</v>
+      </c>
+      <c r="L47" s="156">
         <f>-$O$5</f>
         <v>0</v>
       </c>
-      <c r="M47" s="41">
+      <c r="M47" s="156">
         <f>$M$5</f>
         <v>1</v>
       </c>
-      <c r="N47" s="41">
-        <v>0</v>
-      </c>
-      <c r="O47" s="41">
-        <v>0</v>
-      </c>
-      <c r="P47" s="41">
-        <v>0</v>
-      </c>
-      <c r="Q47" s="41">
-        <v>0</v>
-      </c>
-      <c r="V47" s="41">
+      <c r="N47" s="156">
+        <v>0</v>
+      </c>
+      <c r="O47" s="156">
+        <v>0</v>
+      </c>
+      <c r="P47" s="156">
+        <v>0</v>
+      </c>
+      <c r="Q47" s="156">
+        <v>0</v>
+      </c>
+      <c r="V47" s="156">
         <f>-$E$5</f>
         <v>-1</v>
       </c>
-      <c r="W47" s="41">
+      <c r="W47" s="156">
         <f>$C$5</f>
         <v>6.1257422745431001E-17</v>
       </c>
-      <c r="X47" s="41">
-        <v>0</v>
-      </c>
-      <c r="Y47" s="41">
-        <v>0</v>
-      </c>
-      <c r="Z47" s="41">
-        <v>0</v>
-      </c>
-      <c r="AA47" s="41">
+      <c r="X47" s="156">
+        <v>0</v>
+      </c>
+      <c r="Y47" s="156">
+        <v>0</v>
+      </c>
+      <c r="Z47" s="156">
+        <v>0</v>
+      </c>
+      <c r="AA47" s="156">
         <v>0</v>
       </c>
       <c r="AE47" s="8"/>
@@ -6111,66 +6112,66 @@
       </c>
       <c r="AZ47" s="3">
         <f>AX10+BN10+AX26</f>
-        <v>36280</v>
+        <v>30000</v>
       </c>
       <c r="BS47" s="3"/>
       <c r="CE47" s="2"/>
     </row>
     <row r="48" spans="2:83" x14ac:dyDescent="0.2">
-      <c r="B48" s="41">
-        <v>0</v>
-      </c>
-      <c r="C48" s="41">
-        <v>0</v>
-      </c>
-      <c r="D48" s="41">
-        <v>0</v>
-      </c>
-      <c r="E48" s="41">
+      <c r="B48" s="156">
+        <v>0</v>
+      </c>
+      <c r="C48" s="156">
+        <v>0</v>
+      </c>
+      <c r="D48" s="156">
+        <v>0</v>
+      </c>
+      <c r="E48" s="156">
         <f>$C$5</f>
         <v>6.1257422745431001E-17</v>
       </c>
-      <c r="F48" s="41">
+      <c r="F48" s="156">
         <f>$E$5</f>
         <v>1</v>
       </c>
-      <c r="G48" s="41">
-        <v>0</v>
-      </c>
-      <c r="L48" s="41">
-        <v>0</v>
-      </c>
-      <c r="M48" s="41">
-        <v>0</v>
-      </c>
-      <c r="N48" s="41">
+      <c r="G48" s="156">
+        <v>0</v>
+      </c>
+      <c r="L48" s="156">
+        <v>0</v>
+      </c>
+      <c r="M48" s="156">
+        <v>0</v>
+      </c>
+      <c r="N48" s="156">
         <v>1</v>
       </c>
-      <c r="O48" s="41">
-        <v>0</v>
-      </c>
-      <c r="P48" s="41">
-        <v>0</v>
-      </c>
-      <c r="Q48" s="41">
-        <v>0</v>
-      </c>
-      <c r="V48" s="41">
-        <v>0</v>
-      </c>
-      <c r="W48" s="41">
-        <v>0</v>
-      </c>
-      <c r="X48" s="41">
+      <c r="O48" s="156">
+        <v>0</v>
+      </c>
+      <c r="P48" s="156">
+        <v>0</v>
+      </c>
+      <c r="Q48" s="156">
+        <v>0</v>
+      </c>
+      <c r="V48" s="156">
+        <v>0</v>
+      </c>
+      <c r="W48" s="156">
+        <v>0</v>
+      </c>
+      <c r="X48" s="156">
         <v>1</v>
       </c>
-      <c r="Y48" s="41">
-        <v>0</v>
-      </c>
-      <c r="Z48" s="41">
-        <v>0</v>
-      </c>
-      <c r="AA48" s="41">
+      <c r="Y48" s="156">
+        <v>0</v>
+      </c>
+      <c r="Z48" s="156">
+        <v>0</v>
+      </c>
+      <c r="AA48" s="156">
         <v>0</v>
       </c>
       <c r="AE48" s="8"/>
@@ -6230,68 +6231,68 @@
       </c>
       <c r="AZ48" s="3">
         <f t="shared" si="35"/>
-        <v>21376666.666666664</v>
+        <v>16666666.666666666</v>
       </c>
     </row>
     <row r="49" spans="2:101" x14ac:dyDescent="0.2">
-      <c r="B49" s="41">
-        <v>0</v>
-      </c>
-      <c r="C49" s="41">
-        <v>0</v>
-      </c>
-      <c r="D49" s="41">
-        <v>0</v>
-      </c>
-      <c r="E49" s="41">
+      <c r="B49" s="156">
+        <v>0</v>
+      </c>
+      <c r="C49" s="156">
+        <v>0</v>
+      </c>
+      <c r="D49" s="156">
+        <v>0</v>
+      </c>
+      <c r="E49" s="156">
         <f>-$E$5</f>
         <v>-1</v>
       </c>
-      <c r="F49" s="41">
+      <c r="F49" s="156">
         <f>$C$5</f>
         <v>6.1257422745431001E-17</v>
       </c>
-      <c r="G49" s="41">
-        <v>0</v>
-      </c>
-      <c r="L49" s="41">
-        <v>0</v>
-      </c>
-      <c r="M49" s="41">
-        <v>0</v>
-      </c>
-      <c r="N49" s="41">
-        <v>0</v>
-      </c>
-      <c r="O49" s="41">
+      <c r="G49" s="156">
+        <v>0</v>
+      </c>
+      <c r="L49" s="156">
+        <v>0</v>
+      </c>
+      <c r="M49" s="156">
+        <v>0</v>
+      </c>
+      <c r="N49" s="156">
+        <v>0</v>
+      </c>
+      <c r="O49" s="156">
         <f>$M$5</f>
         <v>1</v>
       </c>
-      <c r="P49" s="41">
+      <c r="P49" s="156">
         <f>$O$5</f>
         <v>0</v>
       </c>
-      <c r="Q49" s="41">
-        <v>0</v>
-      </c>
-      <c r="V49" s="41">
-        <v>0</v>
-      </c>
-      <c r="W49" s="41">
-        <v>0</v>
-      </c>
-      <c r="X49" s="41">
-        <v>0</v>
-      </c>
-      <c r="Y49" s="41">
+      <c r="Q49" s="156">
+        <v>0</v>
+      </c>
+      <c r="V49" s="156">
+        <v>0</v>
+      </c>
+      <c r="W49" s="156">
+        <v>0</v>
+      </c>
+      <c r="X49" s="156">
+        <v>0</v>
+      </c>
+      <c r="Y49" s="156">
         <f>$C$5</f>
         <v>6.1257422745431001E-17</v>
       </c>
-      <c r="Z49" s="41">
+      <c r="Z49" s="156">
         <f>$E$5</f>
         <v>1</v>
       </c>
-      <c r="AA49" s="41">
+      <c r="AA49" s="156">
         <v>0</v>
       </c>
       <c r="AE49" s="10"/>
@@ -6361,63 +6362,63 @@
       <c r="CW49" s="2"/>
     </row>
     <row r="50" spans="2:101" x14ac:dyDescent="0.2">
-      <c r="B50" s="41">
-        <v>0</v>
-      </c>
-      <c r="C50" s="41">
-        <v>0</v>
-      </c>
-      <c r="D50" s="41">
-        <v>0</v>
-      </c>
-      <c r="E50" s="41">
-        <v>0</v>
-      </c>
-      <c r="F50" s="41">
-        <v>0</v>
-      </c>
-      <c r="G50" s="41">
+      <c r="B50" s="156">
+        <v>0</v>
+      </c>
+      <c r="C50" s="156">
+        <v>0</v>
+      </c>
+      <c r="D50" s="156">
+        <v>0</v>
+      </c>
+      <c r="E50" s="156">
+        <v>0</v>
+      </c>
+      <c r="F50" s="156">
+        <v>0</v>
+      </c>
+      <c r="G50" s="156">
         <f>D47</f>
         <v>1</v>
       </c>
-      <c r="L50" s="41">
-        <v>0</v>
-      </c>
-      <c r="M50" s="41">
-        <v>0</v>
-      </c>
-      <c r="N50" s="41">
-        <v>0</v>
-      </c>
-      <c r="O50" s="41">
+      <c r="L50" s="156">
+        <v>0</v>
+      </c>
+      <c r="M50" s="156">
+        <v>0</v>
+      </c>
+      <c r="N50" s="156">
+        <v>0</v>
+      </c>
+      <c r="O50" s="156">
         <f>-$O$5</f>
         <v>0</v>
       </c>
-      <c r="P50" s="41">
+      <c r="P50" s="156">
         <f>$M$5</f>
         <v>1</v>
       </c>
-      <c r="Q50" s="41">
-        <v>0</v>
-      </c>
-      <c r="V50" s="41">
-        <v>0</v>
-      </c>
-      <c r="W50" s="41">
-        <v>0</v>
-      </c>
-      <c r="X50" s="41">
-        <v>0</v>
-      </c>
-      <c r="Y50" s="41">
+      <c r="Q50" s="156">
+        <v>0</v>
+      </c>
+      <c r="V50" s="156">
+        <v>0</v>
+      </c>
+      <c r="W50" s="156">
+        <v>0</v>
+      </c>
+      <c r="X50" s="156">
+        <v>0</v>
+      </c>
+      <c r="Y50" s="156">
         <f>-$E$5</f>
         <v>-1</v>
       </c>
-      <c r="Z50" s="41">
+      <c r="Z50" s="156">
         <f>$C$5</f>
         <v>6.1257422745431001E-17</v>
       </c>
-      <c r="AA50" s="41">
+      <c r="AA50" s="156">
         <v>0</v>
       </c>
       <c r="AE50" s="8"/>
@@ -6479,7 +6480,7 @@
       </c>
       <c r="AZ50" s="3">
         <f t="shared" si="35"/>
-        <v>1569.9999999999989</v>
+        <v>-1.22514845490862E-12</v>
       </c>
       <c r="BA50" s="148" t="s">
         <v>57</v>
@@ -6490,41 +6491,41 @@
     <row r="51" spans="2:101" x14ac:dyDescent="0.2">
       <c r="E51" s="4"/>
       <c r="F51" s="4"/>
-      <c r="L51" s="41">
-        <v>0</v>
-      </c>
-      <c r="M51" s="41">
-        <v>0</v>
-      </c>
-      <c r="N51" s="41">
-        <v>0</v>
-      </c>
-      <c r="O51" s="41">
-        <v>0</v>
-      </c>
-      <c r="P51" s="41">
-        <v>0</v>
-      </c>
-      <c r="Q51" s="41">
+      <c r="L51" s="156">
+        <v>0</v>
+      </c>
+      <c r="M51" s="156">
+        <v>0</v>
+      </c>
+      <c r="N51" s="156">
+        <v>0</v>
+      </c>
+      <c r="O51" s="156">
+        <v>0</v>
+      </c>
+      <c r="P51" s="156">
+        <v>0</v>
+      </c>
+      <c r="Q51" s="156">
         <f>N48</f>
         <v>1</v>
       </c>
-      <c r="V51" s="41">
-        <v>0</v>
-      </c>
-      <c r="W51" s="41">
-        <v>0</v>
-      </c>
-      <c r="X51" s="41">
-        <v>0</v>
-      </c>
-      <c r="Y51" s="41">
-        <v>0</v>
-      </c>
-      <c r="Z51" s="41">
-        <v>0</v>
-      </c>
-      <c r="AA51" s="41">
+      <c r="V51" s="156">
+        <v>0</v>
+      </c>
+      <c r="W51" s="156">
+        <v>0</v>
+      </c>
+      <c r="X51" s="156">
+        <v>0</v>
+      </c>
+      <c r="Y51" s="156">
+        <v>0</v>
+      </c>
+      <c r="Z51" s="156">
+        <v>0</v>
+      </c>
+      <c r="AA51" s="156">
         <f>X48</f>
         <v>1</v>
       </c>
@@ -6739,7 +6740,7 @@
       </c>
       <c r="AZ53" s="3">
         <f t="shared" si="35"/>
-        <v>36280</v>
+        <v>30000</v>
       </c>
       <c r="BB53" s="12"/>
       <c r="BE53" s="16"/>
@@ -6760,24 +6761,24 @@
       <c r="BY53" s="4"/>
     </row>
     <row r="54" spans="2:101" x14ac:dyDescent="0.2">
-      <c r="B54" s="41">
+      <c r="B54" s="156">
         <f>$C$5</f>
         <v>6.1257422745431001E-17</v>
       </c>
-      <c r="C54" s="41">
+      <c r="C54" s="156">
         <f>-$E$5</f>
         <v>-1</v>
       </c>
-      <c r="D54" s="41">
-        <v>0</v>
-      </c>
-      <c r="E54" s="41">
-        <v>0</v>
-      </c>
-      <c r="F54" s="41">
-        <v>0</v>
-      </c>
-      <c r="G54" s="41">
+      <c r="D54" s="156">
+        <v>0</v>
+      </c>
+      <c r="E54" s="156">
+        <v>0</v>
+      </c>
+      <c r="F54" s="156">
+        <v>0</v>
+      </c>
+      <c r="G54" s="156">
         <v>0</v>
       </c>
       <c r="L54" s="2" t="s">
@@ -6845,7 +6846,7 @@
       </c>
       <c r="AZ54" s="3">
         <f t="shared" si="35"/>
-        <v>-21376666.666666664</v>
+        <v>-16666666.666666666</v>
       </c>
       <c r="BB54" s="12"/>
       <c r="BE54" s="16"/>
@@ -6861,64 +6862,64 @@
       <c r="BY54" s="4"/>
     </row>
     <row r="55" spans="2:101" x14ac:dyDescent="0.2">
-      <c r="B55" s="41">
+      <c r="B55" s="156">
         <f>$E$5</f>
         <v>1</v>
       </c>
-      <c r="C55" s="41">
+      <c r="C55" s="156">
         <f>$C$5</f>
         <v>6.1257422745431001E-17</v>
       </c>
-      <c r="D55" s="41">
-        <v>0</v>
-      </c>
-      <c r="E55" s="41">
-        <v>0</v>
-      </c>
-      <c r="F55" s="41">
-        <v>0</v>
-      </c>
-      <c r="G55" s="41">
-        <v>0</v>
-      </c>
-      <c r="L55" s="41">
+      <c r="D55" s="156">
+        <v>0</v>
+      </c>
+      <c r="E55" s="156">
+        <v>0</v>
+      </c>
+      <c r="F55" s="156">
+        <v>0</v>
+      </c>
+      <c r="G55" s="156">
+        <v>0</v>
+      </c>
+      <c r="L55" s="156">
         <f>$M$5</f>
         <v>1</v>
       </c>
-      <c r="M55" s="41">
+      <c r="M55" s="156">
         <f>-$O$5</f>
         <v>0</v>
       </c>
-      <c r="N55" s="41">
-        <v>0</v>
-      </c>
-      <c r="O55" s="41">
-        <v>0</v>
-      </c>
-      <c r="P55" s="41">
-        <v>0</v>
-      </c>
-      <c r="Q55" s="41">
-        <v>0</v>
-      </c>
-      <c r="V55" s="41">
+      <c r="N55" s="156">
+        <v>0</v>
+      </c>
+      <c r="O55" s="156">
+        <v>0</v>
+      </c>
+      <c r="P55" s="156">
+        <v>0</v>
+      </c>
+      <c r="Q55" s="156">
+        <v>0</v>
+      </c>
+      <c r="V55" s="156">
         <f>$C$5</f>
         <v>6.1257422745431001E-17</v>
       </c>
-      <c r="W55" s="41">
+      <c r="W55" s="156">
         <f>-$E$5</f>
         <v>-1</v>
       </c>
-      <c r="X55" s="41">
-        <v>0</v>
-      </c>
-      <c r="Y55" s="41">
-        <v>0</v>
-      </c>
-      <c r="Z55" s="41">
-        <v>0</v>
-      </c>
-      <c r="AA55" s="41">
+      <c r="X55" s="156">
+        <v>0</v>
+      </c>
+      <c r="Y55" s="156">
+        <v>0</v>
+      </c>
+      <c r="Z55" s="156">
+        <v>0</v>
+      </c>
+      <c r="AA55" s="156">
         <v>0</v>
       </c>
       <c r="AB55" s="4"/>
@@ -6939,63 +6940,63 @@
       <c r="BY55" s="4"/>
     </row>
     <row r="56" spans="2:101" x14ac:dyDescent="0.2">
-      <c r="B56" s="41">
-        <v>0</v>
-      </c>
-      <c r="C56" s="41">
-        <v>0</v>
-      </c>
-      <c r="D56" s="41">
+      <c r="B56" s="156">
+        <v>0</v>
+      </c>
+      <c r="C56" s="156">
+        <v>0</v>
+      </c>
+      <c r="D56" s="156">
         <f>D47</f>
         <v>1</v>
       </c>
-      <c r="E56" s="41">
-        <v>0</v>
-      </c>
-      <c r="F56" s="41">
-        <v>0</v>
-      </c>
-      <c r="G56" s="41">
-        <v>0</v>
-      </c>
-      <c r="L56" s="41">
+      <c r="E56" s="156">
+        <v>0</v>
+      </c>
+      <c r="F56" s="156">
+        <v>0</v>
+      </c>
+      <c r="G56" s="156">
+        <v>0</v>
+      </c>
+      <c r="L56" s="156">
         <f>$O$5</f>
         <v>0</v>
       </c>
-      <c r="M56" s="41">
+      <c r="M56" s="156">
         <f>$M$5</f>
         <v>1</v>
       </c>
-      <c r="N56" s="41">
-        <v>0</v>
-      </c>
-      <c r="O56" s="41">
-        <v>0</v>
-      </c>
-      <c r="P56" s="41">
-        <v>0</v>
-      </c>
-      <c r="Q56" s="41">
-        <v>0</v>
-      </c>
-      <c r="V56" s="41">
+      <c r="N56" s="156">
+        <v>0</v>
+      </c>
+      <c r="O56" s="156">
+        <v>0</v>
+      </c>
+      <c r="P56" s="156">
+        <v>0</v>
+      </c>
+      <c r="Q56" s="156">
+        <v>0</v>
+      </c>
+      <c r="V56" s="156">
         <f>$E$5</f>
         <v>1</v>
       </c>
-      <c r="W56" s="41">
+      <c r="W56" s="156">
         <f>$C$5</f>
         <v>6.1257422745431001E-17</v>
       </c>
-      <c r="X56" s="41">
-        <v>0</v>
-      </c>
-      <c r="Y56" s="41">
-        <v>0</v>
-      </c>
-      <c r="Z56" s="41">
-        <v>0</v>
-      </c>
-      <c r="AA56" s="41">
+      <c r="X56" s="156">
+        <v>0</v>
+      </c>
+      <c r="Y56" s="156">
+        <v>0</v>
+      </c>
+      <c r="Z56" s="156">
+        <v>0</v>
+      </c>
+      <c r="AA56" s="156">
         <v>0</v>
       </c>
       <c r="AB56" s="4"/>
@@ -7016,62 +7017,62 @@
       <c r="BY56" s="4"/>
     </row>
     <row r="57" spans="2:101" x14ac:dyDescent="0.2">
-      <c r="B57" s="41">
-        <v>0</v>
-      </c>
-      <c r="C57" s="41">
-        <v>0</v>
-      </c>
-      <c r="D57" s="41">
-        <v>0</v>
-      </c>
-      <c r="E57" s="41">
+      <c r="B57" s="156">
+        <v>0</v>
+      </c>
+      <c r="C57" s="156">
+        <v>0</v>
+      </c>
+      <c r="D57" s="156">
+        <v>0</v>
+      </c>
+      <c r="E57" s="156">
         <f>$C$5</f>
         <v>6.1257422745431001E-17</v>
       </c>
-      <c r="F57" s="41">
+      <c r="F57" s="156">
         <f>-$E$5</f>
         <v>-1</v>
       </c>
-      <c r="G57" s="41">
-        <v>0</v>
-      </c>
-      <c r="L57" s="41">
-        <v>0</v>
-      </c>
-      <c r="M57" s="41">
-        <v>0</v>
-      </c>
-      <c r="N57" s="41">
+      <c r="G57" s="156">
+        <v>0</v>
+      </c>
+      <c r="L57" s="156">
+        <v>0</v>
+      </c>
+      <c r="M57" s="156">
+        <v>0</v>
+      </c>
+      <c r="N57" s="156">
         <f>N48</f>
         <v>1</v>
       </c>
-      <c r="O57" s="41">
-        <v>0</v>
-      </c>
-      <c r="P57" s="41">
-        <v>0</v>
-      </c>
-      <c r="Q57" s="41">
-        <v>0</v>
-      </c>
-      <c r="V57" s="41">
-        <v>0</v>
-      </c>
-      <c r="W57" s="41">
-        <v>0</v>
-      </c>
-      <c r="X57" s="41">
+      <c r="O57" s="156">
+        <v>0</v>
+      </c>
+      <c r="P57" s="156">
+        <v>0</v>
+      </c>
+      <c r="Q57" s="156">
+        <v>0</v>
+      </c>
+      <c r="V57" s="156">
+        <v>0</v>
+      </c>
+      <c r="W57" s="156">
+        <v>0</v>
+      </c>
+      <c r="X57" s="156">
         <f>X48</f>
         <v>1</v>
       </c>
-      <c r="Y57" s="41">
-        <v>0</v>
-      </c>
-      <c r="Z57" s="41">
-        <v>0</v>
-      </c>
-      <c r="AA57" s="41">
+      <c r="Y57" s="156">
+        <v>0</v>
+      </c>
+      <c r="Z57" s="156">
+        <v>0</v>
+      </c>
+      <c r="AA57" s="156">
         <v>0</v>
       </c>
       <c r="AB57" s="4"/>
@@ -7080,64 +7081,64 @@
       <c r="BE57" s="16"/>
     </row>
     <row r="58" spans="2:101" x14ac:dyDescent="0.2">
-      <c r="B58" s="41">
-        <v>0</v>
-      </c>
-      <c r="C58" s="41">
-        <v>0</v>
-      </c>
-      <c r="D58" s="41">
-        <v>0</v>
-      </c>
-      <c r="E58" s="41">
+      <c r="B58" s="156">
+        <v>0</v>
+      </c>
+      <c r="C58" s="156">
+        <v>0</v>
+      </c>
+      <c r="D58" s="156">
+        <v>0</v>
+      </c>
+      <c r="E58" s="156">
         <f>$E$5</f>
         <v>1</v>
       </c>
-      <c r="F58" s="41">
+      <c r="F58" s="156">
         <f>$C$5</f>
         <v>6.1257422745431001E-17</v>
       </c>
-      <c r="G58" s="41">
-        <v>0</v>
-      </c>
-      <c r="L58" s="41">
-        <v>0</v>
-      </c>
-      <c r="M58" s="41">
-        <v>0</v>
-      </c>
-      <c r="N58" s="41">
-        <v>0</v>
-      </c>
-      <c r="O58" s="41">
+      <c r="G58" s="156">
+        <v>0</v>
+      </c>
+      <c r="L58" s="156">
+        <v>0</v>
+      </c>
+      <c r="M58" s="156">
+        <v>0</v>
+      </c>
+      <c r="N58" s="156">
+        <v>0</v>
+      </c>
+      <c r="O58" s="156">
         <f>$M$5</f>
         <v>1</v>
       </c>
-      <c r="P58" s="41">
+      <c r="P58" s="156">
         <f>-$O$5</f>
         <v>0</v>
       </c>
-      <c r="Q58" s="41">
-        <v>0</v>
-      </c>
-      <c r="V58" s="41">
-        <v>0</v>
-      </c>
-      <c r="W58" s="41">
-        <v>0</v>
-      </c>
-      <c r="X58" s="41">
-        <v>0</v>
-      </c>
-      <c r="Y58" s="41">
+      <c r="Q58" s="156">
+        <v>0</v>
+      </c>
+      <c r="V58" s="156">
+        <v>0</v>
+      </c>
+      <c r="W58" s="156">
+        <v>0</v>
+      </c>
+      <c r="X58" s="156">
+        <v>0</v>
+      </c>
+      <c r="Y58" s="156">
         <f>$C$5</f>
         <v>6.1257422745431001E-17</v>
       </c>
-      <c r="Z58" s="41">
+      <c r="Z58" s="156">
         <f>-$E$5</f>
         <v>-1</v>
       </c>
-      <c r="AA58" s="41">
+      <c r="AA58" s="156">
         <v>0</v>
       </c>
       <c r="AB58" s="4"/>
@@ -7154,63 +7155,63 @@
       <c r="BK58" s="2"/>
     </row>
     <row r="59" spans="2:101" x14ac:dyDescent="0.2">
-      <c r="B59" s="41">
-        <v>0</v>
-      </c>
-      <c r="C59" s="41">
-        <v>0</v>
-      </c>
-      <c r="D59" s="41">
-        <v>0</v>
-      </c>
-      <c r="E59" s="41">
-        <v>0</v>
-      </c>
-      <c r="F59" s="41">
-        <v>0</v>
-      </c>
-      <c r="G59" s="41">
+      <c r="B59" s="156">
+        <v>0</v>
+      </c>
+      <c r="C59" s="156">
+        <v>0</v>
+      </c>
+      <c r="D59" s="156">
+        <v>0</v>
+      </c>
+      <c r="E59" s="156">
+        <v>0</v>
+      </c>
+      <c r="F59" s="156">
+        <v>0</v>
+      </c>
+      <c r="G59" s="156">
         <f>D47</f>
         <v>1</v>
       </c>
-      <c r="L59" s="41">
-        <v>0</v>
-      </c>
-      <c r="M59" s="41">
-        <v>0</v>
-      </c>
-      <c r="N59" s="41">
-        <v>0</v>
-      </c>
-      <c r="O59" s="41">
+      <c r="L59" s="156">
+        <v>0</v>
+      </c>
+      <c r="M59" s="156">
+        <v>0</v>
+      </c>
+      <c r="N59" s="156">
+        <v>0</v>
+      </c>
+      <c r="O59" s="156">
         <f>$O$5</f>
         <v>0</v>
       </c>
-      <c r="P59" s="41">
+      <c r="P59" s="156">
         <f>$M$5</f>
         <v>1</v>
       </c>
-      <c r="Q59" s="41">
-        <v>0</v>
-      </c>
-      <c r="V59" s="41">
-        <v>0</v>
-      </c>
-      <c r="W59" s="41">
-        <v>0</v>
-      </c>
-      <c r="X59" s="41">
-        <v>0</v>
-      </c>
-      <c r="Y59" s="41">
+      <c r="Q59" s="156">
+        <v>0</v>
+      </c>
+      <c r="V59" s="156">
+        <v>0</v>
+      </c>
+      <c r="W59" s="156">
+        <v>0</v>
+      </c>
+      <c r="X59" s="156">
+        <v>0</v>
+      </c>
+      <c r="Y59" s="156">
         <f>$E$5</f>
         <v>1</v>
       </c>
-      <c r="Z59" s="41">
+      <c r="Z59" s="156">
         <f>$C$5</f>
         <v>6.1257422745431001E-17</v>
       </c>
-      <c r="AA59" s="41">
+      <c r="AA59" s="156">
         <v>0</v>
       </c>
       <c r="AB59" s="4"/>
@@ -7266,41 +7267,41 @@
       <c r="CA59" s="63"/>
     </row>
     <row r="60" spans="2:101" x14ac:dyDescent="0.2">
-      <c r="L60" s="41">
-        <v>0</v>
-      </c>
-      <c r="M60" s="41">
-        <v>0</v>
-      </c>
-      <c r="N60" s="41">
-        <v>0</v>
-      </c>
-      <c r="O60" s="41">
-        <v>0</v>
-      </c>
-      <c r="P60" s="41">
-        <v>0</v>
-      </c>
-      <c r="Q60" s="41">
+      <c r="L60" s="156">
+        <v>0</v>
+      </c>
+      <c r="M60" s="156">
+        <v>0</v>
+      </c>
+      <c r="N60" s="156">
+        <v>0</v>
+      </c>
+      <c r="O60" s="156">
+        <v>0</v>
+      </c>
+      <c r="P60" s="156">
+        <v>0</v>
+      </c>
+      <c r="Q60" s="156">
         <f>N48</f>
         <v>1</v>
       </c>
-      <c r="V60" s="41">
-        <v>0</v>
-      </c>
-      <c r="W60" s="41">
-        <v>0</v>
-      </c>
-      <c r="X60" s="41">
-        <v>0</v>
-      </c>
-      <c r="Y60" s="41">
-        <v>0</v>
-      </c>
-      <c r="Z60" s="41">
-        <v>0</v>
-      </c>
-      <c r="AA60" s="41">
+      <c r="V60" s="156">
+        <v>0</v>
+      </c>
+      <c r="W60" s="156">
+        <v>0</v>
+      </c>
+      <c r="X60" s="156">
+        <v>0</v>
+      </c>
+      <c r="Y60" s="156">
+        <v>0</v>
+      </c>
+      <c r="Z60" s="156">
+        <v>0</v>
+      </c>
+      <c r="AA60" s="156">
         <f>X48</f>
         <v>1</v>
       </c>
@@ -7465,7 +7466,7 @@
         <v>r22</v>
       </c>
       <c r="AV62" s="146">
-        <v>36280</v>
+        <v>30000</v>
       </c>
       <c r="BB62" s="12"/>
       <c r="BE62" s="12"/>
@@ -7532,7 +7533,7 @@
         <v>r23</v>
       </c>
       <c r="AV63" s="146">
-        <v>21376666.666666664</v>
+        <v>16666666.666666666</v>
       </c>
       <c r="BB63" s="12"/>
       <c r="BE63" s="12"/>
@@ -7779,7 +7780,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="AT67" s="1">
-        <v>36280</v>
+        <v>30000</v>
       </c>
       <c r="AW67" s="1" t="s">
         <v>3</v>
@@ -7821,7 +7822,7 @@
         <v>#VALUE!</v>
       </c>
       <c r="AT68" s="1">
-        <v>21376666.666666664</v>
+        <v>16666666.666666666</v>
       </c>
       <c r="AW68" s="1" t="s">
         <v>60</v>

</xml_diff>

<commit_message>
Handle unknown translation row gathering
Add methods to get rows with unknown translations (rows that are not 0 or knwon translation)
Includes various minor fixes in other files and .idea folder is removed
</commit_message>
<xml_diff>
--- a/theory/FEM matriisit.xlsx
+++ b/theory/FEM matriisit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ohjelmointi\2_Rust\idfem\theory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E28F411-D9C1-469D-BCEC-8315E308FFFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B648D7F7-F766-498B-B267-E95AF951A284}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-22230" yWindow="0" windowWidth="22335" windowHeight="20880" activeTab="1" xr2:uid="{27180542-B0D2-4BFE-946B-7857B24C93C8}"/>
   </bookViews>
@@ -416,7 +416,7 @@
     <numFmt numFmtId="167" formatCode="0.0"/>
     <numFmt numFmtId="168" formatCode="0.00000"/>
     <numFmt numFmtId="169" formatCode="0.0000E+00"/>
-    <numFmt numFmtId="171" formatCode="0.0000"/>
+    <numFmt numFmtId="170" formatCode="0.0000"/>
   </numFmts>
   <fonts count="15" x14ac:knownFonts="1">
     <font>
@@ -697,7 +697,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="163">
+  <cellXfs count="160">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1099,36 +1099,37 @@
     <xf numFmtId="167" fontId="2" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="171" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="170" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutraali" xfId="1" builtinId="28"/>
     <cellStyle name="Normaali" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="11">
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
@@ -1157,39 +1158,9 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
@@ -1215,6 +1186,9 @@
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1432,7 +1406,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>63</xdr:col>
-      <xdr:colOff>542836</xdr:colOff>
+      <xdr:colOff>329924</xdr:colOff>
       <xdr:row>43</xdr:row>
       <xdr:rowOff>28196</xdr:rowOff>
     </xdr:to>
@@ -1887,8 +1861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94F9BDF3-3EE6-4BFB-9734-CB047BC6E804}">
   <dimension ref="B1:CW227"/>
   <sheetViews>
-    <sheetView topLeftCell="P1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U65" sqref="U65"/>
+    <sheetView topLeftCell="AN12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AZ45" sqref="AZ45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -3282,22 +3256,10 @@
       </c>
     </row>
     <row r="16" spans="2:66" x14ac:dyDescent="0.2">
-      <c r="B16" s="161"/>
-      <c r="C16" s="161"/>
-      <c r="D16" s="161"/>
-      <c r="E16" s="162"/>
-      <c r="F16" s="161"/>
-      <c r="L16" s="161"/>
-      <c r="M16" s="161"/>
-      <c r="N16" s="161"/>
-      <c r="O16" s="162"/>
-      <c r="P16" s="161"/>
+      <c r="E16" s="3"/>
+      <c r="O16" s="3"/>
       <c r="S16" s="2"/>
-      <c r="V16" s="161"/>
-      <c r="W16" s="161"/>
-      <c r="X16" s="161"/>
-      <c r="Y16" s="162"/>
-      <c r="Z16" s="161"/>
+      <c r="Y16" s="3"/>
       <c r="AJ16" s="78">
         <v>11</v>
       </c>
@@ -10071,18 +10033,20 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="AK43:AV54">
-    <cfRule type="expression" dxfId="6" priority="1">
-      <formula>ABS(AK43)&lt;0.1</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="5" priority="2">
+    <cfRule type="expression" dxfId="10" priority="2">
       <formula>ABS(AK43)&lt;0.1</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="AZ43:AZ54">
+    <cfRule type="expression" dxfId="9" priority="1">
+      <formula>ABS(AZ43)&lt;0.1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="BR166:BR168">
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
       <formula>"VIRHE!"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
       <formula>"OK!"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10095,8 +10059,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F95DF150-D06E-47EC-89DA-0EC5D53947FD}">
   <dimension ref="A1:CW233"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AN39" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AV74" sqref="AV74"/>
+    <sheetView tabSelected="1" topLeftCell="AH24" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AT92" sqref="AT92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.25"/>
@@ -10115,7 +10079,9 @@
     <col min="47" max="47" width="13.140625" style="80" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="12.42578125" style="80" bestFit="1" customWidth="1"/>
     <col min="49" max="50" width="11.5703125" style="80" bestFit="1" customWidth="1"/>
-    <col min="51" max="16384" width="9.140625" style="80"/>
+    <col min="51" max="53" width="9.140625" style="80"/>
+    <col min="54" max="54" width="12.28515625" style="80" bestFit="1" customWidth="1"/>
+    <col min="55" max="16384" width="9.140625" style="80"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:67" x14ac:dyDescent="0.2">
@@ -11508,7 +11474,7 @@
       <c r="W15" s="4"/>
       <c r="X15" s="4"/>
       <c r="Y15" s="20">
-        <v>10</v>
+        <v>-10</v>
       </c>
       <c r="Z15" s="4" t="s">
         <v>33</v>
@@ -11577,31 +11543,31 @@
     </row>
     <row r="16" spans="1:67" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
-      <c r="B16" s="159"/>
-      <c r="C16" s="154"/>
-      <c r="D16" s="154"/>
-      <c r="E16" s="160"/>
-      <c r="F16" s="154"/>
+      <c r="B16" s="45"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="4"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
-      <c r="L16" s="159"/>
-      <c r="M16" s="154"/>
-      <c r="N16" s="154"/>
-      <c r="O16" s="160"/>
-      <c r="P16" s="154"/>
+      <c r="L16" s="45"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="4"/>
+      <c r="O16" s="7"/>
+      <c r="P16" s="4"/>
       <c r="Q16" s="4"/>
       <c r="R16" s="4"/>
       <c r="S16" s="82"/>
       <c r="T16" s="4"/>
       <c r="U16" s="4"/>
-      <c r="V16" s="159"/>
-      <c r="W16" s="154"/>
-      <c r="X16" s="154"/>
-      <c r="Y16" s="160"/>
-      <c r="Z16" s="154"/>
+      <c r="V16" s="45"/>
+      <c r="W16" s="4"/>
+      <c r="X16" s="4"/>
+      <c r="Y16" s="7"/>
+      <c r="Z16" s="4"/>
       <c r="AA16" s="4"/>
       <c r="AB16" s="4"/>
       <c r="AC16" s="4"/>
@@ -12836,7 +12802,8 @@
         <v>0</v>
       </c>
       <c r="AB28" s="4"/>
-      <c r="AC28" s="41">
+      <c r="AC28" s="38">
+        <f>Y6/2*Y14</f>
         <v>0</v>
       </c>
       <c r="AD28" s="4"/>
@@ -12943,7 +12910,7 @@
       </c>
       <c r="AB29" s="4"/>
       <c r="AC29" s="38">
-        <f>-Y15*Y6/2</f>
+        <f>Y6/2*Y15</f>
         <v>-20000</v>
       </c>
       <c r="AD29" s="4"/>
@@ -13050,7 +13017,7 @@
       </c>
       <c r="AB30" s="4"/>
       <c r="AC30" s="38">
-        <f>-1*(Y15*Y6^2)/12</f>
+        <f>1*(Y15*Y6^2)/12</f>
         <v>-13333333.333333334</v>
       </c>
       <c r="AD30" s="4"/>
@@ -13149,7 +13116,8 @@
         <v>0</v>
       </c>
       <c r="AB31" s="4"/>
-      <c r="AC31" s="41">
+      <c r="AC31" s="38">
+        <f>Y6/2*Y14</f>
         <v>0</v>
       </c>
       <c r="AD31" s="4"/>
@@ -13277,7 +13245,7 @@
       </c>
       <c r="AB32" s="4"/>
       <c r="AC32" s="38">
-        <f>-Y15*Y6/2</f>
+        <f>Y6/2*Y15</f>
         <v>-20000</v>
       </c>
       <c r="AD32" s="4"/>
@@ -13404,7 +13372,7 @@
       </c>
       <c r="AB33" s="4"/>
       <c r="AC33" s="38">
-        <f>1*(Y15*Y6^2)/12</f>
+        <f>-1*(Y15*Y6^2)/12</f>
         <v>13333333.333333334</v>
       </c>
       <c r="AD33" s="4"/>
@@ -14634,17 +14602,17 @@
       <c r="BC46" s="144" t="s">
         <v>52</v>
       </c>
-      <c r="BD46" s="156"/>
-      <c r="BE46" s="156"/>
-      <c r="BF46" s="156"/>
-      <c r="BG46" s="156"/>
-      <c r="BH46" s="156"/>
-      <c r="BI46" s="156"/>
-      <c r="BJ46" s="156"/>
-      <c r="BK46" s="156"/>
-      <c r="BL46" s="156"/>
-      <c r="BM46" s="156"/>
-      <c r="BN46" s="156"/>
+      <c r="BD46" s="4"/>
+      <c r="BE46" s="4"/>
+      <c r="BF46" s="4"/>
+      <c r="BG46" s="4"/>
+      <c r="BH46" s="4"/>
+      <c r="BI46" s="4"/>
+      <c r="BJ46" s="4"/>
+      <c r="BK46" s="4"/>
+      <c r="BL46" s="4"/>
+      <c r="BM46" s="4"/>
+      <c r="BN46" s="4"/>
       <c r="CE46" s="115"/>
     </row>
     <row r="47" spans="1:83" x14ac:dyDescent="0.2">
@@ -14790,17 +14758,16 @@
       <c r="BC47" s="144" t="s">
         <v>51</v>
       </c>
-      <c r="BD47" s="157"/>
-      <c r="BE47" s="155"/>
-      <c r="BF47" s="155"/>
-      <c r="BG47" s="158"/>
-      <c r="BH47" s="158"/>
-      <c r="BI47" s="158"/>
-      <c r="BJ47" s="158"/>
-      <c r="BK47" s="158"/>
-      <c r="BL47" s="158"/>
-      <c r="BM47" s="158"/>
-      <c r="BN47" s="158"/>
+      <c r="BE47" s="154"/>
+      <c r="BF47" s="154"/>
+      <c r="BG47" s="155"/>
+      <c r="BH47" s="155"/>
+      <c r="BI47" s="155"/>
+      <c r="BJ47" s="155"/>
+      <c r="BK47" s="155"/>
+      <c r="BL47" s="155"/>
+      <c r="BM47" s="155"/>
+      <c r="BN47" s="155"/>
       <c r="BS47" s="116"/>
       <c r="CE47" s="115"/>
     </row>
@@ -14945,17 +14912,16 @@
       <c r="BC48" s="144" t="s">
         <v>85</v>
       </c>
-      <c r="BD48" s="157"/>
-      <c r="BE48" s="155"/>
-      <c r="BF48" s="155"/>
-      <c r="BG48" s="158"/>
-      <c r="BH48" s="155"/>
-      <c r="BI48" s="158"/>
-      <c r="BJ48" s="158"/>
-      <c r="BK48" s="158"/>
-      <c r="BL48" s="158"/>
-      <c r="BM48" s="158"/>
-      <c r="BN48" s="158"/>
+      <c r="BE48" s="154"/>
+      <c r="BF48" s="154"/>
+      <c r="BG48" s="155"/>
+      <c r="BH48" s="154"/>
+      <c r="BI48" s="155"/>
+      <c r="BJ48" s="155"/>
+      <c r="BK48" s="155"/>
+      <c r="BL48" s="155"/>
+      <c r="BM48" s="155"/>
+      <c r="BN48" s="155"/>
     </row>
     <row r="49" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A49" s="4"/>
@@ -15102,17 +15068,14 @@
         <v>-20000</v>
       </c>
       <c r="BC49" s="1"/>
-      <c r="BD49" s="157"/>
-      <c r="BE49" s="155"/>
-      <c r="BF49" s="155"/>
-      <c r="BG49" s="158"/>
-      <c r="BH49" s="155"/>
-      <c r="BI49" s="158"/>
-      <c r="BJ49" s="158"/>
-      <c r="BK49" s="158"/>
-      <c r="BL49" s="158"/>
-      <c r="BM49" s="157"/>
-      <c r="BN49" s="157"/>
+      <c r="BE49" s="154"/>
+      <c r="BF49" s="154"/>
+      <c r="BG49" s="155"/>
+      <c r="BH49" s="154"/>
+      <c r="BI49" s="155"/>
+      <c r="BJ49" s="155"/>
+      <c r="BK49" s="155"/>
+      <c r="BL49" s="155"/>
       <c r="CW49" s="115"/>
     </row>
     <row r="50" spans="1:101" x14ac:dyDescent="0.2">
@@ -15259,17 +15222,12 @@
         <v>30000</v>
       </c>
       <c r="BC50" s="1"/>
-      <c r="BD50" s="157"/>
-      <c r="BE50" s="157"/>
-      <c r="BF50" s="157"/>
-      <c r="BG50" s="158"/>
-      <c r="BH50" s="155"/>
-      <c r="BI50" s="158"/>
-      <c r="BJ50" s="158"/>
-      <c r="BK50" s="158"/>
-      <c r="BL50" s="158"/>
-      <c r="BM50" s="157"/>
-      <c r="BN50" s="157"/>
+      <c r="BG50" s="155"/>
+      <c r="BH50" s="154"/>
+      <c r="BI50" s="155"/>
+      <c r="BJ50" s="155"/>
+      <c r="BK50" s="155"/>
+      <c r="BL50" s="155"/>
       <c r="CW50" s="115"/>
     </row>
     <row r="51" spans="1:101" x14ac:dyDescent="0.2">
@@ -15400,17 +15358,14 @@
         <v>30000000</v>
       </c>
       <c r="BC51" s="1"/>
-      <c r="BD51" s="157"/>
-      <c r="BE51" s="155"/>
-      <c r="BF51" s="155"/>
-      <c r="BG51" s="158"/>
-      <c r="BH51" s="155"/>
-      <c r="BI51" s="158"/>
-      <c r="BJ51" s="158"/>
-      <c r="BK51" s="158"/>
-      <c r="BL51" s="158"/>
-      <c r="BM51" s="157"/>
-      <c r="BN51" s="157"/>
+      <c r="BE51" s="154"/>
+      <c r="BF51" s="154"/>
+      <c r="BG51" s="155"/>
+      <c r="BH51" s="154"/>
+      <c r="BI51" s="155"/>
+      <c r="BJ51" s="155"/>
+      <c r="BK51" s="155"/>
+      <c r="BL51" s="155"/>
       <c r="BO51" s="112"/>
       <c r="BP51" s="112"/>
     </row>
@@ -15518,17 +15473,14 @@
       <c r="BC52" s="144" t="s">
         <v>53</v>
       </c>
-      <c r="BD52" s="157"/>
-      <c r="BE52" s="155"/>
-      <c r="BF52" s="155"/>
-      <c r="BG52" s="158"/>
-      <c r="BH52" s="155"/>
-      <c r="BI52" s="158"/>
-      <c r="BJ52" s="158"/>
-      <c r="BK52" s="158"/>
-      <c r="BL52" s="158"/>
-      <c r="BM52" s="157"/>
-      <c r="BN52" s="157"/>
+      <c r="BE52" s="154"/>
+      <c r="BF52" s="154"/>
+      <c r="BG52" s="155"/>
+      <c r="BH52" s="154"/>
+      <c r="BI52" s="155"/>
+      <c r="BJ52" s="155"/>
+      <c r="BK52" s="155"/>
+      <c r="BL52" s="155"/>
       <c r="BO52" s="112"/>
       <c r="BP52" s="112"/>
     </row>
@@ -15638,17 +15590,17 @@
       <c r="BC53" s="144" t="s">
         <v>54</v>
       </c>
-      <c r="BD53" s="158"/>
-      <c r="BE53" s="158"/>
-      <c r="BF53" s="158"/>
-      <c r="BG53" s="158"/>
-      <c r="BH53" s="158"/>
-      <c r="BI53" s="158"/>
-      <c r="BJ53" s="158"/>
-      <c r="BK53" s="158"/>
-      <c r="BL53" s="158"/>
-      <c r="BM53" s="158"/>
-      <c r="BN53" s="158"/>
+      <c r="BD53" s="155"/>
+      <c r="BE53" s="155"/>
+      <c r="BF53" s="155"/>
+      <c r="BG53" s="155"/>
+      <c r="BH53" s="155"/>
+      <c r="BI53" s="155"/>
+      <c r="BJ53" s="155"/>
+      <c r="BK53" s="155"/>
+      <c r="BL53" s="155"/>
+      <c r="BM53" s="155"/>
+      <c r="BN53" s="155"/>
       <c r="BO53" s="112"/>
       <c r="BP53" s="112"/>
     </row>
@@ -15773,17 +15725,16 @@
       <c r="BC54" s="144" t="s">
         <v>88</v>
       </c>
-      <c r="BD54" s="157"/>
-      <c r="BE54" s="155"/>
-      <c r="BF54" s="155"/>
-      <c r="BG54" s="158"/>
-      <c r="BH54" s="155"/>
-      <c r="BI54" s="158"/>
-      <c r="BJ54" s="158"/>
-      <c r="BK54" s="158"/>
-      <c r="BL54" s="158"/>
-      <c r="BM54" s="158"/>
-      <c r="BN54" s="158"/>
+      <c r="BE54" s="154"/>
+      <c r="BF54" s="154"/>
+      <c r="BG54" s="155"/>
+      <c r="BH54" s="154"/>
+      <c r="BI54" s="155"/>
+      <c r="BJ54" s="155"/>
+      <c r="BK54" s="155"/>
+      <c r="BL54" s="155"/>
+      <c r="BM54" s="155"/>
+      <c r="BN54" s="155"/>
       <c r="BO54" s="112"/>
       <c r="BP54" s="112"/>
       <c r="BR54" s="113"/>
@@ -15931,17 +15882,17 @@
         <v>20000</v>
       </c>
       <c r="BC55" s="1"/>
-      <c r="BD55" s="158"/>
-      <c r="BE55" s="158"/>
-      <c r="BF55" s="158"/>
-      <c r="BG55" s="158"/>
-      <c r="BH55" s="158"/>
-      <c r="BI55" s="158"/>
-      <c r="BJ55" s="158"/>
-      <c r="BK55" s="158"/>
-      <c r="BL55" s="158"/>
-      <c r="BM55" s="158"/>
-      <c r="BN55" s="158"/>
+      <c r="BD55" s="155"/>
+      <c r="BE55" s="155"/>
+      <c r="BF55" s="155"/>
+      <c r="BG55" s="155"/>
+      <c r="BH55" s="155"/>
+      <c r="BI55" s="155"/>
+      <c r="BJ55" s="155"/>
+      <c r="BK55" s="155"/>
+      <c r="BL55" s="155"/>
+      <c r="BM55" s="155"/>
+      <c r="BN55" s="155"/>
       <c r="BO55" s="112"/>
       <c r="BP55" s="112"/>
       <c r="BR55" s="113"/>
@@ -16088,17 +16039,17 @@
         <v>30000</v>
       </c>
       <c r="BC56" s="1"/>
-      <c r="BD56" s="158"/>
-      <c r="BE56" s="158"/>
-      <c r="BF56" s="158"/>
-      <c r="BG56" s="158"/>
-      <c r="BH56" s="158"/>
-      <c r="BI56" s="158"/>
-      <c r="BJ56" s="158"/>
-      <c r="BK56" s="158"/>
-      <c r="BL56" s="158"/>
-      <c r="BM56" s="158"/>
-      <c r="BN56" s="158"/>
+      <c r="BD56" s="155"/>
+      <c r="BE56" s="155"/>
+      <c r="BF56" s="155"/>
+      <c r="BG56" s="155"/>
+      <c r="BH56" s="155"/>
+      <c r="BI56" s="155"/>
+      <c r="BJ56" s="155"/>
+      <c r="BK56" s="155"/>
+      <c r="BL56" s="155"/>
+      <c r="BM56" s="155"/>
+      <c r="BN56" s="155"/>
       <c r="BO56" s="112"/>
       <c r="BP56" s="112"/>
       <c r="BR56" s="113"/>
@@ -16242,17 +16193,17 @@
         <v>-30000000</v>
       </c>
       <c r="BC57" s="1"/>
-      <c r="BD57" s="158"/>
-      <c r="BE57" s="158"/>
-      <c r="BF57" s="158"/>
-      <c r="BG57" s="158"/>
-      <c r="BH57" s="158"/>
-      <c r="BI57" s="158"/>
-      <c r="BJ57" s="158"/>
-      <c r="BK57" s="158"/>
-      <c r="BL57" s="158"/>
-      <c r="BM57" s="158"/>
-      <c r="BN57" s="158"/>
+      <c r="BD57" s="155"/>
+      <c r="BE57" s="155"/>
+      <c r="BF57" s="155"/>
+      <c r="BG57" s="155"/>
+      <c r="BH57" s="155"/>
+      <c r="BI57" s="155"/>
+      <c r="BJ57" s="155"/>
+      <c r="BK57" s="155"/>
+      <c r="BL57" s="155"/>
+      <c r="BM57" s="155"/>
+      <c r="BN57" s="155"/>
     </row>
     <row r="58" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A58" s="4"/>
@@ -16389,23 +16340,23 @@
       <c r="AZ58" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="BA58" s="158"/>
+      <c r="BA58" s="155"/>
       <c r="BB58" s="3">
         <f t="shared" si="36"/>
         <v>-13333333.333333334</v>
       </c>
-      <c r="BC58" s="158"/>
-      <c r="BD58" s="158"/>
-      <c r="BE58" s="158"/>
-      <c r="BF58" s="158"/>
-      <c r="BG58" s="158"/>
-      <c r="BH58" s="158"/>
-      <c r="BI58" s="158"/>
-      <c r="BJ58" s="158"/>
-      <c r="BK58" s="158"/>
-      <c r="BL58" s="158"/>
-      <c r="BM58" s="158"/>
-      <c r="BN58" s="158"/>
+      <c r="BC58" s="155"/>
+      <c r="BD58" s="155"/>
+      <c r="BE58" s="155"/>
+      <c r="BF58" s="155"/>
+      <c r="BG58" s="155"/>
+      <c r="BH58" s="155"/>
+      <c r="BI58" s="155"/>
+      <c r="BJ58" s="155"/>
+      <c r="BK58" s="155"/>
+      <c r="BL58" s="155"/>
+      <c r="BM58" s="155"/>
+      <c r="BN58" s="155"/>
     </row>
     <row r="59" spans="1:101" x14ac:dyDescent="0.2">
       <c r="A59" s="4"/>
@@ -16541,23 +16492,17 @@
       <c r="AZ59" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="BA59" s="158"/>
+      <c r="BA59" s="155"/>
       <c r="BB59" s="3">
         <f t="shared" si="36"/>
         <v>13333333.333333334</v>
       </c>
-      <c r="BC59" s="157"/>
-      <c r="BD59" s="157"/>
-      <c r="BE59" s="157"/>
-      <c r="BF59" s="157"/>
-      <c r="BG59" s="158"/>
-      <c r="BH59" s="158"/>
-      <c r="BI59" s="158"/>
-      <c r="BJ59" s="158"/>
-      <c r="BK59" s="158"/>
-      <c r="BL59" s="158"/>
-      <c r="BM59" s="157"/>
-      <c r="BN59" s="157"/>
+      <c r="BG59" s="155"/>
+      <c r="BH59" s="155"/>
+      <c r="BI59" s="155"/>
+      <c r="BJ59" s="155"/>
+      <c r="BK59" s="155"/>
+      <c r="BL59" s="155"/>
       <c r="BT59" s="112"/>
       <c r="BY59" s="117"/>
       <c r="CA59" s="118"/>
@@ -16634,21 +16579,15 @@
       <c r="AW60" s="4"/>
       <c r="AX60" s="4"/>
       <c r="AY60" s="4"/>
-      <c r="AZ60" s="156"/>
-      <c r="BA60" s="158"/>
-      <c r="BB60" s="158"/>
-      <c r="BC60" s="157"/>
-      <c r="BD60" s="157"/>
-      <c r="BE60" s="157"/>
-      <c r="BF60" s="157"/>
-      <c r="BG60" s="158"/>
-      <c r="BH60" s="158"/>
-      <c r="BI60" s="158"/>
-      <c r="BJ60" s="158"/>
-      <c r="BK60" s="158"/>
-      <c r="BL60" s="158"/>
-      <c r="BM60" s="157"/>
-      <c r="BN60" s="157"/>
+      <c r="AZ60" s="4"/>
+      <c r="BA60" s="155"/>
+      <c r="BB60" s="155"/>
+      <c r="BG60" s="155"/>
+      <c r="BH60" s="155"/>
+      <c r="BI60" s="155"/>
+      <c r="BJ60" s="155"/>
+      <c r="BK60" s="155"/>
+      <c r="BL60" s="155"/>
       <c r="BT60" s="112"/>
       <c r="BY60" s="117"/>
       <c r="CA60" s="118"/>
@@ -17805,9 +17744,27 @@
       <c r="BY89" s="117"/>
       <c r="CA89" s="118"/>
     </row>
-    <row r="90" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:79" x14ac:dyDescent="0.2">
+      <c r="AK90" s="16"/>
+      <c r="AL90" s="16"/>
+      <c r="AM90" s="16"/>
+      <c r="AN90" s="16"/>
+      <c r="AO90" s="16"/>
+      <c r="AP90" s="16"/>
+      <c r="AQ90" s="156"/>
+      <c r="AR90" s="156"/>
+      <c r="AS90" s="156"/>
+      <c r="AT90" s="156"/>
+      <c r="AU90" s="156"/>
+      <c r="AV90" s="156"/>
+      <c r="AW90" s="156"/>
+      <c r="AX90" s="156"/>
+      <c r="AY90" s="157"/>
       <c r="AZ90" s="111"/>
+      <c r="BA90" s="157"/>
       <c r="BB90" s="111"/>
+      <c r="BC90" s="157"/>
+      <c r="BD90" s="157"/>
       <c r="BE90" s="111"/>
       <c r="BK90" s="116"/>
       <c r="BL90" s="116"/>
@@ -17820,7 +17777,27 @@
       <c r="BY90" s="117"/>
       <c r="CA90" s="118"/>
     </row>
-    <row r="91" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:79" x14ac:dyDescent="0.2">
+      <c r="AK91" s="16"/>
+      <c r="AL91" s="16"/>
+      <c r="AM91" s="16"/>
+      <c r="AN91" s="16"/>
+      <c r="AO91" s="16"/>
+      <c r="AP91" s="16"/>
+      <c r="AQ91" s="156"/>
+      <c r="AR91" s="156"/>
+      <c r="AS91" s="156"/>
+      <c r="AT91" s="156"/>
+      <c r="AU91" s="156"/>
+      <c r="AV91" s="156"/>
+      <c r="AW91" s="156"/>
+      <c r="AX91" s="156"/>
+      <c r="AY91" s="157"/>
+      <c r="AZ91" s="157"/>
+      <c r="BA91" s="157"/>
+      <c r="BB91" s="157"/>
+      <c r="BC91" s="157"/>
+      <c r="BD91" s="157"/>
       <c r="BE91" s="111"/>
       <c r="BK91" s="116"/>
       <c r="BL91" s="116"/>
@@ -17833,7 +17810,27 @@
       <c r="BY91" s="117"/>
       <c r="CA91" s="118"/>
     </row>
-    <row r="92" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:79" x14ac:dyDescent="0.2">
+      <c r="AK92" s="16"/>
+      <c r="AL92" s="16"/>
+      <c r="AM92" s="16"/>
+      <c r="AN92" s="16"/>
+      <c r="AO92" s="16"/>
+      <c r="AP92" s="16"/>
+      <c r="AQ92" s="156"/>
+      <c r="AR92" s="156"/>
+      <c r="AS92" s="156"/>
+      <c r="AT92" s="156"/>
+      <c r="AU92" s="156"/>
+      <c r="AV92" s="156"/>
+      <c r="AW92" s="156"/>
+      <c r="AX92" s="156"/>
+      <c r="AY92" s="157"/>
+      <c r="AZ92" s="157"/>
+      <c r="BA92" s="157"/>
+      <c r="BB92" s="157"/>
+      <c r="BC92" s="157"/>
+      <c r="BD92" s="157"/>
       <c r="BE92" s="111"/>
       <c r="BK92" s="116"/>
       <c r="BL92" s="116"/>
@@ -17846,7 +17843,27 @@
       <c r="BY92" s="117"/>
       <c r="CA92" s="118"/>
     </row>
-    <row r="93" spans="1:79" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:79" x14ac:dyDescent="0.2">
+      <c r="AK93" s="16"/>
+      <c r="AL93" s="16"/>
+      <c r="AM93" s="16"/>
+      <c r="AN93" s="16"/>
+      <c r="AO93" s="16"/>
+      <c r="AP93" s="16"/>
+      <c r="AQ93" s="16"/>
+      <c r="AR93" s="156"/>
+      <c r="AS93" s="156"/>
+      <c r="AT93" s="156"/>
+      <c r="AU93" s="16"/>
+      <c r="AV93" s="16"/>
+      <c r="AW93" s="156"/>
+      <c r="AX93" s="156"/>
+      <c r="AY93" s="157"/>
+      <c r="AZ93" s="158"/>
+      <c r="BA93" s="157"/>
+      <c r="BB93" s="157"/>
+      <c r="BC93" s="157"/>
+      <c r="BD93" s="157"/>
       <c r="BE93" s="111"/>
       <c r="BK93" s="116"/>
       <c r="BL93" s="116"/>
@@ -17859,9 +17876,225 @@
       <c r="BY93" s="117"/>
       <c r="CA93" s="118"/>
     </row>
-    <row r="100" spans="23:70" x14ac:dyDescent="0.25">
-      <c r="BC100" s="112"/>
-      <c r="BD100" s="112"/>
+    <row r="94" spans="1:79" x14ac:dyDescent="0.2">
+      <c r="AK94" s="16"/>
+      <c r="AL94" s="16"/>
+      <c r="AM94" s="16"/>
+      <c r="AN94" s="16"/>
+      <c r="AO94" s="16"/>
+      <c r="AP94" s="16"/>
+      <c r="AQ94" s="16"/>
+      <c r="AR94" s="156"/>
+      <c r="AS94" s="156"/>
+      <c r="AT94" s="156"/>
+      <c r="AU94" s="16"/>
+      <c r="AV94" s="16"/>
+      <c r="AW94" s="156"/>
+      <c r="AX94" s="156"/>
+      <c r="AY94" s="157"/>
+      <c r="AZ94" s="157"/>
+      <c r="BA94" s="157"/>
+      <c r="BB94" s="157"/>
+      <c r="BC94" s="157"/>
+      <c r="BD94" s="157"/>
+    </row>
+    <row r="95" spans="1:79" x14ac:dyDescent="0.2">
+      <c r="AK95" s="16"/>
+      <c r="AL95" s="16"/>
+      <c r="AM95" s="16"/>
+      <c r="AN95" s="16"/>
+      <c r="AO95" s="16"/>
+      <c r="AP95" s="16"/>
+      <c r="AQ95" s="156"/>
+      <c r="AR95" s="156"/>
+      <c r="AS95" s="156"/>
+      <c r="AT95" s="156"/>
+      <c r="AU95" s="156"/>
+      <c r="AV95" s="156"/>
+      <c r="AW95" s="156"/>
+      <c r="AX95" s="156"/>
+      <c r="AY95" s="157"/>
+      <c r="AZ95" s="157"/>
+      <c r="BA95" s="157"/>
+      <c r="BB95" s="157"/>
+      <c r="BC95" s="157"/>
+      <c r="BD95" s="157"/>
+    </row>
+    <row r="96" spans="1:79" x14ac:dyDescent="0.2">
+      <c r="AK96" s="156"/>
+      <c r="AL96" s="156"/>
+      <c r="AM96" s="156"/>
+      <c r="AN96" s="16"/>
+      <c r="AO96" s="16"/>
+      <c r="AP96" s="156"/>
+      <c r="AQ96" s="16"/>
+      <c r="AR96" s="156"/>
+      <c r="AS96" s="156"/>
+      <c r="AT96" s="156"/>
+      <c r="AU96" s="16"/>
+      <c r="AV96" s="16"/>
+      <c r="AW96" s="156"/>
+      <c r="AX96" s="156"/>
+      <c r="AY96" s="157"/>
+      <c r="AZ96" s="157"/>
+      <c r="BA96" s="157"/>
+      <c r="BB96" s="157"/>
+      <c r="BC96" s="157"/>
+      <c r="BD96" s="157"/>
+    </row>
+    <row r="97" spans="23:70" x14ac:dyDescent="0.2">
+      <c r="AK97" s="156"/>
+      <c r="AL97" s="156"/>
+      <c r="AM97" s="156"/>
+      <c r="AN97" s="156"/>
+      <c r="AO97" s="156"/>
+      <c r="AP97" s="156"/>
+      <c r="AQ97" s="156"/>
+      <c r="AR97" s="16"/>
+      <c r="AS97" s="16"/>
+      <c r="AT97" s="16"/>
+      <c r="AU97" s="16"/>
+      <c r="AV97" s="16"/>
+      <c r="AW97" s="156"/>
+      <c r="AX97" s="156"/>
+      <c r="AY97" s="157"/>
+      <c r="AZ97" s="157"/>
+      <c r="BA97" s="157"/>
+      <c r="BB97" s="157"/>
+      <c r="BC97" s="157"/>
+      <c r="BD97" s="157"/>
+    </row>
+    <row r="98" spans="23:70" x14ac:dyDescent="0.2">
+      <c r="AK98" s="156"/>
+      <c r="AL98" s="156"/>
+      <c r="AM98" s="156"/>
+      <c r="AN98" s="156"/>
+      <c r="AO98" s="156"/>
+      <c r="AP98" s="156"/>
+      <c r="AQ98" s="156"/>
+      <c r="AR98" s="16"/>
+      <c r="AS98" s="16"/>
+      <c r="AT98" s="16"/>
+      <c r="AU98" s="16"/>
+      <c r="AV98" s="16"/>
+      <c r="AW98" s="156"/>
+      <c r="AX98" s="156"/>
+      <c r="AY98" s="157"/>
+      <c r="AZ98" s="157"/>
+      <c r="BA98" s="157"/>
+      <c r="BB98" s="157"/>
+      <c r="BC98" s="157"/>
+      <c r="BD98" s="157"/>
+    </row>
+    <row r="99" spans="23:70" x14ac:dyDescent="0.2">
+      <c r="AK99" s="156"/>
+      <c r="AL99" s="156"/>
+      <c r="AM99" s="156"/>
+      <c r="AN99" s="156"/>
+      <c r="AO99" s="156"/>
+      <c r="AP99" s="156"/>
+      <c r="AQ99" s="156"/>
+      <c r="AR99" s="16"/>
+      <c r="AS99" s="16"/>
+      <c r="AT99" s="16"/>
+      <c r="AU99" s="16"/>
+      <c r="AV99" s="16"/>
+      <c r="AW99" s="156"/>
+      <c r="AX99" s="156"/>
+      <c r="AY99" s="157"/>
+      <c r="AZ99" s="158"/>
+      <c r="BA99" s="157"/>
+      <c r="BB99" s="157"/>
+      <c r="BC99" s="157"/>
+      <c r="BD99" s="157"/>
+    </row>
+    <row r="100" spans="23:70" x14ac:dyDescent="0.2">
+      <c r="AK100" s="156"/>
+      <c r="AL100" s="156"/>
+      <c r="AM100" s="156"/>
+      <c r="AN100" s="16"/>
+      <c r="AO100" s="16"/>
+      <c r="AP100" s="156"/>
+      <c r="AQ100" s="16"/>
+      <c r="AR100" s="16"/>
+      <c r="AS100" s="16"/>
+      <c r="AT100" s="16"/>
+      <c r="AU100" s="16"/>
+      <c r="AV100" s="16"/>
+      <c r="AW100" s="156"/>
+      <c r="AX100" s="156"/>
+      <c r="AY100" s="157"/>
+      <c r="AZ100" s="157"/>
+      <c r="BA100" s="157"/>
+      <c r="BB100" s="157"/>
+      <c r="BC100" s="159"/>
+      <c r="BD100" s="159"/>
+    </row>
+    <row r="101" spans="23:70" x14ac:dyDescent="0.2">
+      <c r="AK101" s="156"/>
+      <c r="AL101" s="156"/>
+      <c r="AM101" s="156"/>
+      <c r="AN101" s="16"/>
+      <c r="AO101" s="16"/>
+      <c r="AP101" s="156"/>
+      <c r="AQ101" s="16"/>
+      <c r="AR101" s="16"/>
+      <c r="AS101" s="16"/>
+      <c r="AT101" s="16"/>
+      <c r="AU101" s="16"/>
+      <c r="AV101" s="16"/>
+      <c r="AW101" s="156"/>
+      <c r="AX101" s="156"/>
+      <c r="AY101" s="157"/>
+      <c r="AZ101" s="157"/>
+      <c r="BA101" s="157"/>
+      <c r="BB101" s="157"/>
+      <c r="BC101" s="157"/>
+      <c r="BD101" s="157"/>
+    </row>
+    <row r="102" spans="23:70" x14ac:dyDescent="0.2">
+      <c r="AK102" s="156"/>
+      <c r="AL102" s="156"/>
+      <c r="AM102" s="156"/>
+      <c r="AN102" s="156"/>
+      <c r="AO102" s="156"/>
+      <c r="AP102" s="156"/>
+      <c r="AQ102" s="156"/>
+      <c r="AR102" s="156"/>
+      <c r="AS102" s="156"/>
+      <c r="AT102" s="156"/>
+      <c r="AU102" s="156"/>
+      <c r="AV102" s="156"/>
+      <c r="AW102" s="156"/>
+      <c r="AX102" s="156"/>
+      <c r="AY102" s="157"/>
+      <c r="AZ102" s="157"/>
+      <c r="BA102" s="157"/>
+      <c r="BB102" s="157"/>
+      <c r="BC102" s="157"/>
+      <c r="BD102" s="157"/>
+    </row>
+    <row r="103" spans="23:70" x14ac:dyDescent="0.2">
+      <c r="AK103" s="156"/>
+      <c r="AL103" s="156"/>
+      <c r="AM103" s="156"/>
+      <c r="AN103" s="156"/>
+      <c r="AO103" s="156"/>
+      <c r="AP103" s="156"/>
+      <c r="AQ103" s="156"/>
+      <c r="AR103" s="156"/>
+      <c r="AS103" s="156"/>
+      <c r="AT103" s="156"/>
+      <c r="AU103" s="156"/>
+      <c r="AV103" s="156"/>
+      <c r="AW103" s="156"/>
+      <c r="AX103" s="156"/>
+      <c r="AY103" s="157"/>
+      <c r="AZ103" s="157"/>
+      <c r="BA103" s="157"/>
+      <c r="BB103" s="157"/>
+      <c r="BC103" s="157"/>
+      <c r="BD103" s="157"/>
     </row>
     <row r="108" spans="23:70" x14ac:dyDescent="0.25">
       <c r="AZ108" s="111"/>
@@ -19011,17 +19244,27 @@
     </row>
   </sheetData>
   <phoneticPr fontId="14" type="noConversion"/>
+  <conditionalFormatting sqref="AK46:AX59">
+    <cfRule type="expression" dxfId="6" priority="3">
+      <formula>ABS(AK46)&lt;0.1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BB46:BB59">
+    <cfRule type="expression" dxfId="5" priority="2">
+      <formula>ABS(BB46)&lt;0.1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="BR172:BR174">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>"VIRHE!"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
       <formula>"OK!"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AK46:AX59">
+  <conditionalFormatting sqref="AK90:AX103">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>ABS(AK46)&lt;0.1</formula>
+      <formula>ABS(AK90)&lt;0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fix eq load sign issue
</commit_message>
<xml_diff>
--- a/theory/FEM matriisit.xlsx
+++ b/theory/FEM matriisit.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ohjelmointi\2_Rust\idfem\theory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B648D7F7-F766-498B-B267-E95AF951A284}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{176A2867-7B30-45AB-BD3B-B940FBC54AA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22230" yWindow="0" windowWidth="22335" windowHeight="20880" activeTab="1" xr2:uid="{27180542-B0D2-4BFE-946B-7857B24C93C8}"/>
+    <workbookView xWindow="-22230" yWindow="0" windowWidth="22335" windowHeight="20880" activeTab="2" xr2:uid="{27180542-B0D2-4BFE-946B-7857B24C93C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Ilman vapautuksia" sheetId="1" r:id="rId1"/>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="94">
   <si>
     <t>°</t>
   </si>
@@ -381,12 +381,6 @@
     <t>N (/Nmm)</t>
   </si>
   <si>
-    <t>Huom! Pystykuorma osoittaa alaspäin! Vaikuttaa siihen, miten ekvivalentit kuormat (horisontaalinen ja momentt)</t>
-  </si>
-  <si>
-    <t>pitää ohjelmassa huomioida (toisin kuin vaakasuuntainen, joka jo osoittaa oikealle (0°))</t>
-  </si>
-  <si>
     <t>Lukkovoimaesimerkissä kuorma osoittaa alaspäin positiivisena</t>
   </si>
   <si>
@@ -403,6 +397,27 @@
   </si>
   <si>
     <t>+Q33</t>
+  </si>
+  <si>
+    <t>=&gt;</t>
+  </si>
+  <si>
+    <t>Reaktiot</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>d/2</t>
+  </si>
+  <si>
+    <t>q</t>
   </si>
 </sst>
 </file>
@@ -697,7 +712,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="160">
+  <cellXfs count="156">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1106,24 +1121,117 @@
     <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutraali" xfId="1" builtinId="28"/>
     <cellStyle name="Normaali" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="40">
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
@@ -1164,6 +1272,12 @@
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -1191,9 +1305,75 @@
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
       <font>
-        <color auto="1"/>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
       </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
   </dxfs>
@@ -1406,7 +1586,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>63</xdr:col>
-      <xdr:colOff>329924</xdr:colOff>
+      <xdr:colOff>166638</xdr:colOff>
       <xdr:row>43</xdr:row>
       <xdr:rowOff>28196</xdr:rowOff>
     </xdr:to>
@@ -1861,7 +2041,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94F9BDF3-3EE6-4BFB-9734-CB047BC6E804}">
   <dimension ref="B1:CW227"/>
   <sheetViews>
-    <sheetView topLeftCell="AN12" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="AI24" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="AZ45" sqref="AZ45"/>
     </sheetView>
   </sheetViews>
@@ -7589,7 +7769,7 @@
         <v>-3.06287113727155E-13</v>
       </c>
       <c r="P64" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="AJ64" s="78">
         <v>9</v>
@@ -7661,7 +7841,7 @@
         <v>5000</v>
       </c>
       <c r="P65" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="AJ65" s="78">
         <v>10</v>
@@ -10033,20 +10213,20 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="AK43:AV54">
-    <cfRule type="expression" dxfId="10" priority="2">
+    <cfRule type="expression" dxfId="9" priority="2">
       <formula>ABS(AK43)&lt;0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AZ43:AZ54">
-    <cfRule type="expression" dxfId="9" priority="1">
+    <cfRule type="expression" dxfId="8" priority="1">
       <formula>ABS(AZ43)&lt;0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BR166:BR168">
-    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
       <formula>"VIRHE!"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
       <formula>"OK!"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10059,8 +10239,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F95DF150-D06E-47EC-89DA-0EC5D53947FD}">
   <dimension ref="A1:CW233"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AH24" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AT92" sqref="AT92"/>
+    <sheetView topLeftCell="AH1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="BD49" sqref="BD49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.25"/>
@@ -10081,7 +10261,9 @@
     <col min="49" max="50" width="11.5703125" style="80" bestFit="1" customWidth="1"/>
     <col min="51" max="53" width="9.140625" style="80"/>
     <col min="54" max="54" width="12.28515625" style="80" bestFit="1" customWidth="1"/>
-    <col min="55" max="16384" width="9.140625" style="80"/>
+    <col min="55" max="57" width="9.140625" style="80"/>
+    <col min="58" max="58" width="11.5703125" style="80" bestFit="1" customWidth="1"/>
+    <col min="59" max="16384" width="9.140625" style="80"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:67" x14ac:dyDescent="0.2">
@@ -14455,7 +14637,15 @@
       <c r="BB45" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="BC45" s="1"/>
+      <c r="BC45" s="146" t="s">
+        <v>87</v>
+      </c>
+      <c r="BD45" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="BF45" s="80" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="46" spans="1:83" x14ac:dyDescent="0.2">
       <c r="A46" s="4"/>
@@ -14602,9 +14792,15 @@
       <c r="BC46" s="144" t="s">
         <v>52</v>
       </c>
-      <c r="BD46" s="4"/>
+      <c r="BD46" s="29" cm="1">
+        <f t="array" ref="BD46:BD48">AZ46:AZ48</f>
+        <v>0</v>
+      </c>
       <c r="BE46" s="4"/>
-      <c r="BF46" s="4"/>
+      <c r="BF46" s="4">
+        <f t="array" ref="BF46:BF59">MMULT(AK46:AX59,BD46:BD59)-BB46:BB59</f>
+        <v>25000.878854754606</v>
+      </c>
       <c r="BG46" s="4"/>
       <c r="BH46" s="4"/>
       <c r="BI46" s="4"/>
@@ -14758,8 +14954,13 @@
       <c r="BC47" s="144" t="s">
         <v>51</v>
       </c>
+      <c r="BD47" s="29">
+        <v>0</v>
+      </c>
       <c r="BE47" s="154"/>
-      <c r="BF47" s="154"/>
+      <c r="BF47" s="154">
+        <v>-30000</v>
+      </c>
       <c r="BG47" s="155"/>
       <c r="BH47" s="155"/>
       <c r="BI47" s="155"/>
@@ -14910,10 +15111,15 @@
         <v>13333333.333333334</v>
       </c>
       <c r="BC48" s="144" t="s">
-        <v>85</v>
+        <v>83</v>
+      </c>
+      <c r="BD48" s="29">
+        <v>0</v>
       </c>
       <c r="BE48" s="154"/>
-      <c r="BF48" s="154"/>
+      <c r="BF48" s="154">
+        <v>-20003515.419018425</v>
+      </c>
       <c r="BG48" s="155"/>
       <c r="BH48" s="154"/>
       <c r="BI48" s="155"/>
@@ -15068,8 +15274,14 @@
         <v>-20000</v>
       </c>
       <c r="BC49" s="1"/>
+      <c r="BD49" s="153" cm="1">
+        <f t="array" ref="BD49:BD51">AV77:AV79</f>
+        <v>-1.0713657960906176E-2</v>
+      </c>
       <c r="BE49" s="154"/>
-      <c r="BF49" s="154"/>
+      <c r="BF49" s="154">
+        <v>2.151500666514039E-8</v>
+      </c>
       <c r="BG49" s="155"/>
       <c r="BH49" s="154"/>
       <c r="BI49" s="155"/>
@@ -15222,6 +15434,12 @@
         <v>30000</v>
       </c>
       <c r="BC50" s="1"/>
+      <c r="BD50" s="153">
+        <v>5.7142857142857141E-2</v>
+      </c>
+      <c r="BF50" s="80">
+        <v>0</v>
+      </c>
       <c r="BG50" s="155"/>
       <c r="BH50" s="154"/>
       <c r="BI50" s="155"/>
@@ -15358,8 +15576,13 @@
         <v>30000000</v>
       </c>
       <c r="BC51" s="1"/>
+      <c r="BD51" s="153">
+        <v>6.4285714285714276E-3</v>
+      </c>
       <c r="BE51" s="154"/>
-      <c r="BF51" s="154"/>
+      <c r="BF51" s="154">
+        <v>0</v>
+      </c>
       <c r="BG51" s="155"/>
       <c r="BH51" s="154"/>
       <c r="BI51" s="155"/>
@@ -15473,8 +15696,14 @@
       <c r="BC52" s="144" t="s">
         <v>53</v>
       </c>
+      <c r="BD52" s="29" cm="1">
+        <f t="array" ref="BD52:BD54">AZ52:AZ54</f>
+        <v>0</v>
+      </c>
       <c r="BE52" s="154"/>
-      <c r="BF52" s="154"/>
+      <c r="BF52" s="154">
+        <v>-25000.878854754599</v>
+      </c>
       <c r="BG52" s="155"/>
       <c r="BH52" s="154"/>
       <c r="BI52" s="155"/>
@@ -15590,9 +15819,13 @@
       <c r="BC53" s="144" t="s">
         <v>54</v>
       </c>
-      <c r="BD53" s="155"/>
+      <c r="BD53" s="29">
+        <v>0</v>
+      </c>
       <c r="BE53" s="155"/>
-      <c r="BF53" s="155"/>
+      <c r="BF53" s="155">
+        <v>-30000</v>
+      </c>
       <c r="BG53" s="155"/>
       <c r="BH53" s="155"/>
       <c r="BI53" s="155"/>
@@ -15723,10 +15956,15 @@
         <v>-13333333.333333334</v>
       </c>
       <c r="BC54" s="144" t="s">
-        <v>88</v>
+        <v>86</v>
+      </c>
+      <c r="BD54" s="29">
+        <v>0</v>
       </c>
       <c r="BE54" s="154"/>
-      <c r="BF54" s="154"/>
+      <c r="BF54" s="154">
+        <v>20003515.419018395</v>
+      </c>
       <c r="BG54" s="155"/>
       <c r="BH54" s="154"/>
       <c r="BI54" s="155"/>
@@ -15882,9 +16120,14 @@
         <v>20000</v>
       </c>
       <c r="BC55" s="1"/>
-      <c r="BD55" s="155"/>
+      <c r="BD55" s="153" cm="1">
+        <f t="array" ref="BD55:BD59">AV80:AV84</f>
+        <v>1.0713657960842227E-2</v>
+      </c>
       <c r="BE55" s="155"/>
-      <c r="BF55" s="155"/>
+      <c r="BF55" s="155">
+        <v>-2.1522282622754574E-8</v>
+      </c>
       <c r="BG55" s="155"/>
       <c r="BH55" s="155"/>
       <c r="BI55" s="155"/>
@@ -16039,9 +16282,13 @@
         <v>30000</v>
       </c>
       <c r="BC56" s="1"/>
-      <c r="BD56" s="155"/>
+      <c r="BD56" s="153">
+        <v>5.7142857142857141E-2</v>
+      </c>
       <c r="BE56" s="155"/>
-      <c r="BF56" s="155"/>
+      <c r="BF56" s="155">
+        <v>0</v>
+      </c>
       <c r="BG56" s="155"/>
       <c r="BH56" s="155"/>
       <c r="BI56" s="155"/>
@@ -16193,9 +16440,13 @@
         <v>-30000000</v>
       </c>
       <c r="BC57" s="1"/>
-      <c r="BD57" s="155"/>
+      <c r="BD57" s="153">
+        <v>-6.4285714285714276E-3</v>
+      </c>
       <c r="BE57" s="155"/>
-      <c r="BF57" s="155"/>
+      <c r="BF57" s="155">
+        <v>0</v>
+      </c>
       <c r="BG57" s="155"/>
       <c r="BH57" s="155"/>
       <c r="BI57" s="155"/>
@@ -16338,7 +16589,7 @@
       </c>
       <c r="AY58" s="4"/>
       <c r="AZ58" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="BA58" s="155"/>
       <c r="BB58" s="3">
@@ -16346,9 +16597,13 @@
         <v>-13333333.333333334</v>
       </c>
       <c r="BC58" s="155"/>
-      <c r="BD58" s="155"/>
+      <c r="BD58" s="153">
+        <v>-7.6150299973122802E-3</v>
+      </c>
       <c r="BE58" s="155"/>
-      <c r="BF58" s="155"/>
+      <c r="BF58" s="155">
+        <v>0</v>
+      </c>
       <c r="BG58" s="155"/>
       <c r="BH58" s="155"/>
       <c r="BI58" s="155"/>
@@ -16490,12 +16745,18 @@
       </c>
       <c r="AY59" s="4"/>
       <c r="AZ59" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="BA59" s="155"/>
       <c r="BB59" s="3">
         <f t="shared" si="36"/>
         <v>13333333.333333334</v>
+      </c>
+      <c r="BD59" s="153">
+        <v>7.6150299973122958E-3</v>
+      </c>
+      <c r="BF59" s="80">
+        <v>0</v>
       </c>
       <c r="BG59" s="155"/>
       <c r="BH59" s="155"/>
@@ -17751,20 +18012,16 @@
       <c r="AN90" s="16"/>
       <c r="AO90" s="16"/>
       <c r="AP90" s="16"/>
-      <c r="AQ90" s="156"/>
-      <c r="AR90" s="156"/>
-      <c r="AS90" s="156"/>
-      <c r="AT90" s="156"/>
-      <c r="AU90" s="156"/>
-      <c r="AV90" s="156"/>
-      <c r="AW90" s="156"/>
-      <c r="AX90" s="156"/>
-      <c r="AY90" s="157"/>
+      <c r="AQ90" s="7"/>
+      <c r="AR90" s="7"/>
+      <c r="AS90" s="7"/>
+      <c r="AT90" s="7"/>
+      <c r="AU90" s="7"/>
+      <c r="AV90" s="7"/>
+      <c r="AW90" s="7"/>
+      <c r="AX90" s="7"/>
       <c r="AZ90" s="111"/>
-      <c r="BA90" s="157"/>
       <c r="BB90" s="111"/>
-      <c r="BC90" s="157"/>
-      <c r="BD90" s="157"/>
       <c r="BE90" s="111"/>
       <c r="BK90" s="116"/>
       <c r="BL90" s="116"/>
@@ -17784,20 +18041,14 @@
       <c r="AN91" s="16"/>
       <c r="AO91" s="16"/>
       <c r="AP91" s="16"/>
-      <c r="AQ91" s="156"/>
-      <c r="AR91" s="156"/>
-      <c r="AS91" s="156"/>
-      <c r="AT91" s="156"/>
-      <c r="AU91" s="156"/>
-      <c r="AV91" s="156"/>
-      <c r="AW91" s="156"/>
-      <c r="AX91" s="156"/>
-      <c r="AY91" s="157"/>
-      <c r="AZ91" s="157"/>
-      <c r="BA91" s="157"/>
-      <c r="BB91" s="157"/>
-      <c r="BC91" s="157"/>
-      <c r="BD91" s="157"/>
+      <c r="AQ91" s="7"/>
+      <c r="AR91" s="7"/>
+      <c r="AS91" s="7"/>
+      <c r="AT91" s="7"/>
+      <c r="AU91" s="7"/>
+      <c r="AV91" s="7"/>
+      <c r="AW91" s="7"/>
+      <c r="AX91" s="7"/>
       <c r="BE91" s="111"/>
       <c r="BK91" s="116"/>
       <c r="BL91" s="116"/>
@@ -17817,20 +18068,14 @@
       <c r="AN92" s="16"/>
       <c r="AO92" s="16"/>
       <c r="AP92" s="16"/>
-      <c r="AQ92" s="156"/>
-      <c r="AR92" s="156"/>
-      <c r="AS92" s="156"/>
-      <c r="AT92" s="156"/>
-      <c r="AU92" s="156"/>
-      <c r="AV92" s="156"/>
-      <c r="AW92" s="156"/>
-      <c r="AX92" s="156"/>
-      <c r="AY92" s="157"/>
-      <c r="AZ92" s="157"/>
-      <c r="BA92" s="157"/>
-      <c r="BB92" s="157"/>
-      <c r="BC92" s="157"/>
-      <c r="BD92" s="157"/>
+      <c r="AQ92" s="7"/>
+      <c r="AR92" s="7"/>
+      <c r="AS92" s="7"/>
+      <c r="AT92" s="7"/>
+      <c r="AU92" s="7"/>
+      <c r="AV92" s="7"/>
+      <c r="AW92" s="7"/>
+      <c r="AX92" s="7"/>
       <c r="BE92" s="111"/>
       <c r="BK92" s="116"/>
       <c r="BL92" s="116"/>
@@ -17851,19 +18096,14 @@
       <c r="AO93" s="16"/>
       <c r="AP93" s="16"/>
       <c r="AQ93" s="16"/>
-      <c r="AR93" s="156"/>
-      <c r="AS93" s="156"/>
-      <c r="AT93" s="156"/>
+      <c r="AR93" s="7"/>
+      <c r="AS93" s="7"/>
+      <c r="AT93" s="7"/>
       <c r="AU93" s="16"/>
       <c r="AV93" s="16"/>
-      <c r="AW93" s="156"/>
-      <c r="AX93" s="156"/>
-      <c r="AY93" s="157"/>
-      <c r="AZ93" s="158"/>
-      <c r="BA93" s="157"/>
-      <c r="BB93" s="157"/>
-      <c r="BC93" s="157"/>
-      <c r="BD93" s="157"/>
+      <c r="AW93" s="7"/>
+      <c r="AX93" s="7"/>
+      <c r="AZ93" s="116"/>
       <c r="BE93" s="111"/>
       <c r="BK93" s="116"/>
       <c r="BL93" s="116"/>
@@ -17884,19 +18124,13 @@
       <c r="AO94" s="16"/>
       <c r="AP94" s="16"/>
       <c r="AQ94" s="16"/>
-      <c r="AR94" s="156"/>
-      <c r="AS94" s="156"/>
-      <c r="AT94" s="156"/>
+      <c r="AR94" s="7"/>
+      <c r="AS94" s="7"/>
+      <c r="AT94" s="7"/>
       <c r="AU94" s="16"/>
       <c r="AV94" s="16"/>
-      <c r="AW94" s="156"/>
-      <c r="AX94" s="156"/>
-      <c r="AY94" s="157"/>
-      <c r="AZ94" s="157"/>
-      <c r="BA94" s="157"/>
-      <c r="BB94" s="157"/>
-      <c r="BC94" s="157"/>
-      <c r="BD94" s="157"/>
+      <c r="AW94" s="7"/>
+      <c r="AX94" s="7"/>
     </row>
     <row r="95" spans="1:79" x14ac:dyDescent="0.2">
       <c r="AK95" s="16"/>
@@ -17905,196 +18139,145 @@
       <c r="AN95" s="16"/>
       <c r="AO95" s="16"/>
       <c r="AP95" s="16"/>
-      <c r="AQ95" s="156"/>
-      <c r="AR95" s="156"/>
-      <c r="AS95" s="156"/>
-      <c r="AT95" s="156"/>
-      <c r="AU95" s="156"/>
-      <c r="AV95" s="156"/>
-      <c r="AW95" s="156"/>
-      <c r="AX95" s="156"/>
-      <c r="AY95" s="157"/>
-      <c r="AZ95" s="157"/>
-      <c r="BA95" s="157"/>
-      <c r="BB95" s="157"/>
-      <c r="BC95" s="157"/>
-      <c r="BD95" s="157"/>
+      <c r="AQ95" s="7"/>
+      <c r="AR95" s="7"/>
+      <c r="AS95" s="7"/>
+      <c r="AT95" s="7"/>
+      <c r="AU95" s="7"/>
+      <c r="AV95" s="7"/>
+      <c r="AW95" s="7"/>
+      <c r="AX95" s="7"/>
     </row>
     <row r="96" spans="1:79" x14ac:dyDescent="0.2">
-      <c r="AK96" s="156"/>
-      <c r="AL96" s="156"/>
-      <c r="AM96" s="156"/>
+      <c r="AK96" s="7"/>
+      <c r="AL96" s="7"/>
+      <c r="AM96" s="7"/>
       <c r="AN96" s="16"/>
       <c r="AO96" s="16"/>
-      <c r="AP96" s="156"/>
+      <c r="AP96" s="7"/>
       <c r="AQ96" s="16"/>
-      <c r="AR96" s="156"/>
-      <c r="AS96" s="156"/>
-      <c r="AT96" s="156"/>
+      <c r="AR96" s="7"/>
+      <c r="AS96" s="7"/>
+      <c r="AT96" s="7"/>
       <c r="AU96" s="16"/>
       <c r="AV96" s="16"/>
-      <c r="AW96" s="156"/>
-      <c r="AX96" s="156"/>
-      <c r="AY96" s="157"/>
-      <c r="AZ96" s="157"/>
-      <c r="BA96" s="157"/>
-      <c r="BB96" s="157"/>
-      <c r="BC96" s="157"/>
-      <c r="BD96" s="157"/>
+      <c r="AW96" s="7"/>
+      <c r="AX96" s="7"/>
     </row>
     <row r="97" spans="23:70" x14ac:dyDescent="0.2">
-      <c r="AK97" s="156"/>
-      <c r="AL97" s="156"/>
-      <c r="AM97" s="156"/>
-      <c r="AN97" s="156"/>
-      <c r="AO97" s="156"/>
-      <c r="AP97" s="156"/>
-      <c r="AQ97" s="156"/>
+      <c r="AK97" s="7"/>
+      <c r="AL97" s="7"/>
+      <c r="AM97" s="7"/>
+      <c r="AN97" s="7"/>
+      <c r="AO97" s="7"/>
+      <c r="AP97" s="7"/>
+      <c r="AQ97" s="7"/>
       <c r="AR97" s="16"/>
       <c r="AS97" s="16"/>
       <c r="AT97" s="16"/>
       <c r="AU97" s="16"/>
       <c r="AV97" s="16"/>
-      <c r="AW97" s="156"/>
-      <c r="AX97" s="156"/>
-      <c r="AY97" s="157"/>
-      <c r="AZ97" s="157"/>
-      <c r="BA97" s="157"/>
-      <c r="BB97" s="157"/>
-      <c r="BC97" s="157"/>
-      <c r="BD97" s="157"/>
+      <c r="AW97" s="7"/>
+      <c r="AX97" s="7"/>
     </row>
     <row r="98" spans="23:70" x14ac:dyDescent="0.2">
-      <c r="AK98" s="156"/>
-      <c r="AL98" s="156"/>
-      <c r="AM98" s="156"/>
-      <c r="AN98" s="156"/>
-      <c r="AO98" s="156"/>
-      <c r="AP98" s="156"/>
-      <c r="AQ98" s="156"/>
+      <c r="AK98" s="7"/>
+      <c r="AL98" s="7"/>
+      <c r="AM98" s="7"/>
+      <c r="AN98" s="7"/>
+      <c r="AO98" s="7"/>
+      <c r="AP98" s="7"/>
+      <c r="AQ98" s="7"/>
       <c r="AR98" s="16"/>
       <c r="AS98" s="16"/>
       <c r="AT98" s="16"/>
       <c r="AU98" s="16"/>
       <c r="AV98" s="16"/>
-      <c r="AW98" s="156"/>
-      <c r="AX98" s="156"/>
-      <c r="AY98" s="157"/>
-      <c r="AZ98" s="157"/>
-      <c r="BA98" s="157"/>
-      <c r="BB98" s="157"/>
-      <c r="BC98" s="157"/>
-      <c r="BD98" s="157"/>
+      <c r="AW98" s="7"/>
+      <c r="AX98" s="7"/>
     </row>
     <row r="99" spans="23:70" x14ac:dyDescent="0.2">
-      <c r="AK99" s="156"/>
-      <c r="AL99" s="156"/>
-      <c r="AM99" s="156"/>
-      <c r="AN99" s="156"/>
-      <c r="AO99" s="156"/>
-      <c r="AP99" s="156"/>
-      <c r="AQ99" s="156"/>
+      <c r="AK99" s="7"/>
+      <c r="AL99" s="7"/>
+      <c r="AM99" s="7"/>
+      <c r="AN99" s="7"/>
+      <c r="AO99" s="7"/>
+      <c r="AP99" s="7"/>
+      <c r="AQ99" s="7"/>
       <c r="AR99" s="16"/>
       <c r="AS99" s="16"/>
       <c r="AT99" s="16"/>
       <c r="AU99" s="16"/>
       <c r="AV99" s="16"/>
-      <c r="AW99" s="156"/>
-      <c r="AX99" s="156"/>
-      <c r="AY99" s="157"/>
-      <c r="AZ99" s="158"/>
-      <c r="BA99" s="157"/>
-      <c r="BB99" s="157"/>
-      <c r="BC99" s="157"/>
-      <c r="BD99" s="157"/>
+      <c r="AW99" s="7"/>
+      <c r="AX99" s="7"/>
+      <c r="AZ99" s="116"/>
     </row>
     <row r="100" spans="23:70" x14ac:dyDescent="0.2">
-      <c r="AK100" s="156"/>
-      <c r="AL100" s="156"/>
-      <c r="AM100" s="156"/>
+      <c r="AK100" s="7"/>
+      <c r="AL100" s="7"/>
+      <c r="AM100" s="7"/>
       <c r="AN100" s="16"/>
       <c r="AO100" s="16"/>
-      <c r="AP100" s="156"/>
+      <c r="AP100" s="7"/>
       <c r="AQ100" s="16"/>
       <c r="AR100" s="16"/>
       <c r="AS100" s="16"/>
       <c r="AT100" s="16"/>
       <c r="AU100" s="16"/>
       <c r="AV100" s="16"/>
-      <c r="AW100" s="156"/>
-      <c r="AX100" s="156"/>
-      <c r="AY100" s="157"/>
-      <c r="AZ100" s="157"/>
-      <c r="BA100" s="157"/>
-      <c r="BB100" s="157"/>
-      <c r="BC100" s="159"/>
-      <c r="BD100" s="159"/>
+      <c r="AW100" s="7"/>
+      <c r="AX100" s="7"/>
+      <c r="BC100" s="112"/>
+      <c r="BD100" s="112"/>
     </row>
     <row r="101" spans="23:70" x14ac:dyDescent="0.2">
-      <c r="AK101" s="156"/>
-      <c r="AL101" s="156"/>
-      <c r="AM101" s="156"/>
+      <c r="AK101" s="7"/>
+      <c r="AL101" s="7"/>
+      <c r="AM101" s="7"/>
       <c r="AN101" s="16"/>
       <c r="AO101" s="16"/>
-      <c r="AP101" s="156"/>
+      <c r="AP101" s="7"/>
       <c r="AQ101" s="16"/>
       <c r="AR101" s="16"/>
       <c r="AS101" s="16"/>
       <c r="AT101" s="16"/>
       <c r="AU101" s="16"/>
       <c r="AV101" s="16"/>
-      <c r="AW101" s="156"/>
-      <c r="AX101" s="156"/>
-      <c r="AY101" s="157"/>
-      <c r="AZ101" s="157"/>
-      <c r="BA101" s="157"/>
-      <c r="BB101" s="157"/>
-      <c r="BC101" s="157"/>
-      <c r="BD101" s="157"/>
+      <c r="AW101" s="7"/>
+      <c r="AX101" s="7"/>
     </row>
     <row r="102" spans="23:70" x14ac:dyDescent="0.2">
-      <c r="AK102" s="156"/>
-      <c r="AL102" s="156"/>
-      <c r="AM102" s="156"/>
-      <c r="AN102" s="156"/>
-      <c r="AO102" s="156"/>
-      <c r="AP102" s="156"/>
-      <c r="AQ102" s="156"/>
-      <c r="AR102" s="156"/>
-      <c r="AS102" s="156"/>
-      <c r="AT102" s="156"/>
-      <c r="AU102" s="156"/>
-      <c r="AV102" s="156"/>
-      <c r="AW102" s="156"/>
-      <c r="AX102" s="156"/>
-      <c r="AY102" s="157"/>
-      <c r="AZ102" s="157"/>
-      <c r="BA102" s="157"/>
-      <c r="BB102" s="157"/>
-      <c r="BC102" s="157"/>
-      <c r="BD102" s="157"/>
+      <c r="AK102" s="7"/>
+      <c r="AL102" s="7"/>
+      <c r="AM102" s="7"/>
+      <c r="AN102" s="7"/>
+      <c r="AO102" s="7"/>
+      <c r="AP102" s="7"/>
+      <c r="AQ102" s="7"/>
+      <c r="AR102" s="7"/>
+      <c r="AS102" s="7"/>
+      <c r="AT102" s="7"/>
+      <c r="AU102" s="7"/>
+      <c r="AV102" s="7"/>
+      <c r="AW102" s="7"/>
+      <c r="AX102" s="7"/>
     </row>
     <row r="103" spans="23:70" x14ac:dyDescent="0.2">
-      <c r="AK103" s="156"/>
-      <c r="AL103" s="156"/>
-      <c r="AM103" s="156"/>
-      <c r="AN103" s="156"/>
-      <c r="AO103" s="156"/>
-      <c r="AP103" s="156"/>
-      <c r="AQ103" s="156"/>
-      <c r="AR103" s="156"/>
-      <c r="AS103" s="156"/>
-      <c r="AT103" s="156"/>
-      <c r="AU103" s="156"/>
-      <c r="AV103" s="156"/>
-      <c r="AW103" s="156"/>
-      <c r="AX103" s="156"/>
-      <c r="AY103" s="157"/>
-      <c r="AZ103" s="157"/>
-      <c r="BA103" s="157"/>
-      <c r="BB103" s="157"/>
-      <c r="BC103" s="157"/>
-      <c r="BD103" s="157"/>
+      <c r="AK103" s="7"/>
+      <c r="AL103" s="7"/>
+      <c r="AM103" s="7"/>
+      <c r="AN103" s="7"/>
+      <c r="AO103" s="7"/>
+      <c r="AP103" s="7"/>
+      <c r="AQ103" s="7"/>
+      <c r="AR103" s="7"/>
+      <c r="AS103" s="7"/>
+      <c r="AT103" s="7"/>
+      <c r="AU103" s="7"/>
+      <c r="AV103" s="7"/>
+      <c r="AW103" s="7"/>
+      <c r="AX103" s="7"/>
     </row>
     <row r="108" spans="23:70" x14ac:dyDescent="0.25">
       <c r="AZ108" s="111"/>
@@ -19244,27 +19427,32 @@
     </row>
   </sheetData>
   <phoneticPr fontId="14" type="noConversion"/>
-  <conditionalFormatting sqref="AK46:AX59">
-    <cfRule type="expression" dxfId="6" priority="3">
-      <formula>ABS(AK46)&lt;0.1</formula>
+  <conditionalFormatting sqref="AK6:AX60">
+    <cfRule type="expression" dxfId="5" priority="2">
+      <formula>ABS(AK6)&lt;0.1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AK90:AX103">
+    <cfRule type="expression" dxfId="4" priority="3">
+      <formula>ABS(AK90)&lt;0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BB46:BB59">
-    <cfRule type="expression" dxfId="5" priority="2">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>ABS(BB46)&lt;0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BR172:BR174">
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
       <formula>"VIRHE!"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="7" operator="equal">
       <formula>"OK!"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AK90:AX103">
+  <conditionalFormatting sqref="AK66:AV73">
     <cfRule type="expression" dxfId="0" priority="1">
-      <formula>ABS(AK90)&lt;0.1</formula>
+      <formula>ABS(AK66)&lt;0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -19274,22 +19462,60 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A31214F-D315-442C-9106-A983B611689D}">
-  <dimension ref="L24:L25"/>
+  <dimension ref="M30:R33"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P20" sqref="P20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O25" sqref="O25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="24" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L24" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="25" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L25" t="s">
-        <v>82</v>
+    <row r="30" spans="13:18" x14ac:dyDescent="0.25">
+      <c r="M30" t="s">
+        <v>89</v>
+      </c>
+      <c r="N30" t="s">
+        <v>90</v>
+      </c>
+      <c r="O30" t="s">
+        <v>76</v>
+      </c>
+      <c r="P30" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>92</v>
+      </c>
+      <c r="R30" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="31" spans="13:18" x14ac:dyDescent="0.25">
+      <c r="M31">
+        <v>4000</v>
+      </c>
+      <c r="N31">
+        <f>1000+(2500/2)</f>
+        <v>2250</v>
+      </c>
+      <c r="O31">
+        <f>500+2500/2</f>
+        <v>1750</v>
+      </c>
+      <c r="P31">
+        <v>2500</v>
+      </c>
+      <c r="Q31">
+        <v>1250</v>
+      </c>
+      <c r="R31">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M33">
+        <f>P31/M31^2*(N31*O31^2+1/12*(N31-2*O31)*P31^2)*R31</f>
+        <v>9749348.9583333321</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Begin implementing internal moment calculation
</commit_message>
<xml_diff>
--- a/theory/FEM matriisit.xlsx
+++ b/theory/FEM matriisit.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ohjelmointi\2_Rust\idfem\theory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{176A2867-7B30-45AB-BD3B-B940FBC54AA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABE8483A-762A-4765-9C2D-546E655B88E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22230" yWindow="0" windowWidth="22335" windowHeight="20880" activeTab="2" xr2:uid="{27180542-B0D2-4BFE-946B-7857B24C93C8}"/>
+    <workbookView xWindow="-22230" yWindow="0" windowWidth="22335" windowHeight="20880" activeTab="1" xr2:uid="{27180542-B0D2-4BFE-946B-7857B24C93C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Ilman vapautuksia" sheetId="1" r:id="rId1"/>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="96">
   <si>
     <t>°</t>
   </si>
@@ -419,6 +419,12 @@
   <si>
     <t>q</t>
   </si>
+  <si>
+    <t>Elem 1 lok</t>
+  </si>
+  <si>
+    <t>Elem 1 glob</t>
+  </si>
 </sst>
 </file>
 
@@ -712,7 +718,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="156">
+  <cellXfs count="159">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1121,126 +1127,17 @@
     <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutraali" xfId="1" builtinId="28"/>
     <cellStyle name="Normaali" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="40">
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
+  <dxfs count="10">
     <dxf>
       <font>
         <b/>
@@ -1305,75 +1202,9 @@
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
+        <color auto="1"/>
       </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
   </dxfs>
@@ -1400,7 +1231,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>61</xdr:col>
-      <xdr:colOff>596105</xdr:colOff>
+      <xdr:colOff>272255</xdr:colOff>
       <xdr:row>40</xdr:row>
       <xdr:rowOff>32279</xdr:rowOff>
     </xdr:to>
@@ -2041,8 +1872,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94F9BDF3-3EE6-4BFB-9734-CB047BC6E804}">
   <dimension ref="B1:CW227"/>
   <sheetViews>
-    <sheetView topLeftCell="AI24" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AZ45" sqref="AZ45"/>
+    <sheetView topLeftCell="AM18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BB48" sqref="BB48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -2076,7 +1907,11 @@
     <col min="44" max="44" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="45" max="48" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="49" max="49" width="9.140625" style="1"/>
-    <col min="50" max="62" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="50" max="53" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="57" max="62" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="63" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -2342,7 +2177,7 @@
       <c r="AW6" s="4"/>
       <c r="AX6" s="3">
         <f>I20</f>
-        <v>-20000</v>
+        <v>20000</v>
       </c>
       <c r="AZ6" s="78">
         <v>1</v>
@@ -2465,7 +2300,7 @@
       <c r="AW7" s="4"/>
       <c r="AX7" s="3">
         <f t="shared" ref="AX7:AX11" si="1">I21</f>
-        <v>1.22514845490862E-12</v>
+        <v>-1.22514845490862E-12</v>
       </c>
       <c r="AZ7" s="78">
         <v>2</v>
@@ -2588,7 +2423,7 @@
       <c r="AW8" s="4"/>
       <c r="AX8" s="3">
         <f t="shared" si="1"/>
-        <v>13333333.333333334</v>
+        <v>-13333333.333333334</v>
       </c>
       <c r="AZ8" s="78">
         <v>3</v>
@@ -2711,7 +2546,7 @@
       <c r="AW9" s="4"/>
       <c r="AX9" s="3">
         <f t="shared" si="1"/>
-        <v>-20000</v>
+        <v>20000</v>
       </c>
       <c r="AZ9" s="78">
         <v>4</v>
@@ -2844,7 +2679,7 @@
       <c r="AW10" s="4"/>
       <c r="AX10" s="3">
         <f>I24</f>
-        <v>1.22514845490862E-12</v>
+        <v>-1.22514845490862E-12</v>
       </c>
       <c r="AZ10" s="78">
         <v>5</v>
@@ -2893,7 +2728,7 @@
       </c>
       <c r="BM10" s="16"/>
       <c r="BN10" s="1">
-        <v>30000</v>
+        <v>-30000</v>
       </c>
     </row>
     <row r="11" spans="2:66" ht="13.5" x14ac:dyDescent="0.2">
@@ -2976,7 +2811,7 @@
       <c r="AW11" s="4"/>
       <c r="AX11" s="3">
         <f t="shared" si="1"/>
-        <v>-13333333.333333334</v>
+        <v>13333333.333333334</v>
       </c>
       <c r="AZ11" s="78">
         <v>6</v>
@@ -3025,7 +2860,7 @@
       </c>
       <c r="BM11" s="16"/>
       <c r="BN11" s="1">
-        <v>30000000</v>
+        <v>-30000000</v>
       </c>
     </row>
     <row r="12" spans="2:66" x14ac:dyDescent="0.2">
@@ -3317,7 +3152,6 @@
         <v>18</v>
       </c>
       <c r="E15" s="14">
-        <f>1000*10/1000</f>
         <v>10</v>
       </c>
       <c r="F15" s="1" t="s">
@@ -3327,7 +3161,6 @@
         <v>18</v>
       </c>
       <c r="O15" s="14">
-        <f>1000*10/1000</f>
         <v>10</v>
       </c>
       <c r="P15" s="1" t="s">
@@ -3337,8 +3170,7 @@
         <v>18</v>
       </c>
       <c r="Y15" s="14">
-        <f>1000*10/1000</f>
-        <v>10</v>
+        <v>-5</v>
       </c>
       <c r="Z15" s="1" t="s">
         <v>56</v>
@@ -3528,7 +3360,7 @@
       </c>
       <c r="BM16" s="16"/>
       <c r="BN16" s="12">
-        <v>30000</v>
+        <v>-30000</v>
       </c>
     </row>
     <row r="17" spans="2:66" x14ac:dyDescent="0.2">
@@ -3620,7 +3452,7 @@
       </c>
       <c r="BM17" s="16"/>
       <c r="BN17" s="12">
-        <v>-30000000</v>
+        <v>30000000</v>
       </c>
     </row>
     <row r="18" spans="2:66" x14ac:dyDescent="0.2">
@@ -3726,7 +3558,7 @@
       </c>
       <c r="I20" s="151">
         <f>B54*I28+C54*I29+D54*I30+E54*I31+F54*I32+G54*I33</f>
-        <v>-20000</v>
+        <v>20000</v>
       </c>
       <c r="L20" s="19">
         <f t="shared" ref="L20:Q25" si="7">$L37*L$46+$M37*L$47+$N37*L$48+$O37*L$49+$P37*L$50+$Q37*L$51</f>
@@ -3782,7 +3614,7 @@
       </c>
       <c r="AC20" s="40">
         <f>V55*AC28+W55*AC29+X55*AC30+Y55*AC31+Z55*AC32+AA55*AC33</f>
-        <v>20000</v>
+        <v>-10000</v>
       </c>
       <c r="AJ20" s="2" t="s">
         <v>38</v>
@@ -3815,7 +3647,7 @@
       </c>
       <c r="I21" s="151">
         <f>B55*I28+C55*I29+D55*I30+E55*I31+F55*I32+G55*I33</f>
-        <v>1.22514845490862E-12</v>
+        <v>-1.22514845490862E-12</v>
       </c>
       <c r="L21" s="19">
         <f t="shared" si="7"/>
@@ -3843,7 +3675,7 @@
       </c>
       <c r="S21" s="40">
         <f>L56*S28+M56*S29+N56*S30+O56*S31+P56*S32+Q56*S33</f>
-        <v>30000</v>
+        <v>-30000</v>
       </c>
       <c r="V21" s="20">
         <f t="shared" si="8"/>
@@ -3871,7 +3703,7 @@
       </c>
       <c r="AC21" s="40">
         <f>V56*AC28+W56*AC29+X56*AC30+Y56*AC31+Z56*AC32+AA56*AC33</f>
-        <v>-1.22514845490862E-12</v>
+        <v>6.1257422745431001E-13</v>
       </c>
       <c r="AJ21" s="9"/>
       <c r="AK21" s="78">
@@ -3942,7 +3774,7 @@
       </c>
       <c r="I22" s="151">
         <f>B56*I28+C56*I29+D56*I30+E56*I31+F56*I32+G56*I33</f>
-        <v>13333333.333333334</v>
+        <v>-13333333.333333334</v>
       </c>
       <c r="L22" s="19">
         <f t="shared" si="7"/>
@@ -3970,7 +3802,7 @@
       </c>
       <c r="S22" s="40">
         <f>L57*S28+M57*S29+N57*S30+O57*S31+P57*S32+Q57*S33</f>
-        <v>30000000</v>
+        <v>-30000000</v>
       </c>
       <c r="V22" s="20">
         <f t="shared" ref="V22:Z25" si="10">$V39*B$45+$W39*B$46+$X39*B$47+$Y39*B$48+$Z39*B$49+$AA39*B$50</f>
@@ -3998,7 +3830,7 @@
       </c>
       <c r="AC22" s="40">
         <f>V57*AC28+W57*AC29+X57*AC30+Y57*AC31+Z57*AC32+AA57*AC33</f>
-        <v>-13333333.333333334</v>
+        <v>6666666.666666667</v>
       </c>
       <c r="AJ22" s="78">
         <v>1</v>
@@ -4068,7 +3900,7 @@
       </c>
       <c r="I23" s="151">
         <f>B57*I28+C57*I29+D57*I30+E57*I31+F57*I32+G57*I33</f>
-        <v>-20000</v>
+        <v>20000</v>
       </c>
       <c r="L23" s="19">
         <f t="shared" si="7"/>
@@ -4124,7 +3956,7 @@
       </c>
       <c r="AC23" s="40">
         <f>V58*AC28+W58*AC29+X58*AC30+Y58*AC31+Z58*AC32+AA58*AC33</f>
-        <v>20000</v>
+        <v>-10000</v>
       </c>
       <c r="AJ23" s="78">
         <v>2</v>
@@ -4194,7 +4026,7 @@
       </c>
       <c r="I24" s="151">
         <f>B58*I28+C58*I29+D58*I30+E58*I31+F58*I32+G58*I33</f>
-        <v>1.22514845490862E-12</v>
+        <v>-1.22514845490862E-12</v>
       </c>
       <c r="L24" s="19">
         <f t="shared" si="7"/>
@@ -4222,7 +4054,7 @@
       </c>
       <c r="S24" s="40">
         <f>L59*S28+M59*S29+N59*S30+O59*S31+P59*S32+Q59*S33</f>
-        <v>30000</v>
+        <v>-30000</v>
       </c>
       <c r="V24" s="20">
         <f t="shared" si="10"/>
@@ -4250,7 +4082,7 @@
       </c>
       <c r="AC24" s="40">
         <f>V59*AC28+W59*AC29+X59*AC30+Y59*AC31+Z59*AC32+AA59*AC33</f>
-        <v>-1.22514845490862E-12</v>
+        <v>6.1257422745431001E-13</v>
       </c>
       <c r="AJ24" s="78">
         <v>3</v>
@@ -4320,7 +4152,7 @@
       </c>
       <c r="I25" s="151">
         <f>B59*I28+C59*I29+D59*I30+E59*I31+F59*I32+G59*I33</f>
-        <v>-13333333.333333334</v>
+        <v>13333333.333333334</v>
       </c>
       <c r="K25" s="2"/>
       <c r="L25" s="19">
@@ -4349,7 +4181,7 @@
       </c>
       <c r="S25" s="40">
         <f>L60*S28+M60*S29+N60*S30+O60*S31+P60*S32+Q60*S33</f>
-        <v>-30000000</v>
+        <v>30000000</v>
       </c>
       <c r="U25" s="2"/>
       <c r="V25" s="20">
@@ -4378,7 +4210,7 @@
       </c>
       <c r="AC25" s="40">
         <f>V60*AC28+W60*AC29+X60*AC30+Y60*AC31+Z60*AC32+AA60*AC33</f>
-        <v>13333333.333333334</v>
+        <v>-6666666.666666667</v>
       </c>
       <c r="AE25" s="2"/>
       <c r="AJ25" s="78">
@@ -4553,7 +4385,7 @@
         <v>0</v>
       </c>
       <c r="I28" s="38">
-        <f>E6/2*E14</f>
+        <f>-E6/2*E14</f>
         <v>0</v>
       </c>
       <c r="L28" s="38">
@@ -4600,7 +4432,7 @@
         <v>0</v>
       </c>
       <c r="AC28" s="38">
-        <f>Y6/2*Y14</f>
+        <f>-Y6/2*Y14</f>
         <v>0</v>
       </c>
       <c r="AJ28" s="78">
@@ -4651,7 +4483,7 @@
       <c r="AW28" s="4"/>
       <c r="AX28" s="3">
         <f>AC20</f>
-        <v>20000</v>
+        <v>-10000</v>
       </c>
       <c r="AY28" s="8"/>
     </row>
@@ -4679,8 +4511,8 @@
         <v>656250</v>
       </c>
       <c r="I29" s="38">
-        <f>E6/2*E15</f>
-        <v>20000</v>
+        <f>-E6/2*E15</f>
+        <v>-20000</v>
       </c>
       <c r="L29" s="39">
         <v>0</v>
@@ -4705,8 +4537,8 @@
         <v>2333333.3333333335</v>
       </c>
       <c r="S29" s="38">
-        <f>O6/2*(O14+O15)</f>
-        <v>30000</v>
+        <f>-O6/2*(O14+O15)</f>
+        <v>-30000</v>
       </c>
       <c r="V29" s="39">
         <v>0</v>
@@ -4731,8 +4563,8 @@
         <v>656250</v>
       </c>
       <c r="AC29" s="38">
-        <f>-Y15*Y6/2</f>
-        <v>-20000</v>
+        <f>-Y6/2*Y15</f>
+        <v>10000</v>
       </c>
       <c r="AJ29" s="78">
         <v>8</v>
@@ -4782,7 +4614,7 @@
       <c r="AW29" s="4"/>
       <c r="AX29" s="3">
         <f t="shared" ref="AX29:AX33" si="12">AC21</f>
-        <v>-1.22514845490862E-12</v>
+        <v>6.1257422745431001E-13</v>
       </c>
       <c r="AY29" s="10"/>
     </row>
@@ -4810,8 +4642,8 @@
         <v>875000000</v>
       </c>
       <c r="I30" s="38">
-        <f>1*(E15*E6^2)/12</f>
-        <v>13333333.333333334</v>
+        <f>-1*(E15*E6^2)/12</f>
+        <v>-13333333.333333334</v>
       </c>
       <c r="L30" s="39">
         <v>0</v>
@@ -4836,8 +4668,8 @@
         <v>4666666666.666667</v>
       </c>
       <c r="S30" s="38">
-        <f>1*((O14+O15)*O6^2)/12</f>
-        <v>30000000</v>
+        <f>-1*((O14+O15)*O6^2)/12</f>
+        <v>-30000000</v>
       </c>
       <c r="V30" s="39">
         <v>0</v>
@@ -4863,7 +4695,7 @@
       </c>
       <c r="AC30" s="38">
         <f>-1*(Y15*Y6^2)/12</f>
-        <v>-13333333.333333334</v>
+        <v>6666666.666666667</v>
       </c>
       <c r="AJ30" s="78">
         <v>9</v>
@@ -4913,7 +4745,7 @@
       <c r="AW30" s="4"/>
       <c r="AX30" s="3">
         <f t="shared" si="12"/>
-        <v>-13333333.333333334</v>
+        <v>6666666.666666667</v>
       </c>
       <c r="AY30" s="8"/>
     </row>
@@ -4939,7 +4771,7 @@
         <v>0</v>
       </c>
       <c r="I31" s="38">
-        <f>E6/2*E14</f>
+        <f>-E6/2*E14</f>
         <v>0</v>
       </c>
       <c r="L31" s="38">
@@ -4986,7 +4818,7 @@
         <v>0</v>
       </c>
       <c r="AC31" s="38">
-        <f>Y6/2*Y14</f>
+        <f>-Y6/2*Y14</f>
         <v>0</v>
       </c>
       <c r="AJ31" s="78">
@@ -5037,7 +4869,7 @@
       <c r="AW31" s="4"/>
       <c r="AX31" s="3">
         <f t="shared" si="12"/>
-        <v>20000</v>
+        <v>-10000</v>
       </c>
       <c r="AY31" s="8"/>
     </row>
@@ -5065,8 +4897,8 @@
         <v>-656250</v>
       </c>
       <c r="I32" s="38">
-        <f>E6/2*E15</f>
-        <v>20000</v>
+        <f>-E6/2*E15</f>
+        <v>-20000</v>
       </c>
       <c r="L32" s="39">
         <v>0</v>
@@ -5092,8 +4924,8 @@
       </c>
       <c r="R32" s="2"/>
       <c r="S32" s="38">
-        <f>O6/2*(O14+O15)</f>
-        <v>30000</v>
+        <f>-O6/2*(O14+O15)</f>
+        <v>-30000</v>
       </c>
       <c r="V32" s="39">
         <v>0</v>
@@ -5118,8 +4950,8 @@
         <v>-656250</v>
       </c>
       <c r="AC32" s="38">
-        <f>-Y15*Y6/2</f>
-        <v>-20000</v>
+        <f>-Y6/2*Y15</f>
+        <v>10000</v>
       </c>
       <c r="AJ32" s="78">
         <v>11</v>
@@ -5169,7 +5001,7 @@
       <c r="AW32" s="4"/>
       <c r="AX32" s="3">
         <f t="shared" si="12"/>
-        <v>-1.22514845490862E-12</v>
+        <v>6.1257422745431001E-13</v>
       </c>
       <c r="AY32" s="10"/>
     </row>
@@ -5197,8 +5029,8 @@
         <v>1750000000</v>
       </c>
       <c r="I33" s="38">
-        <f>-1*(E15*E6^2)/12</f>
-        <v>-13333333.333333334</v>
+        <f>1*(E15*E6^2)/12</f>
+        <v>13333333.333333334</v>
       </c>
       <c r="L33" s="39">
         <v>0</v>
@@ -5223,8 +5055,8 @@
         <v>9333333333.333334</v>
       </c>
       <c r="S33" s="38">
-        <f>-1*((O14+O15)*O6^2)/12</f>
-        <v>-30000000</v>
+        <f>1*((O14+O15)*O6^2)/12</f>
+        <v>30000000</v>
       </c>
       <c r="V33" s="39">
         <v>0</v>
@@ -5250,7 +5082,7 @@
       </c>
       <c r="AC33" s="38">
         <f>1*(Y15*Y6^2)/12</f>
-        <v>13333333.333333334</v>
+        <v>-6666666.666666667</v>
       </c>
       <c r="AJ33" s="78">
         <v>12</v>
@@ -5300,7 +5132,7 @@
       <c r="AW33" s="4"/>
       <c r="AX33" s="3">
         <f t="shared" si="12"/>
-        <v>13333333.333333334</v>
+        <v>-6666666.666666667</v>
       </c>
       <c r="AY33" s="8"/>
     </row>
@@ -5845,6 +5677,13 @@
       <c r="AZ42" s="9" t="s">
         <v>50</v>
       </c>
+      <c r="BB42" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="BC42" s="80"/>
+      <c r="BD42" s="80" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="43" spans="2:83" x14ac:dyDescent="0.2">
       <c r="H43" s="27"/>
@@ -5905,10 +5744,19 @@
       </c>
       <c r="AZ43" s="3">
         <f>AX6+BN6+AX22</f>
-        <v>-20000</v>
+        <v>20000</v>
       </c>
       <c r="BA43" s="144" t="s">
         <v>52</v>
+      </c>
+      <c r="BB43" s="153" cm="1">
+        <f t="array" ref="BB43:BB44">AX43:AX44</f>
+        <v>0</v>
+      </c>
+      <c r="BC43" s="4"/>
+      <c r="BD43" s="4">
+        <f t="array" ref="BD43:BD54">MMULT(AK43:AV54,BB43:BB54)-AZ43:AZ54</f>
+        <v>-20427.724341873007</v>
       </c>
     </row>
     <row r="44" spans="2:83" x14ac:dyDescent="0.2">
@@ -5972,10 +5820,17 @@
       </c>
       <c r="AZ44" s="3">
         <f t="shared" ref="AZ44:AZ54" si="35">AX7+BN7+AX23</f>
-        <v>1.22514845490862E-12</v>
+        <v>-1.22514845490862E-12</v>
       </c>
       <c r="BA44" s="144" t="s">
         <v>51</v>
+      </c>
+      <c r="BB44" s="153">
+        <v>0</v>
+      </c>
+      <c r="BC44" s="154"/>
+      <c r="BD44" s="156">
+        <v>23333.33333332961</v>
       </c>
     </row>
     <row r="45" spans="2:83" x14ac:dyDescent="0.2">
@@ -6062,7 +5917,15 @@
       </c>
       <c r="AZ45" s="3">
         <f t="shared" si="35"/>
-        <v>13333333.333333334</v>
+        <v>-13333333.333333334</v>
+      </c>
+      <c r="BB45" s="153" cm="1">
+        <f t="array" ref="BB45:BB48">AV71:AV74</f>
+        <v>-3.6373783993449142E-2</v>
+      </c>
+      <c r="BC45" s="154"/>
+      <c r="BD45" s="156">
+        <v>-2.2351741790771484E-8</v>
       </c>
     </row>
     <row r="46" spans="2:83" x14ac:dyDescent="0.2">
@@ -6183,7 +6046,14 @@
       </c>
       <c r="AZ46" s="3">
         <f t="shared" si="35"/>
-        <v>-20000</v>
+        <v>20000</v>
+      </c>
+      <c r="BB46" s="153">
+        <v>81.935673318570522</v>
+      </c>
+      <c r="BC46" s="154"/>
+      <c r="BD46" s="156">
+        <v>-7.4505805969238281E-9</v>
       </c>
       <c r="CE46" s="2"/>
     </row>
@@ -6303,7 +6173,14 @@
       </c>
       <c r="AZ47" s="3">
         <f>AX10+BN10+AX26</f>
-        <v>30000</v>
+        <v>-30000</v>
+      </c>
+      <c r="BB47" s="153">
+        <v>-4.4444444444442371E-2</v>
+      </c>
+      <c r="BC47" s="80"/>
+      <c r="BD47" s="80">
+        <v>5.8535079006105661E-9</v>
       </c>
       <c r="BS47" s="3"/>
       <c r="CE47" s="2"/>
@@ -6422,7 +6299,14 @@
       </c>
       <c r="AZ48" s="3">
         <f t="shared" si="35"/>
-        <v>16666666.666666666</v>
+        <v>-16666666.666666666</v>
+      </c>
+      <c r="BB48" s="157">
+        <v>-3.9422822401248706E-3</v>
+      </c>
+      <c r="BC48" s="154"/>
+      <c r="BD48" s="156">
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="2:101" x14ac:dyDescent="0.2">
@@ -6545,10 +6429,18 @@
       </c>
       <c r="AZ49" s="3">
         <f t="shared" si="35"/>
-        <v>20000</v>
+        <v>-10000</v>
       </c>
       <c r="BA49" s="144" t="s">
         <v>53</v>
+      </c>
+      <c r="BB49" s="153" cm="1">
+        <f t="array" ref="BB49:BB50">AX49:AX50</f>
+        <v>0</v>
+      </c>
+      <c r="BC49" s="154"/>
+      <c r="BD49" s="156">
+        <v>427.7243418762082</v>
       </c>
       <c r="CW49" s="2"/>
     </row>
@@ -6671,10 +6563,17 @@
       </c>
       <c r="AZ50" s="3">
         <f t="shared" si="35"/>
-        <v>-1.22514845490862E-12</v>
+        <v>6.1257422745431001E-13</v>
       </c>
       <c r="BA50" s="144" t="s">
         <v>54</v>
+      </c>
+      <c r="BB50" s="153">
+        <v>0</v>
+      </c>
+      <c r="BC50" s="155"/>
+      <c r="BD50" s="4">
+        <v>36666.666666664547</v>
       </c>
       <c r="BK50" s="2"/>
       <c r="CW50" s="2"/>
@@ -6778,9 +6677,16 @@
       </c>
       <c r="AZ51" s="3">
         <f t="shared" si="35"/>
-        <v>-13333333.333333334</v>
-      </c>
-      <c r="BB51" s="4"/>
+        <v>6666666.666666667</v>
+      </c>
+      <c r="BB51" s="153" cm="1">
+        <f t="array" ref="BB51:BB54">AV75:AV78</f>
+        <v>-2.7444205424524807E-2</v>
+      </c>
+      <c r="BC51" s="154"/>
+      <c r="BD51" s="156">
+        <v>-9.3132257461547852E-9</v>
+      </c>
       <c r="BK51" s="6"/>
       <c r="BL51" s="6"/>
       <c r="BM51" s="6"/>
@@ -6853,9 +6759,15 @@
       </c>
       <c r="AZ52" s="3">
         <f t="shared" si="35"/>
-        <v>20000</v>
-      </c>
-      <c r="BB52" s="12"/>
+        <v>-10000</v>
+      </c>
+      <c r="BB52" s="153">
+        <v>81.907712924773207</v>
+      </c>
+      <c r="BC52" s="155"/>
+      <c r="BD52" s="4">
+        <v>1.597072696313262E-9</v>
+      </c>
       <c r="BE52" s="16"/>
       <c r="BK52" s="6"/>
       <c r="BL52" s="6"/>
@@ -6931,9 +6843,15 @@
       </c>
       <c r="AZ53" s="3">
         <f t="shared" si="35"/>
-        <v>30000</v>
-      </c>
-      <c r="BB53" s="12"/>
+        <v>-30000</v>
+      </c>
+      <c r="BB53" s="153">
+        <v>-6.9841269841270814E-2</v>
+      </c>
+      <c r="BC53" s="155"/>
+      <c r="BD53" s="4">
+        <v>0</v>
+      </c>
       <c r="BE53" s="16"/>
       <c r="BK53" s="6"/>
       <c r="BL53" s="6"/>
@@ -7037,9 +6955,15 @@
       </c>
       <c r="AZ54" s="3">
         <f t="shared" si="35"/>
-        <v>-16666666.666666666</v>
-      </c>
-      <c r="BB54" s="12"/>
+        <v>23333333.333333332</v>
+      </c>
+      <c r="BB54" s="158">
+        <v>1.0766737745173162E-3</v>
+      </c>
+      <c r="BC54" s="155"/>
+      <c r="BD54" s="4">
+        <v>0</v>
+      </c>
       <c r="BE54" s="16"/>
       <c r="BK54" s="6"/>
       <c r="BL54" s="6"/>
@@ -7117,7 +7041,9 @@
       <c r="AH55" s="10"/>
       <c r="AI55" s="10"/>
       <c r="AZ55" s="12"/>
-      <c r="BB55" s="7"/>
+      <c r="BB55" s="153"/>
+      <c r="BC55" s="155"/>
+      <c r="BD55" s="155"/>
       <c r="BE55" s="16"/>
       <c r="BK55" s="6"/>
       <c r="BL55" s="6"/>
@@ -7194,7 +7120,9 @@
       <c r="AH56" s="8"/>
       <c r="AI56" s="8"/>
       <c r="AZ56" s="12"/>
-      <c r="BB56" s="7"/>
+      <c r="BB56" s="153"/>
+      <c r="BC56" s="80"/>
+      <c r="BD56" s="80"/>
       <c r="BE56" s="16"/>
       <c r="BK56" s="6"/>
       <c r="BL56" s="6"/>
@@ -7533,7 +7461,7 @@
       </c>
       <c r="AV60" s="145" cm="1">
         <f t="array" ref="AV60:AV63">AZ45:AZ48</f>
-        <v>13333333.333333334</v>
+        <v>-13333333.333333334</v>
       </c>
       <c r="BB60" s="12"/>
       <c r="BE60" s="12"/>
@@ -7585,7 +7513,7 @@
         <v>r21</v>
       </c>
       <c r="AV61" s="142">
-        <v>-20000</v>
+        <v>20000</v>
       </c>
       <c r="BA61" s="4"/>
       <c r="BB61" s="12"/>
@@ -7657,7 +7585,7 @@
         <v>r22</v>
       </c>
       <c r="AV62" s="142">
-        <v>30000</v>
+        <v>-30000</v>
       </c>
       <c r="BB62" s="12"/>
       <c r="BE62" s="12"/>
@@ -7724,7 +7652,7 @@
         <v>r23</v>
       </c>
       <c r="AV63" s="142">
-        <v>16666666.666666666</v>
+        <v>-16666666.666666666</v>
       </c>
       <c r="BB63" s="12"/>
       <c r="BE63" s="12"/>
@@ -7808,7 +7736,7 @@
       </c>
       <c r="AV64" s="3" cm="1">
         <f t="array" ref="AV64:AV67">AZ51:AZ54</f>
-        <v>-13333333.333333334</v>
+        <v>6666666.666666667</v>
       </c>
       <c r="BR64" s="66"/>
     </row>
@@ -7874,7 +7802,7 @@
         <v>45</v>
       </c>
       <c r="AV65" s="1">
-        <v>20000</v>
+        <v>-10000</v>
       </c>
       <c r="BR65" s="66"/>
     </row>
@@ -7933,7 +7861,7 @@
         <v>46</v>
       </c>
       <c r="AV66" s="1">
-        <v>30000</v>
+        <v>-30000</v>
       </c>
       <c r="BC66" s="29"/>
       <c r="BD66" s="29"/>
@@ -7979,7 +7907,7 @@
         <v>47</v>
       </c>
       <c r="AV67" s="1">
-        <v>-16666666.666666666</v>
+        <v>23333333.333333332</v>
       </c>
       <c r="BR67" s="66"/>
     </row>
@@ -8105,18 +8033,18 @@
       </c>
       <c r="AT71" s="3" cm="1">
         <f t="array" ref="AT71:AT74">AV60:AV63</f>
-        <v>13333333.333333334</v>
+        <v>-13333333.333333334</v>
       </c>
       <c r="AV71" s="153" cm="1">
         <f t="array" ref="AV71:AV78">MMULT(AK71:AR78,AT71:AT78)</f>
-        <v>6.7891530802525538E-3</v>
+        <v>-3.6373783993449142E-2</v>
       </c>
       <c r="AW71" s="1" t="s">
         <v>57</v>
       </c>
       <c r="AX71" s="1">
         <f>1000*AV71</f>
-        <v>6.7891530802525537</v>
+        <v>-36.373783993449145</v>
       </c>
       <c r="AY71" s="1" t="s">
         <v>55</v>
@@ -8157,10 +8085,10 @@
         <v>-1.4326082487351951E-7</v>
       </c>
       <c r="AT72" s="1">
-        <v>-20000</v>
+        <v>20000</v>
       </c>
       <c r="AV72" s="153">
-        <v>-1.8248294394143993E-2</v>
+        <v>81.935673318570522</v>
       </c>
       <c r="AW72" s="1" t="s">
         <v>3</v>
@@ -8201,10 +8129,10 @@
         <v>-3.1746031746016089E-10</v>
       </c>
       <c r="AT73" s="1">
-        <v>30000</v>
+        <v>-30000</v>
       </c>
       <c r="AV73" s="153">
-        <v>5.7142857142852277E-2</v>
+        <v>-4.4444444444442371E-2</v>
       </c>
       <c r="AW73" s="1" t="s">
         <v>3</v>
@@ -8244,17 +8172,17 @@
         <v>-4.780466308201401E-11</v>
       </c>
       <c r="AT74" s="1">
-        <v>16666666.666666666</v>
+        <v>-16666666.666666666</v>
       </c>
       <c r="AV74" s="153">
-        <v>1.6734752983857441E-3</v>
+        <v>-3.9422822401248706E-3</v>
       </c>
       <c r="AW74" s="1" t="s">
         <v>57</v>
       </c>
       <c r="AX74" s="1">
         <f>1000*AV74</f>
-        <v>1.6734752983857442</v>
+        <v>-3.9422822401248707</v>
       </c>
       <c r="AY74" s="1" t="s">
         <v>55</v>
@@ -8304,17 +8232,17 @@
       </c>
       <c r="AT75" s="3" cm="1">
         <f t="array" ref="AT75:AT78">_xlfn.ANCHORARRAY(AV64)</f>
-        <v>-13333333.333333334</v>
+        <v>6666666.666666667</v>
       </c>
       <c r="AV75" s="153">
-        <v>-6.7891530802525885E-3</v>
+        <v>-2.7444205424524807E-2</v>
       </c>
       <c r="AW75" s="1" t="s">
         <v>57</v>
       </c>
       <c r="AX75" s="1">
         <f>1000*AV75</f>
-        <v>-6.7891530802525883</v>
+        <v>-27.444205424524807</v>
       </c>
       <c r="AY75" s="1" t="s">
         <v>55</v>
@@ -8365,10 +8293,10 @@
         <v>-1.4330002168725404E-7</v>
       </c>
       <c r="AT76" s="1">
-        <v>20000</v>
+        <v>-10000</v>
       </c>
       <c r="AV76" s="153">
-        <v>1.8248294394228814E-2</v>
+        <v>81.907712924773207</v>
       </c>
       <c r="AW76" s="1" t="s">
         <v>3</v>
@@ -8419,10 +8347,10 @@
         <v>3.1746031746031929E-10</v>
       </c>
       <c r="AT77" s="1">
-        <v>30000</v>
+        <v>-30000</v>
       </c>
       <c r="AV77" s="153">
-        <v>5.7142857142857134E-2</v>
+        <v>-6.9841269841270814E-2</v>
       </c>
       <c r="AW77" s="1" t="s">
         <v>3</v>
@@ -8469,17 +8397,17 @@
         <v>1.1944487472222405E-10</v>
       </c>
       <c r="AT78" s="1">
-        <v>-16666666.666666666</v>
+        <v>23333333.333333332</v>
       </c>
       <c r="AV78" s="153">
-        <v>-1.6734752983857447E-3</v>
+        <v>1.0766737745173162E-3</v>
       </c>
       <c r="AW78" s="1" t="s">
         <v>57</v>
       </c>
       <c r="AX78" s="1">
         <f>1000*AV78</f>
-        <v>-1.6734752983857448</v>
+        <v>1.0766737745173163</v>
       </c>
       <c r="AY78" s="1" t="s">
         <v>55</v>
@@ -10239,8 +10167,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F95DF150-D06E-47EC-89DA-0EC5D53947FD}">
   <dimension ref="A1:CW233"/>
   <sheetViews>
-    <sheetView topLeftCell="AH1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="BD49" sqref="BD49"/>
+    <sheetView tabSelected="1" topLeftCell="AS18" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="BB63" sqref="BB63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.25"/>
@@ -10783,7 +10711,7 @@
       <c r="AX6" s="69"/>
       <c r="AY6" s="7">
         <f>I20</f>
-        <v>-20000</v>
+        <v>20000</v>
       </c>
       <c r="AZ6" s="78">
         <v>1</v>
@@ -10892,7 +10820,7 @@
       <c r="AX7" s="69"/>
       <c r="AY7" s="7">
         <f t="shared" ref="AY7:AY10" si="1">I21</f>
-        <v>1.22514845490862E-12</v>
+        <v>-1.22514845490862E-12</v>
       </c>
       <c r="AZ7" s="78">
         <v>2</v>
@@ -11001,7 +10929,7 @@
       <c r="AX8" s="69"/>
       <c r="AY8" s="7">
         <f t="shared" si="1"/>
-        <v>13333333.333333334</v>
+        <v>-13333333.333333334</v>
       </c>
       <c r="AZ8" s="78">
         <v>3</v>
@@ -11110,7 +11038,7 @@
       <c r="AX9" s="69"/>
       <c r="AY9" s="7">
         <f t="shared" si="1"/>
-        <v>-20000</v>
+        <v>20000</v>
       </c>
       <c r="AZ9" s="78">
         <v>4</v>
@@ -11241,7 +11169,7 @@
       <c r="AX10" s="69"/>
       <c r="AY10" s="7">
         <f t="shared" si="1"/>
-        <v>1.22514845490862E-12</v>
+        <v>-1.22514845490862E-12</v>
       </c>
       <c r="AZ10" s="78">
         <v>5</v>
@@ -11279,7 +11207,7 @@
       <c r="BM10" s="16"/>
       <c r="BN10" s="72"/>
       <c r="BO10" s="80">
-        <v>30000</v>
+        <v>-30000</v>
       </c>
     </row>
     <row r="11" spans="1:67" ht="13.5" x14ac:dyDescent="0.2">
@@ -11388,7 +11316,7 @@
       <c r="BM11" s="16"/>
       <c r="BN11" s="72"/>
       <c r="BO11" s="80">
-        <v>30000000</v>
+        <v>-30000000</v>
       </c>
     </row>
     <row r="12" spans="1:67" x14ac:dyDescent="0.2">
@@ -11656,7 +11584,7 @@
       <c r="W15" s="4"/>
       <c r="X15" s="4"/>
       <c r="Y15" s="20">
-        <v>-10</v>
+        <v>-5</v>
       </c>
       <c r="Z15" s="4" t="s">
         <v>33</v>
@@ -11808,7 +11736,7 @@
       <c r="BM16" s="16"/>
       <c r="BN16" s="72"/>
       <c r="BO16" s="80">
-        <v>30000</v>
+        <v>-30000</v>
       </c>
     </row>
     <row r="17" spans="1:67" x14ac:dyDescent="0.2">
@@ -11896,7 +11824,7 @@
       <c r="BM17" s="16"/>
       <c r="BN17" s="72"/>
       <c r="BO17" s="80">
-        <v>-30000000</v>
+        <v>30000000</v>
       </c>
     </row>
     <row r="18" spans="1:67" x14ac:dyDescent="0.2">
@@ -11967,7 +11895,7 @@
       <c r="AX18" s="69"/>
       <c r="AY18" s="7">
         <f>I25</f>
-        <v>-13333333.333333334</v>
+        <v>13333333.333333334</v>
       </c>
       <c r="AZ18" s="78">
         <v>13</v>
@@ -12095,7 +12023,7 @@
       <c r="H20" s="4"/>
       <c r="I20" s="40">
         <f>B54*I28+C54*I29+D54*I30+E54*I31+F54*I32+G54*I33</f>
-        <v>-20000</v>
+        <v>20000</v>
       </c>
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
@@ -12157,7 +12085,7 @@
       <c r="AB20" s="4"/>
       <c r="AC20" s="40">
         <f>V55*AC28+W55*AC29+X55*AC30+Y55*AC31+Z55*AC32+AA55*AC33</f>
-        <v>20000</v>
+        <v>-10000</v>
       </c>
       <c r="AD20" s="4"/>
       <c r="AJ20" s="4"/>
@@ -12221,7 +12149,7 @@
       <c r="H21" s="4"/>
       <c r="I21" s="40">
         <f>B55*I28+C55*I29+D55*I30+E55*I31+F55*I32+G55*I33</f>
-        <v>1.22514845490862E-12</v>
+        <v>-1.22514845490862E-12</v>
       </c>
       <c r="J21" s="4"/>
       <c r="K21" s="4"/>
@@ -12252,7 +12180,7 @@
       <c r="R21" s="4"/>
       <c r="S21" s="40">
         <f>L56*S28+M56*S29+N56*S30+O56*S31+P56*S32+Q56*S33</f>
-        <v>30000</v>
+        <v>-30000</v>
       </c>
       <c r="T21" s="4"/>
       <c r="U21" s="4"/>
@@ -12283,7 +12211,7 @@
       <c r="AB21" s="4"/>
       <c r="AC21" s="40">
         <f>V56*AC28+W56*AC29+X56*AC30+Y56*AC31+Z56*AC32+AA56*AC33</f>
-        <v>-1.22514845490862E-12</v>
+        <v>6.1257422745431001E-13</v>
       </c>
       <c r="AD21" s="4"/>
       <c r="AJ21" s="4"/>
@@ -12347,7 +12275,7 @@
       <c r="H22" s="4"/>
       <c r="I22" s="40">
         <f>B56*I28+C56*I29+D56*I30+E56*I31+F56*I32+G56*I33</f>
-        <v>13333333.333333334</v>
+        <v>-13333333.333333334</v>
       </c>
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
@@ -12378,7 +12306,7 @@
       <c r="R22" s="4"/>
       <c r="S22" s="40">
         <f>L57*S28+M57*S29+N57*S30+O57*S31+P57*S32+Q57*S33</f>
-        <v>30000000</v>
+        <v>-30000000</v>
       </c>
       <c r="T22" s="4"/>
       <c r="U22" s="4"/>
@@ -12409,7 +12337,7 @@
       <c r="AB22" s="4"/>
       <c r="AC22" s="40">
         <f>V57*AC28+W57*AC29+X57*AC30+Y57*AC31+Z57*AC32+AA57*AC33</f>
-        <v>-13333333.333333334</v>
+        <v>6666666.666666667</v>
       </c>
       <c r="AD22" s="4"/>
       <c r="AJ22" s="4"/>
@@ -12458,7 +12386,7 @@
       <c r="H23" s="4"/>
       <c r="I23" s="40">
         <f>B57*I28+C57*I29+D57*I30+E57*I31+F57*I32+G57*I33</f>
-        <v>-20000</v>
+        <v>20000</v>
       </c>
       <c r="J23" s="4"/>
       <c r="K23" s="4"/>
@@ -12520,7 +12448,7 @@
       <c r="AB23" s="4"/>
       <c r="AC23" s="40">
         <f>V58*AC28+W58*AC29+X58*AC30+Y58*AC31+Z58*AC32+AA58*AC33</f>
-        <v>20000</v>
+        <v>-10000</v>
       </c>
       <c r="AD23" s="4"/>
       <c r="AJ23" s="79" t="s">
@@ -12571,7 +12499,7 @@
       <c r="H24" s="4"/>
       <c r="I24" s="40">
         <f>B58*I28+C58*I29+D58*I30+E58*I31+F58*I32+G58*I33</f>
-        <v>1.22514845490862E-12</v>
+        <v>-1.22514845490862E-12</v>
       </c>
       <c r="J24" s="4"/>
       <c r="K24" s="4"/>
@@ -12602,7 +12530,7 @@
       <c r="R24" s="4"/>
       <c r="S24" s="40">
         <f>L59*S28+M59*S29+N59*S30+O59*S31+P59*S32+Q59*S33</f>
-        <v>30000</v>
+        <v>-30000</v>
       </c>
       <c r="T24" s="4"/>
       <c r="U24" s="4"/>
@@ -12633,7 +12561,7 @@
       <c r="AB24" s="4"/>
       <c r="AC24" s="40">
         <f>V59*AC28+W59*AC29+X59*AC30+Y59*AC31+Z59*AC32+AA59*AC33</f>
-        <v>-1.22514845490862E-12</v>
+        <v>6.1257422745431001E-13</v>
       </c>
       <c r="AD24" s="4"/>
       <c r="AJ24" s="78"/>
@@ -12710,7 +12638,7 @@
       <c r="H25" s="4"/>
       <c r="I25" s="40">
         <f>B59*I28+C59*I29+D59*I30+E59*I31+F59*I32+G59*I33</f>
-        <v>-13333333.333333334</v>
+        <v>13333333.333333334</v>
       </c>
       <c r="J25" s="4"/>
       <c r="K25" s="82"/>
@@ -12741,7 +12669,7 @@
       <c r="R25" s="4"/>
       <c r="S25" s="40">
         <f>L60*S28+M60*S29+N60*S30+O60*S31+P60*S32+Q60*S33</f>
-        <v>-30000000</v>
+        <v>30000000</v>
       </c>
       <c r="T25" s="4"/>
       <c r="U25" s="82"/>
@@ -12772,7 +12700,7 @@
       <c r="AB25" s="4"/>
       <c r="AC25" s="40">
         <f>V60*AC28+W60*AC29+X60*AC30+Y60*AC31+Z60*AC32+AA60*AC33</f>
-        <v>13333333.333333334</v>
+        <v>-6666666.666666667</v>
       </c>
       <c r="AD25" s="4"/>
       <c r="AE25" s="115"/>
@@ -12985,7 +12913,7 @@
       </c>
       <c r="AB28" s="4"/>
       <c r="AC28" s="38">
-        <f>Y6/2*Y14</f>
+        <f>-Y6/2*Y14</f>
         <v>0</v>
       </c>
       <c r="AD28" s="4"/>
@@ -13034,8 +12962,8 @@
       </c>
       <c r="H29" s="4"/>
       <c r="I29" s="38">
-        <f>E6/2*E15</f>
-        <v>20000</v>
+        <f>-E6/2*E15</f>
+        <v>-20000</v>
       </c>
       <c r="J29" s="4"/>
       <c r="K29" s="4"/>
@@ -13063,8 +12991,8 @@
       </c>
       <c r="R29" s="4"/>
       <c r="S29" s="38">
-        <f>O6/2*(O14+O15)</f>
-        <v>30000</v>
+        <f>-O6/2*(O14+O15)</f>
+        <v>-30000</v>
       </c>
       <c r="T29" s="4"/>
       <c r="U29" s="4"/>
@@ -13092,8 +13020,8 @@
       </c>
       <c r="AB29" s="4"/>
       <c r="AC29" s="38">
-        <f>Y6/2*Y15</f>
-        <v>-20000</v>
+        <f>-Y6/2*Y15</f>
+        <v>10000</v>
       </c>
       <c r="AD29" s="4"/>
       <c r="AJ29" s="78">
@@ -13141,8 +13069,8 @@
       </c>
       <c r="H30" s="4"/>
       <c r="I30" s="38">
-        <f>1*(E15*E6^2)/12</f>
-        <v>13333333.333333334</v>
+        <f>-1*(E15*E6^2)/12</f>
+        <v>-13333333.333333334</v>
       </c>
       <c r="J30" s="4"/>
       <c r="K30" s="4"/>
@@ -13170,8 +13098,8 @@
       </c>
       <c r="R30" s="4"/>
       <c r="S30" s="38">
-        <f>1*((O14+O15)*O6^2)/12</f>
-        <v>30000000</v>
+        <f>-1*((O14+O15)*O6^2)/12</f>
+        <v>-30000000</v>
       </c>
       <c r="T30" s="4"/>
       <c r="U30" s="4"/>
@@ -13199,8 +13127,8 @@
       </c>
       <c r="AB30" s="4"/>
       <c r="AC30" s="38">
-        <f>1*(Y15*Y6^2)/12</f>
-        <v>-13333333.333333334</v>
+        <f>-1*(Y15*Y6^2)/12</f>
+        <v>6666666.666666667</v>
       </c>
       <c r="AD30" s="4"/>
       <c r="AJ30" s="78">
@@ -13299,7 +13227,7 @@
       </c>
       <c r="AB31" s="4"/>
       <c r="AC31" s="38">
-        <f>Y6/2*Y14</f>
+        <f>-Y6/2*Y14</f>
         <v>0</v>
       </c>
       <c r="AD31" s="4"/>
@@ -13340,7 +13268,7 @@
       </c>
       <c r="AY31" s="8" cm="1">
         <f t="array" ref="AY31:AY35">AC20:AC24</f>
-        <v>20000</v>
+        <v>-10000</v>
       </c>
     </row>
     <row r="32" spans="1:67" x14ac:dyDescent="0.2">
@@ -13369,8 +13297,8 @@
       </c>
       <c r="H32" s="4"/>
       <c r="I32" s="38">
-        <f>E6/2*E15</f>
-        <v>20000</v>
+        <f>-E6/2*E15</f>
+        <v>-20000</v>
       </c>
       <c r="J32" s="4"/>
       <c r="K32" s="4"/>
@@ -13398,8 +13326,8 @@
       </c>
       <c r="R32" s="82"/>
       <c r="S32" s="38">
-        <f>O6/2*(O14+O15)</f>
-        <v>30000</v>
+        <f>-O6/2*(O14+O15)</f>
+        <v>-30000</v>
       </c>
       <c r="T32" s="4"/>
       <c r="U32" s="4"/>
@@ -13427,8 +13355,8 @@
       </c>
       <c r="AB32" s="4"/>
       <c r="AC32" s="38">
-        <f>Y6/2*Y15</f>
-        <v>-20000</v>
+        <f>-Y6/2*Y15</f>
+        <v>10000</v>
       </c>
       <c r="AD32" s="4"/>
       <c r="AJ32" s="78">
@@ -13467,7 +13395,7 @@
         <v>4.0200183676689094E-11</v>
       </c>
       <c r="AY32" s="10">
-        <v>-1.22514845490862E-12</v>
+        <v>6.1257422745431001E-13</v>
       </c>
     </row>
     <row r="33" spans="1:83" x14ac:dyDescent="0.2">
@@ -13496,8 +13424,8 @@
       </c>
       <c r="H33" s="4"/>
       <c r="I33" s="38">
-        <f>-1*(E15*E6^2)/12</f>
-        <v>-13333333.333333334</v>
+        <f>1*(E15*E6^2)/12</f>
+        <v>13333333.333333334</v>
       </c>
       <c r="J33" s="4"/>
       <c r="K33" s="4"/>
@@ -13525,8 +13453,8 @@
       </c>
       <c r="R33" s="4"/>
       <c r="S33" s="38">
-        <f>-1*((O14+O15)*O6^2)/12</f>
-        <v>-30000000</v>
+        <f>1*((O14+O15)*O6^2)/12</f>
+        <v>30000000</v>
       </c>
       <c r="T33" s="4"/>
       <c r="U33" s="4"/>
@@ -13554,8 +13482,8 @@
       </c>
       <c r="AB33" s="4"/>
       <c r="AC33" s="38">
-        <f>-1*(Y15*Y6^2)/12</f>
-        <v>13333333.333333334</v>
+        <f>1*(Y15*Y6^2)/12</f>
+        <v>-6666666.666666667</v>
       </c>
       <c r="AD33" s="4"/>
       <c r="AJ33" s="78">
@@ -13594,7 +13522,7 @@
         <v>875000000</v>
       </c>
       <c r="AY33" s="8">
-        <v>-13333333.333333334</v>
+        <v>6666666.666666667</v>
       </c>
     </row>
     <row r="34" spans="1:83" x14ac:dyDescent="0.2">
@@ -13664,7 +13592,7 @@
         <v>656250</v>
       </c>
       <c r="AY34" s="8">
-        <v>20000</v>
+        <v>-10000</v>
       </c>
     </row>
     <row r="35" spans="1:83" x14ac:dyDescent="0.2">
@@ -13736,7 +13664,7 @@
         <v>-4.0200183676689094E-11</v>
       </c>
       <c r="AY35" s="10">
-        <v>-1.22514845490862E-12</v>
+        <v>6.1257422745431001E-13</v>
       </c>
     </row>
     <row r="36" spans="1:83" x14ac:dyDescent="0.2">
@@ -14037,7 +13965,7 @@
       </c>
       <c r="AY38" s="7">
         <f>AC25</f>
-        <v>13333333.333333334</v>
+        <v>-6666666.666666667</v>
       </c>
     </row>
     <row r="39" spans="1:83" x14ac:dyDescent="0.2">
@@ -14787,19 +14715,19 @@
       <c r="BA46" s="1"/>
       <c r="BB46" s="3">
         <f>AY6+BO6+AY25</f>
-        <v>-20000</v>
+        <v>20000</v>
       </c>
       <c r="BC46" s="144" t="s">
         <v>52</v>
       </c>
-      <c r="BD46" s="29" cm="1">
+      <c r="BD46" s="32" cm="1">
         <f t="array" ref="BD46:BD48">AZ46:AZ48</f>
         <v>0</v>
       </c>
       <c r="BE46" s="4"/>
       <c r="BF46" s="4">
         <f t="array" ref="BF46:BF59">MMULT(AK46:AX59,BD46:BD59)-BB46:BB59</f>
-        <v>25000.878854754606</v>
+        <v>-28750.65914106604</v>
       </c>
       <c r="BG46" s="4"/>
       <c r="BH46" s="4"/>
@@ -14949,17 +14877,17 @@
       <c r="BA47" s="1"/>
       <c r="BB47" s="3">
         <f t="shared" ref="BB47:BB59" si="36">AY7+BO7+AY26</f>
-        <v>1.22514845490862E-12</v>
+        <v>-1.22514845490862E-12</v>
       </c>
       <c r="BC47" s="144" t="s">
         <v>51</v>
       </c>
-      <c r="BD47" s="29">
+      <c r="BD47" s="32">
         <v>0</v>
       </c>
       <c r="BE47" s="154"/>
       <c r="BF47" s="154">
-        <v>-30000</v>
+        <v>29999.999999999996</v>
       </c>
       <c r="BG47" s="155"/>
       <c r="BH47" s="155"/>
@@ -15108,17 +15036,17 @@
       <c r="BA48" s="1"/>
       <c r="BB48" s="3">
         <f t="shared" si="36"/>
-        <v>13333333.333333334</v>
+        <v>-13333333.333333334</v>
       </c>
       <c r="BC48" s="144" t="s">
         <v>83</v>
       </c>
-      <c r="BD48" s="29">
+      <c r="BD48" s="32">
         <v>0</v>
       </c>
       <c r="BE48" s="154"/>
       <c r="BF48" s="154">
-        <v>-20003515.419018425</v>
+        <v>35002636.564264163</v>
       </c>
       <c r="BG48" s="155"/>
       <c r="BH48" s="154"/>
@@ -15271,16 +15199,16 @@
       <c r="BA49" s="1"/>
       <c r="BB49" s="3">
         <f t="shared" si="36"/>
-        <v>-20000</v>
+        <v>20000</v>
       </c>
       <c r="BC49" s="1"/>
       <c r="BD49" s="153" cm="1">
         <f t="array" ref="BD49:BD51">AV77:AV79</f>
-        <v>-1.0713657960906176E-2</v>
+        <v>45.722320957757432</v>
       </c>
       <c r="BE49" s="154"/>
       <c r="BF49" s="154">
-        <v>2.151500666514039E-8</v>
+        <v>-1.076841726899147E-8</v>
       </c>
       <c r="BG49" s="155"/>
       <c r="BH49" s="154"/>
@@ -15431,11 +15359,11 @@
       <c r="BA50" s="1"/>
       <c r="BB50" s="3">
         <f t="shared" si="36"/>
-        <v>30000</v>
+        <v>-30000</v>
       </c>
       <c r="BC50" s="1"/>
       <c r="BD50" s="153">
-        <v>5.7142857142857141E-2</v>
+        <v>-5.7142857142859937E-2</v>
       </c>
       <c r="BF50" s="80">
         <v>0</v>
@@ -15573,11 +15501,11 @@
       <c r="BA51" s="1"/>
       <c r="BB51" s="3">
         <f t="shared" si="36"/>
-        <v>30000000</v>
+        <v>-30000000</v>
       </c>
       <c r="BC51" s="1"/>
-      <c r="BD51" s="153">
-        <v>6.4285714285714276E-3</v>
+      <c r="BD51" s="157">
+        <v>-6.4285714285714276E-3</v>
       </c>
       <c r="BE51" s="154"/>
       <c r="BF51" s="154">
@@ -15691,18 +15619,18 @@
       <c r="BA52" s="1"/>
       <c r="BB52" s="3">
         <f t="shared" si="36"/>
-        <v>20000</v>
+        <v>-10000</v>
       </c>
       <c r="BC52" s="144" t="s">
         <v>53</v>
       </c>
-      <c r="BD52" s="29" cm="1">
+      <c r="BD52" s="32" cm="1">
         <f t="array" ref="BD52:BD54">AZ52:AZ54</f>
         <v>0</v>
       </c>
       <c r="BE52" s="154"/>
       <c r="BF52" s="154">
-        <v>-25000.878854754599</v>
+        <v>8750.6591410658639</v>
       </c>
       <c r="BG52" s="155"/>
       <c r="BH52" s="154"/>
@@ -15814,17 +15742,17 @@
       <c r="BA53" s="1"/>
       <c r="BB53" s="3">
         <f t="shared" si="36"/>
-        <v>-1.22514845490862E-12</v>
+        <v>6.1257422745431001E-13</v>
       </c>
       <c r="BC53" s="144" t="s">
         <v>54</v>
       </c>
-      <c r="BD53" s="29">
+      <c r="BD53" s="32">
         <v>0</v>
       </c>
       <c r="BE53" s="155"/>
       <c r="BF53" s="155">
-        <v>-30000</v>
+        <v>30000</v>
       </c>
       <c r="BG53" s="155"/>
       <c r="BH53" s="155"/>
@@ -15953,17 +15881,17 @@
       <c r="BA54" s="1"/>
       <c r="BB54" s="3">
         <f t="shared" si="36"/>
-        <v>-13333333.333333334</v>
+        <v>6666666.666666667</v>
       </c>
       <c r="BC54" s="144" t="s">
         <v>86</v>
       </c>
-      <c r="BD54" s="29">
+      <c r="BD54" s="32">
         <v>0</v>
       </c>
       <c r="BE54" s="154"/>
       <c r="BF54" s="154">
-        <v>20003515.419018395</v>
+        <v>4997363.4357365454</v>
       </c>
       <c r="BG54" s="155"/>
       <c r="BH54" s="154"/>
@@ -16117,16 +16045,16 @@
       <c r="BA55" s="1"/>
       <c r="BB55" s="3">
         <f t="shared" si="36"/>
-        <v>20000</v>
+        <v>-10000</v>
       </c>
       <c r="BC55" s="1"/>
       <c r="BD55" s="153" cm="1">
         <f t="array" ref="BD55:BD59">AV80:AV84</f>
-        <v>1.0713657960842227E-2</v>
+        <v>45.706250470816116</v>
       </c>
       <c r="BE55" s="155"/>
       <c r="BF55" s="155">
-        <v>-2.1522282622754574E-8</v>
+        <v>1.3978933566249907E-8</v>
       </c>
       <c r="BG55" s="155"/>
       <c r="BH55" s="155"/>
@@ -16279,11 +16207,11 @@
       <c r="BA56" s="1"/>
       <c r="BB56" s="3">
         <f t="shared" si="36"/>
-        <v>30000</v>
+        <v>-30000</v>
       </c>
       <c r="BC56" s="1"/>
       <c r="BD56" s="153">
-        <v>5.7142857142857141E-2</v>
+        <v>-5.7142857142859944E-2</v>
       </c>
       <c r="BE56" s="155"/>
       <c r="BF56" s="155">
@@ -16437,11 +16365,11 @@
       <c r="BA57" s="1"/>
       <c r="BB57" s="3">
         <f t="shared" si="36"/>
-        <v>-30000000</v>
+        <v>30000000</v>
       </c>
       <c r="BC57" s="1"/>
-      <c r="BD57" s="153">
-        <v>-6.4285714285714276E-3</v>
+      <c r="BD57" s="157">
+        <v>6.4285714285714276E-3</v>
       </c>
       <c r="BE57" s="155"/>
       <c r="BF57" s="155">
@@ -16594,11 +16522,11 @@
       <c r="BA58" s="155"/>
       <c r="BB58" s="3">
         <f t="shared" si="36"/>
-        <v>-13333333.333333334</v>
+        <v>13333333.333333334</v>
       </c>
       <c r="BC58" s="155"/>
-      <c r="BD58" s="153">
-        <v>-7.6150299973122802E-3</v>
+      <c r="BD58" s="157">
+        <v>-9.5268227401114139E-3</v>
       </c>
       <c r="BE58" s="155"/>
       <c r="BF58" s="155">
@@ -16750,13 +16678,13 @@
       <c r="BA59" s="155"/>
       <c r="BB59" s="3">
         <f t="shared" si="36"/>
-        <v>13333333.333333334</v>
-      </c>
-      <c r="BD59" s="153">
-        <v>7.6150299973122958E-3</v>
+        <v>-6666666.666666667</v>
+      </c>
+      <c r="BD59" s="157">
+        <v>-2.0949367736079846E-2</v>
       </c>
       <c r="BF59" s="80">
-        <v>0</v>
+        <v>1.3969838619232178E-8</v>
       </c>
       <c r="BG59" s="155"/>
       <c r="BH59" s="155"/>
@@ -16950,7 +16878,12 @@
       <c r="AX63"/>
       <c r="AY63"/>
       <c r="AZ63" s="111"/>
-      <c r="BB63" s="111"/>
+      <c r="BB63" s="111" t="s">
+        <v>95</v>
+      </c>
+      <c r="BC63" s="80" t="s">
+        <v>94</v>
+      </c>
       <c r="BE63" s="111"/>
       <c r="BK63" s="116"/>
       <c r="BT63" s="112"/>
@@ -16976,7 +16909,14 @@
       <c r="AW64" s="1"/>
       <c r="AX64" s="1"/>
       <c r="AY64"/>
-      <c r="BB64" s="111"/>
+      <c r="BB64" s="111" cm="1">
+        <f t="array" ref="BB64:BB68">BF46:BF50</f>
+        <v>-28750.65914106604</v>
+      </c>
+      <c r="BC64" s="80" cm="1">
+        <f t="array" ref="BC64:BC69">MMULT(B45:G50,BB64:BB69)</f>
+        <v>29999.999999999996</v>
+      </c>
       <c r="BE64" s="111"/>
       <c r="BK64" s="116"/>
       <c r="BT64" s="112"/>
@@ -17024,7 +16964,12 @@
       <c r="AW65" s="1"/>
       <c r="AX65" s="1"/>
       <c r="AY65"/>
-      <c r="BB65" s="111"/>
+      <c r="BB65" s="111">
+        <v>29999.999999999996</v>
+      </c>
+      <c r="BC65" s="80">
+        <v>28750.659141066044</v>
+      </c>
       <c r="BE65" s="111"/>
     </row>
     <row r="66" spans="5:74" ht="15" x14ac:dyDescent="0.25">
@@ -17065,11 +17010,17 @@
       <c r="AU66" s="1"/>
       <c r="AV66" s="145" cm="1">
         <f t="array" ref="AV66:AV68">BB49:BB51</f>
-        <v>-20000</v>
+        <v>20000</v>
       </c>
       <c r="AW66" s="1"/>
       <c r="AX66" s="1"/>
       <c r="AY66"/>
+      <c r="BB66" s="80">
+        <v>35002636.564264163</v>
+      </c>
+      <c r="BC66" s="80">
+        <v>35002636.564264163</v>
+      </c>
     </row>
     <row r="67" spans="5:74" ht="15" x14ac:dyDescent="0.25">
       <c r="AJ67" s="78">
@@ -17105,11 +17056,17 @@
       </c>
       <c r="AU67" s="1"/>
       <c r="AV67" s="142">
-        <v>30000</v>
+        <v>-30000</v>
       </c>
       <c r="AW67" s="1"/>
       <c r="AX67" s="1"/>
       <c r="AY67"/>
+      <c r="BB67" s="80">
+        <v>-1.076841726899147E-8</v>
+      </c>
+      <c r="BC67" s="80">
+        <v>-6.5964548894581007E-25</v>
+      </c>
     </row>
     <row r="68" spans="5:74" ht="15" x14ac:dyDescent="0.25">
       <c r="AJ68" s="78">
@@ -17145,11 +17102,17 @@
       </c>
       <c r="AU68" s="1"/>
       <c r="AV68" s="142">
-        <v>30000000</v>
+        <v>-30000000</v>
       </c>
       <c r="AW68" s="1"/>
       <c r="AX68" s="1"/>
       <c r="AY68"/>
+      <c r="BB68" s="80">
+        <v>0</v>
+      </c>
+      <c r="BC68" s="80">
+        <v>1.076841726899147E-8</v>
+      </c>
       <c r="BO68" s="115"/>
       <c r="BR68" s="139"/>
     </row>
@@ -17191,11 +17154,18 @@
       <c r="AU69" s="1"/>
       <c r="AV69" s="145" cm="1">
         <f t="array" ref="AV69:AV73">BB55:BB59</f>
-        <v>20000</v>
+        <v>-10000</v>
       </c>
       <c r="AW69" s="1"/>
       <c r="AX69" s="1"/>
       <c r="AY69"/>
+      <c r="BB69" s="80">
+        <f>BF59</f>
+        <v>1.3969838619232178E-8</v>
+      </c>
+      <c r="BC69" s="80">
+        <v>1.3969838619232178E-8</v>
+      </c>
       <c r="BR69" s="139"/>
     </row>
     <row r="70" spans="5:74" ht="15" x14ac:dyDescent="0.25">
@@ -17234,7 +17204,7 @@
       </c>
       <c r="AU70" s="1"/>
       <c r="AV70" s="3">
-        <v>30000</v>
+        <v>-30000</v>
       </c>
       <c r="AW70" s="1"/>
       <c r="AX70" s="1"/>
@@ -17275,7 +17245,7 @@
       </c>
       <c r="AU71" s="1"/>
       <c r="AV71" s="1">
-        <v>-30000000</v>
+        <v>30000000</v>
       </c>
       <c r="AW71" s="1"/>
       <c r="AX71" s="1"/>
@@ -17316,7 +17286,7 @@
       </c>
       <c r="AU72" s="1"/>
       <c r="AV72" s="1">
-        <v>-13333333.333333334</v>
+        <v>13333333.333333334</v>
       </c>
       <c r="AW72" s="1"/>
       <c r="AX72" s="1"/>
@@ -17359,7 +17329,7 @@
       </c>
       <c r="AU73" s="1"/>
       <c r="AV73" s="1">
-        <v>13333333.333333334</v>
+        <v>-6666666.666666667</v>
       </c>
       <c r="AW73" s="1"/>
       <c r="AX73" s="1"/>
@@ -17485,12 +17455,12 @@
       <c r="AS77" s="1"/>
       <c r="AT77" s="3" cm="1">
         <f t="array" ref="AT77:AT84">AV66:AV73</f>
-        <v>-20000</v>
+        <v>20000</v>
       </c>
       <c r="AU77" s="1"/>
       <c r="AV77" s="153" cm="1">
         <f t="array" ref="AV77:AV84">MMULT(AK77:AR84,AT77:AT84)</f>
-        <v>-1.0713657960906176E-2</v>
+        <v>45.722320957757432</v>
       </c>
       <c r="AW77" s="1" t="s">
         <v>3</v>
@@ -17528,11 +17498,11 @@
       </c>
       <c r="AS78" s="1"/>
       <c r="AT78" s="80">
-        <v>30000</v>
+        <v>-30000</v>
       </c>
       <c r="AU78" s="1"/>
       <c r="AV78" s="153">
-        <v>5.7142857142857141E-2</v>
+        <v>-5.7142857142859937E-2</v>
       </c>
       <c r="AW78" s="1" t="s">
         <v>3</v>
@@ -17570,18 +17540,18 @@
       </c>
       <c r="AS79" s="1"/>
       <c r="AT79" s="1">
-        <v>30000000</v>
+        <v>-30000000</v>
       </c>
       <c r="AU79" s="1"/>
       <c r="AV79" s="153">
-        <v>6.4285714285714276E-3</v>
+        <v>-6.4285714285714276E-3</v>
       </c>
       <c r="AW79" s="1" t="s">
         <v>57</v>
       </c>
       <c r="AX79" s="1">
         <f>1000*AV79</f>
-        <v>6.4285714285714279</v>
+        <v>-6.4285714285714279</v>
       </c>
       <c r="AY79" s="4"/>
       <c r="BK79" s="115"/>
@@ -17616,11 +17586,11 @@
       </c>
       <c r="AS80" s="1"/>
       <c r="AT80" s="1">
-        <v>20000</v>
+        <v>-10000</v>
       </c>
       <c r="AU80" s="1"/>
       <c r="AV80" s="153">
-        <v>1.0713657960842227E-2</v>
+        <v>45.706250470816116</v>
       </c>
       <c r="AW80" s="1" t="s">
         <v>3</v>
@@ -17669,11 +17639,11 @@
       </c>
       <c r="AS81" s="1"/>
       <c r="AT81" s="3">
-        <v>30000</v>
+        <v>-30000</v>
       </c>
       <c r="AU81" s="1"/>
       <c r="AV81" s="153">
-        <v>5.7142857142857141E-2</v>
+        <v>-5.7142857142859944E-2</v>
       </c>
       <c r="AW81" s="1" t="s">
         <v>3</v>
@@ -17722,18 +17692,18 @@
       </c>
       <c r="AS82" s="1"/>
       <c r="AT82" s="1">
-        <v>-30000000</v>
+        <v>30000000</v>
       </c>
       <c r="AU82" s="1"/>
       <c r="AV82" s="153">
-        <v>-6.4285714285714276E-3</v>
+        <v>6.4285714285714276E-3</v>
       </c>
       <c r="AW82" s="1" t="s">
         <v>57</v>
       </c>
       <c r="AX82" s="1">
         <f>1000*AV82</f>
-        <v>-6.4285714285714279</v>
+        <v>6.4285714285714279</v>
       </c>
       <c r="AY82" s="4"/>
       <c r="AZ82" s="111"/>
@@ -17813,18 +17783,18 @@
       </c>
       <c r="AS83" s="1"/>
       <c r="AT83" s="1">
-        <v>-13333333.333333334</v>
+        <v>13333333.333333334</v>
       </c>
       <c r="AU83" s="1"/>
       <c r="AV83" s="153">
-        <v>-7.6150299973122802E-3</v>
+        <v>-9.5268227401114139E-3</v>
       </c>
       <c r="AW83" s="1" t="s">
         <v>57</v>
       </c>
       <c r="AX83" s="1">
         <f>1000*AV83</f>
-        <v>-7.6150299973122806</v>
+        <v>-9.5268227401114132</v>
       </c>
       <c r="AY83" s="4"/>
       <c r="AZ83" s="109"/>
@@ -17902,18 +17872,18 @@
       </c>
       <c r="AS84" s="1"/>
       <c r="AT84" s="1">
-        <v>13333333.333333334</v>
+        <v>-6666666.666666667</v>
       </c>
       <c r="AU84" s="1"/>
       <c r="AV84" s="153">
-        <v>7.6150299973122958E-3</v>
+        <v>-2.0949367736079846E-2</v>
       </c>
       <c r="AW84" s="1" t="s">
         <v>57</v>
       </c>
       <c r="AX84" s="1">
         <f>1000*AV84</f>
-        <v>7.6150299973122957</v>
+        <v>-20.949367736079846</v>
       </c>
       <c r="AY84" s="4"/>
       <c r="AZ84" s="4"/>
@@ -19427,32 +19397,32 @@
     </row>
   </sheetData>
   <phoneticPr fontId="14" type="noConversion"/>
+  <conditionalFormatting sqref="AK66:AV73">
+    <cfRule type="expression" dxfId="5" priority="1">
+      <formula>ABS(AK66)&lt;0.1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="AK6:AX60">
-    <cfRule type="expression" dxfId="5" priority="2">
+    <cfRule type="expression" dxfId="4" priority="2">
       <formula>ABS(AK6)&lt;0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK90:AX103">
-    <cfRule type="expression" dxfId="4" priority="3">
+    <cfRule type="expression" dxfId="3" priority="3">
       <formula>ABS(AK90)&lt;0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BB46:BB59">
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="2" priority="4">
       <formula>ABS(BB46)&lt;0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BR172:BR174">
-    <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="6" operator="equal">
       <formula>"VIRHE!"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="7" operator="equal">
       <formula>"OK!"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AK66:AV73">
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>ABS(AK66)&lt;0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -19462,10 +19432,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A31214F-D315-442C-9106-A983B611689D}">
-  <dimension ref="M30:R33"/>
+  <dimension ref="M30:R34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O25" sqref="O25"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M34" sqref="M34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19514,6 +19484,12 @@
     </row>
     <row r="33" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M33">
+        <f>P31/M31^3*((2*N31+M31)*O31^2+1/4*(N31-O31)*P31^2)*R31</f>
+        <v>10473.6328125</v>
+      </c>
+    </row>
+    <row r="34" spans="13:13" x14ac:dyDescent="0.25">
+      <c r="M34">
         <f>P31/M31^2*(N31*O31^2+1/12*(N31-2*O31)*P31^2)*R31</f>
         <v>9749348.9583333321</v>
       </c>

</xml_diff>

<commit_message>
Increment version and method to API to check which version the library is
</commit_message>
<xml_diff>
--- a/theory/FEM matriisit.xlsx
+++ b/theory/FEM matriisit.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ohjelmointi\2_Rust\idfem\theory\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ohjelmointi\2_Rust\vefem\theory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{428CB022-27BE-4935-923A-805D8E674509}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FF1CBCC-04AA-4158-9486-FC4E1A11FAFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38295" yWindow="0" windowWidth="23460" windowHeight="20880" activeTab="2" xr2:uid="{27180542-B0D2-4BFE-946B-7857B24C93C8}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="3" xr2:uid="{27180542-B0D2-4BFE-946B-7857B24C93C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Ilman vapautuksia" sheetId="1" r:id="rId1"/>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="103">
   <si>
     <t>°</t>
   </si>
@@ -740,7 +740,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="159">
+  <cellXfs count="160">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1154,6 +1154,7 @@
     </xf>
     <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutraali" xfId="1" builtinId="28"/>
@@ -19587,7 +19588,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A219C33C-A99E-4D9D-A1C8-724BB0D5FC4F}">
   <dimension ref="A1:CW233"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AU3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="BG49" sqref="BG49"/>
     </sheetView>
   </sheetViews>
@@ -29813,14 +29814,32 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A31214F-D315-442C-9106-A983B611689D}">
-  <dimension ref="M30:R34"/>
+  <dimension ref="L14:R34"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M34" sqref="M34"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
+    <row r="14" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L14" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="12:14" x14ac:dyDescent="0.25">
+      <c r="L15" s="159">
+        <v>10000000</v>
+      </c>
+      <c r="M15">
+        <f>6*N31*O31/M31^3*L15</f>
+        <v>3750</v>
+      </c>
+      <c r="N15">
+        <f>O31*(2*N31-O31)/M31^2*L15</f>
+        <v>2500000</v>
+      </c>
+    </row>
     <row r="30" spans="13:18" x14ac:dyDescent="0.25">
       <c r="M30" t="s">
         <v>89</v>
@@ -29846,12 +29865,11 @@
         <v>4000</v>
       </c>
       <c r="N31">
-        <f>1000+(2500/2)</f>
-        <v>2250</v>
+        <v>2000</v>
       </c>
       <c r="O31">
-        <f>500+2500/2</f>
-        <v>1750</v>
+        <f>M31-N31</f>
+        <v>2000</v>
       </c>
       <c r="P31">
         <v>2500</v>
@@ -29866,13 +29884,13 @@
     <row r="33" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M33">
         <f>P31/M31^3*((2*N31+M31)*O31^2+1/4*(N31-O31)*P31^2)*R31</f>
-        <v>10473.6328125</v>
+        <v>12500</v>
       </c>
     </row>
     <row r="34" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M34">
         <f>P31/M31^2*(N31*O31^2+1/12*(N31-2*O31)*P31^2)*R31</f>
-        <v>9749348.9583333321</v>
+        <v>10872395.833333332</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add test for element local nodal force vectors
</commit_message>
<xml_diff>
--- a/theory/FEM matriisit.xlsx
+++ b/theory/FEM matriisit.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ohjelmointi\2_Rust\vefem\theory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FF1CBCC-04AA-4158-9486-FC4E1A11FAFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1377142-8139-465E-AF87-9D282E5BCB9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="3" xr2:uid="{27180542-B0D2-4BFE-946B-7857B24C93C8}"/>
+    <workbookView xWindow="-25875" yWindow="0" windowWidth="25980" windowHeight="20880" xr2:uid="{27180542-B0D2-4BFE-946B-7857B24C93C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Ilman vapautuksia" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="109">
   <si>
     <t>°</t>
   </si>
@@ -447,6 +447,24 @@
   <si>
     <t>Yleinen jousivakio</t>
   </si>
+  <si>
+    <t>siirtymät (lok)</t>
+  </si>
+  <si>
+    <t>lukkovoimat (lok, kierretyt)</t>
+  </si>
+  <si>
+    <t>Elementin 1 lokaalit solmupisteiden voimasuureet</t>
+  </si>
+  <si>
+    <t>solmupisteiden voimavektorit</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Jäykkyysmatriisi * lokaalit siirtymät - lokaalit lukkovoimat</t>
+  </si>
 </sst>
 </file>
 
@@ -740,7 +758,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="160">
+  <cellXfs count="161">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1155,6 +1173,9 @@
     <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutraali" xfId="1" builtinId="28"/>
@@ -2026,8 +2047,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94F9BDF3-3EE6-4BFB-9734-CB047BC6E804}">
   <dimension ref="B1:CW227"/>
   <sheetViews>
-    <sheetView topLeftCell="AM18" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BB48" sqref="BB48"/>
+    <sheetView tabSelected="1" topLeftCell="AG47" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AQ79" sqref="AQ79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -8615,13 +8636,13 @@
       <c r="BD80" s="28"/>
       <c r="BE80" s="12"/>
     </row>
-    <row r="81" spans="52:83" x14ac:dyDescent="0.2">
+    <row r="81" spans="36:83" x14ac:dyDescent="0.2">
       <c r="AZ81" s="4"/>
       <c r="BB81" s="12"/>
       <c r="BE81" s="12"/>
       <c r="BK81" s="2"/>
     </row>
-    <row r="82" spans="52:83" x14ac:dyDescent="0.2">
+    <row r="82" spans="36:83" x14ac:dyDescent="0.2">
       <c r="AZ82" s="4"/>
       <c r="BB82" s="12"/>
       <c r="BE82" s="12"/>
@@ -8637,7 +8658,10 @@
       <c r="BY82" s="65"/>
       <c r="CA82" s="63"/>
     </row>
-    <row r="83" spans="52:83" x14ac:dyDescent="0.2">
+    <row r="83" spans="36:83" x14ac:dyDescent="0.2">
+      <c r="AJ83" s="1" t="s">
+        <v>105</v>
+      </c>
       <c r="AZ83" s="12"/>
       <c r="BB83" s="12"/>
       <c r="BE83" s="12"/>
@@ -8654,7 +8678,13 @@
       <c r="CA83" s="63"/>
       <c r="CE83" s="45"/>
     </row>
-    <row r="84" spans="52:83" x14ac:dyDescent="0.2">
+    <row r="84" spans="36:83" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AJ84" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="AT84" s="160" t="s">
+        <v>104</v>
+      </c>
       <c r="AZ84" s="12"/>
       <c r="BB84" s="12"/>
       <c r="BE84" s="12"/>
@@ -8676,7 +8706,42 @@
       <c r="BZ84" s="4"/>
       <c r="CA84" s="63"/>
     </row>
-    <row r="85" spans="52:83" x14ac:dyDescent="0.2">
+    <row r="85" spans="36:83" x14ac:dyDescent="0.2">
+      <c r="AJ85" s="9"/>
+      <c r="AK85" s="9">
+        <v>1</v>
+      </c>
+      <c r="AL85" s="9">
+        <v>2</v>
+      </c>
+      <c r="AM85" s="9">
+        <v>3</v>
+      </c>
+      <c r="AN85" s="9">
+        <v>4</v>
+      </c>
+      <c r="AO85" s="9">
+        <v>5</v>
+      </c>
+      <c r="AP85" s="9">
+        <v>6</v>
+      </c>
+      <c r="AQ85" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AR85" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="AS85" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="AT85" s="160"/>
+      <c r="AU85" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="AV85" s="9" t="s">
+        <v>106</v>
+      </c>
       <c r="AZ85" s="4"/>
       <c r="BB85" s="4"/>
       <c r="BE85" s="12"/>
@@ -8692,7 +8757,46 @@
       <c r="BY85" s="65"/>
       <c r="CA85" s="63"/>
     </row>
-    <row r="86" spans="52:83" x14ac:dyDescent="0.2">
+    <row r="86" spans="36:83" x14ac:dyDescent="0.2">
+      <c r="AJ86" s="9">
+        <v>1</v>
+      </c>
+      <c r="AK86" s="3">
+        <f>B28</f>
+        <v>525000</v>
+      </c>
+      <c r="AL86" s="3">
+        <f t="shared" ref="AL86:AP86" si="36">C28</f>
+        <v>0</v>
+      </c>
+      <c r="AM86" s="3">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="AN86" s="3">
+        <f t="shared" si="36"/>
+        <v>-525000</v>
+      </c>
+      <c r="AO86" s="3">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="AP86" s="3">
+        <f t="shared" si="36"/>
+        <v>0</v>
+      </c>
+      <c r="AR86" s="1" cm="1">
+        <f t="array" ref="AR86:AR91">MMULT(B45:G50,BB43:BB48)</f>
+        <v>0</v>
+      </c>
+      <c r="AT86" s="3">
+        <f>I20</f>
+        <v>20000</v>
+      </c>
+      <c r="AV86" s="3" cm="1">
+        <f t="array" ref="AV86:AV91">MMULT(AK86:AP91,_xlfn.ANCHORARRAY(AR86))-AT86:AT91</f>
+        <v>3333.3333333296105</v>
+      </c>
       <c r="AZ86" s="4"/>
       <c r="BB86" s="4"/>
       <c r="BE86" s="12"/>
@@ -8708,7 +8812,44 @@
       <c r="BY86" s="65"/>
       <c r="CA86" s="63"/>
     </row>
-    <row r="87" spans="52:83" x14ac:dyDescent="0.2">
+    <row r="87" spans="36:83" x14ac:dyDescent="0.2">
+      <c r="AJ87" s="9">
+        <v>2</v>
+      </c>
+      <c r="AK87" s="3">
+        <f t="shared" ref="AK87:AK91" si="37">B29</f>
+        <v>0</v>
+      </c>
+      <c r="AL87" s="3">
+        <f t="shared" ref="AL87:AL91" si="38">C29</f>
+        <v>328.125</v>
+      </c>
+      <c r="AM87" s="3">
+        <f t="shared" ref="AM87:AM91" si="39">D29</f>
+        <v>656250</v>
+      </c>
+      <c r="AN87" s="3">
+        <f t="shared" ref="AN87:AN91" si="40">E29</f>
+        <v>0</v>
+      </c>
+      <c r="AO87" s="3">
+        <f t="shared" ref="AO87:AO91" si="41">F29</f>
+        <v>-328.125</v>
+      </c>
+      <c r="AP87" s="3">
+        <f t="shared" ref="AP87:AP91" si="42">G29</f>
+        <v>656250</v>
+      </c>
+      <c r="AR87" s="1">
+        <v>0</v>
+      </c>
+      <c r="AT87" s="3">
+        <f t="shared" ref="AT87:AT91" si="43">I21</f>
+        <v>-1.22514845490862E-12</v>
+      </c>
+      <c r="AV87" s="1">
+        <v>427.7243418730103</v>
+      </c>
       <c r="AZ87" s="4"/>
       <c r="BB87" s="4"/>
       <c r="BE87" s="12"/>
@@ -8724,7 +8865,163 @@
       <c r="BY87" s="65"/>
       <c r="CA87" s="63"/>
     </row>
-    <row r="94" spans="52:83" x14ac:dyDescent="0.2">
+    <row r="88" spans="36:83" x14ac:dyDescent="0.2">
+      <c r="AJ88" s="9">
+        <v>3</v>
+      </c>
+      <c r="AK88" s="3">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="AL88" s="3">
+        <f t="shared" si="38"/>
+        <v>656250</v>
+      </c>
+      <c r="AM88" s="3">
+        <f t="shared" si="39"/>
+        <v>1750000000</v>
+      </c>
+      <c r="AN88" s="3">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+      <c r="AO88" s="3">
+        <f t="shared" si="41"/>
+        <v>-656250</v>
+      </c>
+      <c r="AP88" s="3">
+        <f t="shared" si="42"/>
+        <v>875000000</v>
+      </c>
+      <c r="AR88" s="1">
+        <v>-3.6373783993449142E-2</v>
+      </c>
+      <c r="AT88" s="3">
+        <f t="shared" si="43"/>
+        <v>-13333333.333333334</v>
+      </c>
+      <c r="AV88" s="1">
+        <v>-2.2351741790771484E-8</v>
+      </c>
+    </row>
+    <row r="89" spans="36:83" x14ac:dyDescent="0.2">
+      <c r="AJ89" s="9">
+        <v>4</v>
+      </c>
+      <c r="AK89" s="3">
+        <f t="shared" si="37"/>
+        <v>-525000</v>
+      </c>
+      <c r="AL89" s="3">
+        <f t="shared" si="38"/>
+        <v>0</v>
+      </c>
+      <c r="AM89" s="3">
+        <f t="shared" si="39"/>
+        <v>0</v>
+      </c>
+      <c r="AN89" s="3">
+        <f t="shared" si="40"/>
+        <v>525000</v>
+      </c>
+      <c r="AO89" s="3">
+        <f t="shared" si="41"/>
+        <v>0</v>
+      </c>
+      <c r="AP89" s="3">
+        <f t="shared" si="42"/>
+        <v>0</v>
+      </c>
+      <c r="AR89" s="1">
+        <v>-4.4444444444437355E-2</v>
+      </c>
+      <c r="AT89" s="3">
+        <f t="shared" si="43"/>
+        <v>20000</v>
+      </c>
+      <c r="AV89" s="1">
+        <v>-43333.33333332961</v>
+      </c>
+    </row>
+    <row r="90" spans="36:83" x14ac:dyDescent="0.2">
+      <c r="AJ90" s="9">
+        <v>5</v>
+      </c>
+      <c r="AK90" s="3">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="AL90" s="3">
+        <f t="shared" si="38"/>
+        <v>-328.125</v>
+      </c>
+      <c r="AM90" s="3">
+        <f t="shared" si="39"/>
+        <v>-656250</v>
+      </c>
+      <c r="AN90" s="3">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+      <c r="AO90" s="3">
+        <f t="shared" si="41"/>
+        <v>328.125</v>
+      </c>
+      <c r="AP90" s="3">
+        <f t="shared" si="42"/>
+        <v>-656250</v>
+      </c>
+      <c r="AR90" s="1">
+        <v>-81.935673318570522</v>
+      </c>
+      <c r="AT90" s="3">
+        <f t="shared" si="43"/>
+        <v>-1.22514845490862E-12</v>
+      </c>
+      <c r="AV90" s="1">
+        <v>-427.7243418730078</v>
+      </c>
+    </row>
+    <row r="91" spans="36:83" x14ac:dyDescent="0.2">
+      <c r="AJ91" s="9">
+        <v>6</v>
+      </c>
+      <c r="AK91" s="3">
+        <f t="shared" si="37"/>
+        <v>0</v>
+      </c>
+      <c r="AL91" s="3">
+        <f t="shared" si="38"/>
+        <v>656250</v>
+      </c>
+      <c r="AM91" s="3">
+        <f t="shared" si="39"/>
+        <v>875000000</v>
+      </c>
+      <c r="AN91" s="3">
+        <f t="shared" si="40"/>
+        <v>0</v>
+      </c>
+      <c r="AO91" s="3">
+        <f t="shared" si="41"/>
+        <v>-656250</v>
+      </c>
+      <c r="AP91" s="3">
+        <f t="shared" si="42"/>
+        <v>1750000000</v>
+      </c>
+      <c r="AR91" s="1">
+        <v>-3.9422822401248706E-3</v>
+      </c>
+      <c r="AT91" s="3">
+        <f t="shared" si="43"/>
+        <v>13333333.333333334</v>
+      </c>
+      <c r="AV91" s="1">
+        <v>1710897.3674920481</v>
+      </c>
+    </row>
+    <row r="94" spans="36:83" x14ac:dyDescent="0.2">
       <c r="BC94" s="29"/>
       <c r="BD94" s="29"/>
     </row>
@@ -10294,6 +10591,9 @@
       <c r="BF227" s="50"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="AT84:AT85"/>
+  </mergeCells>
   <conditionalFormatting sqref="AK43:AV54">
     <cfRule type="expression" dxfId="14" priority="2">
       <formula>ABS(AK43)&lt;0.1</formula>
@@ -29816,7 +30116,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A31214F-D315-442C-9106-A983B611689D}">
   <dimension ref="L14:R34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Implement axial deformation calculations with strain
</commit_message>
<xml_diff>
--- a/theory/FEM matriisit.xlsx
+++ b/theory/FEM matriisit.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ohjelmointi\2_Rust\vefem\theory\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1377142-8139-465E-AF87-9D282E5BCB9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA924C09-161D-42C5-8E06-D7DA51F3630D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25875" yWindow="0" windowWidth="25980" windowHeight="20880" xr2:uid="{27180542-B0D2-4BFE-946B-7857B24C93C8}"/>
   </bookViews>
@@ -2047,8 +2047,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94F9BDF3-3EE6-4BFB-9734-CB047BC6E804}">
   <dimension ref="B1:CW227"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AG47" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AQ79" sqref="AQ79"/>
+    <sheetView tabSelected="1" topLeftCell="AG42" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AW81" sqref="AW81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -8790,12 +8790,12 @@
         <v>0</v>
       </c>
       <c r="AT86" s="3">
-        <f>I20</f>
-        <v>20000</v>
+        <f>I28</f>
+        <v>0</v>
       </c>
       <c r="AV86" s="3" cm="1">
         <f t="array" ref="AV86:AV91">MMULT(AK86:AP91,_xlfn.ANCHORARRAY(AR86))-AT86:AT91</f>
-        <v>3333.3333333296105</v>
+        <v>23333.33333332961</v>
       </c>
       <c r="AZ86" s="4"/>
       <c r="BB86" s="4"/>
@@ -8844,11 +8844,11 @@
         <v>0</v>
       </c>
       <c r="AT87" s="3">
-        <f t="shared" ref="AT87:AT91" si="43">I21</f>
-        <v>-1.22514845490862E-12</v>
+        <f t="shared" ref="AT87:AT91" si="43">I29</f>
+        <v>-20000</v>
       </c>
       <c r="AV87" s="1">
-        <v>427.7243418730103</v>
+        <v>20427.72434187301</v>
       </c>
       <c r="AZ87" s="4"/>
       <c r="BB87" s="4"/>
@@ -8937,10 +8937,10 @@
       </c>
       <c r="AT89" s="3">
         <f t="shared" si="43"/>
-        <v>20000</v>
+        <v>0</v>
       </c>
       <c r="AV89" s="1">
-        <v>-43333.33333332961</v>
+        <v>-23333.33333332961</v>
       </c>
     </row>
     <row r="90" spans="36:83" x14ac:dyDescent="0.2">
@@ -8976,10 +8976,10 @@
       </c>
       <c r="AT90" s="3">
         <f t="shared" si="43"/>
-        <v>-1.22514845490862E-12</v>
+        <v>-20000</v>
       </c>
       <c r="AV90" s="1">
-        <v>-427.7243418730078</v>
+        <v>19572.27565812699</v>
       </c>
     </row>
     <row r="91" spans="36:83" x14ac:dyDescent="0.2">

</xml_diff>